<commit_message>
Rw Usage Updates S.1.0.0.1
Boat Enabled -
InCapacity - [0] , NodeW - [-3] , BirdW - [6] , FuelW - [19] , OnHost - [5] .

Rw- Local(Left Running With Cost ) - [For Business/Shop/Market only] -
</commit_message>
<xml_diff>
--- a/System_2.2.1.xlsx
+++ b/System_2.2.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{169B9324-107E-4572-9A06-DCEB10911A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD06CC0C-C8BB-476C-84D1-A9F06C6B65B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5018,6 +5018,159 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5036,12 +5189,6 @@
     <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5096,169 +5243,61 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5300,43 +5339,70 @@
     <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="52" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="52" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="14" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5360,112 +5426,25 @@
     <xf numFmtId="0" fontId="29" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="52" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="52" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="14" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5543,25 +5522,46 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -6894,7 +6894,7 @@
       <c r="H1" s="97" t="s">
         <v>343</v>
       </c>
-      <c r="I1" s="659" t="s">
+      <c r="I1" s="613" t="s">
         <v>369</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -6930,7 +6930,7 @@
       <c r="X1" s="430" t="s">
         <v>155</v>
       </c>
-      <c r="Y1" s="653" t="s">
+      <c r="Y1" s="657" t="s">
         <v>528</v>
       </c>
       <c r="Z1" s="406">
@@ -6955,7 +6955,7 @@
         <v>498</v>
       </c>
       <c r="AM1" s="402"/>
-      <c r="AN1" s="635"/>
+      <c r="AN1" s="640"/>
       <c r="AO1" s="338" t="s">
         <v>469</v>
       </c>
@@ -6964,23 +6964,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="617">
+      <c r="A2" s="666">
         <f ca="1">TODAY()</f>
         <v>45289</v>
       </c>
-      <c r="B2" s="619" t="s">
+      <c r="B2" s="668" t="s">
         <v>370</v>
       </c>
-      <c r="C2" s="615" t="s">
+      <c r="C2" s="645" t="s">
         <v>357</v>
       </c>
-      <c r="D2" s="621" t="s">
+      <c r="D2" s="670" t="s">
         <v>355</v>
       </c>
-      <c r="E2" s="669" t="s">
+      <c r="E2" s="609" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="640" t="s">
+      <c r="F2" s="619" t="s">
         <v>102</v>
       </c>
       <c r="G2" s="393" t="s">
@@ -6989,31 +6989,31 @@
       <c r="H2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="660"/>
+      <c r="I2" s="614"/>
       <c r="J2" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="671" t="s">
+      <c r="K2" s="611" t="s">
         <v>342</v>
       </c>
-      <c r="L2" s="672"/>
-      <c r="M2" s="640" t="s">
+      <c r="L2" s="612"/>
+      <c r="M2" s="619" t="s">
         <v>102</v>
       </c>
       <c r="N2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="644" t="s">
+      <c r="O2" s="649" t="s">
         <v>102</v>
       </c>
       <c r="P2" s="85" t="s">
         <v>147</v>
       </c>
-      <c r="Q2" s="615" t="s">
+      <c r="Q2" s="645" t="s">
         <v>143</v>
       </c>
       <c r="R2" s="598"/>
-      <c r="S2" s="657" t="s">
+      <c r="S2" s="634" t="s">
         <v>148</v>
       </c>
       <c r="T2" s="89"/>
@@ -7023,7 +7023,7 @@
       <c r="X2" s="431" t="s">
         <v>156</v>
       </c>
-      <c r="Y2" s="654"/>
+      <c r="Y2" s="658"/>
       <c r="Z2" s="407">
         <v>1</v>
       </c>
@@ -7046,15 +7046,15 @@
         <v>463</v>
       </c>
       <c r="AM2" s="428"/>
-      <c r="AN2" s="636"/>
+      <c r="AN2" s="641"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="618"/>
-      <c r="B3" s="620"/>
-      <c r="C3" s="616"/>
-      <c r="D3" s="622"/>
-      <c r="E3" s="670"/>
-      <c r="F3" s="641"/>
+      <c r="A3" s="667"/>
+      <c r="B3" s="669"/>
+      <c r="C3" s="646"/>
+      <c r="D3" s="671"/>
+      <c r="E3" s="610"/>
+      <c r="F3" s="620"/>
       <c r="G3" s="394" t="s">
         <v>28</v>
       </c>
@@ -7073,17 +7073,17 @@
       <c r="L3" s="201" t="s">
         <v>107</v>
       </c>
-      <c r="M3" s="641"/>
+      <c r="M3" s="620"/>
       <c r="N3" s="69" t="s">
         <v>146</v>
       </c>
-      <c r="O3" s="645"/>
+      <c r="O3" s="650"/>
       <c r="P3" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="Q3" s="616"/>
+      <c r="Q3" s="646"/>
       <c r="R3" s="600"/>
-      <c r="S3" s="658"/>
+      <c r="S3" s="636"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -7091,7 +7091,7 @@
       <c r="X3" s="431" t="s">
         <v>157</v>
       </c>
-      <c r="Y3" s="654"/>
+      <c r="Y3" s="658"/>
       <c r="Z3" s="408">
         <v>1</v>
       </c>
@@ -7100,7 +7100,7 @@
       <c r="AC3" s="100" t="s">
         <v>480</v>
       </c>
-      <c r="AD3" s="656" t="s">
+      <c r="AD3" s="631" t="s">
         <v>455</v>
       </c>
       <c r="AE3" s="257"/>
@@ -7112,16 +7112,16 @@
       <c r="AK3" s="257"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="428"/>
-      <c r="AN3" s="636"/>
+      <c r="AN3" s="641"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="238" t="s">
         <v>183</v>
       </c>
-      <c r="B4" s="633" t="s">
+      <c r="B4" s="682" t="s">
         <v>373</v>
       </c>
-      <c r="C4" s="615" t="s">
+      <c r="C4" s="645" t="s">
         <v>154</v>
       </c>
       <c r="D4" s="347" t="s">
@@ -7130,7 +7130,7 @@
       <c r="E4" s="378">
         <v>2</v>
       </c>
-      <c r="F4" s="641"/>
+      <c r="F4" s="620"/>
       <c r="G4" s="381" t="s">
         <v>201</v>
       </c>
@@ -7147,11 +7147,11 @@
         <v>150</v>
       </c>
       <c r="L4" s="204"/>
-      <c r="M4" s="641"/>
+      <c r="M4" s="620"/>
       <c r="N4" s="174" t="s">
         <v>69</v>
       </c>
-      <c r="O4" s="645"/>
+      <c r="O4" s="650"/>
       <c r="P4" s="2" t="s">
         <v>191</v>
       </c>
@@ -7173,12 +7173,12 @@
       <c r="X4" s="431" t="s">
         <v>158</v>
       </c>
-      <c r="Y4" s="654"/>
+      <c r="Y4" s="658"/>
       <c r="Z4" s="409"/>
       <c r="AA4" s="307"/>
       <c r="AB4" s="209"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="656"/>
+      <c r="AD4" s="631"/>
       <c r="AE4" s="257"/>
       <c r="AF4" s="257"/>
       <c r="AG4" s="16"/>
@@ -7188,37 +7188,37 @@
       <c r="AK4" s="257"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="428"/>
-      <c r="AN4" s="636"/>
+      <c r="AN4" s="641"/>
       <c r="AO4" s="338" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="659" t="s">
+      <c r="A5" s="613" t="s">
         <v>418</v>
       </c>
-      <c r="B5" s="634"/>
-      <c r="C5" s="616"/>
+      <c r="B5" s="683"/>
+      <c r="C5" s="646"/>
       <c r="D5" s="61" t="s">
         <v>153</v>
       </c>
       <c r="E5" s="379">
         <v>1</v>
       </c>
-      <c r="F5" s="641"/>
-      <c r="G5" s="625" t="s">
+      <c r="F5" s="620"/>
+      <c r="G5" s="674" t="s">
         <v>192</v>
       </c>
-      <c r="H5" s="625"/>
-      <c r="I5" s="625"/>
-      <c r="J5" s="625"/>
-      <c r="K5" s="625"/>
-      <c r="L5" s="626"/>
-      <c r="M5" s="641"/>
+      <c r="H5" s="674"/>
+      <c r="I5" s="674"/>
+      <c r="J5" s="674"/>
+      <c r="K5" s="674"/>
+      <c r="L5" s="675"/>
+      <c r="M5" s="620"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
-      <c r="O5" s="645"/>
+      <c r="O5" s="650"/>
       <c r="T5" s="89"/>
       <c r="U5" s="124"/>
       <c r="V5" s="120"/>
@@ -7226,7 +7226,7 @@
       <c r="X5" s="431" t="s">
         <v>159</v>
       </c>
-      <c r="Y5" s="654"/>
+      <c r="Y5" s="658"/>
       <c r="Z5" s="409">
         <v>1</v>
       </c>
@@ -7249,24 +7249,24 @@
       <c r="AK5" s="257"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="428"/>
-      <c r="AN5" s="636"/>
+      <c r="AN5" s="641"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="660"/>
-      <c r="B6" s="631" t="s">
+      <c r="A6" s="614"/>
+      <c r="B6" s="680" t="s">
         <v>177</v>
       </c>
-      <c r="C6" s="661"/>
-      <c r="D6" s="662"/>
-      <c r="F6" s="641"/>
-      <c r="G6" s="627"/>
-      <c r="H6" s="627"/>
-      <c r="I6" s="627"/>
-      <c r="J6" s="627"/>
-      <c r="K6" s="627"/>
-      <c r="L6" s="628"/>
-      <c r="M6" s="641"/>
-      <c r="O6" s="645"/>
+      <c r="C6" s="628"/>
+      <c r="D6" s="629"/>
+      <c r="F6" s="620"/>
+      <c r="G6" s="676"/>
+      <c r="H6" s="676"/>
+      <c r="I6" s="676"/>
+      <c r="J6" s="676"/>
+      <c r="K6" s="676"/>
+      <c r="L6" s="677"/>
+      <c r="M6" s="620"/>
+      <c r="O6" s="650"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
       <c r="V6" s="98" t="s">
@@ -7276,7 +7276,7 @@
       <c r="X6" s="431" t="s">
         <v>160</v>
       </c>
-      <c r="Y6" s="654"/>
+      <c r="Y6" s="658"/>
       <c r="Z6" s="407">
         <v>1</v>
       </c>
@@ -7290,16 +7290,16 @@
       <c r="AF6" s="257"/>
       <c r="AG6" s="257"/>
       <c r="AH6" s="257"/>
-      <c r="AI6" s="650"/>
+      <c r="AI6" s="630"/>
       <c r="AJ6" s="441" t="s">
         <v>458</v>
       </c>
-      <c r="AK6" s="650" t="s">
+      <c r="AK6" s="630" t="s">
         <v>251</v>
       </c>
       <c r="AL6" s="257"/>
       <c r="AM6" s="428"/>
-      <c r="AN6" s="636"/>
+      <c r="AN6" s="641"/>
       <c r="AO6" s="338" t="s">
         <v>470</v>
       </c>
@@ -7308,7 +7308,7 @@
       <c r="A7" s="232" t="s">
         <v>571</v>
       </c>
-      <c r="B7" s="632"/>
+      <c r="B7" s="681"/>
       <c r="C7" s="202" t="s">
         <v>374</v>
       </c>
@@ -7318,7 +7318,7 @@
       <c r="E7" s="265">
         <v>3</v>
       </c>
-      <c r="F7" s="641"/>
+      <c r="F7" s="620"/>
       <c r="G7" s="395">
         <v>0</v>
       </c>
@@ -7337,8 +7337,8 @@
       <c r="L7" s="212">
         <v>0</v>
       </c>
-      <c r="M7" s="641"/>
-      <c r="O7" s="645"/>
+      <c r="M7" s="620"/>
+      <c r="O7" s="650"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
       </c>
@@ -7352,7 +7352,7 @@
       <c r="X7" s="431" t="s">
         <v>161</v>
       </c>
-      <c r="Y7" s="654"/>
+      <c r="Y7" s="658"/>
       <c r="Z7" s="407">
         <v>1</v>
       </c>
@@ -7362,18 +7362,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="257"/>
       <c r="AF7" s="257"/>
-      <c r="AG7" s="656" t="s">
+      <c r="AG7" s="631" t="s">
         <v>454</v>
       </c>
       <c r="AH7" s="257"/>
-      <c r="AI7" s="650"/>
+      <c r="AI7" s="630"/>
       <c r="AJ7" s="257"/>
-      <c r="AK7" s="650"/>
+      <c r="AK7" s="630"/>
       <c r="AL7" s="80" t="s">
         <v>496</v>
       </c>
       <c r="AM7" s="428"/>
-      <c r="AN7" s="636"/>
+      <c r="AN7" s="641"/>
       <c r="AP7" s="76" t="s">
         <v>471</v>
       </c>
@@ -7390,27 +7390,27 @@
         <f>SUM(G7:N9)</f>
         <v>15</v>
       </c>
-      <c r="F8" s="641"/>
-      <c r="G8" s="626">
-        <v>0</v>
-      </c>
-      <c r="H8" s="623" t="s">
+      <c r="F8" s="620"/>
+      <c r="G8" s="675">
+        <v>0</v>
+      </c>
+      <c r="H8" s="672" t="s">
         <v>104</v>
       </c>
       <c r="I8" s="598">
         <v>0</v>
       </c>
-      <c r="J8" s="623" t="s">
+      <c r="J8" s="672" t="s">
         <v>104</v>
       </c>
-      <c r="K8" s="629"/>
-      <c r="L8" s="663"/>
-      <c r="M8" s="642"/>
-      <c r="N8" s="666">
+      <c r="K8" s="678"/>
+      <c r="L8" s="632"/>
+      <c r="M8" s="647"/>
+      <c r="N8" s="637">
         <f>N5+N11</f>
         <v>15</v>
       </c>
-      <c r="O8" s="645"/>
+      <c r="O8" s="650"/>
       <c r="T8" s="103" t="s">
         <v>44</v>
       </c>
@@ -7420,7 +7420,7 @@
       <c r="X8" s="431" t="s">
         <v>162</v>
       </c>
-      <c r="Y8" s="654"/>
+      <c r="Y8" s="658"/>
       <c r="Z8" s="409"/>
       <c r="AA8" s="307"/>
       <c r="AB8" s="209"/>
@@ -7428,14 +7428,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="257"/>
       <c r="AF8" s="257"/>
-      <c r="AG8" s="656"/>
+      <c r="AG8" s="631"/>
       <c r="AH8" s="257"/>
-      <c r="AI8" s="650"/>
+      <c r="AI8" s="630"/>
       <c r="AJ8" s="257"/>
       <c r="AK8" s="257"/>
       <c r="AL8" s="257"/>
       <c r="AM8" s="428"/>
-      <c r="AN8" s="636"/>
+      <c r="AN8" s="641"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="232" t="s">
@@ -7450,17 +7450,17 @@
       <c r="D9" s="348" t="s">
         <v>281</v>
       </c>
-      <c r="F9" s="641"/>
-      <c r="G9" s="628"/>
-      <c r="H9" s="624"/>
+      <c r="F9" s="620"/>
+      <c r="G9" s="677"/>
+      <c r="H9" s="673"/>
       <c r="I9" s="600"/>
-      <c r="J9" s="624"/>
-      <c r="K9" s="630"/>
-      <c r="L9" s="664"/>
-      <c r="M9" s="643"/>
-      <c r="N9" s="667"/>
-      <c r="O9" s="646"/>
-      <c r="S9" s="657" t="s">
+      <c r="J9" s="673"/>
+      <c r="K9" s="679"/>
+      <c r="L9" s="633"/>
+      <c r="M9" s="648"/>
+      <c r="N9" s="638"/>
+      <c r="O9" s="651"/>
+      <c r="S9" s="634" t="s">
         <v>61</v>
       </c>
       <c r="T9" s="89"/>
@@ -7472,7 +7472,7 @@
       <c r="X9" s="431" t="s">
         <v>163</v>
       </c>
-      <c r="Y9" s="654"/>
+      <c r="Y9" s="658"/>
       <c r="Z9" s="410"/>
       <c r="AA9" s="307"/>
       <c r="AB9" s="209"/>
@@ -7482,16 +7482,16 @@
       </c>
       <c r="AE9" s="257"/>
       <c r="AF9" s="257"/>
-      <c r="AG9" s="656"/>
+      <c r="AG9" s="631"/>
       <c r="AH9" s="257"/>
-      <c r="AI9" s="650"/>
+      <c r="AI9" s="630"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="650" t="s">
+      <c r="AK9" s="630" t="s">
         <v>251</v>
       </c>
       <c r="AL9" s="257"/>
       <c r="AM9" s="428"/>
-      <c r="AN9" s="636"/>
+      <c r="AN9" s="641"/>
       <c r="AP9" s="2" t="s">
         <v>508</v>
       </c>
@@ -7508,20 +7508,20 @@
         <f>Boat!W8</f>
         <v>37</v>
       </c>
-      <c r="F10" s="641"/>
+      <c r="F10" s="620"/>
       <c r="N10" s="418" t="s">
         <v>396</v>
       </c>
-      <c r="O10" s="678" t="s">
+      <c r="O10" s="622" t="s">
         <v>102</v>
       </c>
-      <c r="P10" s="647" t="s">
+      <c r="P10" s="652" t="s">
         <v>400</v>
       </c>
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="665"/>
+      <c r="S10" s="635"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>176</v>
@@ -7533,7 +7533,7 @@
       <c r="X10" s="431" t="s">
         <v>164</v>
       </c>
-      <c r="Y10" s="654"/>
+      <c r="Y10" s="658"/>
       <c r="Z10" s="409">
         <v>0</v>
       </c>
@@ -7551,16 +7551,16 @@
       <c r="AF10" s="238" t="s">
         <v>311</v>
       </c>
-      <c r="AG10" s="656"/>
+      <c r="AG10" s="631"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="650"/>
+      <c r="AI10" s="630"/>
       <c r="AJ10" s="257"/>
-      <c r="AK10" s="650"/>
+      <c r="AK10" s="630"/>
       <c r="AL10" s="257"/>
       <c r="AM10" s="442" t="s">
         <v>318</v>
       </c>
-      <c r="AN10" s="636"/>
+      <c r="AN10" s="641"/>
       <c r="AO10" s="204" t="s">
         <v>94</v>
       </c>
@@ -7578,18 +7578,18 @@
       <c r="D11" s="170" t="s">
         <v>355</v>
       </c>
-      <c r="F11" s="641"/>
+      <c r="F11" s="620"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="679"/>
-      <c r="P11" s="648"/>
+      <c r="O11" s="623"/>
+      <c r="P11" s="653"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>220</v>
       </c>
-      <c r="S11" s="665"/>
+      <c r="S11" s="635"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -7599,7 +7599,7 @@
       <c r="X11" s="431" t="s">
         <v>165</v>
       </c>
-      <c r="Y11" s="654"/>
+      <c r="Y11" s="658"/>
       <c r="Z11" s="409"/>
       <c r="AA11" s="307">
         <v>1</v>
@@ -7613,14 +7613,14 @@
       <c r="AF11" s="257" t="s">
         <v>476</v>
       </c>
-      <c r="AG11" s="656"/>
+      <c r="AG11" s="631"/>
       <c r="AH11" s="257"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="257"/>
       <c r="AK11" s="257"/>
       <c r="AL11" s="257"/>
       <c r="AM11" s="428"/>
-      <c r="AN11" s="636"/>
+      <c r="AN11" s="641"/>
       <c r="AP11" s="76" t="s">
         <v>484</v>
       </c>
@@ -7639,7 +7639,7 @@
       <c r="E12" s="224">
         <v>3</v>
       </c>
-      <c r="F12" s="641"/>
+      <c r="F12" s="620"/>
       <c r="G12" s="337" t="s">
         <v>400</v>
       </c>
@@ -7648,16 +7648,16 @@
       </c>
       <c r="I12" s="605"/>
       <c r="J12" s="605"/>
-      <c r="K12" s="683"/>
+      <c r="K12" s="627"/>
       <c r="L12" s="203"/>
       <c r="M12" s="203"/>
       <c r="N12" s="203"/>
-      <c r="O12" s="679"/>
-      <c r="P12" s="648"/>
+      <c r="O12" s="623"/>
+      <c r="P12" s="653"/>
       <c r="R12" s="122" t="s">
         <v>180</v>
       </c>
-      <c r="S12" s="658"/>
+      <c r="S12" s="636"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -7667,7 +7667,7 @@
       <c r="X12" s="431" t="s">
         <v>166</v>
       </c>
-      <c r="Y12" s="654"/>
+      <c r="Y12" s="658"/>
       <c r="Z12" s="407">
         <v>1</v>
       </c>
@@ -7678,16 +7678,16 @@
       <c r="AC12" s="100" t="s">
         <v>481</v>
       </c>
-      <c r="AD12" s="668" t="s">
+      <c r="AD12" s="639" t="s">
         <v>240</v>
       </c>
       <c r="AE12" s="441" t="s">
         <v>239</v>
       </c>
-      <c r="AF12" s="656" t="s">
+      <c r="AF12" s="631" t="s">
         <v>228</v>
       </c>
-      <c r="AG12" s="656"/>
+      <c r="AG12" s="631"/>
       <c r="AH12" s="238" t="s">
         <v>259</v>
       </c>
@@ -7697,10 +7697,10 @@
       <c r="AJ12" s="257"/>
       <c r="AK12" s="257"/>
       <c r="AL12" s="257"/>
-      <c r="AM12" s="651" t="s">
+      <c r="AM12" s="655" t="s">
         <v>249</v>
       </c>
-      <c r="AN12" s="636"/>
+      <c r="AN12" s="641"/>
       <c r="AO12" s="338" t="s">
         <v>96</v>
       </c>
@@ -7712,17 +7712,17 @@
       <c r="E13" s="448">
         <v>-3</v>
       </c>
-      <c r="F13" s="641"/>
+      <c r="F13" s="620"/>
       <c r="G13" s="605" t="s">
         <v>430</v>
       </c>
       <c r="H13" s="605"/>
       <c r="I13" s="605"/>
-      <c r="J13" s="683"/>
+      <c r="J13" s="627"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="679"/>
-      <c r="P13" s="649"/>
+      <c r="O13" s="623"/>
+      <c r="P13" s="654"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
       </c>
@@ -7732,7 +7732,7 @@
       <c r="X13" s="431" t="s">
         <v>167</v>
       </c>
-      <c r="Y13" s="654"/>
+      <c r="Y13" s="658"/>
       <c r="Z13" s="407">
         <v>1</v>
       </c>
@@ -7743,8 +7743,8 @@
         <v>500</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="668"/>
-      <c r="AF13" s="656"/>
+      <c r="AD13" s="639"/>
+      <c r="AF13" s="631"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="238" t="s">
         <v>308</v>
@@ -7755,8 +7755,8 @@
       <c r="AJ13" s="80"/>
       <c r="AK13" s="257"/>
       <c r="AL13" s="257"/>
-      <c r="AM13" s="651"/>
-      <c r="AN13" s="636"/>
+      <c r="AM13" s="655"/>
+      <c r="AN13" s="641"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="450"/>
@@ -7764,18 +7764,18 @@
       <c r="C14" s="459"/>
       <c r="D14" s="452"/>
       <c r="E14" s="453"/>
-      <c r="F14" s="641"/>
+      <c r="F14" s="620"/>
       <c r="G14" s="605" t="s">
         <v>429</v>
       </c>
       <c r="H14" s="605"/>
       <c r="I14" s="605"/>
-      <c r="J14" s="683"/>
+      <c r="J14" s="627"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="679"/>
+      <c r="O14" s="623"/>
       <c r="Q14" s="61" t="s">
         <v>532</v>
       </c>
@@ -7789,24 +7789,24 @@
       <c r="X14" s="431" t="s">
         <v>168</v>
       </c>
-      <c r="Y14" s="654"/>
+      <c r="Y14" s="658"/>
       <c r="Z14" s="407">
         <v>1</v>
       </c>
       <c r="AA14" s="307"/>
       <c r="AB14" s="209"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="668"/>
+      <c r="AD14" s="639"/>
       <c r="AE14" s="257"/>
-      <c r="AF14" s="656"/>
+      <c r="AF14" s="631"/>
       <c r="AG14" s="257"/>
       <c r="AH14" s="257"/>
       <c r="AI14" s="70"/>
       <c r="AJ14" s="257"/>
       <c r="AK14" s="257"/>
       <c r="AL14" s="257"/>
-      <c r="AM14" s="651"/>
-      <c r="AN14" s="636"/>
+      <c r="AM14" s="655"/>
+      <c r="AN14" s="641"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="449" t="s">
@@ -7815,8 +7815,8 @@
       <c r="C15" s="598" t="s">
         <v>373</v>
       </c>
-      <c r="F15" s="641"/>
-      <c r="O15" s="679"/>
+      <c r="F15" s="620"/>
+      <c r="O15" s="623"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -7829,7 +7829,7 @@
       <c r="X15" s="431" t="s">
         <v>169</v>
       </c>
-      <c r="Y15" s="654"/>
+      <c r="Y15" s="658"/>
       <c r="Z15" s="409">
         <v>1</v>
       </c>
@@ -7838,8 +7838,8 @@
       <c r="AC15" s="76" t="s">
         <v>479</v>
       </c>
-      <c r="AD15" s="668"/>
-      <c r="AF15" s="656"/>
+      <c r="AD15" s="639"/>
+      <c r="AF15" s="631"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="238" t="s">
         <v>448</v>
@@ -7852,8 +7852,8 @@
       </c>
       <c r="AK15" s="257"/>
       <c r="AL15" s="257"/>
-      <c r="AM15" s="651"/>
-      <c r="AN15" s="636"/>
+      <c r="AM15" s="655"/>
+      <c r="AN15" s="641"/>
       <c r="AP15" s="76" t="s">
         <v>73</v>
       </c>
@@ -7875,13 +7875,13 @@
       <c r="E16" s="224">
         <v>1</v>
       </c>
-      <c r="F16" s="641"/>
+      <c r="F16" s="620"/>
       <c r="G16" s="337" t="s">
         <v>488</v>
       </c>
       <c r="I16" s="469"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="679"/>
+      <c r="O16" s="623"/>
       <c r="R16" s="435" t="s">
         <v>184</v>
       </c>
@@ -7892,7 +7892,7 @@
       <c r="X16" s="431" t="s">
         <v>170</v>
       </c>
-      <c r="Y16" s="654"/>
+      <c r="Y16" s="658"/>
       <c r="Z16" s="407">
         <v>1</v>
       </c>
@@ -7913,18 +7913,18 @@
       <c r="AM16" s="428" t="s">
         <v>317</v>
       </c>
-      <c r="AN16" s="636"/>
+      <c r="AN16" s="641"/>
       <c r="AP16" s="76" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="641"/>
+      <c r="F17" s="620"/>
       <c r="I17" s="470"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="679"/>
+      <c r="O17" s="623"/>
       <c r="Q17" s="21" t="s">
         <v>530</v>
       </c>
@@ -7944,7 +7944,7 @@
       <c r="X17" s="431" t="s">
         <v>171</v>
       </c>
-      <c r="Y17" s="654"/>
+      <c r="Y17" s="658"/>
       <c r="Z17" s="409"/>
       <c r="AA17" s="307"/>
       <c r="AB17" s="209"/>
@@ -7969,7 +7969,7 @@
       <c r="AK17" s="257"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="428"/>
-      <c r="AN17" s="636"/>
+      <c r="AN17" s="641"/>
       <c r="AO17" s="204" t="s">
         <v>497</v>
       </c>
@@ -7993,21 +7993,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="641"/>
+      <c r="F18" s="620"/>
       <c r="G18" s="337" t="s">
         <v>527</v>
       </c>
       <c r="I18" s="24"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="679"/>
+      <c r="O18" s="623"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="673" t="s">
+      <c r="R18" s="615" t="s">
         <v>535</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="612" t="s">
+      <c r="U18" s="663" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -8017,7 +8017,7 @@
       <c r="X18" s="431" t="s">
         <v>172</v>
       </c>
-      <c r="Y18" s="654"/>
+      <c r="Y18" s="658"/>
       <c r="Z18" s="409">
         <v>1</v>
       </c>
@@ -8028,38 +8028,38 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="257"/>
-      <c r="AF18" s="650" t="s">
+      <c r="AF18" s="630" t="s">
         <v>475</v>
       </c>
       <c r="AG18" s="257"/>
       <c r="AH18" s="70"/>
       <c r="AI18" s="70"/>
-      <c r="AJ18" s="652" t="s">
+      <c r="AJ18" s="656" t="s">
         <v>315</v>
       </c>
       <c r="AK18" s="257"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="428"/>
-      <c r="AN18" s="636"/>
+      <c r="AN18" s="641"/>
       <c r="AP18" s="76" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="641"/>
+      <c r="F19" s="620"/>
       <c r="I19" s="219"/>
-      <c r="O19" s="679"/>
-      <c r="R19" s="674"/>
+      <c r="O19" s="623"/>
+      <c r="R19" s="616"/>
       <c r="S19" s="30" t="s">
         <v>533</v>
       </c>
-      <c r="U19" s="613"/>
+      <c r="U19" s="664"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="431" t="s">
         <v>173</v>
       </c>
-      <c r="Y19" s="654"/>
+      <c r="Y19" s="658"/>
       <c r="Z19" s="407">
         <v>1</v>
       </c>
@@ -8068,17 +8068,17 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="257"/>
-      <c r="AF19" s="650"/>
+      <c r="AF19" s="630"/>
       <c r="AG19" s="257"/>
       <c r="AH19" s="257"/>
       <c r="AI19" s="70"/>
-      <c r="AJ19" s="652"/>
+      <c r="AJ19" s="656"/>
       <c r="AK19" s="460" t="s">
         <v>251</v>
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="428"/>
-      <c r="AN19" s="636"/>
+      <c r="AN19" s="641"/>
       <c r="AP19" s="76" t="s">
         <v>468</v>
       </c>
@@ -8099,24 +8099,24 @@
       <c r="E20" s="437">
         <v>-1</v>
       </c>
-      <c r="F20" s="641"/>
+      <c r="F20" s="620"/>
       <c r="G20" s="337" t="s">
         <v>491</v>
       </c>
       <c r="I20" s="219"/>
-      <c r="O20" s="679"/>
-      <c r="Q20" s="681" t="s">
+      <c r="O20" s="623"/>
+      <c r="Q20" s="625" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="404" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="614"/>
+      <c r="U20" s="665"/>
       <c r="W20" s="405"/>
       <c r="X20" s="432" t="s">
         <v>174</v>
       </c>
-      <c r="Y20" s="654"/>
+      <c r="Y20" s="658"/>
       <c r="Z20" s="411">
         <v>1</v>
       </c>
@@ -8141,7 +8141,7 @@
       <c r="AM20" s="381" t="s">
         <v>249</v>
       </c>
-      <c r="AN20" s="636"/>
+      <c r="AN20" s="641"/>
       <c r="AO20" s="338" t="s">
         <v>460</v>
       </c>
@@ -8162,20 +8162,20 @@
       <c r="E21" s="265">
         <v>0</v>
       </c>
-      <c r="F21" s="641"/>
+      <c r="F21" s="620"/>
       <c r="I21" s="219"/>
-      <c r="O21" s="679"/>
-      <c r="Q21" s="682"/>
+      <c r="O21" s="623"/>
+      <c r="Q21" s="626"/>
       <c r="T21" s="422"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="609"/>
+      <c r="V21" s="660"/>
       <c r="W21" s="426" t="s">
         <v>175</v>
       </c>
       <c r="X21" s="429" t="s">
         <v>186</v>
       </c>
-      <c r="Y21" s="654"/>
+      <c r="Y21" s="658"/>
       <c r="Z21" s="445">
         <v>3</v>
       </c>
@@ -8206,15 +8206,15 @@
       <c r="AM21" s="428" t="s">
         <v>544</v>
       </c>
-      <c r="AN21" s="636"/>
+      <c r="AN21" s="641"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="641"/>
+      <c r="F22" s="620"/>
       <c r="G22" s="337" t="s">
         <v>489</v>
       </c>
       <c r="I22" s="219"/>
-      <c r="O22" s="679"/>
+      <c r="O22" s="623"/>
       <c r="R22" s="434" t="s">
         <v>44</v>
       </c>
@@ -8222,14 +8222,14 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="610"/>
+      <c r="V22" s="661"/>
       <c r="W22" s="426" t="s">
         <v>175</v>
       </c>
       <c r="X22" s="429" t="s">
         <v>187</v>
       </c>
-      <c r="Y22" s="654"/>
+      <c r="Y22" s="658"/>
       <c r="Z22" s="415"/>
       <c r="AA22" s="10"/>
       <c r="AB22" s="415"/>
@@ -8240,7 +8240,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="650" t="s">
+      <c r="AJ22" s="630" t="s">
         <v>472</v>
       </c>
       <c r="AK22" s="257"/>
@@ -8248,7 +8248,7 @@
         <v>478</v>
       </c>
       <c r="AM22" s="300"/>
-      <c r="AN22" s="636"/>
+      <c r="AN22" s="641"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="231" t="s">
@@ -8266,22 +8266,22 @@
       <c r="E23" s="225">
         <v>1</v>
       </c>
-      <c r="F23" s="641"/>
+      <c r="F23" s="620"/>
       <c r="I23" s="219"/>
-      <c r="O23" s="679"/>
-      <c r="Q23" s="681" t="s">
+      <c r="O23" s="623"/>
+      <c r="Q23" s="625" t="s">
         <v>144</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="420" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="610"/>
+      <c r="V23" s="661"/>
       <c r="W23" s="148"/>
       <c r="X23" s="429" t="s">
         <v>188</v>
       </c>
-      <c r="Y23" s="654"/>
+      <c r="Y23" s="658"/>
       <c r="Z23" s="17"/>
       <c r="AA23" s="10"/>
       <c r="AB23" s="415"/>
@@ -8292,13 +8292,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="650"/>
+      <c r="AJ23" s="630"/>
       <c r="AK23" s="257"/>
       <c r="AL23" s="80" t="s">
         <v>507</v>
       </c>
       <c r="AM23" s="300"/>
-      <c r="AN23" s="636"/>
+      <c r="AN23" s="641"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="440" t="s">
@@ -8316,23 +8316,23 @@
       <c r="E24" s="436">
         <v>1</v>
       </c>
-      <c r="F24" s="641"/>
+      <c r="F24" s="620"/>
       <c r="G24" s="61" t="s">
         <v>490</v>
       </c>
       <c r="I24" s="219"/>
-      <c r="O24" s="679"/>
-      <c r="Q24" s="682"/>
+      <c r="O24" s="623"/>
+      <c r="Q24" s="626"/>
       <c r="T24" s="17"/>
       <c r="U24" s="227" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="610"/>
+      <c r="V24" s="661"/>
       <c r="W24" s="148"/>
       <c r="X24" s="429" t="s">
         <v>185</v>
       </c>
-      <c r="Y24" s="654"/>
+      <c r="Y24" s="658"/>
       <c r="Z24" s="17"/>
       <c r="AA24" s="10"/>
       <c r="AB24" s="415"/>
@@ -8351,12 +8351,12 @@
         <v>463</v>
       </c>
       <c r="AM24" s="300"/>
-      <c r="AN24" s="636"/>
+      <c r="AN24" s="641"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="641"/>
+      <c r="F25" s="620"/>
       <c r="I25" s="219"/>
-      <c r="O25" s="679"/>
+      <c r="O25" s="623"/>
       <c r="P25" s="204" t="s">
         <v>280</v>
       </c>
@@ -8369,12 +8369,12 @@
       <c r="U25" s="400" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="611"/>
+      <c r="V25" s="662"/>
       <c r="W25" s="148"/>
       <c r="X25" s="429" t="s">
         <v>189</v>
       </c>
-      <c r="Y25" s="654"/>
+      <c r="Y25" s="658"/>
       <c r="Z25" s="17"/>
       <c r="AA25" s="10"/>
       <c r="AB25" s="415"/>
@@ -8391,7 +8391,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="300"/>
-      <c r="AN25" s="636"/>
+      <c r="AN25" s="641"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="231" t="s">
@@ -8409,17 +8409,17 @@
       <c r="E26" s="380">
         <v>1</v>
       </c>
-      <c r="F26" s="641"/>
+      <c r="F26" s="620"/>
       <c r="G26" s="337" t="s">
         <v>487</v>
       </c>
       <c r="I26" s="219"/>
-      <c r="O26" s="679"/>
-      <c r="P26" s="638" t="s">
+      <c r="O26" s="623"/>
+      <c r="P26" s="643" t="s">
         <v>525</v>
       </c>
-      <c r="Q26" s="639"/>
-      <c r="R26" s="675" t="s">
+      <c r="Q26" s="644"/>
+      <c r="R26" s="617" t="s">
         <v>534</v>
       </c>
       <c r="T26" s="178"/>
@@ -8431,7 +8431,7 @@
       <c r="X26" s="429" t="s">
         <v>181</v>
       </c>
-      <c r="Y26" s="654"/>
+      <c r="Y26" s="658"/>
       <c r="Z26" s="17"/>
       <c r="AA26" s="10"/>
       <c r="AB26" s="415"/>
@@ -8458,7 +8458,7 @@
       <c r="AM26" s="442" t="s">
         <v>456</v>
       </c>
-      <c r="AN26" s="636"/>
+      <c r="AN26" s="641"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -8470,13 +8470,13 @@
       <c r="E27" s="265" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="677"/>
+      <c r="F27" s="621"/>
       <c r="G27" s="61" t="s">
         <v>543</v>
       </c>
       <c r="I27" s="220"/>
-      <c r="O27" s="680"/>
-      <c r="R27" s="676"/>
+      <c r="O27" s="624"/>
+      <c r="R27" s="618"/>
       <c r="S27" s="421" t="s">
         <v>54</v>
       </c>
@@ -8489,7 +8489,7 @@
       <c r="X27" s="429" t="s">
         <v>529</v>
       </c>
-      <c r="Y27" s="655"/>
+      <c r="Y27" s="659"/>
       <c r="Z27" s="161"/>
       <c r="AA27" s="13"/>
       <c r="AB27" s="416"/>
@@ -8506,32 +8506,26 @@
       <c r="AM27" s="381" t="s">
         <v>319</v>
       </c>
-      <c r="AN27" s="637"/>
+      <c r="AN27" s="642"/>
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="F2:F27"/>
-    <mergeCell ref="O10:O27"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AI6:AI10"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AG7:AG12"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="V21:V25"/>
+    <mergeCell ref="U18:U20"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="G5:L6"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B4:B5"/>
     <mergeCell ref="AN1:AN27"/>
     <mergeCell ref="P26:Q26"/>
     <mergeCell ref="Q2:Q3"/>
@@ -8548,22 +8542,28 @@
     <mergeCell ref="AD3:AD4"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="R2:R3"/>
-    <mergeCell ref="V21:V25"/>
-    <mergeCell ref="U18:U20"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="G5:L6"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="AI6:AI10"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AG7:AG12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="O10:O27"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8600,12 +8600,12 @@
       <c r="B1" s="603" t="s">
         <v>310</v>
       </c>
-      <c r="C1" s="683"/>
+      <c r="C1" s="627"/>
       <c r="D1" s="204"/>
       <c r="J1" s="603" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="683"/>
+      <c r="K1" s="627"/>
       <c r="L1" s="195" t="s">
         <v>330</v>
       </c>
@@ -9008,7 +9008,7 @@
       <c r="P1" s="398" t="s">
         <v>397</v>
       </c>
-      <c r="Q1" s="714" t="s">
+      <c r="Q1" s="701" t="s">
         <v>180</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -9032,7 +9032,7 @@
       <c r="AA1" s="517" t="s">
         <v>437</v>
       </c>
-      <c r="AB1" s="708" t="s">
+      <c r="AB1" s="695" t="s">
         <v>593</v>
       </c>
       <c r="AC1" s="99" t="s">
@@ -9054,32 +9054,32 @@
       </c>
     </row>
     <row r="2" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="693">
+      <c r="A2" s="706">
         <f ca="1">TODAY()</f>
         <v>45289</v>
       </c>
-      <c r="B2" s="695" t="s">
+      <c r="B2" s="708" t="s">
         <v>379</v>
       </c>
-      <c r="C2" s="615" t="s">
+      <c r="C2" s="645" t="s">
         <v>357</v>
       </c>
-      <c r="D2" s="697" t="s">
+      <c r="D2" s="710" t="s">
         <v>102</v>
       </c>
-      <c r="E2" s="699" t="s">
+      <c r="E2" s="712" t="s">
         <v>64</v>
       </c>
       <c r="F2" s="191" t="s">
         <v>218</v>
       </c>
-      <c r="G2" s="659" t="s">
+      <c r="G2" s="613" t="s">
         <v>372</v>
       </c>
       <c r="H2" s="206" t="s">
         <v>218</v>
       </c>
-      <c r="I2" s="705" t="s">
+      <c r="I2" s="692" t="s">
         <v>102</v>
       </c>
       <c r="J2" s="396" t="s">
@@ -9103,7 +9103,7 @@
       <c r="P2" s="399">
         <v>40</v>
       </c>
-      <c r="Q2" s="715"/>
+      <c r="Q2" s="702"/>
       <c r="R2" s="21">
         <f>R7+R20</f>
         <v>4</v>
@@ -9128,7 +9128,7 @@
         <f>IF((Z2+T2)&gt;0,0,-1)</f>
         <v>0</v>
       </c>
-      <c r="AB2" s="709"/>
+      <c r="AB2" s="696"/>
       <c r="AC2" s="35"/>
       <c r="AH2" s="6" t="s">
         <v>344</v>
@@ -9143,14 +9143,14 @@
       </c>
     </row>
     <row r="3" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="694"/>
-      <c r="B3" s="696"/>
-      <c r="C3" s="616"/>
-      <c r="D3" s="698"/>
-      <c r="E3" s="700"/>
-      <c r="G3" s="660"/>
+      <c r="A3" s="707"/>
+      <c r="B3" s="709"/>
+      <c r="C3" s="646"/>
+      <c r="D3" s="711"/>
+      <c r="E3" s="713"/>
+      <c r="G3" s="614"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="706"/>
+      <c r="I3" s="693"/>
       <c r="K3" s="24">
         <v>2</v>
       </c>
@@ -9165,7 +9165,7 @@
       <c r="V3" s="470"/>
       <c r="W3" s="6"/>
       <c r="X3" s="470"/>
-      <c r="AB3" s="709"/>
+      <c r="AB3" s="696"/>
       <c r="AC3" s="35"/>
       <c r="AE3" s="100" t="s">
         <v>588</v>
@@ -9194,10 +9194,10 @@
         <v>380</v>
       </c>
       <c r="B4" s="243"/>
-      <c r="C4" s="701" t="s">
+      <c r="C4" s="714" t="s">
         <v>177</v>
       </c>
-      <c r="I4" s="706"/>
+      <c r="I4" s="693"/>
       <c r="R4" s="471" t="s">
         <v>588</v>
       </c>
@@ -9209,7 +9209,7 @@
       <c r="V4" s="470"/>
       <c r="W4" s="6"/>
       <c r="X4" s="470"/>
-      <c r="AB4" s="709"/>
+      <c r="AB4" s="696"/>
       <c r="AC4" s="35"/>
       <c r="AE4" s="20"/>
       <c r="AF4" s="100" t="s">
@@ -9234,7 +9234,7 @@
       <c r="B5" s="100" t="s">
         <v>357</v>
       </c>
-      <c r="C5" s="702"/>
+      <c r="C5" s="715"/>
       <c r="D5" s="222" t="s">
         <v>102</v>
       </c>
@@ -9250,7 +9250,7 @@
       <c r="H5" s="206" t="s">
         <v>218</v>
       </c>
-      <c r="I5" s="706"/>
+      <c r="I5" s="693"/>
       <c r="J5" s="397" t="s">
         <v>268</v>
       </c>
@@ -9277,7 +9277,7 @@
       <c r="V5" s="468"/>
       <c r="W5" s="6"/>
       <c r="X5" s="468"/>
-      <c r="AB5" s="709"/>
+      <c r="AB5" s="696"/>
       <c r="AC5" s="2" t="s">
         <v>591</v>
       </c>
@@ -9297,19 +9297,19 @@
       <c r="AL5" s="468"/>
     </row>
     <row r="6" spans="1:38" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="690" t="s">
+      <c r="A6" s="703" t="s">
         <v>285</v>
       </c>
       <c r="B6" s="105" t="s">
         <v>198</v>
       </c>
-      <c r="C6" s="661"/>
-      <c r="D6" s="662"/>
+      <c r="C6" s="628"/>
+      <c r="D6" s="629"/>
       <c r="E6" s="96">
         <v>1</v>
       </c>
       <c r="G6" s="599"/>
-      <c r="I6" s="706"/>
+      <c r="I6" s="693"/>
       <c r="P6" s="61" t="s">
         <v>591</v>
       </c>
@@ -9321,7 +9321,7 @@
         <f>S7+S11-SUM(V2:V10)</f>
         <v>3</v>
       </c>
-      <c r="AB6" s="709"/>
+      <c r="AB6" s="696"/>
       <c r="AC6" s="35"/>
       <c r="AE6" s="64">
         <f>AE7-SUM(AL2:AL10)+AE11</f>
@@ -9337,7 +9337,7 @@
       <c r="AL6" s="112"/>
     </row>
     <row r="7" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="691"/>
+      <c r="A7" s="704"/>
       <c r="B7" s="100" t="s">
         <v>154</v>
       </c>
@@ -9348,7 +9348,7 @@
         <v>135</v>
       </c>
       <c r="G7" s="599"/>
-      <c r="I7" s="706"/>
+      <c r="I7" s="693"/>
       <c r="M7" s="16" t="s">
         <v>347</v>
       </c>
@@ -9378,7 +9378,7 @@
         <v>249</v>
       </c>
       <c r="X7" s="469"/>
-      <c r="AB7" s="709"/>
+      <c r="AB7" s="696"/>
       <c r="AC7" s="99" t="s">
         <v>592</v>
       </c>
@@ -9406,7 +9406,7 @@
       <c r="AL7" s="24"/>
     </row>
     <row r="8" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="692"/>
+      <c r="A8" s="705"/>
       <c r="B8" s="212" t="s">
         <v>28</v>
       </c>
@@ -9415,7 +9415,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="599"/>
-      <c r="I8" s="706"/>
+      <c r="I8" s="693"/>
       <c r="N8" s="80"/>
       <c r="U8" s="6"/>
       <c r="V8" s="24"/>
@@ -9423,7 +9423,7 @@
         <v>611</v>
       </c>
       <c r="X8" s="470"/>
-      <c r="AB8" s="709"/>
+      <c r="AB8" s="696"/>
       <c r="AC8" s="515"/>
       <c r="AH8" s="6" t="s">
         <v>610</v>
@@ -9452,7 +9452,7 @@
       </c>
       <c r="G9" s="599"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="706"/>
+      <c r="I9" s="693"/>
       <c r="M9" s="19" t="s">
         <v>524</v>
       </c>
@@ -9463,7 +9463,7 @@
         <v>603</v>
       </c>
       <c r="X9" s="470"/>
-      <c r="AB9" s="709"/>
+      <c r="AB9" s="696"/>
       <c r="AC9" s="515"/>
       <c r="AE9" s="20"/>
       <c r="AF9" s="20"/>
@@ -9491,7 +9491,7 @@
         <v>37</v>
       </c>
       <c r="G10" s="599"/>
-      <c r="I10" s="706"/>
+      <c r="I10" s="693"/>
       <c r="J10" s="24" t="s">
         <v>372</v>
       </c>
@@ -9506,7 +9506,7 @@
       <c r="V10" s="470"/>
       <c r="W10" s="6"/>
       <c r="X10" s="470"/>
-      <c r="AB10" s="709"/>
+      <c r="AB10" s="696"/>
       <c r="AC10" s="515"/>
       <c r="AE10" s="20"/>
       <c r="AF10" s="20"/>
@@ -9534,7 +9534,7 @@
         <v>265</v>
       </c>
       <c r="G11" s="599"/>
-      <c r="I11" s="706"/>
+      <c r="I11" s="693"/>
       <c r="J11" s="24" t="s">
         <v>194</v>
       </c>
@@ -9560,13 +9560,13 @@
       <c r="S11" s="24">
         <v>3</v>
       </c>
-      <c r="U11" s="711" t="s">
+      <c r="U11" s="698" t="s">
         <v>557</v>
       </c>
-      <c r="V11" s="712"/>
-      <c r="W11" s="712"/>
-      <c r="X11" s="713"/>
-      <c r="AB11" s="710"/>
+      <c r="V11" s="699"/>
+      <c r="W11" s="699"/>
+      <c r="X11" s="700"/>
+      <c r="AB11" s="697"/>
       <c r="AC11" s="99" t="s">
         <v>594</v>
       </c>
@@ -9580,13 +9580,13 @@
         <v>5</v>
       </c>
       <c r="AG11" s="414"/>
-      <c r="AH11" s="711" t="s">
+      <c r="AH11" s="698" t="s">
         <v>602</v>
       </c>
-      <c r="AI11" s="712"/>
-      <c r="AJ11" s="712"/>
-      <c r="AK11" s="712"/>
-      <c r="AL11" s="713"/>
+      <c r="AI11" s="699"/>
+      <c r="AJ11" s="699"/>
+      <c r="AK11" s="699"/>
+      <c r="AL11" s="700"/>
     </row>
     <row r="12" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="227" t="s">
@@ -9597,7 +9597,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="599"/>
-      <c r="I12" s="706"/>
+      <c r="I12" s="693"/>
       <c r="J12" s="24" t="s">
         <v>515</v>
       </c>
@@ -9630,7 +9630,7 @@
       </c>
       <c r="D13" s="20"/>
       <c r="G13" s="599"/>
-      <c r="I13" s="706"/>
+      <c r="I13" s="693"/>
       <c r="J13" s="108" t="s">
         <v>547</v>
       </c>
@@ -9674,7 +9674,7 @@
       <c r="H14" s="206" t="s">
         <v>218</v>
       </c>
-      <c r="I14" s="706"/>
+      <c r="I14" s="693"/>
       <c r="U14" s="67" t="s">
         <v>80</v>
       </c>
@@ -9701,7 +9701,7 @@
       <c r="H15" s="271">
         <v>0</v>
       </c>
-      <c r="I15" s="706"/>
+      <c r="I15" s="693"/>
       <c r="J15" s="108" t="s">
         <v>153</v>
       </c>
@@ -9732,7 +9732,7 @@
       <c r="D16" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="I16" s="706"/>
+      <c r="I16" s="693"/>
       <c r="K16" s="100" t="s">
         <v>44</v>
       </c>
@@ -9776,7 +9776,7 @@
       <c r="G17" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="I17" s="706"/>
+      <c r="I17" s="693"/>
       <c r="L17" s="2" t="s">
         <v>426</v>
       </c>
@@ -9790,13 +9790,13 @@
     </row>
     <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
-      <c r="I18" s="706"/>
+      <c r="I18" s="693"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="703" t="s">
+      <c r="O18" s="690" t="s">
         <v>516</v>
       </c>
-      <c r="P18" s="704"/>
+      <c r="P18" s="691"/>
       <c r="Q18" s="127" t="s">
         <v>44</v>
       </c>
@@ -9816,7 +9816,7 @@
       <c r="X18" s="24"/>
     </row>
     <row r="19" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="706"/>
+      <c r="I19" s="693"/>
       <c r="M19" s="21" t="s">
         <v>425</v>
       </c>
@@ -9846,7 +9846,7 @@
       <c r="G20" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="I20" s="706"/>
+      <c r="I20" s="693"/>
       <c r="K20" s="19" t="s">
         <v>422</v>
       </c>
@@ -9875,7 +9875,7 @@
       <c r="X20" s="468"/>
     </row>
     <row r="21" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="706"/>
+      <c r="I21" s="693"/>
       <c r="M21" s="216" t="s">
         <v>411</v>
       </c>
@@ -9905,7 +9905,7 @@
       <c r="G22" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="I22" s="706"/>
+      <c r="I22" s="693"/>
       <c r="P22" s="99" t="s">
         <v>590</v>
       </c>
@@ -9920,7 +9920,7 @@
       <c r="E23" s="283" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="706"/>
+      <c r="I23" s="693"/>
       <c r="Q23" s="24">
         <f>SUM(V23:V31)</f>
         <v>7</v>
@@ -9937,7 +9937,7 @@
       </c>
     </row>
     <row r="24" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="706"/>
+      <c r="I24" s="693"/>
       <c r="U24" s="35"/>
       <c r="V24" s="509">
         <v>1</v>
@@ -9965,7 +9965,7 @@
       <c r="H25" s="191" t="s">
         <v>266</v>
       </c>
-      <c r="I25" s="706"/>
+      <c r="I25" s="693"/>
       <c r="J25" s="397" t="s">
         <v>269</v>
       </c>
@@ -10010,7 +10010,7 @@
       <c r="H26" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="I26" s="706"/>
+      <c r="I26" s="693"/>
       <c r="K26" s="24">
         <v>15</v>
       </c>
@@ -10045,7 +10045,7 @@
       </c>
     </row>
     <row r="27" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="706"/>
+      <c r="I27" s="693"/>
       <c r="O27" s="2" t="s">
         <v>98</v>
       </c>
@@ -10072,7 +10072,7 @@
       <c r="E28" s="215">
         <v>2</v>
       </c>
-      <c r="I28" s="706"/>
+      <c r="I28" s="693"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="142"/>
@@ -10094,7 +10094,7 @@
       <c r="H29" s="191" t="s">
         <v>267</v>
       </c>
-      <c r="I29" s="707"/>
+      <c r="I29" s="694"/>
       <c r="J29" s="324"/>
       <c r="L29" s="96" t="s">
         <v>273</v>
@@ -10152,13 +10152,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I2:I29"/>
-    <mergeCell ref="AB1:AB11"/>
-    <mergeCell ref="AH11:AL11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="U11:X11"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="G5:G14"/>
     <mergeCell ref="A2:A3"/>
@@ -10170,6 +10163,13 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C2:C3"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I2:I29"/>
+    <mergeCell ref="AB1:AB11"/>
+    <mergeCell ref="AH11:AL11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="U11:X11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10180,8 +10180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AT37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AF10" sqref="AF10"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4:P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10281,14 +10281,14 @@
         <f ca="1">TODAY()</f>
         <v>45289</v>
       </c>
-      <c r="T1" s="742"/>
+      <c r="T1" s="735"/>
       <c r="U1" s="142"/>
       <c r="V1" s="6"/>
       <c r="W1" s="6"/>
-      <c r="X1" s="726" t="s">
+      <c r="X1" s="719" t="s">
         <v>441</v>
       </c>
-      <c r="Y1" s="727"/>
+      <c r="Y1" s="720"/>
       <c r="Z1" s="306">
         <f>68-(W8+Y3+X3+U3)</f>
         <v>0</v>
@@ -10304,27 +10304,27 @@
       <c r="AD1" s="302" t="s">
         <v>44</v>
       </c>
-      <c r="AE1" s="728" t="s">
+      <c r="AE1" s="721" t="s">
         <v>190</v>
       </c>
-      <c r="AF1" s="729"/>
-      <c r="AG1" s="730"/>
-      <c r="AH1" s="731" t="s">
+      <c r="AF1" s="722"/>
+      <c r="AG1" s="723"/>
+      <c r="AH1" s="724" t="s">
         <v>293</v>
       </c>
-      <c r="AI1" s="732"/>
-      <c r="AJ1" s="733"/>
-      <c r="AK1" s="659" t="s">
+      <c r="AI1" s="725"/>
+      <c r="AJ1" s="726"/>
+      <c r="AK1" s="613" t="s">
         <v>613</v>
       </c>
       <c r="AL1" s="550" t="s">
         <v>614</v>
       </c>
-      <c r="AM1" s="723" t="s">
+      <c r="AM1" s="716" t="s">
         <v>444</v>
       </c>
-      <c r="AN1" s="724"/>
-      <c r="AO1" s="725"/>
+      <c r="AN1" s="717"/>
+      <c r="AO1" s="718"/>
       <c r="AR1" s="142"/>
     </row>
     <row r="2" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10337,29 +10337,29 @@
       </c>
       <c r="J2" s="318">
         <f>K2+L2</f>
-        <v>11</v>
-      </c>
-      <c r="K2" s="721">
+        <v>25</v>
+      </c>
+      <c r="K2" s="743">
         <f>SUM(K4:K37)</f>
         <v>6</v>
       </c>
-      <c r="L2" s="719">
+      <c r="L2" s="741">
         <f>SUM(L4:L37)</f>
-        <v>5</v>
-      </c>
-      <c r="M2" s="734">
+        <v>19</v>
+      </c>
+      <c r="M2" s="727">
         <f>SUM(M5:M30)</f>
         <v>0</v>
       </c>
-      <c r="N2" s="736">
+      <c r="N2" s="729">
         <f>SUM(N4:N29)</f>
         <v>8</v>
       </c>
-      <c r="O2" s="738">
+      <c r="O2" s="731">
         <f>SUM(O4:O29)</f>
         <v>10</v>
       </c>
-      <c r="P2" s="666">
+      <c r="P2" s="637">
         <f>SUM(N30:N37)* (-1)</f>
         <v>0</v>
       </c>
@@ -10372,14 +10372,14 @@
       <c r="S2" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="T2" s="743"/>
+      <c r="T2" s="736"/>
       <c r="U2" s="537" t="s">
         <v>262</v>
       </c>
       <c r="V2" s="482" t="s">
         <v>219</v>
       </c>
-      <c r="W2" s="740" t="s">
+      <c r="W2" s="733" t="s">
         <v>234</v>
       </c>
       <c r="X2" s="483" t="s">
@@ -10421,7 +10421,7 @@
       <c r="AJ2" s="150" t="s">
         <v>288</v>
       </c>
-      <c r="AK2" s="660"/>
+      <c r="AK2" s="614"/>
       <c r="AL2" s="591" t="s">
         <v>288</v>
       </c>
@@ -10449,12 +10449,12 @@
         <f>V3+X3+Y3+U3</f>
         <v>68</v>
       </c>
-      <c r="K3" s="722"/>
-      <c r="L3" s="720"/>
-      <c r="M3" s="735"/>
-      <c r="N3" s="737"/>
-      <c r="O3" s="739"/>
-      <c r="P3" s="667"/>
+      <c r="K3" s="744"/>
+      <c r="L3" s="742"/>
+      <c r="M3" s="728"/>
+      <c r="N3" s="730"/>
+      <c r="O3" s="732"/>
+      <c r="P3" s="638"/>
       <c r="Q3" s="172">
         <f>(M2+N2)-Y3</f>
         <v>0</v>
@@ -10462,7 +10462,7 @@
       <c r="S3" s="159" t="s">
         <v>244</v>
       </c>
-      <c r="T3" s="744"/>
+      <c r="T3" s="737"/>
       <c r="U3" s="538">
         <f>SUM(U4:U29)</f>
         <v>14</v>
@@ -10471,7 +10471,7 @@
         <f>SUM(V4:V29)</f>
         <v>37</v>
       </c>
-      <c r="W3" s="741"/>
+      <c r="W3" s="734"/>
       <c r="X3" s="485">
         <f t="shared" ref="X3:AC3" si="0">SUM(X4:X29)</f>
         <v>9</v>
@@ -10567,7 +10567,7 @@
       <c r="J4" s="569"/>
       <c r="K4" s="573"/>
       <c r="L4" s="579">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4" s="325"/>
       <c r="N4" s="107">
@@ -10577,7 +10577,7 @@
         <f>AC4</f>
         <v>0</v>
       </c>
-      <c r="P4" s="716"/>
+      <c r="P4" s="738"/>
       <c r="Q4" s="20"/>
       <c r="R4" s="2" t="s">
         <v>334</v>
@@ -10661,7 +10661,7 @@
         <f>AC5</f>
         <v>0</v>
       </c>
-      <c r="P5" s="717"/>
+      <c r="P5" s="739"/>
       <c r="Q5" s="20"/>
       <c r="R5" s="2" t="s">
         <v>340</v>
@@ -10745,7 +10745,7 @@
       </c>
       <c r="K6" s="574"/>
       <c r="L6" s="581">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M6" s="326"/>
       <c r="N6" s="107">
@@ -10755,7 +10755,7 @@
         <f>AC6</f>
         <v>1</v>
       </c>
-      <c r="P6" s="717"/>
+      <c r="P6" s="739"/>
       <c r="Q6" s="54" t="s">
         <v>335</v>
       </c>
@@ -10848,7 +10848,7 @@
       <c r="J7" s="570"/>
       <c r="K7" s="574"/>
       <c r="L7" s="580">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7" s="326">
         <v>0</v>
@@ -10860,7 +10860,7 @@
         <f>AC7</f>
         <v>0</v>
       </c>
-      <c r="P7" s="717"/>
+      <c r="P7" s="739"/>
       <c r="Q7" s="20"/>
       <c r="R7" s="2" t="s">
         <v>335</v>
@@ -10976,7 +10976,7 @@
         <f t="shared" ref="O8:O37" si="10">AC8</f>
         <v>0</v>
       </c>
-      <c r="P8" s="717"/>
+      <c r="P8" s="739"/>
       <c r="Q8" s="108" t="s">
         <v>233</v>
       </c>
@@ -11067,7 +11067,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P9" s="717"/>
+      <c r="P9" s="739"/>
       <c r="Q9" s="108" t="s">
         <v>335</v>
       </c>
@@ -11172,7 +11172,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P10" s="717"/>
+      <c r="P10" s="739"/>
       <c r="Q10" s="20"/>
       <c r="R10" s="2" t="s">
         <v>340</v>
@@ -11262,7 +11262,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P11" s="717"/>
+      <c r="P11" s="739"/>
       <c r="Q11" s="108" t="s">
         <v>335</v>
       </c>
@@ -11327,14 +11327,14 @@
       <c r="AR11" s="508"/>
     </row>
     <row r="12" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="626" t="s">
+      <c r="A12" s="675" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
         <v>13</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="E12" s="681" t="s">
+      <c r="E12" s="625" t="s">
         <v>56</v>
       </c>
       <c r="G12" s="262"/>
@@ -11359,7 +11359,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P12" s="717"/>
+      <c r="P12" s="739"/>
       <c r="Q12" s="108" t="s">
         <v>335</v>
       </c>
@@ -11436,14 +11436,14 @@
       </c>
     </row>
     <row r="13" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="628"/>
+      <c r="A13" s="677"/>
       <c r="B13" s="583">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="682"/>
+      <c r="E13" s="626"/>
       <c r="F13" s="172">
         <v>0</v>
       </c>
@@ -11467,7 +11467,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P13" s="717"/>
+      <c r="P13" s="739"/>
       <c r="Q13" s="108" t="s">
         <v>335</v>
       </c>
@@ -11539,7 +11539,7 @@
       <c r="J14" s="570"/>
       <c r="K14" s="574"/>
       <c r="L14" s="580">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14" s="328"/>
       <c r="N14" s="291">
@@ -11549,7 +11549,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P14" s="717"/>
+      <c r="P14" s="739"/>
       <c r="Q14" s="20"/>
       <c r="R14" s="200" t="s">
         <v>339</v>
@@ -11641,7 +11641,9 @@
         <v>194</v>
       </c>
       <c r="K15" s="575"/>
-      <c r="L15" s="581"/>
+      <c r="L15" s="581">
+        <v>1</v>
+      </c>
       <c r="M15" s="328"/>
       <c r="N15" s="291">
         <v>1</v>
@@ -11650,7 +11652,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P15" s="717"/>
+      <c r="P15" s="739"/>
       <c r="Q15" s="20"/>
       <c r="R15" s="200" t="s">
         <v>339</v>
@@ -11744,7 +11746,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P16" s="717"/>
+      <c r="P16" s="739"/>
       <c r="Q16" s="108" t="s">
         <v>335</v>
       </c>
@@ -11845,7 +11847,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P17" s="717"/>
+      <c r="P17" s="739"/>
       <c r="Q17" s="20"/>
       <c r="R17" s="2" t="s">
         <v>341</v>
@@ -11945,7 +11947,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P18" s="717"/>
+      <c r="P18" s="739"/>
       <c r="Q18" s="108" t="s">
         <v>335</v>
       </c>
@@ -12035,7 +12037,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P19" s="717"/>
+      <c r="P19" s="739"/>
       <c r="Q19" s="20"/>
       <c r="R19" s="2" t="s">
         <v>334</v>
@@ -12143,11 +12145,11 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P20" s="718"/>
+      <c r="P20" s="740"/>
       <c r="Q20" s="605" t="s">
         <v>335</v>
       </c>
-      <c r="R20" s="683"/>
+      <c r="R20" s="627"/>
       <c r="S20" s="534" t="s">
         <v>85</v>
       </c>
@@ -12236,7 +12238,7 @@
       </c>
       <c r="K21" s="574"/>
       <c r="L21" s="580">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M21" s="330"/>
       <c r="N21" s="107">
@@ -12409,7 +12411,7 @@
     </row>
     <row r="23" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="24"/>
-      <c r="E23" s="633" t="s">
+      <c r="E23" s="682" t="s">
         <v>289</v>
       </c>
       <c r="F23" s="180"/>
@@ -12514,7 +12516,7 @@
       <c r="C24" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="E24" s="634"/>
+      <c r="E24" s="683"/>
       <c r="F24" s="172"/>
       <c r="H24" s="42"/>
       <c r="J24" s="570" t="s">
@@ -12540,7 +12542,7 @@
       <c r="Q24" s="605" t="s">
         <v>335</v>
       </c>
-      <c r="R24" s="683"/>
+      <c r="R24" s="627"/>
       <c r="S24" s="534" t="s">
         <v>249</v>
       </c>
@@ -12626,7 +12628,7 @@
       </c>
       <c r="K25" s="574"/>
       <c r="L25" s="580">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M25" s="525">
         <v>0</v>
@@ -12985,7 +12987,9 @@
         <v>358</v>
       </c>
       <c r="K29" s="577"/>
-      <c r="L29" s="581"/>
+      <c r="L29" s="581">
+        <v>1</v>
+      </c>
       <c r="M29" s="324"/>
       <c r="N29" s="64">
         <v>0</v>
@@ -13204,12 +13208,12 @@
       <c r="AR31" s="508"/>
     </row>
     <row r="32" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="650"/>
-      <c r="B32" s="650"/>
+      <c r="A32" s="630"/>
+      <c r="B32" s="630"/>
       <c r="J32" s="571"/>
       <c r="K32" s="586"/>
       <c r="L32" s="580">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M32" s="510">
         <v>0</v>
@@ -13312,7 +13316,7 @@
       <c r="J33" s="572"/>
       <c r="K33" s="587"/>
       <c r="L33" s="580">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M33" s="334"/>
       <c r="N33" s="247">
@@ -13415,7 +13419,7 @@
         <v>0</v>
       </c>
       <c r="L34" s="580">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M34" s="334"/>
       <c r="N34" s="248">
@@ -13507,7 +13511,7 @@
       </c>
       <c r="K35" s="586"/>
       <c r="L35" s="580">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M35" s="334"/>
       <c r="N35" s="250">
@@ -13599,7 +13603,7 @@
       </c>
       <c r="K36" s="586"/>
       <c r="L36" s="580">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M36" s="334"/>
       <c r="N36" s="250">
@@ -13697,7 +13701,7 @@
       </c>
       <c r="K37" s="588"/>
       <c r="L37" s="582">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M37" s="335"/>
       <c r="N37" s="249">
@@ -13786,6 +13790,15 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="P4:P20"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="Q20:R20"/>
     <mergeCell ref="AM1:AO1"/>
     <mergeCell ref="X1:Y1"/>
     <mergeCell ref="AE1:AG1"/>
@@ -13797,15 +13810,6 @@
     <mergeCell ref="W2:W3"/>
     <mergeCell ref="T1:T3"/>
     <mergeCell ref="AK1:AK2"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="P4:P20"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="Q20:R20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13873,7 +13877,7 @@
       <c r="V1" s="603" t="s">
         <v>70</v>
       </c>
-      <c r="W1" s="683"/>
+      <c r="W1" s="627"/>
       <c r="X1" s="62" t="s">
         <v>101</v>
       </c>
@@ -13892,7 +13896,7 @@
       <c r="AC1" s="116" t="s">
         <v>190</v>
       </c>
-      <c r="AD1" s="759" t="s">
+      <c r="AD1" s="752" t="s">
         <v>211</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -13909,10 +13913,10 @@
       <c r="E2" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="790" t="s">
+      <c r="F2" s="751" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="747" t="s">
+      <c r="G2" s="779" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -13940,10 +13944,10 @@
       <c r="U2" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="V2" s="726" t="s">
+      <c r="V2" s="719" t="s">
         <v>120</v>
       </c>
-      <c r="W2" s="727"/>
+      <c r="W2" s="720"/>
       <c r="X2" s="64" t="s">
         <v>109</v>
       </c>
@@ -13962,7 +13966,7 @@
       <c r="AC2" s="117" t="s">
         <v>98</v>
       </c>
-      <c r="AD2" s="760"/>
+      <c r="AD2" s="753"/>
       <c r="AE2" s="64" t="s">
         <v>98</v>
       </c>
@@ -13981,8 +13985,8 @@
       <c r="E3" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="F3" s="630"/>
-      <c r="G3" s="748"/>
+      <c r="F3" s="679"/>
+      <c r="G3" s="780"/>
       <c r="H3" s="40" t="s">
         <v>80</v>
       </c>
@@ -13993,13 +13997,13 @@
         <v>81</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="757" t="s">
+      <c r="O3" s="789" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="778" t="s">
+      <c r="P3" s="771" t="s">
         <v>217</v>
       </c>
-      <c r="Q3" s="779"/>
+      <c r="Q3" s="772"/>
       <c r="S3" s="57" t="s">
         <v>218</v>
       </c>
@@ -14009,15 +14013,15 @@
       <c r="W3" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="AD3" s="760"/>
+      <c r="AD3" s="753"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="748"/>
+      <c r="G4" s="780"/>
       <c r="H4" s="6"/>
       <c r="L4" s="687" t="s">
         <v>82</v>
       </c>
-      <c r="O4" s="758"/>
+      <c r="O4" s="790"/>
       <c r="T4" s="55" t="s">
         <v>97</v>
       </c>
@@ -14031,8 +14035,8 @@
         <v>194</v>
       </c>
       <c r="Z4" s="605"/>
-      <c r="AA4" s="683"/>
-      <c r="AD4" s="760"/>
+      <c r="AA4" s="627"/>
+      <c r="AD4" s="753"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -14047,21 +14051,21 @@
       <c r="F5" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="G5" s="748"/>
+      <c r="G5" s="780"/>
       <c r="H5" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="K5" s="765" t="s">
+      <c r="K5" s="758" t="s">
         <v>215</v>
       </c>
-      <c r="L5" s="780"/>
+      <c r="L5" s="773"/>
       <c r="M5" s="2" t="s">
         <v>213</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>212</v>
       </c>
-      <c r="O5" s="758"/>
+      <c r="O5" s="790"/>
       <c r="P5" s="108" t="s">
         <v>214</v>
       </c>
@@ -14077,11 +14081,11 @@
       <c r="U5" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="Y5" s="768" t="s">
+      <c r="Y5" s="761" t="s">
         <v>282</v>
       </c>
-      <c r="Z5" s="769"/>
-      <c r="AD5" s="760"/>
+      <c r="Z5" s="762"/>
+      <c r="AD5" s="753"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -14091,16 +14095,16 @@
       <c r="E6" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="G6" s="748"/>
+      <c r="G6" s="780"/>
       <c r="H6" s="46" t="s">
         <v>80</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="766"/>
-      <c r="L6" s="780"/>
-      <c r="O6" s="758"/>
+      <c r="K6" s="759"/>
+      <c r="L6" s="773"/>
+      <c r="O6" s="790"/>
       <c r="T6" s="2" t="s">
         <v>100</v>
       </c>
@@ -14110,23 +14114,23 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="760"/>
+      <c r="AD6" s="753"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="748"/>
+      <c r="G7" s="780"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="766"/>
-      <c r="L7" s="780"/>
+      <c r="K7" s="759"/>
+      <c r="L7" s="773"/>
       <c r="N7" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="O7" s="758"/>
+      <c r="O7" s="790"/>
       <c r="P7" s="73"/>
       <c r="U7" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="760"/>
+      <c r="AD7" s="753"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -14139,7 +14143,7 @@
       <c r="F8" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="G8" s="748"/>
+      <c r="G8" s="780"/>
       <c r="H8" s="50" t="s">
         <v>75</v>
       </c>
@@ -14149,41 +14153,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="766"/>
-      <c r="L8" s="780"/>
-      <c r="O8" s="758"/>
+      <c r="K8" s="759"/>
+      <c r="L8" s="773"/>
+      <c r="O8" s="790"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="762" t="s">
+      <c r="S8" s="755" t="s">
         <v>210</v>
       </c>
-      <c r="T8" s="763"/>
-      <c r="U8" s="763"/>
-      <c r="V8" s="763"/>
-      <c r="W8" s="763"/>
-      <c r="X8" s="763"/>
-      <c r="Y8" s="763"/>
-      <c r="Z8" s="763"/>
-      <c r="AA8" s="763"/>
-      <c r="AB8" s="763"/>
-      <c r="AC8" s="764"/>
-      <c r="AD8" s="760"/>
+      <c r="T8" s="756"/>
+      <c r="U8" s="756"/>
+      <c r="V8" s="756"/>
+      <c r="W8" s="756"/>
+      <c r="X8" s="756"/>
+      <c r="Y8" s="756"/>
+      <c r="Z8" s="756"/>
+      <c r="AA8" s="756"/>
+      <c r="AB8" s="756"/>
+      <c r="AC8" s="757"/>
+      <c r="AD8" s="753"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="784"/>
-      <c r="G9" s="748"/>
+      <c r="C9" s="745"/>
+      <c r="G9" s="780"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="766"/>
-      <c r="L9" s="751" t="s">
+      <c r="K9" s="759"/>
+      <c r="L9" s="783" t="s">
         <v>216</v>
       </c>
-      <c r="M9" s="752"/>
-      <c r="N9" s="753"/>
-      <c r="O9" s="758"/>
+      <c r="M9" s="784"/>
+      <c r="N9" s="785"/>
+      <c r="O9" s="790"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="760"/>
+      <c r="AD9" s="753"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="785"/>
+      <c r="C10" s="746"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>87</v>
@@ -14191,7 +14195,7 @@
       <c r="F10" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="G10" s="748"/>
+      <c r="G10" s="780"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>80</v>
@@ -14199,33 +14203,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="766"/>
-      <c r="M10" s="787" t="s">
+      <c r="K10" s="759"/>
+      <c r="M10" s="748" t="s">
         <v>89</v>
       </c>
-      <c r="N10" s="788"/>
-      <c r="O10" s="788"/>
-      <c r="P10" s="788"/>
-      <c r="Q10" s="788"/>
-      <c r="R10" s="788"/>
-      <c r="S10" s="788"/>
-      <c r="T10" s="788"/>
-      <c r="U10" s="788"/>
-      <c r="V10" s="788"/>
-      <c r="W10" s="788"/>
-      <c r="X10" s="788"/>
-      <c r="Y10" s="788"/>
-      <c r="Z10" s="788"/>
-      <c r="AA10" s="788"/>
-      <c r="AB10" s="788"/>
-      <c r="AC10" s="789"/>
-      <c r="AD10" s="760"/>
+      <c r="N10" s="749"/>
+      <c r="O10" s="749"/>
+      <c r="P10" s="749"/>
+      <c r="Q10" s="749"/>
+      <c r="R10" s="749"/>
+      <c r="S10" s="749"/>
+      <c r="T10" s="749"/>
+      <c r="U10" s="749"/>
+      <c r="V10" s="749"/>
+      <c r="W10" s="749"/>
+      <c r="X10" s="749"/>
+      <c r="Y10" s="749"/>
+      <c r="Z10" s="749"/>
+      <c r="AA10" s="749"/>
+      <c r="AB10" s="749"/>
+      <c r="AC10" s="750"/>
+      <c r="AD10" s="753"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="786"/>
-      <c r="G11" s="748"/>
+      <c r="C11" s="747"/>
+      <c r="G11" s="780"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="766"/>
+      <c r="K11" s="759"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -14233,17 +14237,17 @@
       <c r="Y11" s="68" t="s">
         <v>120</v>
       </c>
-      <c r="Z11" s="776" t="s">
+      <c r="Z11" s="769" t="s">
         <v>120</v>
       </c>
-      <c r="AA11" s="777"/>
+      <c r="AA11" s="770"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>120</v>
       </c>
-      <c r="AD11" s="760"/>
+      <c r="AD11" s="753"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -14256,7 +14260,7 @@
       <c r="F12" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="G12" s="748"/>
+      <c r="G12" s="780"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>80</v>
@@ -14264,8 +14268,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="766"/>
-      <c r="L12" s="781" t="s">
+      <c r="K12" s="759"/>
+      <c r="L12" s="774" t="s">
         <v>92</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -14296,25 +14300,25 @@
         <v>115</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="770" t="s">
+      <c r="AA12" s="763" t="s">
         <v>125</v>
       </c>
-      <c r="AB12" s="771"/>
+      <c r="AB12" s="764"/>
       <c r="AC12" s="21" t="s">
         <v>230</v>
       </c>
-      <c r="AD12" s="760"/>
+      <c r="AD12" s="753"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="784"/>
-      <c r="G13" s="748"/>
-      <c r="K13" s="766"/>
-      <c r="L13" s="782"/>
+      <c r="C13" s="745"/>
+      <c r="G13" s="780"/>
+      <c r="K13" s="759"/>
+      <c r="L13" s="775"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="750" t="s">
+      <c r="Q13" s="782" t="s">
         <v>208</v>
       </c>
-      <c r="R13" s="639"/>
+      <c r="R13" s="644"/>
       <c r="S13" s="599"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
@@ -14323,17 +14327,17 @@
       <c r="X13" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="AA13" s="772"/>
-      <c r="AB13" s="773"/>
-      <c r="AD13" s="760"/>
+      <c r="AA13" s="765"/>
+      <c r="AB13" s="766"/>
+      <c r="AD13" s="753"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="C14" s="786"/>
+      <c r="C14" s="747"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="748"/>
+      <c r="G14" s="780"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -14341,8 +14345,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="766"/>
-      <c r="L14" s="782"/>
+      <c r="K14" s="759"/>
+      <c r="L14" s="775"/>
       <c r="M14" s="21" t="s">
         <v>110</v>
       </c>
@@ -14363,9 +14367,9 @@
       <c r="Y14" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="AA14" s="772"/>
-      <c r="AB14" s="773"/>
-      <c r="AD14" s="760"/>
+      <c r="AA14" s="765"/>
+      <c r="AB14" s="766"/>
+      <c r="AD14" s="753"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -14380,19 +14384,19 @@
       <c r="F15" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="G15" s="748"/>
+      <c r="G15" s="780"/>
       <c r="H15" s="2" t="s">
         <v>80</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="K15" s="766"/>
-      <c r="L15" s="783"/>
-      <c r="Q15" s="750" t="s">
+      <c r="K15" s="759"/>
+      <c r="L15" s="776"/>
+      <c r="Q15" s="782" t="s">
         <v>209</v>
       </c>
-      <c r="R15" s="639"/>
+      <c r="R15" s="644"/>
       <c r="S15" s="599"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
@@ -14401,14 +14405,14 @@
       <c r="X15" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="AA15" s="772"/>
-      <c r="AB15" s="773"/>
-      <c r="AD15" s="760"/>
+      <c r="AA15" s="765"/>
+      <c r="AB15" s="766"/>
+      <c r="AD15" s="753"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="748"/>
-      <c r="K16" s="766"/>
+      <c r="G16" s="780"/>
+      <c r="K16" s="759"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>108</v>
@@ -14427,24 +14431,24 @@
       <c r="Z16" s="76" t="s">
         <v>126</v>
       </c>
-      <c r="AA16" s="772"/>
-      <c r="AB16" s="773"/>
-      <c r="AD16" s="760"/>
+      <c r="AA16" s="765"/>
+      <c r="AB16" s="766"/>
+      <c r="AD16" s="753"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F17" s="745" t="s">
+      <c r="F17" s="777" t="s">
         <v>95</v>
       </c>
-      <c r="G17" s="748"/>
+      <c r="G17" s="780"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>80</v>
       </c>
-      <c r="K17" s="766"/>
+      <c r="K17" s="759"/>
       <c r="S17" s="599"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
@@ -14452,9 +14456,9 @@
       <c r="X17" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA17" s="772"/>
-      <c r="AB17" s="773"/>
-      <c r="AD17" s="760"/>
+      <c r="AA17" s="765"/>
+      <c r="AB17" s="766"/>
+      <c r="AD17" s="753"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -14464,15 +14468,15 @@
       <c r="E18" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F18" s="746"/>
-      <c r="G18" s="748"/>
+      <c r="F18" s="778"/>
+      <c r="G18" s="780"/>
       <c r="H18" s="108" t="s">
         <v>75</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="K18" s="766"/>
+      <c r="K18" s="759"/>
       <c r="O18" s="64" t="s">
         <v>114</v>
       </c>
@@ -14483,39 +14487,42 @@
       <c r="X18" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AA18" s="774"/>
-      <c r="AB18" s="775"/>
-      <c r="AD18" s="760"/>
+      <c r="AA18" s="767"/>
+      <c r="AB18" s="768"/>
+      <c r="AD18" s="753"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>207</v>
       </c>
-      <c r="G19" s="749"/>
-      <c r="K19" s="767"/>
+      <c r="G19" s="781"/>
+      <c r="K19" s="760"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="754" t="s">
+      <c r="R19" s="786" t="s">
         <v>123</v>
       </c>
-      <c r="S19" s="755"/>
-      <c r="T19" s="756"/>
+      <c r="S19" s="787"/>
+      <c r="T19" s="788"/>
       <c r="V19" s="77" t="s">
         <v>114</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="AD19" s="761"/>
+      <c r="AD19" s="754"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="M10:AC10"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="S12:S18"/>
+    <mergeCell ref="O3:O9"/>
     <mergeCell ref="AD1:AD19"/>
     <mergeCell ref="S8:AC8"/>
     <mergeCell ref="K5:K19"/>
@@ -14527,14 +14534,11 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L12:L15"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G19"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="S12:S18"/>
-    <mergeCell ref="O3:O9"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="M10:AC10"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rw Usage Updates S.1.0.0.1 _7:55PM
Boat Enabled -
InCapacity - [13] , NodeW - [-3] , BirdW - [6] , FuelW - [19] , OnHost - [5] .

Rw- Local(Left Running With Cost ) - [For Business/Shop/Market only] -
</commit_message>
<xml_diff>
--- a/System_2.2.1.xlsx
+++ b/System_2.2.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD06CC0C-C8BB-476C-84D1-A9F06C6B65B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01161D83-8F66-4FAB-9D1C-FAB8083118A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BoardRW" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1113" uniqueCount="621">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="624">
   <si>
     <t>Zone</t>
   </si>
@@ -1902,6 +1902,15 @@
   </si>
   <si>
     <t>tv9</t>
+  </si>
+  <si>
+    <t>Taiwan News</t>
+  </si>
+  <si>
+    <t>TaiwanNews</t>
+  </si>
+  <si>
+    <t>7F in Capacity</t>
   </si>
 </sst>
 </file>
@@ -5018,6 +5027,186 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5030,12 +5219,6 @@
     <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5047,12 +5230,6 @@
     </xf>
     <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
@@ -5075,190 +5252,61 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5300,43 +5348,25 @@
     <xf numFmtId="0" fontId="39" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5405,46 +5435,46 @@
     <xf numFmtId="14" fontId="5" fillId="14" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5522,46 +5552,25 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5859,8 +5868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:X28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="X5" sqref="X5"/>
+    <sheetView topLeftCell="C9" workbookViewId="0">
+      <selection activeCell="X14" sqref="X14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6583,7 +6592,9 @@
       </c>
       <c r="P22" s="313"/>
       <c r="T22" s="607"/>
-      <c r="X22" s="19"/>
+      <c r="X22" s="2" t="s">
+        <v>623</v>
+      </c>
     </row>
     <row r="23" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
@@ -6894,7 +6905,7 @@
       <c r="H1" s="97" t="s">
         <v>343</v>
       </c>
-      <c r="I1" s="613" t="s">
+      <c r="I1" s="659" t="s">
         <v>369</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -6930,7 +6941,7 @@
       <c r="X1" s="430" t="s">
         <v>155</v>
       </c>
-      <c r="Y1" s="657" t="s">
+      <c r="Y1" s="653" t="s">
         <v>528</v>
       </c>
       <c r="Z1" s="406">
@@ -6955,7 +6966,7 @@
         <v>498</v>
       </c>
       <c r="AM1" s="402"/>
-      <c r="AN1" s="640"/>
+      <c r="AN1" s="635"/>
       <c r="AO1" s="338" t="s">
         <v>469</v>
       </c>
@@ -6964,23 +6975,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="666">
+      <c r="A2" s="617">
         <f ca="1">TODAY()</f>
         <v>45289</v>
       </c>
-      <c r="B2" s="668" t="s">
+      <c r="B2" s="619" t="s">
         <v>370</v>
       </c>
-      <c r="C2" s="645" t="s">
+      <c r="C2" s="615" t="s">
         <v>357</v>
       </c>
-      <c r="D2" s="670" t="s">
+      <c r="D2" s="621" t="s">
         <v>355</v>
       </c>
-      <c r="E2" s="609" t="s">
+      <c r="E2" s="669" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="619" t="s">
+      <c r="F2" s="640" t="s">
         <v>102</v>
       </c>
       <c r="G2" s="393" t="s">
@@ -6989,31 +7000,31 @@
       <c r="H2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="614"/>
+      <c r="I2" s="660"/>
       <c r="J2" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="611" t="s">
+      <c r="K2" s="671" t="s">
         <v>342</v>
       </c>
-      <c r="L2" s="612"/>
-      <c r="M2" s="619" t="s">
+      <c r="L2" s="672"/>
+      <c r="M2" s="640" t="s">
         <v>102</v>
       </c>
       <c r="N2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="649" t="s">
+      <c r="O2" s="644" t="s">
         <v>102</v>
       </c>
       <c r="P2" s="85" t="s">
         <v>147</v>
       </c>
-      <c r="Q2" s="645" t="s">
+      <c r="Q2" s="615" t="s">
         <v>143</v>
       </c>
       <c r="R2" s="598"/>
-      <c r="S2" s="634" t="s">
+      <c r="S2" s="657" t="s">
         <v>148</v>
       </c>
       <c r="T2" s="89"/>
@@ -7023,7 +7034,7 @@
       <c r="X2" s="431" t="s">
         <v>156</v>
       </c>
-      <c r="Y2" s="658"/>
+      <c r="Y2" s="654"/>
       <c r="Z2" s="407">
         <v>1</v>
       </c>
@@ -7046,15 +7057,15 @@
         <v>463</v>
       </c>
       <c r="AM2" s="428"/>
-      <c r="AN2" s="641"/>
+      <c r="AN2" s="636"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="667"/>
-      <c r="B3" s="669"/>
-      <c r="C3" s="646"/>
-      <c r="D3" s="671"/>
-      <c r="E3" s="610"/>
-      <c r="F3" s="620"/>
+      <c r="A3" s="618"/>
+      <c r="B3" s="620"/>
+      <c r="C3" s="616"/>
+      <c r="D3" s="622"/>
+      <c r="E3" s="670"/>
+      <c r="F3" s="641"/>
       <c r="G3" s="394" t="s">
         <v>28</v>
       </c>
@@ -7073,17 +7084,17 @@
       <c r="L3" s="201" t="s">
         <v>107</v>
       </c>
-      <c r="M3" s="620"/>
+      <c r="M3" s="641"/>
       <c r="N3" s="69" t="s">
         <v>146</v>
       </c>
-      <c r="O3" s="650"/>
+      <c r="O3" s="645"/>
       <c r="P3" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="Q3" s="646"/>
+      <c r="Q3" s="616"/>
       <c r="R3" s="600"/>
-      <c r="S3" s="636"/>
+      <c r="S3" s="658"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -7091,7 +7102,7 @@
       <c r="X3" s="431" t="s">
         <v>157</v>
       </c>
-      <c r="Y3" s="658"/>
+      <c r="Y3" s="654"/>
       <c r="Z3" s="408">
         <v>1</v>
       </c>
@@ -7100,7 +7111,7 @@
       <c r="AC3" s="100" t="s">
         <v>480</v>
       </c>
-      <c r="AD3" s="631" t="s">
+      <c r="AD3" s="656" t="s">
         <v>455</v>
       </c>
       <c r="AE3" s="257"/>
@@ -7112,16 +7123,16 @@
       <c r="AK3" s="257"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="428"/>
-      <c r="AN3" s="641"/>
+      <c r="AN3" s="636"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="238" t="s">
         <v>183</v>
       </c>
-      <c r="B4" s="682" t="s">
+      <c r="B4" s="633" t="s">
         <v>373</v>
       </c>
-      <c r="C4" s="645" t="s">
+      <c r="C4" s="615" t="s">
         <v>154</v>
       </c>
       <c r="D4" s="347" t="s">
@@ -7130,7 +7141,7 @@
       <c r="E4" s="378">
         <v>2</v>
       </c>
-      <c r="F4" s="620"/>
+      <c r="F4" s="641"/>
       <c r="G4" s="381" t="s">
         <v>201</v>
       </c>
@@ -7147,11 +7158,11 @@
         <v>150</v>
       </c>
       <c r="L4" s="204"/>
-      <c r="M4" s="620"/>
+      <c r="M4" s="641"/>
       <c r="N4" s="174" t="s">
         <v>69</v>
       </c>
-      <c r="O4" s="650"/>
+      <c r="O4" s="645"/>
       <c r="P4" s="2" t="s">
         <v>191</v>
       </c>
@@ -7173,12 +7184,12 @@
       <c r="X4" s="431" t="s">
         <v>158</v>
       </c>
-      <c r="Y4" s="658"/>
+      <c r="Y4" s="654"/>
       <c r="Z4" s="409"/>
       <c r="AA4" s="307"/>
       <c r="AB4" s="209"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="631"/>
+      <c r="AD4" s="656"/>
       <c r="AE4" s="257"/>
       <c r="AF4" s="257"/>
       <c r="AG4" s="16"/>
@@ -7188,37 +7199,37 @@
       <c r="AK4" s="257"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="428"/>
-      <c r="AN4" s="641"/>
+      <c r="AN4" s="636"/>
       <c r="AO4" s="338" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="613" t="s">
+      <c r="A5" s="659" t="s">
         <v>418</v>
       </c>
-      <c r="B5" s="683"/>
-      <c r="C5" s="646"/>
+      <c r="B5" s="634"/>
+      <c r="C5" s="616"/>
       <c r="D5" s="61" t="s">
         <v>153</v>
       </c>
       <c r="E5" s="379">
         <v>1</v>
       </c>
-      <c r="F5" s="620"/>
-      <c r="G5" s="674" t="s">
+      <c r="F5" s="641"/>
+      <c r="G5" s="625" t="s">
         <v>192</v>
       </c>
-      <c r="H5" s="674"/>
-      <c r="I5" s="674"/>
-      <c r="J5" s="674"/>
-      <c r="K5" s="674"/>
-      <c r="L5" s="675"/>
-      <c r="M5" s="620"/>
+      <c r="H5" s="625"/>
+      <c r="I5" s="625"/>
+      <c r="J5" s="625"/>
+      <c r="K5" s="625"/>
+      <c r="L5" s="626"/>
+      <c r="M5" s="641"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
-      <c r="O5" s="650"/>
+      <c r="O5" s="645"/>
       <c r="T5" s="89"/>
       <c r="U5" s="124"/>
       <c r="V5" s="120"/>
@@ -7226,7 +7237,7 @@
       <c r="X5" s="431" t="s">
         <v>159</v>
       </c>
-      <c r="Y5" s="658"/>
+      <c r="Y5" s="654"/>
       <c r="Z5" s="409">
         <v>1</v>
       </c>
@@ -7249,24 +7260,24 @@
       <c r="AK5" s="257"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="428"/>
-      <c r="AN5" s="641"/>
+      <c r="AN5" s="636"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="614"/>
-      <c r="B6" s="680" t="s">
+      <c r="A6" s="660"/>
+      <c r="B6" s="631" t="s">
         <v>177</v>
       </c>
-      <c r="C6" s="628"/>
-      <c r="D6" s="629"/>
-      <c r="F6" s="620"/>
-      <c r="G6" s="676"/>
-      <c r="H6" s="676"/>
-      <c r="I6" s="676"/>
-      <c r="J6" s="676"/>
-      <c r="K6" s="676"/>
-      <c r="L6" s="677"/>
-      <c r="M6" s="620"/>
-      <c r="O6" s="650"/>
+      <c r="C6" s="661"/>
+      <c r="D6" s="662"/>
+      <c r="F6" s="641"/>
+      <c r="G6" s="627"/>
+      <c r="H6" s="627"/>
+      <c r="I6" s="627"/>
+      <c r="J6" s="627"/>
+      <c r="K6" s="627"/>
+      <c r="L6" s="628"/>
+      <c r="M6" s="641"/>
+      <c r="O6" s="645"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
       <c r="V6" s="98" t="s">
@@ -7276,7 +7287,7 @@
       <c r="X6" s="431" t="s">
         <v>160</v>
       </c>
-      <c r="Y6" s="658"/>
+      <c r="Y6" s="654"/>
       <c r="Z6" s="407">
         <v>1</v>
       </c>
@@ -7290,16 +7301,16 @@
       <c r="AF6" s="257"/>
       <c r="AG6" s="257"/>
       <c r="AH6" s="257"/>
-      <c r="AI6" s="630"/>
+      <c r="AI6" s="650"/>
       <c r="AJ6" s="441" t="s">
         <v>458</v>
       </c>
-      <c r="AK6" s="630" t="s">
+      <c r="AK6" s="650" t="s">
         <v>251</v>
       </c>
       <c r="AL6" s="257"/>
       <c r="AM6" s="428"/>
-      <c r="AN6" s="641"/>
+      <c r="AN6" s="636"/>
       <c r="AO6" s="338" t="s">
         <v>470</v>
       </c>
@@ -7308,7 +7319,7 @@
       <c r="A7" s="232" t="s">
         <v>571</v>
       </c>
-      <c r="B7" s="681"/>
+      <c r="B7" s="632"/>
       <c r="C7" s="202" t="s">
         <v>374</v>
       </c>
@@ -7318,7 +7329,7 @@
       <c r="E7" s="265">
         <v>3</v>
       </c>
-      <c r="F7" s="620"/>
+      <c r="F7" s="641"/>
       <c r="G7" s="395">
         <v>0</v>
       </c>
@@ -7337,8 +7348,8 @@
       <c r="L7" s="212">
         <v>0</v>
       </c>
-      <c r="M7" s="620"/>
-      <c r="O7" s="650"/>
+      <c r="M7" s="641"/>
+      <c r="O7" s="645"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
       </c>
@@ -7352,7 +7363,7 @@
       <c r="X7" s="431" t="s">
         <v>161</v>
       </c>
-      <c r="Y7" s="658"/>
+      <c r="Y7" s="654"/>
       <c r="Z7" s="407">
         <v>1</v>
       </c>
@@ -7362,18 +7373,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="257"/>
       <c r="AF7" s="257"/>
-      <c r="AG7" s="631" t="s">
+      <c r="AG7" s="656" t="s">
         <v>454</v>
       </c>
       <c r="AH7" s="257"/>
-      <c r="AI7" s="630"/>
+      <c r="AI7" s="650"/>
       <c r="AJ7" s="257"/>
-      <c r="AK7" s="630"/>
+      <c r="AK7" s="650"/>
       <c r="AL7" s="80" t="s">
         <v>496</v>
       </c>
       <c r="AM7" s="428"/>
-      <c r="AN7" s="641"/>
+      <c r="AN7" s="636"/>
       <c r="AP7" s="76" t="s">
         <v>471</v>
       </c>
@@ -7390,27 +7401,27 @@
         <f>SUM(G7:N9)</f>
         <v>15</v>
       </c>
-      <c r="F8" s="620"/>
-      <c r="G8" s="675">
-        <v>0</v>
-      </c>
-      <c r="H8" s="672" t="s">
+      <c r="F8" s="641"/>
+      <c r="G8" s="626">
+        <v>0</v>
+      </c>
+      <c r="H8" s="623" t="s">
         <v>104</v>
       </c>
       <c r="I8" s="598">
         <v>0</v>
       </c>
-      <c r="J8" s="672" t="s">
+      <c r="J8" s="623" t="s">
         <v>104</v>
       </c>
-      <c r="K8" s="678"/>
-      <c r="L8" s="632"/>
-      <c r="M8" s="647"/>
-      <c r="N8" s="637">
+      <c r="K8" s="629"/>
+      <c r="L8" s="663"/>
+      <c r="M8" s="642"/>
+      <c r="N8" s="666">
         <f>N5+N11</f>
         <v>15</v>
       </c>
-      <c r="O8" s="650"/>
+      <c r="O8" s="645"/>
       <c r="T8" s="103" t="s">
         <v>44</v>
       </c>
@@ -7420,7 +7431,7 @@
       <c r="X8" s="431" t="s">
         <v>162</v>
       </c>
-      <c r="Y8" s="658"/>
+      <c r="Y8" s="654"/>
       <c r="Z8" s="409"/>
       <c r="AA8" s="307"/>
       <c r="AB8" s="209"/>
@@ -7428,14 +7439,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="257"/>
       <c r="AF8" s="257"/>
-      <c r="AG8" s="631"/>
+      <c r="AG8" s="656"/>
       <c r="AH8" s="257"/>
-      <c r="AI8" s="630"/>
+      <c r="AI8" s="650"/>
       <c r="AJ8" s="257"/>
       <c r="AK8" s="257"/>
       <c r="AL8" s="257"/>
       <c r="AM8" s="428"/>
-      <c r="AN8" s="641"/>
+      <c r="AN8" s="636"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="232" t="s">
@@ -7450,17 +7461,17 @@
       <c r="D9" s="348" t="s">
         <v>281</v>
       </c>
-      <c r="F9" s="620"/>
-      <c r="G9" s="677"/>
-      <c r="H9" s="673"/>
+      <c r="F9" s="641"/>
+      <c r="G9" s="628"/>
+      <c r="H9" s="624"/>
       <c r="I9" s="600"/>
-      <c r="J9" s="673"/>
-      <c r="K9" s="679"/>
-      <c r="L9" s="633"/>
-      <c r="M9" s="648"/>
-      <c r="N9" s="638"/>
-      <c r="O9" s="651"/>
-      <c r="S9" s="634" t="s">
+      <c r="J9" s="624"/>
+      <c r="K9" s="630"/>
+      <c r="L9" s="664"/>
+      <c r="M9" s="643"/>
+      <c r="N9" s="667"/>
+      <c r="O9" s="646"/>
+      <c r="S9" s="657" t="s">
         <v>61</v>
       </c>
       <c r="T9" s="89"/>
@@ -7472,7 +7483,7 @@
       <c r="X9" s="431" t="s">
         <v>163</v>
       </c>
-      <c r="Y9" s="658"/>
+      <c r="Y9" s="654"/>
       <c r="Z9" s="410"/>
       <c r="AA9" s="307"/>
       <c r="AB9" s="209"/>
@@ -7482,16 +7493,16 @@
       </c>
       <c r="AE9" s="257"/>
       <c r="AF9" s="257"/>
-      <c r="AG9" s="631"/>
+      <c r="AG9" s="656"/>
       <c r="AH9" s="257"/>
-      <c r="AI9" s="630"/>
+      <c r="AI9" s="650"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="630" t="s">
+      <c r="AK9" s="650" t="s">
         <v>251</v>
       </c>
       <c r="AL9" s="257"/>
       <c r="AM9" s="428"/>
-      <c r="AN9" s="641"/>
+      <c r="AN9" s="636"/>
       <c r="AP9" s="2" t="s">
         <v>508</v>
       </c>
@@ -7508,20 +7519,20 @@
         <f>Boat!W8</f>
         <v>37</v>
       </c>
-      <c r="F10" s="620"/>
+      <c r="F10" s="641"/>
       <c r="N10" s="418" t="s">
         <v>396</v>
       </c>
-      <c r="O10" s="622" t="s">
+      <c r="O10" s="678" t="s">
         <v>102</v>
       </c>
-      <c r="P10" s="652" t="s">
+      <c r="P10" s="647" t="s">
         <v>400</v>
       </c>
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="635"/>
+      <c r="S10" s="665"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>176</v>
@@ -7533,7 +7544,7 @@
       <c r="X10" s="431" t="s">
         <v>164</v>
       </c>
-      <c r="Y10" s="658"/>
+      <c r="Y10" s="654"/>
       <c r="Z10" s="409">
         <v>0</v>
       </c>
@@ -7551,16 +7562,16 @@
       <c r="AF10" s="238" t="s">
         <v>311</v>
       </c>
-      <c r="AG10" s="631"/>
+      <c r="AG10" s="656"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="630"/>
+      <c r="AI10" s="650"/>
       <c r="AJ10" s="257"/>
-      <c r="AK10" s="630"/>
+      <c r="AK10" s="650"/>
       <c r="AL10" s="257"/>
       <c r="AM10" s="442" t="s">
         <v>318</v>
       </c>
-      <c r="AN10" s="641"/>
+      <c r="AN10" s="636"/>
       <c r="AO10" s="204" t="s">
         <v>94</v>
       </c>
@@ -7578,18 +7589,18 @@
       <c r="D11" s="170" t="s">
         <v>355</v>
       </c>
-      <c r="F11" s="620"/>
+      <c r="F11" s="641"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="623"/>
-      <c r="P11" s="653"/>
+      <c r="O11" s="679"/>
+      <c r="P11" s="648"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>220</v>
       </c>
-      <c r="S11" s="635"/>
+      <c r="S11" s="665"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -7599,7 +7610,7 @@
       <c r="X11" s="431" t="s">
         <v>165</v>
       </c>
-      <c r="Y11" s="658"/>
+      <c r="Y11" s="654"/>
       <c r="Z11" s="409"/>
       <c r="AA11" s="307">
         <v>1</v>
@@ -7613,14 +7624,14 @@
       <c r="AF11" s="257" t="s">
         <v>476</v>
       </c>
-      <c r="AG11" s="631"/>
+      <c r="AG11" s="656"/>
       <c r="AH11" s="257"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="257"/>
       <c r="AK11" s="257"/>
       <c r="AL11" s="257"/>
       <c r="AM11" s="428"/>
-      <c r="AN11" s="641"/>
+      <c r="AN11" s="636"/>
       <c r="AP11" s="76" t="s">
         <v>484</v>
       </c>
@@ -7639,7 +7650,7 @@
       <c r="E12" s="224">
         <v>3</v>
       </c>
-      <c r="F12" s="620"/>
+      <c r="F12" s="641"/>
       <c r="G12" s="337" t="s">
         <v>400</v>
       </c>
@@ -7648,16 +7659,16 @@
       </c>
       <c r="I12" s="605"/>
       <c r="J12" s="605"/>
-      <c r="K12" s="627"/>
+      <c r="K12" s="683"/>
       <c r="L12" s="203"/>
       <c r="M12" s="203"/>
       <c r="N12" s="203"/>
-      <c r="O12" s="623"/>
-      <c r="P12" s="653"/>
+      <c r="O12" s="679"/>
+      <c r="P12" s="648"/>
       <c r="R12" s="122" t="s">
         <v>180</v>
       </c>
-      <c r="S12" s="636"/>
+      <c r="S12" s="658"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -7667,7 +7678,7 @@
       <c r="X12" s="431" t="s">
         <v>166</v>
       </c>
-      <c r="Y12" s="658"/>
+      <c r="Y12" s="654"/>
       <c r="Z12" s="407">
         <v>1</v>
       </c>
@@ -7678,16 +7689,16 @@
       <c r="AC12" s="100" t="s">
         <v>481</v>
       </c>
-      <c r="AD12" s="639" t="s">
+      <c r="AD12" s="668" t="s">
         <v>240</v>
       </c>
       <c r="AE12" s="441" t="s">
         <v>239</v>
       </c>
-      <c r="AF12" s="631" t="s">
+      <c r="AF12" s="656" t="s">
         <v>228</v>
       </c>
-      <c r="AG12" s="631"/>
+      <c r="AG12" s="656"/>
       <c r="AH12" s="238" t="s">
         <v>259</v>
       </c>
@@ -7697,10 +7708,10 @@
       <c r="AJ12" s="257"/>
       <c r="AK12" s="257"/>
       <c r="AL12" s="257"/>
-      <c r="AM12" s="655" t="s">
+      <c r="AM12" s="651" t="s">
         <v>249</v>
       </c>
-      <c r="AN12" s="641"/>
+      <c r="AN12" s="636"/>
       <c r="AO12" s="338" t="s">
         <v>96</v>
       </c>
@@ -7712,17 +7723,17 @@
       <c r="E13" s="448">
         <v>-3</v>
       </c>
-      <c r="F13" s="620"/>
+      <c r="F13" s="641"/>
       <c r="G13" s="605" t="s">
         <v>430</v>
       </c>
       <c r="H13" s="605"/>
       <c r="I13" s="605"/>
-      <c r="J13" s="627"/>
+      <c r="J13" s="683"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="623"/>
-      <c r="P13" s="654"/>
+      <c r="O13" s="679"/>
+      <c r="P13" s="649"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
       </c>
@@ -7732,7 +7743,7 @@
       <c r="X13" s="431" t="s">
         <v>167</v>
       </c>
-      <c r="Y13" s="658"/>
+      <c r="Y13" s="654"/>
       <c r="Z13" s="407">
         <v>1</v>
       </c>
@@ -7743,8 +7754,8 @@
         <v>500</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="639"/>
-      <c r="AF13" s="631"/>
+      <c r="AD13" s="668"/>
+      <c r="AF13" s="656"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="238" t="s">
         <v>308</v>
@@ -7755,8 +7766,8 @@
       <c r="AJ13" s="80"/>
       <c r="AK13" s="257"/>
       <c r="AL13" s="257"/>
-      <c r="AM13" s="655"/>
-      <c r="AN13" s="641"/>
+      <c r="AM13" s="651"/>
+      <c r="AN13" s="636"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="450"/>
@@ -7764,18 +7775,18 @@
       <c r="C14" s="459"/>
       <c r="D14" s="452"/>
       <c r="E14" s="453"/>
-      <c r="F14" s="620"/>
+      <c r="F14" s="641"/>
       <c r="G14" s="605" t="s">
         <v>429</v>
       </c>
       <c r="H14" s="605"/>
       <c r="I14" s="605"/>
-      <c r="J14" s="627"/>
+      <c r="J14" s="683"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="623"/>
+      <c r="O14" s="679"/>
       <c r="Q14" s="61" t="s">
         <v>532</v>
       </c>
@@ -7789,24 +7800,24 @@
       <c r="X14" s="431" t="s">
         <v>168</v>
       </c>
-      <c r="Y14" s="658"/>
+      <c r="Y14" s="654"/>
       <c r="Z14" s="407">
         <v>1</v>
       </c>
       <c r="AA14" s="307"/>
       <c r="AB14" s="209"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="639"/>
+      <c r="AD14" s="668"/>
       <c r="AE14" s="257"/>
-      <c r="AF14" s="631"/>
+      <c r="AF14" s="656"/>
       <c r="AG14" s="257"/>
       <c r="AH14" s="257"/>
       <c r="AI14" s="70"/>
       <c r="AJ14" s="257"/>
       <c r="AK14" s="257"/>
       <c r="AL14" s="257"/>
-      <c r="AM14" s="655"/>
-      <c r="AN14" s="641"/>
+      <c r="AM14" s="651"/>
+      <c r="AN14" s="636"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="449" t="s">
@@ -7815,8 +7826,8 @@
       <c r="C15" s="598" t="s">
         <v>373</v>
       </c>
-      <c r="F15" s="620"/>
-      <c r="O15" s="623"/>
+      <c r="F15" s="641"/>
+      <c r="O15" s="679"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -7829,7 +7840,7 @@
       <c r="X15" s="431" t="s">
         <v>169</v>
       </c>
-      <c r="Y15" s="658"/>
+      <c r="Y15" s="654"/>
       <c r="Z15" s="409">
         <v>1</v>
       </c>
@@ -7838,8 +7849,8 @@
       <c r="AC15" s="76" t="s">
         <v>479</v>
       </c>
-      <c r="AD15" s="639"/>
-      <c r="AF15" s="631"/>
+      <c r="AD15" s="668"/>
+      <c r="AF15" s="656"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="238" t="s">
         <v>448</v>
@@ -7852,8 +7863,8 @@
       </c>
       <c r="AK15" s="257"/>
       <c r="AL15" s="257"/>
-      <c r="AM15" s="655"/>
-      <c r="AN15" s="641"/>
+      <c r="AM15" s="651"/>
+      <c r="AN15" s="636"/>
       <c r="AP15" s="76" t="s">
         <v>73</v>
       </c>
@@ -7875,13 +7886,13 @@
       <c r="E16" s="224">
         <v>1</v>
       </c>
-      <c r="F16" s="620"/>
+      <c r="F16" s="641"/>
       <c r="G16" s="337" t="s">
         <v>488</v>
       </c>
       <c r="I16" s="469"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="623"/>
+      <c r="O16" s="679"/>
       <c r="R16" s="435" t="s">
         <v>184</v>
       </c>
@@ -7892,7 +7903,7 @@
       <c r="X16" s="431" t="s">
         <v>170</v>
       </c>
-      <c r="Y16" s="658"/>
+      <c r="Y16" s="654"/>
       <c r="Z16" s="407">
         <v>1</v>
       </c>
@@ -7913,18 +7924,18 @@
       <c r="AM16" s="428" t="s">
         <v>317</v>
       </c>
-      <c r="AN16" s="641"/>
+      <c r="AN16" s="636"/>
       <c r="AP16" s="76" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="620"/>
+      <c r="F17" s="641"/>
       <c r="I17" s="470"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="623"/>
+      <c r="O17" s="679"/>
       <c r="Q17" s="21" t="s">
         <v>530</v>
       </c>
@@ -7944,7 +7955,7 @@
       <c r="X17" s="431" t="s">
         <v>171</v>
       </c>
-      <c r="Y17" s="658"/>
+      <c r="Y17" s="654"/>
       <c r="Z17" s="409"/>
       <c r="AA17" s="307"/>
       <c r="AB17" s="209"/>
@@ -7969,7 +7980,7 @@
       <c r="AK17" s="257"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="428"/>
-      <c r="AN17" s="641"/>
+      <c r="AN17" s="636"/>
       <c r="AO17" s="204" t="s">
         <v>497</v>
       </c>
@@ -7993,21 +8004,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="620"/>
+      <c r="F18" s="641"/>
       <c r="G18" s="337" t="s">
         <v>527</v>
       </c>
       <c r="I18" s="24"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="623"/>
+      <c r="O18" s="679"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="615" t="s">
+      <c r="R18" s="673" t="s">
         <v>535</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="663" t="s">
+      <c r="U18" s="612" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -8017,7 +8028,7 @@
       <c r="X18" s="431" t="s">
         <v>172</v>
       </c>
-      <c r="Y18" s="658"/>
+      <c r="Y18" s="654"/>
       <c r="Z18" s="409">
         <v>1</v>
       </c>
@@ -8028,38 +8039,38 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="257"/>
-      <c r="AF18" s="630" t="s">
+      <c r="AF18" s="650" t="s">
         <v>475</v>
       </c>
       <c r="AG18" s="257"/>
       <c r="AH18" s="70"/>
       <c r="AI18" s="70"/>
-      <c r="AJ18" s="656" t="s">
+      <c r="AJ18" s="652" t="s">
         <v>315</v>
       </c>
       <c r="AK18" s="257"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="428"/>
-      <c r="AN18" s="641"/>
+      <c r="AN18" s="636"/>
       <c r="AP18" s="76" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="620"/>
+      <c r="F19" s="641"/>
       <c r="I19" s="219"/>
-      <c r="O19" s="623"/>
-      <c r="R19" s="616"/>
+      <c r="O19" s="679"/>
+      <c r="R19" s="674"/>
       <c r="S19" s="30" t="s">
         <v>533</v>
       </c>
-      <c r="U19" s="664"/>
+      <c r="U19" s="613"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="431" t="s">
         <v>173</v>
       </c>
-      <c r="Y19" s="658"/>
+      <c r="Y19" s="654"/>
       <c r="Z19" s="407">
         <v>1</v>
       </c>
@@ -8068,17 +8079,17 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="257"/>
-      <c r="AF19" s="630"/>
+      <c r="AF19" s="650"/>
       <c r="AG19" s="257"/>
       <c r="AH19" s="257"/>
       <c r="AI19" s="70"/>
-      <c r="AJ19" s="656"/>
+      <c r="AJ19" s="652"/>
       <c r="AK19" s="460" t="s">
         <v>251</v>
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="428"/>
-      <c r="AN19" s="641"/>
+      <c r="AN19" s="636"/>
       <c r="AP19" s="76" t="s">
         <v>468</v>
       </c>
@@ -8099,24 +8110,24 @@
       <c r="E20" s="437">
         <v>-1</v>
       </c>
-      <c r="F20" s="620"/>
+      <c r="F20" s="641"/>
       <c r="G20" s="337" t="s">
         <v>491</v>
       </c>
       <c r="I20" s="219"/>
-      <c r="O20" s="623"/>
-      <c r="Q20" s="625" t="s">
+      <c r="O20" s="679"/>
+      <c r="Q20" s="681" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="404" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="665"/>
+      <c r="U20" s="614"/>
       <c r="W20" s="405"/>
       <c r="X20" s="432" t="s">
         <v>174</v>
       </c>
-      <c r="Y20" s="658"/>
+      <c r="Y20" s="654"/>
       <c r="Z20" s="411">
         <v>1</v>
       </c>
@@ -8141,7 +8152,7 @@
       <c r="AM20" s="381" t="s">
         <v>249</v>
       </c>
-      <c r="AN20" s="641"/>
+      <c r="AN20" s="636"/>
       <c r="AO20" s="338" t="s">
         <v>460</v>
       </c>
@@ -8162,20 +8173,20 @@
       <c r="E21" s="265">
         <v>0</v>
       </c>
-      <c r="F21" s="620"/>
+      <c r="F21" s="641"/>
       <c r="I21" s="219"/>
-      <c r="O21" s="623"/>
-      <c r="Q21" s="626"/>
+      <c r="O21" s="679"/>
+      <c r="Q21" s="682"/>
       <c r="T21" s="422"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="660"/>
+      <c r="V21" s="609"/>
       <c r="W21" s="426" t="s">
         <v>175</v>
       </c>
       <c r="X21" s="429" t="s">
         <v>186</v>
       </c>
-      <c r="Y21" s="658"/>
+      <c r="Y21" s="654"/>
       <c r="Z21" s="445">
         <v>3</v>
       </c>
@@ -8206,15 +8217,15 @@
       <c r="AM21" s="428" t="s">
         <v>544</v>
       </c>
-      <c r="AN21" s="641"/>
+      <c r="AN21" s="636"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="620"/>
+      <c r="F22" s="641"/>
       <c r="G22" s="337" t="s">
         <v>489</v>
       </c>
       <c r="I22" s="219"/>
-      <c r="O22" s="623"/>
+      <c r="O22" s="679"/>
       <c r="R22" s="434" t="s">
         <v>44</v>
       </c>
@@ -8222,14 +8233,14 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="661"/>
+      <c r="V22" s="610"/>
       <c r="W22" s="426" t="s">
         <v>175</v>
       </c>
       <c r="X22" s="429" t="s">
         <v>187</v>
       </c>
-      <c r="Y22" s="658"/>
+      <c r="Y22" s="654"/>
       <c r="Z22" s="415"/>
       <c r="AA22" s="10"/>
       <c r="AB22" s="415"/>
@@ -8240,7 +8251,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="630" t="s">
+      <c r="AJ22" s="650" t="s">
         <v>472</v>
       </c>
       <c r="AK22" s="257"/>
@@ -8248,7 +8259,7 @@
         <v>478</v>
       </c>
       <c r="AM22" s="300"/>
-      <c r="AN22" s="641"/>
+      <c r="AN22" s="636"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="231" t="s">
@@ -8266,22 +8277,22 @@
       <c r="E23" s="225">
         <v>1</v>
       </c>
-      <c r="F23" s="620"/>
+      <c r="F23" s="641"/>
       <c r="I23" s="219"/>
-      <c r="O23" s="623"/>
-      <c r="Q23" s="625" t="s">
+      <c r="O23" s="679"/>
+      <c r="Q23" s="681" t="s">
         <v>144</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="420" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="661"/>
+      <c r="V23" s="610"/>
       <c r="W23" s="148"/>
       <c r="X23" s="429" t="s">
         <v>188</v>
       </c>
-      <c r="Y23" s="658"/>
+      <c r="Y23" s="654"/>
       <c r="Z23" s="17"/>
       <c r="AA23" s="10"/>
       <c r="AB23" s="415"/>
@@ -8292,13 +8303,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="630"/>
+      <c r="AJ23" s="650"/>
       <c r="AK23" s="257"/>
       <c r="AL23" s="80" t="s">
         <v>507</v>
       </c>
       <c r="AM23" s="300"/>
-      <c r="AN23" s="641"/>
+      <c r="AN23" s="636"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="440" t="s">
@@ -8316,23 +8327,23 @@
       <c r="E24" s="436">
         <v>1</v>
       </c>
-      <c r="F24" s="620"/>
+      <c r="F24" s="641"/>
       <c r="G24" s="61" t="s">
         <v>490</v>
       </c>
       <c r="I24" s="219"/>
-      <c r="O24" s="623"/>
-      <c r="Q24" s="626"/>
+      <c r="O24" s="679"/>
+      <c r="Q24" s="682"/>
       <c r="T24" s="17"/>
       <c r="U24" s="227" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="661"/>
+      <c r="V24" s="610"/>
       <c r="W24" s="148"/>
       <c r="X24" s="429" t="s">
         <v>185</v>
       </c>
-      <c r="Y24" s="658"/>
+      <c r="Y24" s="654"/>
       <c r="Z24" s="17"/>
       <c r="AA24" s="10"/>
       <c r="AB24" s="415"/>
@@ -8351,12 +8362,12 @@
         <v>463</v>
       </c>
       <c r="AM24" s="300"/>
-      <c r="AN24" s="641"/>
+      <c r="AN24" s="636"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="620"/>
+      <c r="F25" s="641"/>
       <c r="I25" s="219"/>
-      <c r="O25" s="623"/>
+      <c r="O25" s="679"/>
       <c r="P25" s="204" t="s">
         <v>280</v>
       </c>
@@ -8369,12 +8380,12 @@
       <c r="U25" s="400" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="662"/>
+      <c r="V25" s="611"/>
       <c r="W25" s="148"/>
       <c r="X25" s="429" t="s">
         <v>189</v>
       </c>
-      <c r="Y25" s="658"/>
+      <c r="Y25" s="654"/>
       <c r="Z25" s="17"/>
       <c r="AA25" s="10"/>
       <c r="AB25" s="415"/>
@@ -8391,7 +8402,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="300"/>
-      <c r="AN25" s="641"/>
+      <c r="AN25" s="636"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="231" t="s">
@@ -8409,17 +8420,17 @@
       <c r="E26" s="380">
         <v>1</v>
       </c>
-      <c r="F26" s="620"/>
+      <c r="F26" s="641"/>
       <c r="G26" s="337" t="s">
         <v>487</v>
       </c>
       <c r="I26" s="219"/>
-      <c r="O26" s="623"/>
-      <c r="P26" s="643" t="s">
+      <c r="O26" s="679"/>
+      <c r="P26" s="638" t="s">
         <v>525</v>
       </c>
-      <c r="Q26" s="644"/>
-      <c r="R26" s="617" t="s">
+      <c r="Q26" s="639"/>
+      <c r="R26" s="675" t="s">
         <v>534</v>
       </c>
       <c r="T26" s="178"/>
@@ -8431,7 +8442,7 @@
       <c r="X26" s="429" t="s">
         <v>181</v>
       </c>
-      <c r="Y26" s="658"/>
+      <c r="Y26" s="654"/>
       <c r="Z26" s="17"/>
       <c r="AA26" s="10"/>
       <c r="AB26" s="415"/>
@@ -8458,7 +8469,7 @@
       <c r="AM26" s="442" t="s">
         <v>456</v>
       </c>
-      <c r="AN26" s="641"/>
+      <c r="AN26" s="636"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -8470,13 +8481,13 @@
       <c r="E27" s="265" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="621"/>
+      <c r="F27" s="677"/>
       <c r="G27" s="61" t="s">
         <v>543</v>
       </c>
       <c r="I27" s="220"/>
-      <c r="O27" s="624"/>
-      <c r="R27" s="618"/>
+      <c r="O27" s="680"/>
+      <c r="R27" s="676"/>
       <c r="S27" s="421" t="s">
         <v>54</v>
       </c>
@@ -8489,7 +8500,7 @@
       <c r="X27" s="429" t="s">
         <v>529</v>
       </c>
-      <c r="Y27" s="659"/>
+      <c r="Y27" s="655"/>
       <c r="Z27" s="161"/>
       <c r="AA27" s="13"/>
       <c r="AB27" s="416"/>
@@ -8506,10 +8517,48 @@
       <c r="AM27" s="381" t="s">
         <v>319</v>
       </c>
-      <c r="AN27" s="642"/>
+      <c r="AN27" s="637"/>
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="O10:O27"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="AI6:AI10"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AG7:AG12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="AN1:AN27"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="M2:M9"/>
+    <mergeCell ref="O2:O9"/>
+    <mergeCell ref="P10:P13"/>
+    <mergeCell ref="AK6:AK7"/>
+    <mergeCell ref="AM12:AM15"/>
+    <mergeCell ref="AF18:AF19"/>
+    <mergeCell ref="AJ18:AJ19"/>
+    <mergeCell ref="Y1:Y27"/>
+    <mergeCell ref="AJ22:AJ23"/>
+    <mergeCell ref="AK9:AK10"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="R2:R3"/>
     <mergeCell ref="V21:V25"/>
     <mergeCell ref="U18:U20"/>
     <mergeCell ref="C2:C3"/>
@@ -8526,44 +8575,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="AN1:AN27"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="M2:M9"/>
-    <mergeCell ref="O2:O9"/>
-    <mergeCell ref="P10:P13"/>
-    <mergeCell ref="AK6:AK7"/>
-    <mergeCell ref="AM12:AM15"/>
-    <mergeCell ref="AF18:AF19"/>
-    <mergeCell ref="AJ18:AJ19"/>
-    <mergeCell ref="Y1:Y27"/>
-    <mergeCell ref="AJ22:AJ23"/>
-    <mergeCell ref="AK9:AK10"/>
-    <mergeCell ref="AD3:AD4"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AI6:AI10"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AG7:AG12"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="F2:F27"/>
-    <mergeCell ref="O10:O27"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8600,12 +8611,12 @@
       <c r="B1" s="603" t="s">
         <v>310</v>
       </c>
-      <c r="C1" s="627"/>
+      <c r="C1" s="683"/>
       <c r="D1" s="204"/>
       <c r="J1" s="603" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="627"/>
+      <c r="K1" s="683"/>
       <c r="L1" s="195" t="s">
         <v>330</v>
       </c>
@@ -8939,8 +8950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB54FD83-008D-4F8B-87AC-83E7F70047CB}">
   <dimension ref="A1:AL31"/>
   <sheetViews>
-    <sheetView topLeftCell="N12" workbookViewId="0">
-      <selection activeCell="AH17" sqref="AH17"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8966,7 +8977,7 @@
     <col min="19" max="19" width="3.140625" style="20" customWidth="1"/>
     <col min="20" max="20" width="9.7109375" style="20" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="3.7109375" style="20" customWidth="1"/>
-    <col min="23" max="23" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="3.85546875" style="20" customWidth="1"/>
     <col min="25" max="25" width="3.28515625" customWidth="1"/>
     <col min="26" max="26" width="7" style="20" bestFit="1" customWidth="1"/>
@@ -9008,7 +9019,7 @@
       <c r="P1" s="398" t="s">
         <v>397</v>
       </c>
-      <c r="Q1" s="701" t="s">
+      <c r="Q1" s="714" t="s">
         <v>180</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -9032,7 +9043,7 @@
       <c r="AA1" s="517" t="s">
         <v>437</v>
       </c>
-      <c r="AB1" s="695" t="s">
+      <c r="AB1" s="708" t="s">
         <v>593</v>
       </c>
       <c r="AC1" s="99" t="s">
@@ -9054,32 +9065,32 @@
       </c>
     </row>
     <row r="2" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="706">
+      <c r="A2" s="693">
         <f ca="1">TODAY()</f>
         <v>45289</v>
       </c>
-      <c r="B2" s="708" t="s">
+      <c r="B2" s="695" t="s">
         <v>379</v>
       </c>
-      <c r="C2" s="645" t="s">
+      <c r="C2" s="615" t="s">
         <v>357</v>
       </c>
-      <c r="D2" s="710" t="s">
+      <c r="D2" s="697" t="s">
         <v>102</v>
       </c>
-      <c r="E2" s="712" t="s">
+      <c r="E2" s="699" t="s">
         <v>64</v>
       </c>
       <c r="F2" s="191" t="s">
         <v>218</v>
       </c>
-      <c r="G2" s="613" t="s">
+      <c r="G2" s="659" t="s">
         <v>372</v>
       </c>
       <c r="H2" s="206" t="s">
         <v>218</v>
       </c>
-      <c r="I2" s="692" t="s">
+      <c r="I2" s="705" t="s">
         <v>102</v>
       </c>
       <c r="J2" s="396" t="s">
@@ -9103,10 +9114,10 @@
       <c r="P2" s="399">
         <v>40</v>
       </c>
-      <c r="Q2" s="702"/>
+      <c r="Q2" s="715"/>
       <c r="R2" s="21">
         <f>R7+R20</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S2" s="21">
         <f>S7+S20</f>
@@ -9128,7 +9139,7 @@
         <f>IF((Z2+T2)&gt;0,0,-1)</f>
         <v>0</v>
       </c>
-      <c r="AB2" s="696"/>
+      <c r="AB2" s="709"/>
       <c r="AC2" s="35"/>
       <c r="AH2" s="6" t="s">
         <v>344</v>
@@ -9143,14 +9154,14 @@
       </c>
     </row>
     <row r="3" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="707"/>
-      <c r="B3" s="709"/>
-      <c r="C3" s="646"/>
-      <c r="D3" s="711"/>
-      <c r="E3" s="713"/>
-      <c r="G3" s="614"/>
+      <c r="A3" s="694"/>
+      <c r="B3" s="696"/>
+      <c r="C3" s="616"/>
+      <c r="D3" s="698"/>
+      <c r="E3" s="700"/>
+      <c r="G3" s="660"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="693"/>
+      <c r="I3" s="706"/>
       <c r="K3" s="24">
         <v>2</v>
       </c>
@@ -9165,7 +9176,7 @@
       <c r="V3" s="470"/>
       <c r="W3" s="6"/>
       <c r="X3" s="470"/>
-      <c r="AB3" s="696"/>
+      <c r="AB3" s="709"/>
       <c r="AC3" s="35"/>
       <c r="AE3" s="100" t="s">
         <v>588</v>
@@ -9194,10 +9205,10 @@
         <v>380</v>
       </c>
       <c r="B4" s="243"/>
-      <c r="C4" s="714" t="s">
+      <c r="C4" s="701" t="s">
         <v>177</v>
       </c>
-      <c r="I4" s="693"/>
+      <c r="I4" s="706"/>
       <c r="R4" s="471" t="s">
         <v>588</v>
       </c>
@@ -9209,7 +9220,7 @@
       <c r="V4" s="470"/>
       <c r="W4" s="6"/>
       <c r="X4" s="470"/>
-      <c r="AB4" s="696"/>
+      <c r="AB4" s="709"/>
       <c r="AC4" s="35"/>
       <c r="AE4" s="20"/>
       <c r="AF4" s="100" t="s">
@@ -9217,7 +9228,7 @@
       </c>
       <c r="AG4" s="24">
         <f>IF((AF7-SUM(AI2:AI10)&lt;0),AF7-SUM(AI2:AI10),0)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AH4" s="6" t="s">
         <v>251</v>
@@ -9234,7 +9245,7 @@
       <c r="B5" s="100" t="s">
         <v>357</v>
       </c>
-      <c r="C5" s="715"/>
+      <c r="C5" s="702"/>
       <c r="D5" s="222" t="s">
         <v>102</v>
       </c>
@@ -9250,7 +9261,7 @@
       <c r="H5" s="206" t="s">
         <v>218</v>
       </c>
-      <c r="I5" s="693"/>
+      <c r="I5" s="706"/>
       <c r="J5" s="397" t="s">
         <v>268</v>
       </c>
@@ -9277,7 +9288,7 @@
       <c r="V5" s="468"/>
       <c r="W5" s="6"/>
       <c r="X5" s="468"/>
-      <c r="AB5" s="696"/>
+      <c r="AB5" s="709"/>
       <c r="AC5" s="2" t="s">
         <v>591</v>
       </c>
@@ -9297,19 +9308,19 @@
       <c r="AL5" s="468"/>
     </row>
     <row r="6" spans="1:38" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="703" t="s">
+      <c r="A6" s="690" t="s">
         <v>285</v>
       </c>
       <c r="B6" s="105" t="s">
         <v>198</v>
       </c>
-      <c r="C6" s="628"/>
-      <c r="D6" s="629"/>
+      <c r="C6" s="661"/>
+      <c r="D6" s="662"/>
       <c r="E6" s="96">
         <v>1</v>
       </c>
       <c r="G6" s="599"/>
-      <c r="I6" s="693"/>
+      <c r="I6" s="706"/>
       <c r="P6" s="61" t="s">
         <v>591</v>
       </c>
@@ -9321,7 +9332,7 @@
         <f>S7+S11-SUM(V2:V10)</f>
         <v>3</v>
       </c>
-      <c r="AB6" s="696"/>
+      <c r="AB6" s="709"/>
       <c r="AC6" s="35"/>
       <c r="AE6" s="64">
         <f>AE7-SUM(AL2:AL10)+AE11</f>
@@ -9329,7 +9340,7 @@
       </c>
       <c r="AF6" s="64">
         <f>AF7-SUM(AI2:AI10)+AF11</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH6" s="6"/>
       <c r="AI6" s="525"/>
@@ -9337,7 +9348,7 @@
       <c r="AL6" s="112"/>
     </row>
     <row r="7" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="704"/>
+      <c r="A7" s="691"/>
       <c r="B7" s="100" t="s">
         <v>154</v>
       </c>
@@ -9348,7 +9359,7 @@
         <v>135</v>
       </c>
       <c r="G7" s="599"/>
-      <c r="I7" s="693"/>
+      <c r="I7" s="706"/>
       <c r="M7" s="16" t="s">
         <v>347</v>
       </c>
@@ -9378,7 +9389,7 @@
         <v>249</v>
       </c>
       <c r="X7" s="469"/>
-      <c r="AB7" s="696"/>
+      <c r="AB7" s="709"/>
       <c r="AC7" s="99" t="s">
         <v>592</v>
       </c>
@@ -9391,7 +9402,7 @@
       </c>
       <c r="AF7" s="295">
         <f>8-AF11</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AH7" s="6" t="s">
         <v>249</v>
@@ -9406,7 +9417,7 @@
       <c r="AL7" s="24"/>
     </row>
     <row r="8" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="705"/>
+      <c r="A8" s="692"/>
       <c r="B8" s="212" t="s">
         <v>28</v>
       </c>
@@ -9415,7 +9426,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="599"/>
-      <c r="I8" s="693"/>
+      <c r="I8" s="706"/>
       <c r="N8" s="80"/>
       <c r="U8" s="6"/>
       <c r="V8" s="24"/>
@@ -9423,12 +9434,14 @@
         <v>611</v>
       </c>
       <c r="X8" s="470"/>
-      <c r="AB8" s="696"/>
+      <c r="AB8" s="709"/>
       <c r="AC8" s="515"/>
       <c r="AH8" s="6" t="s">
         <v>610</v>
       </c>
-      <c r="AI8" s="470"/>
+      <c r="AI8" s="470">
+        <v>1</v>
+      </c>
       <c r="AJ8" s="552"/>
       <c r="AK8" s="6" t="s">
         <v>610</v>
@@ -9452,7 +9465,7 @@
       </c>
       <c r="G9" s="599"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="693"/>
+      <c r="I9" s="706"/>
       <c r="M9" s="19" t="s">
         <v>524</v>
       </c>
@@ -9463,7 +9476,7 @@
         <v>603</v>
       </c>
       <c r="X9" s="470"/>
-      <c r="AB9" s="696"/>
+      <c r="AB9" s="709"/>
       <c r="AC9" s="515"/>
       <c r="AE9" s="20"/>
       <c r="AF9" s="20"/>
@@ -9491,7 +9504,7 @@
         <v>37</v>
       </c>
       <c r="G10" s="599"/>
-      <c r="I10" s="693"/>
+      <c r="I10" s="706"/>
       <c r="J10" s="24" t="s">
         <v>372</v>
       </c>
@@ -9506,7 +9519,7 @@
       <c r="V10" s="470"/>
       <c r="W10" s="6"/>
       <c r="X10" s="470"/>
-      <c r="AB10" s="696"/>
+      <c r="AB10" s="709"/>
       <c r="AC10" s="515"/>
       <c r="AE10" s="20"/>
       <c r="AF10" s="20"/>
@@ -9534,7 +9547,7 @@
         <v>265</v>
       </c>
       <c r="G11" s="599"/>
-      <c r="I11" s="693"/>
+      <c r="I11" s="706"/>
       <c r="J11" s="24" t="s">
         <v>194</v>
       </c>
@@ -9560,13 +9573,13 @@
       <c r="S11" s="24">
         <v>3</v>
       </c>
-      <c r="U11" s="698" t="s">
+      <c r="U11" s="711" t="s">
         <v>557</v>
       </c>
-      <c r="V11" s="699"/>
-      <c r="W11" s="699"/>
-      <c r="X11" s="700"/>
-      <c r="AB11" s="697"/>
+      <c r="V11" s="712"/>
+      <c r="W11" s="712"/>
+      <c r="X11" s="713"/>
+      <c r="AB11" s="710"/>
       <c r="AC11" s="99" t="s">
         <v>594</v>
       </c>
@@ -9577,16 +9590,16 @@
         <v>3</v>
       </c>
       <c r="AF11" s="24">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AG11" s="414"/>
-      <c r="AH11" s="698" t="s">
+      <c r="AH11" s="711" t="s">
         <v>602</v>
       </c>
-      <c r="AI11" s="699"/>
-      <c r="AJ11" s="699"/>
-      <c r="AK11" s="699"/>
-      <c r="AL11" s="700"/>
+      <c r="AI11" s="712"/>
+      <c r="AJ11" s="712"/>
+      <c r="AK11" s="712"/>
+      <c r="AL11" s="713"/>
     </row>
     <row r="12" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="227" t="s">
@@ -9597,7 +9610,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="599"/>
-      <c r="I12" s="693"/>
+      <c r="I12" s="706"/>
       <c r="J12" s="24" t="s">
         <v>515</v>
       </c>
@@ -9630,7 +9643,7 @@
       </c>
       <c r="D13" s="20"/>
       <c r="G13" s="599"/>
-      <c r="I13" s="693"/>
+      <c r="I13" s="706"/>
       <c r="J13" s="108" t="s">
         <v>547</v>
       </c>
@@ -9674,7 +9687,7 @@
       <c r="H14" s="206" t="s">
         <v>218</v>
       </c>
-      <c r="I14" s="693"/>
+      <c r="I14" s="706"/>
       <c r="U14" s="67" t="s">
         <v>80</v>
       </c>
@@ -9701,7 +9714,7 @@
       <c r="H15" s="271">
         <v>0</v>
       </c>
-      <c r="I15" s="693"/>
+      <c r="I15" s="706"/>
       <c r="J15" s="108" t="s">
         <v>153</v>
       </c>
@@ -9732,7 +9745,7 @@
       <c r="D16" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="I16" s="693"/>
+      <c r="I16" s="706"/>
       <c r="K16" s="100" t="s">
         <v>44</v>
       </c>
@@ -9776,7 +9789,7 @@
       <c r="G17" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="I17" s="693"/>
+      <c r="I17" s="706"/>
       <c r="L17" s="2" t="s">
         <v>426</v>
       </c>
@@ -9790,19 +9803,19 @@
     </row>
     <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
-      <c r="I18" s="693"/>
+      <c r="I18" s="706"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="690" t="s">
+      <c r="O18" s="703" t="s">
         <v>516</v>
       </c>
-      <c r="P18" s="691"/>
+      <c r="P18" s="704"/>
       <c r="Q18" s="127" t="s">
         <v>44</v>
       </c>
       <c r="R18" s="24">
         <f>5-R26</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S18" s="24">
         <f>5-S26</f>
@@ -9811,12 +9824,14 @@
       <c r="U18" s="19"/>
       <c r="V18" s="24"/>
       <c r="W18" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="X18" s="24"/>
+        <v>622</v>
+      </c>
+      <c r="X18" s="24">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="693"/>
+      <c r="I19" s="706"/>
       <c r="M19" s="21" t="s">
         <v>425</v>
       </c>
@@ -9846,7 +9861,7 @@
       <c r="G20" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="I20" s="693"/>
+      <c r="I20" s="706"/>
       <c r="K20" s="19" t="s">
         <v>422</v>
       </c>
@@ -9861,7 +9876,7 @@
       </c>
       <c r="R20" s="24">
         <f>R18-SUM(X16:X21)+R26</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S20" s="24">
         <f>S18-SUM(V16:V21)+S26</f>
@@ -9875,7 +9890,7 @@
       <c r="X20" s="468"/>
     </row>
     <row r="21" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="693"/>
+      <c r="I21" s="706"/>
       <c r="M21" s="216" t="s">
         <v>411</v>
       </c>
@@ -9905,7 +9920,7 @@
       <c r="G22" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="I22" s="693"/>
+      <c r="I22" s="706"/>
       <c r="P22" s="99" t="s">
         <v>590</v>
       </c>
@@ -9920,7 +9935,7 @@
       <c r="E23" s="283" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="693"/>
+      <c r="I23" s="706"/>
       <c r="Q23" s="24">
         <f>SUM(V23:V31)</f>
         <v>7</v>
@@ -9937,7 +9952,7 @@
       </c>
     </row>
     <row r="24" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="693"/>
+      <c r="I24" s="706"/>
       <c r="U24" s="35"/>
       <c r="V24" s="509">
         <v>1</v>
@@ -9965,7 +9980,7 @@
       <c r="H25" s="191" t="s">
         <v>266</v>
       </c>
-      <c r="I25" s="693"/>
+      <c r="I25" s="706"/>
       <c r="J25" s="397" t="s">
         <v>269</v>
       </c>
@@ -10010,7 +10025,7 @@
       <c r="H26" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="I26" s="693"/>
+      <c r="I26" s="706"/>
       <c r="K26" s="24">
         <v>15</v>
       </c>
@@ -10025,7 +10040,7 @@
         <v>44</v>
       </c>
       <c r="R26" s="24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S26" s="24">
         <v>4</v>
@@ -10045,7 +10060,7 @@
       </c>
     </row>
     <row r="27" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="693"/>
+      <c r="I27" s="706"/>
       <c r="O27" s="2" t="s">
         <v>98</v>
       </c>
@@ -10072,7 +10087,7 @@
       <c r="E28" s="215">
         <v>2</v>
       </c>
-      <c r="I28" s="693"/>
+      <c r="I28" s="706"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="142"/>
@@ -10094,7 +10109,7 @@
       <c r="H29" s="191" t="s">
         <v>267</v>
       </c>
-      <c r="I29" s="694"/>
+      <c r="I29" s="707"/>
       <c r="J29" s="324"/>
       <c r="L29" s="96" t="s">
         <v>273</v>
@@ -10152,6 +10167,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I2:I29"/>
+    <mergeCell ref="AB1:AB11"/>
+    <mergeCell ref="AH11:AL11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="U11:X11"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="G5:G14"/>
     <mergeCell ref="A2:A3"/>
@@ -10163,13 +10185,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I2:I29"/>
-    <mergeCell ref="AB1:AB11"/>
-    <mergeCell ref="AH11:AL11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="U11:X11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10180,8 +10195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AT37"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4:P20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10281,14 +10296,14 @@
         <f ca="1">TODAY()</f>
         <v>45289</v>
       </c>
-      <c r="T1" s="735"/>
+      <c r="T1" s="742"/>
       <c r="U1" s="142"/>
       <c r="V1" s="6"/>
       <c r="W1" s="6"/>
-      <c r="X1" s="719" t="s">
+      <c r="X1" s="726" t="s">
         <v>441</v>
       </c>
-      <c r="Y1" s="720"/>
+      <c r="Y1" s="727"/>
       <c r="Z1" s="306">
         <f>68-(W8+Y3+X3+U3)</f>
         <v>0</v>
@@ -10304,27 +10319,27 @@
       <c r="AD1" s="302" t="s">
         <v>44</v>
       </c>
-      <c r="AE1" s="721" t="s">
+      <c r="AE1" s="728" t="s">
         <v>190</v>
       </c>
-      <c r="AF1" s="722"/>
-      <c r="AG1" s="723"/>
-      <c r="AH1" s="724" t="s">
+      <c r="AF1" s="729"/>
+      <c r="AG1" s="730"/>
+      <c r="AH1" s="731" t="s">
         <v>293</v>
       </c>
-      <c r="AI1" s="725"/>
-      <c r="AJ1" s="726"/>
-      <c r="AK1" s="613" t="s">
+      <c r="AI1" s="732"/>
+      <c r="AJ1" s="733"/>
+      <c r="AK1" s="659" t="s">
         <v>613</v>
       </c>
       <c r="AL1" s="550" t="s">
         <v>614</v>
       </c>
-      <c r="AM1" s="716" t="s">
+      <c r="AM1" s="723" t="s">
         <v>444</v>
       </c>
-      <c r="AN1" s="717"/>
-      <c r="AO1" s="718"/>
+      <c r="AN1" s="724"/>
+      <c r="AO1" s="725"/>
       <c r="AR1" s="142"/>
     </row>
     <row r="2" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10339,27 +10354,27 @@
         <f>K2+L2</f>
         <v>25</v>
       </c>
-      <c r="K2" s="743">
+      <c r="K2" s="721">
         <f>SUM(K4:K37)</f>
         <v>6</v>
       </c>
-      <c r="L2" s="741">
+      <c r="L2" s="719">
         <f>SUM(L4:L37)</f>
         <v>19</v>
       </c>
-      <c r="M2" s="727">
+      <c r="M2" s="734">
         <f>SUM(M5:M30)</f>
         <v>0</v>
       </c>
-      <c r="N2" s="729">
+      <c r="N2" s="736">
         <f>SUM(N4:N29)</f>
         <v>8</v>
       </c>
-      <c r="O2" s="731">
+      <c r="O2" s="738">
         <f>SUM(O4:O29)</f>
         <v>10</v>
       </c>
-      <c r="P2" s="637">
+      <c r="P2" s="666">
         <f>SUM(N30:N37)* (-1)</f>
         <v>0</v>
       </c>
@@ -10372,14 +10387,14 @@
       <c r="S2" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="T2" s="736"/>
+      <c r="T2" s="743"/>
       <c r="U2" s="537" t="s">
         <v>262</v>
       </c>
       <c r="V2" s="482" t="s">
         <v>219</v>
       </c>
-      <c r="W2" s="733" t="s">
+      <c r="W2" s="740" t="s">
         <v>234</v>
       </c>
       <c r="X2" s="483" t="s">
@@ -10421,7 +10436,7 @@
       <c r="AJ2" s="150" t="s">
         <v>288</v>
       </c>
-      <c r="AK2" s="614"/>
+      <c r="AK2" s="660"/>
       <c r="AL2" s="591" t="s">
         <v>288</v>
       </c>
@@ -10449,12 +10464,12 @@
         <f>V3+X3+Y3+U3</f>
         <v>68</v>
       </c>
-      <c r="K3" s="744"/>
-      <c r="L3" s="742"/>
-      <c r="M3" s="728"/>
-      <c r="N3" s="730"/>
-      <c r="O3" s="732"/>
-      <c r="P3" s="638"/>
+      <c r="K3" s="722"/>
+      <c r="L3" s="720"/>
+      <c r="M3" s="735"/>
+      <c r="N3" s="737"/>
+      <c r="O3" s="739"/>
+      <c r="P3" s="667"/>
       <c r="Q3" s="172">
         <f>(M2+N2)-Y3</f>
         <v>0</v>
@@ -10462,7 +10477,7 @@
       <c r="S3" s="159" t="s">
         <v>244</v>
       </c>
-      <c r="T3" s="737"/>
+      <c r="T3" s="744"/>
       <c r="U3" s="538">
         <f>SUM(U4:U29)</f>
         <v>14</v>
@@ -10471,7 +10486,7 @@
         <f>SUM(V4:V29)</f>
         <v>37</v>
       </c>
-      <c r="W3" s="734"/>
+      <c r="W3" s="741"/>
       <c r="X3" s="485">
         <f t="shared" ref="X3:AC3" si="0">SUM(X4:X29)</f>
         <v>9</v>
@@ -10522,7 +10537,7 @@
       </c>
       <c r="AJ3" s="404">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AK3" s="404">
         <f>SUM(AK4:AK37)</f>
@@ -10577,7 +10592,7 @@
         <f>AC4</f>
         <v>0</v>
       </c>
-      <c r="P4" s="738"/>
+      <c r="P4" s="716"/>
       <c r="Q4" s="20"/>
       <c r="R4" s="2" t="s">
         <v>334</v>
@@ -10661,7 +10676,7 @@
         <f>AC5</f>
         <v>0</v>
       </c>
-      <c r="P5" s="739"/>
+      <c r="P5" s="717"/>
       <c r="Q5" s="20"/>
       <c r="R5" s="2" t="s">
         <v>340</v>
@@ -10755,7 +10770,7 @@
         <f>AC6</f>
         <v>1</v>
       </c>
-      <c r="P6" s="739"/>
+      <c r="P6" s="717"/>
       <c r="Q6" s="54" t="s">
         <v>335</v>
       </c>
@@ -10810,7 +10825,7 @@
         <v>0</v>
       </c>
       <c r="AJ6" s="509">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK6" s="558">
         <v>1</v>
@@ -10860,7 +10875,7 @@
         <f>AC7</f>
         <v>0</v>
       </c>
-      <c r="P7" s="739"/>
+      <c r="P7" s="717"/>
       <c r="Q7" s="20"/>
       <c r="R7" s="2" t="s">
         <v>335</v>
@@ -10976,7 +10991,7 @@
         <f t="shared" ref="O8:O37" si="10">AC8</f>
         <v>0</v>
       </c>
-      <c r="P8" s="739"/>
+      <c r="P8" s="717"/>
       <c r="Q8" s="108" t="s">
         <v>233</v>
       </c>
@@ -11067,7 +11082,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P9" s="739"/>
+      <c r="P9" s="717"/>
       <c r="Q9" s="108" t="s">
         <v>335</v>
       </c>
@@ -11172,7 +11187,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P10" s="739"/>
+      <c r="P10" s="717"/>
       <c r="Q10" s="20"/>
       <c r="R10" s="2" t="s">
         <v>340</v>
@@ -11262,7 +11277,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P11" s="739"/>
+      <c r="P11" s="717"/>
       <c r="Q11" s="108" t="s">
         <v>335</v>
       </c>
@@ -11327,14 +11342,14 @@
       <c r="AR11" s="508"/>
     </row>
     <row r="12" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="675" t="s">
+      <c r="A12" s="626" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
         <v>13</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="E12" s="625" t="s">
+      <c r="E12" s="681" t="s">
         <v>56</v>
       </c>
       <c r="G12" s="262"/>
@@ -11359,7 +11374,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P12" s="739"/>
+      <c r="P12" s="717"/>
       <c r="Q12" s="108" t="s">
         <v>335</v>
       </c>
@@ -11436,14 +11451,14 @@
       </c>
     </row>
     <row r="13" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="677"/>
+      <c r="A13" s="628"/>
       <c r="B13" s="583">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="626"/>
+      <c r="E13" s="682"/>
       <c r="F13" s="172">
         <v>0</v>
       </c>
@@ -11467,7 +11482,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P13" s="739"/>
+      <c r="P13" s="717"/>
       <c r="Q13" s="108" t="s">
         <v>335</v>
       </c>
@@ -11549,7 +11564,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P14" s="739"/>
+      <c r="P14" s="717"/>
       <c r="Q14" s="20"/>
       <c r="R14" s="200" t="s">
         <v>339</v>
@@ -11652,7 +11667,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P15" s="739"/>
+      <c r="P15" s="717"/>
       <c r="Q15" s="20"/>
       <c r="R15" s="200" t="s">
         <v>339</v>
@@ -11746,7 +11761,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P16" s="739"/>
+      <c r="P16" s="717"/>
       <c r="Q16" s="108" t="s">
         <v>335</v>
       </c>
@@ -11847,7 +11862,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P17" s="739"/>
+      <c r="P17" s="717"/>
       <c r="Q17" s="20"/>
       <c r="R17" s="2" t="s">
         <v>341</v>
@@ -11947,7 +11962,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P18" s="739"/>
+      <c r="P18" s="717"/>
       <c r="Q18" s="108" t="s">
         <v>335</v>
       </c>
@@ -12037,7 +12052,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P19" s="739"/>
+      <c r="P19" s="717"/>
       <c r="Q19" s="20"/>
       <c r="R19" s="2" t="s">
         <v>334</v>
@@ -12145,11 +12160,11 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P20" s="740"/>
+      <c r="P20" s="718"/>
       <c r="Q20" s="605" t="s">
         <v>335</v>
       </c>
-      <c r="R20" s="627"/>
+      <c r="R20" s="683"/>
       <c r="S20" s="534" t="s">
         <v>85</v>
       </c>
@@ -12411,7 +12426,7 @@
     </row>
     <row r="23" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="24"/>
-      <c r="E23" s="682" t="s">
+      <c r="E23" s="633" t="s">
         <v>289</v>
       </c>
       <c r="F23" s="180"/>
@@ -12516,7 +12531,7 @@
       <c r="C24" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="E24" s="683"/>
+      <c r="E24" s="634"/>
       <c r="F24" s="172"/>
       <c r="H24" s="42"/>
       <c r="J24" s="570" t="s">
@@ -12542,7 +12557,7 @@
       <c r="Q24" s="605" t="s">
         <v>335</v>
       </c>
-      <c r="R24" s="627"/>
+      <c r="R24" s="683"/>
       <c r="S24" s="534" t="s">
         <v>249</v>
       </c>
@@ -12976,7 +12991,9 @@
         <v>0</v>
       </c>
       <c r="AQ28" s="566"/>
-      <c r="AR28" s="508"/>
+      <c r="AR28" s="540" t="s">
+        <v>562</v>
+      </c>
     </row>
     <row r="29" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E29" s="258" t="s">
@@ -13208,8 +13225,8 @@
       <c r="AR31" s="508"/>
     </row>
     <row r="32" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="630"/>
-      <c r="B32" s="630"/>
+      <c r="A32" s="650"/>
+      <c r="B32" s="650"/>
       <c r="J32" s="571"/>
       <c r="K32" s="586"/>
       <c r="L32" s="580">
@@ -13306,7 +13323,9 @@
     </row>
     <row r="33" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="80"/>
-      <c r="B33" s="24"/>
+      <c r="B33" s="21">
+        <v>6</v>
+      </c>
       <c r="G33" s="382">
         <v>-1</v>
       </c>
@@ -13406,6 +13425,9 @@
       </c>
     </row>
     <row r="34" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="21">
+        <v>7</v>
+      </c>
       <c r="C34" s="2" t="s">
         <v>257</v>
       </c>
@@ -13685,7 +13707,9 @@
       </c>
     </row>
     <row r="37" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="21"/>
+      <c r="B37" s="21">
+        <v>0</v>
+      </c>
       <c r="D37" s="382">
         <v>1</v>
       </c>
@@ -13709,7 +13733,7 @@
       </c>
       <c r="O37" s="175">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P37" s="110"/>
       <c r="Q37" s="20"/>
@@ -13736,27 +13760,27 @@
       <c r="Z37" s="65"/>
       <c r="AA37" s="117">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB37" s="64">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC37" s="64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD37" s="301">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AE37" s="350">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF37" s="356"/>
       <c r="AG37" s="357"/>
       <c r="AH37" s="351">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI37" s="556">
         <v>0</v>
@@ -13768,15 +13792,15 @@
       <c r="AL37" s="320"/>
       <c r="AM37" s="68">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN37" s="308">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO37" s="309">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP37" s="6" t="s">
         <v>468</v>
@@ -13785,20 +13809,11 @@
         <v>563</v>
       </c>
       <c r="AR37" s="540" t="s">
-        <v>562</v>
+        <v>621</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="P4:P20"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="Q20:R20"/>
     <mergeCell ref="AM1:AO1"/>
     <mergeCell ref="X1:Y1"/>
     <mergeCell ref="AE1:AG1"/>
@@ -13810,6 +13825,15 @@
     <mergeCell ref="W2:W3"/>
     <mergeCell ref="T1:T3"/>
     <mergeCell ref="AK1:AK2"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="P4:P20"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="Q20:R20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13877,7 +13901,7 @@
       <c r="V1" s="603" t="s">
         <v>70</v>
       </c>
-      <c r="W1" s="627"/>
+      <c r="W1" s="683"/>
       <c r="X1" s="62" t="s">
         <v>101</v>
       </c>
@@ -13896,7 +13920,7 @@
       <c r="AC1" s="116" t="s">
         <v>190</v>
       </c>
-      <c r="AD1" s="752" t="s">
+      <c r="AD1" s="759" t="s">
         <v>211</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -13913,10 +13937,10 @@
       <c r="E2" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="751" t="s">
+      <c r="F2" s="790" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="779" t="s">
+      <c r="G2" s="747" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -13944,10 +13968,10 @@
       <c r="U2" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="V2" s="719" t="s">
+      <c r="V2" s="726" t="s">
         <v>120</v>
       </c>
-      <c r="W2" s="720"/>
+      <c r="W2" s="727"/>
       <c r="X2" s="64" t="s">
         <v>109</v>
       </c>
@@ -13966,7 +13990,7 @@
       <c r="AC2" s="117" t="s">
         <v>98</v>
       </c>
-      <c r="AD2" s="753"/>
+      <c r="AD2" s="760"/>
       <c r="AE2" s="64" t="s">
         <v>98</v>
       </c>
@@ -13985,8 +14009,8 @@
       <c r="E3" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="F3" s="679"/>
-      <c r="G3" s="780"/>
+      <c r="F3" s="630"/>
+      <c r="G3" s="748"/>
       <c r="H3" s="40" t="s">
         <v>80</v>
       </c>
@@ -13997,13 +14021,13 @@
         <v>81</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="789" t="s">
+      <c r="O3" s="757" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="771" t="s">
+      <c r="P3" s="778" t="s">
         <v>217</v>
       </c>
-      <c r="Q3" s="772"/>
+      <c r="Q3" s="779"/>
       <c r="S3" s="57" t="s">
         <v>218</v>
       </c>
@@ -14013,15 +14037,15 @@
       <c r="W3" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="AD3" s="753"/>
+      <c r="AD3" s="760"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="780"/>
+      <c r="G4" s="748"/>
       <c r="H4" s="6"/>
       <c r="L4" s="687" t="s">
         <v>82</v>
       </c>
-      <c r="O4" s="790"/>
+      <c r="O4" s="758"/>
       <c r="T4" s="55" t="s">
         <v>97</v>
       </c>
@@ -14035,8 +14059,8 @@
         <v>194</v>
       </c>
       <c r="Z4" s="605"/>
-      <c r="AA4" s="627"/>
-      <c r="AD4" s="753"/>
+      <c r="AA4" s="683"/>
+      <c r="AD4" s="760"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -14051,21 +14075,21 @@
       <c r="F5" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="G5" s="780"/>
+      <c r="G5" s="748"/>
       <c r="H5" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="K5" s="758" t="s">
+      <c r="K5" s="765" t="s">
         <v>215</v>
       </c>
-      <c r="L5" s="773"/>
+      <c r="L5" s="780"/>
       <c r="M5" s="2" t="s">
         <v>213</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>212</v>
       </c>
-      <c r="O5" s="790"/>
+      <c r="O5" s="758"/>
       <c r="P5" s="108" t="s">
         <v>214</v>
       </c>
@@ -14081,11 +14105,11 @@
       <c r="U5" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="Y5" s="761" t="s">
+      <c r="Y5" s="768" t="s">
         <v>282</v>
       </c>
-      <c r="Z5" s="762"/>
-      <c r="AD5" s="753"/>
+      <c r="Z5" s="769"/>
+      <c r="AD5" s="760"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -14095,16 +14119,16 @@
       <c r="E6" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="G6" s="780"/>
+      <c r="G6" s="748"/>
       <c r="H6" s="46" t="s">
         <v>80</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="759"/>
-      <c r="L6" s="773"/>
-      <c r="O6" s="790"/>
+      <c r="K6" s="766"/>
+      <c r="L6" s="780"/>
+      <c r="O6" s="758"/>
       <c r="T6" s="2" t="s">
         <v>100</v>
       </c>
@@ -14114,23 +14138,23 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="753"/>
+      <c r="AD6" s="760"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="780"/>
+      <c r="G7" s="748"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="759"/>
-      <c r="L7" s="773"/>
+      <c r="K7" s="766"/>
+      <c r="L7" s="780"/>
       <c r="N7" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="O7" s="790"/>
+      <c r="O7" s="758"/>
       <c r="P7" s="73"/>
       <c r="U7" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="753"/>
+      <c r="AD7" s="760"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -14143,7 +14167,7 @@
       <c r="F8" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="G8" s="780"/>
+      <c r="G8" s="748"/>
       <c r="H8" s="50" t="s">
         <v>75</v>
       </c>
@@ -14153,41 +14177,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="759"/>
-      <c r="L8" s="773"/>
-      <c r="O8" s="790"/>
+      <c r="K8" s="766"/>
+      <c r="L8" s="780"/>
+      <c r="O8" s="758"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="755" t="s">
+      <c r="S8" s="762" t="s">
         <v>210</v>
       </c>
-      <c r="T8" s="756"/>
-      <c r="U8" s="756"/>
-      <c r="V8" s="756"/>
-      <c r="W8" s="756"/>
-      <c r="X8" s="756"/>
-      <c r="Y8" s="756"/>
-      <c r="Z8" s="756"/>
-      <c r="AA8" s="756"/>
-      <c r="AB8" s="756"/>
-      <c r="AC8" s="757"/>
-      <c r="AD8" s="753"/>
+      <c r="T8" s="763"/>
+      <c r="U8" s="763"/>
+      <c r="V8" s="763"/>
+      <c r="W8" s="763"/>
+      <c r="X8" s="763"/>
+      <c r="Y8" s="763"/>
+      <c r="Z8" s="763"/>
+      <c r="AA8" s="763"/>
+      <c r="AB8" s="763"/>
+      <c r="AC8" s="764"/>
+      <c r="AD8" s="760"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="745"/>
-      <c r="G9" s="780"/>
+      <c r="C9" s="784"/>
+      <c r="G9" s="748"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="759"/>
-      <c r="L9" s="783" t="s">
+      <c r="K9" s="766"/>
+      <c r="L9" s="751" t="s">
         <v>216</v>
       </c>
-      <c r="M9" s="784"/>
-      <c r="N9" s="785"/>
-      <c r="O9" s="790"/>
+      <c r="M9" s="752"/>
+      <c r="N9" s="753"/>
+      <c r="O9" s="758"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="753"/>
+      <c r="AD9" s="760"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="746"/>
+      <c r="C10" s="785"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>87</v>
@@ -14195,7 +14219,7 @@
       <c r="F10" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="G10" s="780"/>
+      <c r="G10" s="748"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>80</v>
@@ -14203,33 +14227,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="759"/>
-      <c r="M10" s="748" t="s">
+      <c r="K10" s="766"/>
+      <c r="M10" s="787" t="s">
         <v>89</v>
       </c>
-      <c r="N10" s="749"/>
-      <c r="O10" s="749"/>
-      <c r="P10" s="749"/>
-      <c r="Q10" s="749"/>
-      <c r="R10" s="749"/>
-      <c r="S10" s="749"/>
-      <c r="T10" s="749"/>
-      <c r="U10" s="749"/>
-      <c r="V10" s="749"/>
-      <c r="W10" s="749"/>
-      <c r="X10" s="749"/>
-      <c r="Y10" s="749"/>
-      <c r="Z10" s="749"/>
-      <c r="AA10" s="749"/>
-      <c r="AB10" s="749"/>
-      <c r="AC10" s="750"/>
-      <c r="AD10" s="753"/>
+      <c r="N10" s="788"/>
+      <c r="O10" s="788"/>
+      <c r="P10" s="788"/>
+      <c r="Q10" s="788"/>
+      <c r="R10" s="788"/>
+      <c r="S10" s="788"/>
+      <c r="T10" s="788"/>
+      <c r="U10" s="788"/>
+      <c r="V10" s="788"/>
+      <c r="W10" s="788"/>
+      <c r="X10" s="788"/>
+      <c r="Y10" s="788"/>
+      <c r="Z10" s="788"/>
+      <c r="AA10" s="788"/>
+      <c r="AB10" s="788"/>
+      <c r="AC10" s="789"/>
+      <c r="AD10" s="760"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="747"/>
-      <c r="G11" s="780"/>
+      <c r="C11" s="786"/>
+      <c r="G11" s="748"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="759"/>
+      <c r="K11" s="766"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -14237,17 +14261,17 @@
       <c r="Y11" s="68" t="s">
         <v>120</v>
       </c>
-      <c r="Z11" s="769" t="s">
+      <c r="Z11" s="776" t="s">
         <v>120</v>
       </c>
-      <c r="AA11" s="770"/>
+      <c r="AA11" s="777"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>120</v>
       </c>
-      <c r="AD11" s="753"/>
+      <c r="AD11" s="760"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -14260,7 +14284,7 @@
       <c r="F12" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="G12" s="780"/>
+      <c r="G12" s="748"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>80</v>
@@ -14268,8 +14292,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="759"/>
-      <c r="L12" s="774" t="s">
+      <c r="K12" s="766"/>
+      <c r="L12" s="781" t="s">
         <v>92</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -14300,25 +14324,25 @@
         <v>115</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="763" t="s">
+      <c r="AA12" s="770" t="s">
         <v>125</v>
       </c>
-      <c r="AB12" s="764"/>
+      <c r="AB12" s="771"/>
       <c r="AC12" s="21" t="s">
         <v>230</v>
       </c>
-      <c r="AD12" s="753"/>
+      <c r="AD12" s="760"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="745"/>
-      <c r="G13" s="780"/>
-      <c r="K13" s="759"/>
-      <c r="L13" s="775"/>
+      <c r="C13" s="784"/>
+      <c r="G13" s="748"/>
+      <c r="K13" s="766"/>
+      <c r="L13" s="782"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="782" t="s">
+      <c r="Q13" s="750" t="s">
         <v>208</v>
       </c>
-      <c r="R13" s="644"/>
+      <c r="R13" s="639"/>
       <c r="S13" s="599"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
@@ -14327,17 +14351,17 @@
       <c r="X13" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="AA13" s="765"/>
-      <c r="AB13" s="766"/>
-      <c r="AD13" s="753"/>
+      <c r="AA13" s="772"/>
+      <c r="AB13" s="773"/>
+      <c r="AD13" s="760"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="C14" s="747"/>
+      <c r="C14" s="786"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="780"/>
+      <c r="G14" s="748"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -14345,8 +14369,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="759"/>
-      <c r="L14" s="775"/>
+      <c r="K14" s="766"/>
+      <c r="L14" s="782"/>
       <c r="M14" s="21" t="s">
         <v>110</v>
       </c>
@@ -14367,9 +14391,9 @@
       <c r="Y14" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="AA14" s="765"/>
-      <c r="AB14" s="766"/>
-      <c r="AD14" s="753"/>
+      <c r="AA14" s="772"/>
+      <c r="AB14" s="773"/>
+      <c r="AD14" s="760"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -14384,19 +14408,19 @@
       <c r="F15" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="G15" s="780"/>
+      <c r="G15" s="748"/>
       <c r="H15" s="2" t="s">
         <v>80</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="K15" s="759"/>
-      <c r="L15" s="776"/>
-      <c r="Q15" s="782" t="s">
+      <c r="K15" s="766"/>
+      <c r="L15" s="783"/>
+      <c r="Q15" s="750" t="s">
         <v>209</v>
       </c>
-      <c r="R15" s="644"/>
+      <c r="R15" s="639"/>
       <c r="S15" s="599"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
@@ -14405,14 +14429,14 @@
       <c r="X15" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="AA15" s="765"/>
-      <c r="AB15" s="766"/>
-      <c r="AD15" s="753"/>
+      <c r="AA15" s="772"/>
+      <c r="AB15" s="773"/>
+      <c r="AD15" s="760"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="780"/>
-      <c r="K16" s="759"/>
+      <c r="G16" s="748"/>
+      <c r="K16" s="766"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>108</v>
@@ -14431,24 +14455,24 @@
       <c r="Z16" s="76" t="s">
         <v>126</v>
       </c>
-      <c r="AA16" s="765"/>
-      <c r="AB16" s="766"/>
-      <c r="AD16" s="753"/>
+      <c r="AA16" s="772"/>
+      <c r="AB16" s="773"/>
+      <c r="AD16" s="760"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F17" s="777" t="s">
+      <c r="F17" s="745" t="s">
         <v>95</v>
       </c>
-      <c r="G17" s="780"/>
+      <c r="G17" s="748"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>80</v>
       </c>
-      <c r="K17" s="759"/>
+      <c r="K17" s="766"/>
       <c r="S17" s="599"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
@@ -14456,9 +14480,9 @@
       <c r="X17" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA17" s="765"/>
-      <c r="AB17" s="766"/>
-      <c r="AD17" s="753"/>
+      <c r="AA17" s="772"/>
+      <c r="AB17" s="773"/>
+      <c r="AD17" s="760"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -14468,15 +14492,15 @@
       <c r="E18" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F18" s="778"/>
-      <c r="G18" s="780"/>
+      <c r="F18" s="746"/>
+      <c r="G18" s="748"/>
       <c r="H18" s="108" t="s">
         <v>75</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="K18" s="759"/>
+      <c r="K18" s="766"/>
       <c r="O18" s="64" t="s">
         <v>114</v>
       </c>
@@ -14487,42 +14511,39 @@
       <c r="X18" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AA18" s="767"/>
-      <c r="AB18" s="768"/>
-      <c r="AD18" s="753"/>
+      <c r="AA18" s="774"/>
+      <c r="AB18" s="775"/>
+      <c r="AD18" s="760"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>207</v>
       </c>
-      <c r="G19" s="781"/>
-      <c r="K19" s="760"/>
+      <c r="G19" s="749"/>
+      <c r="K19" s="767"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="786" t="s">
+      <c r="R19" s="754" t="s">
         <v>123</v>
       </c>
-      <c r="S19" s="787"/>
-      <c r="T19" s="788"/>
+      <c r="S19" s="755"/>
+      <c r="T19" s="756"/>
       <c r="V19" s="77" t="s">
         <v>114</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="AD19" s="754"/>
+      <c r="AD19" s="761"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G19"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="S12:S18"/>
-    <mergeCell ref="O3:O9"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="M10:AC10"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="AD1:AD19"/>
     <mergeCell ref="S8:AC8"/>
     <mergeCell ref="K5:K19"/>
@@ -14534,11 +14555,14 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L12:L15"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="M10:AC10"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="S12:S18"/>
+    <mergeCell ref="O3:O9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rw Usage Updates S.1.0.0.2 _4:30PM
Boat Enabled -
InCapacity - [13] , NodeW - [-3] , BirdW - [6] , FuelW - [19] , OnHost - [5] . VillageW=[5]

Rw- Local(Left Running With Cost ) - [For Business/Shop/Market only] -
</commit_message>
<xml_diff>
--- a/System_2.2.1.xlsx
+++ b/System_2.2.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01161D83-8F66-4FAB-9D1C-FAB8083118A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F8A19B-A9BC-4CB9-846E-299A2B8F0702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1116" uniqueCount="625">
   <si>
     <t>Zone</t>
   </si>
@@ -1911,6 +1911,9 @@
   </si>
   <si>
     <t>7F in Capacity</t>
+  </si>
+  <si>
+    <t>bharat24</t>
   </si>
 </sst>
 </file>
@@ -5868,8 +5871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:X28"/>
   <sheetViews>
-    <sheetView topLeftCell="C9" workbookViewId="0">
-      <selection activeCell="X14" sqref="X14"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6052,7 +6055,7 @@
         <v>225</v>
       </c>
       <c r="V5" s="24">
-        <v>7440</v>
+        <v>7560</v>
       </c>
     </row>
     <row r="6" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6265,7 +6268,7 @@
         <v>224</v>
       </c>
       <c r="V11" s="64">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6977,7 +6980,7 @@
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="617">
         <f ca="1">TODAY()</f>
-        <v>45289</v>
+        <v>45290</v>
       </c>
       <c r="B2" s="619" t="s">
         <v>370</v>
@@ -8950,8 +8953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB54FD83-008D-4F8B-87AC-83E7F70047CB}">
   <dimension ref="A1:AL31"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AH14" sqref="AH14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9067,7 +9070,7 @@
     <row r="2" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="693">
         <f ca="1">TODAY()</f>
-        <v>45289</v>
+        <v>45290</v>
       </c>
       <c r="B2" s="695" t="s">
         <v>379</v>
@@ -9117,7 +9120,7 @@
       <c r="Q2" s="715"/>
       <c r="R2" s="21">
         <f>R7+R20</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S2" s="21">
         <f>S7+S20</f>
@@ -9235,8 +9238,12 @@
       </c>
       <c r="AI4" s="470"/>
       <c r="AJ4" s="552"/>
-      <c r="AK4" s="6"/>
-      <c r="AL4" s="24"/>
+      <c r="AK4" s="6" t="s">
+        <v>624</v>
+      </c>
+      <c r="AL4" s="24">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="221" t="s">
@@ -9336,7 +9343,7 @@
       <c r="AC6" s="35"/>
       <c r="AE6" s="64">
         <f>AE7-SUM(AL2:AL10)+AE11</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AF6" s="64">
         <f>AF7-SUM(AI2:AI10)+AF11</f>
@@ -9398,7 +9405,7 @@
       </c>
       <c r="AE7" s="24">
         <f>8-AE11</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AF7" s="295">
         <f>8-AF11</f>
@@ -9587,7 +9594,7 @@
         <v>44</v>
       </c>
       <c r="AE11" s="24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AF11" s="24">
         <v>3</v>
@@ -9840,7 +9847,9 @@
       <c r="W19" s="19" t="s">
         <v>344</v>
       </c>
-      <c r="X19" s="24"/>
+      <c r="X19" s="24">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="231" t="s">
@@ -9876,7 +9885,7 @@
       </c>
       <c r="R20" s="24">
         <f>R18-SUM(X16:X21)+R26</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S20" s="24">
         <f>S18-SUM(V16:V21)+S26</f>
@@ -10195,8 +10204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AT37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10294,7 +10303,7 @@
       </c>
       <c r="S1" s="151">
         <f ca="1">TODAY()</f>
-        <v>45289</v>
+        <v>45290</v>
       </c>
       <c r="T1" s="742"/>
       <c r="U1" s="142"/>
@@ -10352,7 +10361,7 @@
       </c>
       <c r="J2" s="318">
         <f>K2+L2</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K2" s="721">
         <f>SUM(K4:K37)</f>
@@ -10360,7 +10369,7 @@
       </c>
       <c r="L2" s="719">
         <f>SUM(L4:L37)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M2" s="734">
         <f>SUM(M5:M30)</f>
@@ -10372,11 +10381,11 @@
       </c>
       <c r="O2" s="738">
         <f>SUM(O4:O29)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P2" s="666">
         <f>SUM(N30:N37)* (-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Q2" s="269" t="s">
         <v>238</v>
@@ -10501,15 +10510,15 @@
       </c>
       <c r="AA3" s="66">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AB3" s="66">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AC3" s="66">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AD3" s="66">
         <f t="shared" ref="AD3:AO3" si="1">SUM(AD4:AD29)</f>
@@ -10517,7 +10526,7 @@
       </c>
       <c r="AE3" s="66">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AF3" s="66">
         <f t="shared" si="1"/>
@@ -10529,7 +10538,7 @@
       </c>
       <c r="AH3" s="66">
         <f>SUM(AH4:AH29)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AI3" s="374">
         <f t="shared" si="1"/>
@@ -10549,15 +10558,15 @@
       </c>
       <c r="AM3" s="100">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AN3" s="310">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AO3" s="311">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AR3" s="142"/>
     </row>
@@ -10873,7 +10882,7 @@
       </c>
       <c r="O7" s="293">
         <f>AC7</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P7" s="717"/>
       <c r="Q7" s="20"/>
@@ -10905,21 +10914,21 @@
       <c r="Z7" s="296"/>
       <c r="AA7" s="117">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB7" s="290">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC7" s="290">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD7" s="290">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AE7" s="294">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF7" s="107">
         <v>0</v>
@@ -10929,7 +10938,7 @@
       </c>
       <c r="AH7" s="296">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI7" s="375"/>
       <c r="AJ7" s="509"/>
@@ -10937,15 +10946,15 @@
       <c r="AL7" s="317"/>
       <c r="AM7" s="336">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN7" s="308">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO7" s="309">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP7" s="6" t="s">
         <v>240</v>
@@ -13323,9 +13332,7 @@
     </row>
     <row r="33" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="80"/>
-      <c r="B33" s="21">
-        <v>6</v>
-      </c>
+      <c r="B33" s="21"/>
       <c r="G33" s="382">
         <v>-1</v>
       </c>
@@ -13335,15 +13342,15 @@
       <c r="J33" s="572"/>
       <c r="K33" s="587"/>
       <c r="L33" s="580">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M33" s="334"/>
       <c r="N33" s="247">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O33" s="293">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P33" s="109"/>
       <c r="Q33" s="20"/>
@@ -13357,7 +13364,7 @@
         <v>1</v>
       </c>
       <c r="V33" s="160">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W33" s="589">
         <v>-1</v>
@@ -13367,32 +13374,32 @@
       </c>
       <c r="Y33" s="183">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z33" s="65"/>
       <c r="AA33" s="117">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB33" s="64">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AC33" s="64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD33" s="301">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AE33" s="350">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF33" s="354"/>
       <c r="AG33" s="355"/>
       <c r="AH33" s="316">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI33" s="375"/>
       <c r="AJ33" s="155"/>
@@ -13404,15 +13411,15 @@
       </c>
       <c r="AM33" s="568">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN33" s="308">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO33" s="309">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP33" s="6" t="s">
         <v>344</v>
@@ -13426,7 +13433,7 @@
     </row>
     <row r="34" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="21">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>257</v>
@@ -13896,7 +13903,7 @@
       <c r="P1" s="38"/>
       <c r="S1" s="58">
         <f ca="1">TODAY()</f>
-        <v>45289</v>
+        <v>45290</v>
       </c>
       <c r="V1" s="603" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
Rw Usage Updates S.1.0.0.4 _2:20PM
Boat Enabled -
InCapacity - [7] , NodeW - [-3] , BirdW - [6] , FuelW - [20] , OnHost - [8+1]
 VillageW=[5]
Rw - Local(Left Running With Cost ) - [For Business/Shop/Market only] -
</commit_message>
<xml_diff>
--- a/System_2.2.1.xlsx
+++ b/System_2.2.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F8A19B-A9BC-4CB9-846E-299A2B8F0702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4B3DBD-6C41-4908-BAC9-276AA5D93695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1116" uniqueCount="625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="624">
   <si>
     <t>Zone</t>
   </si>
@@ -1896,9 +1896,6 @@
   </si>
   <si>
     <t>Rbangla</t>
-  </si>
-  <si>
-    <t>2M11F</t>
   </si>
   <si>
     <t>tv9</t>
@@ -5030,6 +5027,159 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5048,12 +5198,6 @@
     <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5108,169 +5252,61 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5312,43 +5348,70 @@
     <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="52" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="52" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="14" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5372,112 +5435,25 @@
     <xf numFmtId="0" fontId="29" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="52" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="52" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="14" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5555,25 +5531,46 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5871,8 +5868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:X28"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="W10" sqref="W10"/>
+    <sheetView topLeftCell="C9" workbookViewId="0">
+      <selection activeCell="V26" sqref="V26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6596,7 +6593,7 @@
       <c r="P22" s="313"/>
       <c r="T22" s="607"/>
       <c r="X22" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="23" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6742,9 +6739,7 @@
       </c>
       <c r="P26" s="313"/>
       <c r="T26" s="607"/>
-      <c r="V26" s="24" t="s">
-        <v>619</v>
-      </c>
+      <c r="V26" s="24"/>
     </row>
     <row r="27" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="256" t="s">
@@ -6908,7 +6903,7 @@
       <c r="H1" s="97" t="s">
         <v>343</v>
       </c>
-      <c r="I1" s="659" t="s">
+      <c r="I1" s="613" t="s">
         <v>369</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -6944,7 +6939,7 @@
       <c r="X1" s="430" t="s">
         <v>155</v>
       </c>
-      <c r="Y1" s="653" t="s">
+      <c r="Y1" s="657" t="s">
         <v>528</v>
       </c>
       <c r="Z1" s="406">
@@ -6969,7 +6964,7 @@
         <v>498</v>
       </c>
       <c r="AM1" s="402"/>
-      <c r="AN1" s="635"/>
+      <c r="AN1" s="640"/>
       <c r="AO1" s="338" t="s">
         <v>469</v>
       </c>
@@ -6978,23 +6973,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="617">
+      <c r="A2" s="666">
         <f ca="1">TODAY()</f>
-        <v>45290</v>
-      </c>
-      <c r="B2" s="619" t="s">
+        <v>45291</v>
+      </c>
+      <c r="B2" s="668" t="s">
         <v>370</v>
       </c>
-      <c r="C2" s="615" t="s">
+      <c r="C2" s="645" t="s">
         <v>357</v>
       </c>
-      <c r="D2" s="621" t="s">
+      <c r="D2" s="670" t="s">
         <v>355</v>
       </c>
-      <c r="E2" s="669" t="s">
+      <c r="E2" s="609" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="640" t="s">
+      <c r="F2" s="619" t="s">
         <v>102</v>
       </c>
       <c r="G2" s="393" t="s">
@@ -7003,31 +6998,31 @@
       <c r="H2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="660"/>
+      <c r="I2" s="614"/>
       <c r="J2" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="671" t="s">
+      <c r="K2" s="611" t="s">
         <v>342</v>
       </c>
-      <c r="L2" s="672"/>
-      <c r="M2" s="640" t="s">
+      <c r="L2" s="612"/>
+      <c r="M2" s="619" t="s">
         <v>102</v>
       </c>
       <c r="N2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="644" t="s">
+      <c r="O2" s="649" t="s">
         <v>102</v>
       </c>
       <c r="P2" s="85" t="s">
         <v>147</v>
       </c>
-      <c r="Q2" s="615" t="s">
+      <c r="Q2" s="645" t="s">
         <v>143</v>
       </c>
       <c r="R2" s="598"/>
-      <c r="S2" s="657" t="s">
+      <c r="S2" s="634" t="s">
         <v>148</v>
       </c>
       <c r="T2" s="89"/>
@@ -7037,7 +7032,7 @@
       <c r="X2" s="431" t="s">
         <v>156</v>
       </c>
-      <c r="Y2" s="654"/>
+      <c r="Y2" s="658"/>
       <c r="Z2" s="407">
         <v>1</v>
       </c>
@@ -7060,15 +7055,15 @@
         <v>463</v>
       </c>
       <c r="AM2" s="428"/>
-      <c r="AN2" s="636"/>
+      <c r="AN2" s="641"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="618"/>
-      <c r="B3" s="620"/>
-      <c r="C3" s="616"/>
-      <c r="D3" s="622"/>
-      <c r="E3" s="670"/>
-      <c r="F3" s="641"/>
+      <c r="A3" s="667"/>
+      <c r="B3" s="669"/>
+      <c r="C3" s="646"/>
+      <c r="D3" s="671"/>
+      <c r="E3" s="610"/>
+      <c r="F3" s="620"/>
       <c r="G3" s="394" t="s">
         <v>28</v>
       </c>
@@ -7087,17 +7082,17 @@
       <c r="L3" s="201" t="s">
         <v>107</v>
       </c>
-      <c r="M3" s="641"/>
+      <c r="M3" s="620"/>
       <c r="N3" s="69" t="s">
         <v>146</v>
       </c>
-      <c r="O3" s="645"/>
+      <c r="O3" s="650"/>
       <c r="P3" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="Q3" s="616"/>
+      <c r="Q3" s="646"/>
       <c r="R3" s="600"/>
-      <c r="S3" s="658"/>
+      <c r="S3" s="636"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -7105,7 +7100,7 @@
       <c r="X3" s="431" t="s">
         <v>157</v>
       </c>
-      <c r="Y3" s="654"/>
+      <c r="Y3" s="658"/>
       <c r="Z3" s="408">
         <v>1</v>
       </c>
@@ -7114,7 +7109,7 @@
       <c r="AC3" s="100" t="s">
         <v>480</v>
       </c>
-      <c r="AD3" s="656" t="s">
+      <c r="AD3" s="631" t="s">
         <v>455</v>
       </c>
       <c r="AE3" s="257"/>
@@ -7126,16 +7121,16 @@
       <c r="AK3" s="257"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="428"/>
-      <c r="AN3" s="636"/>
+      <c r="AN3" s="641"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="238" t="s">
         <v>183</v>
       </c>
-      <c r="B4" s="633" t="s">
+      <c r="B4" s="682" t="s">
         <v>373</v>
       </c>
-      <c r="C4" s="615" t="s">
+      <c r="C4" s="645" t="s">
         <v>154</v>
       </c>
       <c r="D4" s="347" t="s">
@@ -7144,7 +7139,7 @@
       <c r="E4" s="378">
         <v>2</v>
       </c>
-      <c r="F4" s="641"/>
+      <c r="F4" s="620"/>
       <c r="G4" s="381" t="s">
         <v>201</v>
       </c>
@@ -7161,11 +7156,11 @@
         <v>150</v>
       </c>
       <c r="L4" s="204"/>
-      <c r="M4" s="641"/>
+      <c r="M4" s="620"/>
       <c r="N4" s="174" t="s">
         <v>69</v>
       </c>
-      <c r="O4" s="645"/>
+      <c r="O4" s="650"/>
       <c r="P4" s="2" t="s">
         <v>191</v>
       </c>
@@ -7187,12 +7182,12 @@
       <c r="X4" s="431" t="s">
         <v>158</v>
       </c>
-      <c r="Y4" s="654"/>
+      <c r="Y4" s="658"/>
       <c r="Z4" s="409"/>
       <c r="AA4" s="307"/>
       <c r="AB4" s="209"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="656"/>
+      <c r="AD4" s="631"/>
       <c r="AE4" s="257"/>
       <c r="AF4" s="257"/>
       <c r="AG4" s="16"/>
@@ -7202,37 +7197,37 @@
       <c r="AK4" s="257"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="428"/>
-      <c r="AN4" s="636"/>
+      <c r="AN4" s="641"/>
       <c r="AO4" s="338" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="659" t="s">
+      <c r="A5" s="613" t="s">
         <v>418</v>
       </c>
-      <c r="B5" s="634"/>
-      <c r="C5" s="616"/>
+      <c r="B5" s="683"/>
+      <c r="C5" s="646"/>
       <c r="D5" s="61" t="s">
         <v>153</v>
       </c>
       <c r="E5" s="379">
         <v>1</v>
       </c>
-      <c r="F5" s="641"/>
-      <c r="G5" s="625" t="s">
+      <c r="F5" s="620"/>
+      <c r="G5" s="674" t="s">
         <v>192</v>
       </c>
-      <c r="H5" s="625"/>
-      <c r="I5" s="625"/>
-      <c r="J5" s="625"/>
-      <c r="K5" s="625"/>
-      <c r="L5" s="626"/>
-      <c r="M5" s="641"/>
+      <c r="H5" s="674"/>
+      <c r="I5" s="674"/>
+      <c r="J5" s="674"/>
+      <c r="K5" s="674"/>
+      <c r="L5" s="675"/>
+      <c r="M5" s="620"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
-      <c r="O5" s="645"/>
+      <c r="O5" s="650"/>
       <c r="T5" s="89"/>
       <c r="U5" s="124"/>
       <c r="V5" s="120"/>
@@ -7240,7 +7235,7 @@
       <c r="X5" s="431" t="s">
         <v>159</v>
       </c>
-      <c r="Y5" s="654"/>
+      <c r="Y5" s="658"/>
       <c r="Z5" s="409">
         <v>1</v>
       </c>
@@ -7263,24 +7258,24 @@
       <c r="AK5" s="257"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="428"/>
-      <c r="AN5" s="636"/>
+      <c r="AN5" s="641"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="660"/>
-      <c r="B6" s="631" t="s">
+      <c r="A6" s="614"/>
+      <c r="B6" s="680" t="s">
         <v>177</v>
       </c>
-      <c r="C6" s="661"/>
-      <c r="D6" s="662"/>
-      <c r="F6" s="641"/>
-      <c r="G6" s="627"/>
-      <c r="H6" s="627"/>
-      <c r="I6" s="627"/>
-      <c r="J6" s="627"/>
-      <c r="K6" s="627"/>
-      <c r="L6" s="628"/>
-      <c r="M6" s="641"/>
-      <c r="O6" s="645"/>
+      <c r="C6" s="628"/>
+      <c r="D6" s="629"/>
+      <c r="F6" s="620"/>
+      <c r="G6" s="676"/>
+      <c r="H6" s="676"/>
+      <c r="I6" s="676"/>
+      <c r="J6" s="676"/>
+      <c r="K6" s="676"/>
+      <c r="L6" s="677"/>
+      <c r="M6" s="620"/>
+      <c r="O6" s="650"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
       <c r="V6" s="98" t="s">
@@ -7290,7 +7285,7 @@
       <c r="X6" s="431" t="s">
         <v>160</v>
       </c>
-      <c r="Y6" s="654"/>
+      <c r="Y6" s="658"/>
       <c r="Z6" s="407">
         <v>1</v>
       </c>
@@ -7304,16 +7299,16 @@
       <c r="AF6" s="257"/>
       <c r="AG6" s="257"/>
       <c r="AH6" s="257"/>
-      <c r="AI6" s="650"/>
+      <c r="AI6" s="630"/>
       <c r="AJ6" s="441" t="s">
         <v>458</v>
       </c>
-      <c r="AK6" s="650" t="s">
+      <c r="AK6" s="630" t="s">
         <v>251</v>
       </c>
       <c r="AL6" s="257"/>
       <c r="AM6" s="428"/>
-      <c r="AN6" s="636"/>
+      <c r="AN6" s="641"/>
       <c r="AO6" s="338" t="s">
         <v>470</v>
       </c>
@@ -7322,7 +7317,7 @@
       <c r="A7" s="232" t="s">
         <v>571</v>
       </c>
-      <c r="B7" s="632"/>
+      <c r="B7" s="681"/>
       <c r="C7" s="202" t="s">
         <v>374</v>
       </c>
@@ -7332,7 +7327,7 @@
       <c r="E7" s="265">
         <v>3</v>
       </c>
-      <c r="F7" s="641"/>
+      <c r="F7" s="620"/>
       <c r="G7" s="395">
         <v>0</v>
       </c>
@@ -7351,8 +7346,8 @@
       <c r="L7" s="212">
         <v>0</v>
       </c>
-      <c r="M7" s="641"/>
-      <c r="O7" s="645"/>
+      <c r="M7" s="620"/>
+      <c r="O7" s="650"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
       </c>
@@ -7366,7 +7361,7 @@
       <c r="X7" s="431" t="s">
         <v>161</v>
       </c>
-      <c r="Y7" s="654"/>
+      <c r="Y7" s="658"/>
       <c r="Z7" s="407">
         <v>1</v>
       </c>
@@ -7376,18 +7371,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="257"/>
       <c r="AF7" s="257"/>
-      <c r="AG7" s="656" t="s">
+      <c r="AG7" s="631" t="s">
         <v>454</v>
       </c>
       <c r="AH7" s="257"/>
-      <c r="AI7" s="650"/>
+      <c r="AI7" s="630"/>
       <c r="AJ7" s="257"/>
-      <c r="AK7" s="650"/>
+      <c r="AK7" s="630"/>
       <c r="AL7" s="80" t="s">
         <v>496</v>
       </c>
       <c r="AM7" s="428"/>
-      <c r="AN7" s="636"/>
+      <c r="AN7" s="641"/>
       <c r="AP7" s="76" t="s">
         <v>471</v>
       </c>
@@ -7404,27 +7399,27 @@
         <f>SUM(G7:N9)</f>
         <v>15</v>
       </c>
-      <c r="F8" s="641"/>
-      <c r="G8" s="626">
-        <v>0</v>
-      </c>
-      <c r="H8" s="623" t="s">
+      <c r="F8" s="620"/>
+      <c r="G8" s="675">
+        <v>0</v>
+      </c>
+      <c r="H8" s="672" t="s">
         <v>104</v>
       </c>
       <c r="I8" s="598">
         <v>0</v>
       </c>
-      <c r="J8" s="623" t="s">
+      <c r="J8" s="672" t="s">
         <v>104</v>
       </c>
-      <c r="K8" s="629"/>
-      <c r="L8" s="663"/>
-      <c r="M8" s="642"/>
-      <c r="N8" s="666">
+      <c r="K8" s="678"/>
+      <c r="L8" s="632"/>
+      <c r="M8" s="647"/>
+      <c r="N8" s="637">
         <f>N5+N11</f>
         <v>15</v>
       </c>
-      <c r="O8" s="645"/>
+      <c r="O8" s="650"/>
       <c r="T8" s="103" t="s">
         <v>44</v>
       </c>
@@ -7434,7 +7429,7 @@
       <c r="X8" s="431" t="s">
         <v>162</v>
       </c>
-      <c r="Y8" s="654"/>
+      <c r="Y8" s="658"/>
       <c r="Z8" s="409"/>
       <c r="AA8" s="307"/>
       <c r="AB8" s="209"/>
@@ -7442,14 +7437,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="257"/>
       <c r="AF8" s="257"/>
-      <c r="AG8" s="656"/>
+      <c r="AG8" s="631"/>
       <c r="AH8" s="257"/>
-      <c r="AI8" s="650"/>
+      <c r="AI8" s="630"/>
       <c r="AJ8" s="257"/>
       <c r="AK8" s="257"/>
       <c r="AL8" s="257"/>
       <c r="AM8" s="428"/>
-      <c r="AN8" s="636"/>
+      <c r="AN8" s="641"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="232" t="s">
@@ -7464,17 +7459,17 @@
       <c r="D9" s="348" t="s">
         <v>281</v>
       </c>
-      <c r="F9" s="641"/>
-      <c r="G9" s="628"/>
-      <c r="H9" s="624"/>
+      <c r="F9" s="620"/>
+      <c r="G9" s="677"/>
+      <c r="H9" s="673"/>
       <c r="I9" s="600"/>
-      <c r="J9" s="624"/>
-      <c r="K9" s="630"/>
-      <c r="L9" s="664"/>
-      <c r="M9" s="643"/>
-      <c r="N9" s="667"/>
-      <c r="O9" s="646"/>
-      <c r="S9" s="657" t="s">
+      <c r="J9" s="673"/>
+      <c r="K9" s="679"/>
+      <c r="L9" s="633"/>
+      <c r="M9" s="648"/>
+      <c r="N9" s="638"/>
+      <c r="O9" s="651"/>
+      <c r="S9" s="634" t="s">
         <v>61</v>
       </c>
       <c r="T9" s="89"/>
@@ -7486,7 +7481,7 @@
       <c r="X9" s="431" t="s">
         <v>163</v>
       </c>
-      <c r="Y9" s="654"/>
+      <c r="Y9" s="658"/>
       <c r="Z9" s="410"/>
       <c r="AA9" s="307"/>
       <c r="AB9" s="209"/>
@@ -7496,16 +7491,16 @@
       </c>
       <c r="AE9" s="257"/>
       <c r="AF9" s="257"/>
-      <c r="AG9" s="656"/>
+      <c r="AG9" s="631"/>
       <c r="AH9" s="257"/>
-      <c r="AI9" s="650"/>
+      <c r="AI9" s="630"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="650" t="s">
+      <c r="AK9" s="630" t="s">
         <v>251</v>
       </c>
       <c r="AL9" s="257"/>
       <c r="AM9" s="428"/>
-      <c r="AN9" s="636"/>
+      <c r="AN9" s="641"/>
       <c r="AP9" s="2" t="s">
         <v>508</v>
       </c>
@@ -7522,20 +7517,20 @@
         <f>Boat!W8</f>
         <v>37</v>
       </c>
-      <c r="F10" s="641"/>
+      <c r="F10" s="620"/>
       <c r="N10" s="418" t="s">
         <v>396</v>
       </c>
-      <c r="O10" s="678" t="s">
+      <c r="O10" s="622" t="s">
         <v>102</v>
       </c>
-      <c r="P10" s="647" t="s">
+      <c r="P10" s="652" t="s">
         <v>400</v>
       </c>
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="665"/>
+      <c r="S10" s="635"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>176</v>
@@ -7547,7 +7542,7 @@
       <c r="X10" s="431" t="s">
         <v>164</v>
       </c>
-      <c r="Y10" s="654"/>
+      <c r="Y10" s="658"/>
       <c r="Z10" s="409">
         <v>0</v>
       </c>
@@ -7565,16 +7560,16 @@
       <c r="AF10" s="238" t="s">
         <v>311</v>
       </c>
-      <c r="AG10" s="656"/>
+      <c r="AG10" s="631"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="650"/>
+      <c r="AI10" s="630"/>
       <c r="AJ10" s="257"/>
-      <c r="AK10" s="650"/>
+      <c r="AK10" s="630"/>
       <c r="AL10" s="257"/>
       <c r="AM10" s="442" t="s">
         <v>318</v>
       </c>
-      <c r="AN10" s="636"/>
+      <c r="AN10" s="641"/>
       <c r="AO10" s="204" t="s">
         <v>94</v>
       </c>
@@ -7592,18 +7587,18 @@
       <c r="D11" s="170" t="s">
         <v>355</v>
       </c>
-      <c r="F11" s="641"/>
+      <c r="F11" s="620"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="679"/>
-      <c r="P11" s="648"/>
+      <c r="O11" s="623"/>
+      <c r="P11" s="653"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>220</v>
       </c>
-      <c r="S11" s="665"/>
+      <c r="S11" s="635"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -7613,7 +7608,7 @@
       <c r="X11" s="431" t="s">
         <v>165</v>
       </c>
-      <c r="Y11" s="654"/>
+      <c r="Y11" s="658"/>
       <c r="Z11" s="409"/>
       <c r="AA11" s="307">
         <v>1</v>
@@ -7627,14 +7622,14 @@
       <c r="AF11" s="257" t="s">
         <v>476</v>
       </c>
-      <c r="AG11" s="656"/>
+      <c r="AG11" s="631"/>
       <c r="AH11" s="257"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="257"/>
       <c r="AK11" s="257"/>
       <c r="AL11" s="257"/>
       <c r="AM11" s="428"/>
-      <c r="AN11" s="636"/>
+      <c r="AN11" s="641"/>
       <c r="AP11" s="76" t="s">
         <v>484</v>
       </c>
@@ -7653,7 +7648,7 @@
       <c r="E12" s="224">
         <v>3</v>
       </c>
-      <c r="F12" s="641"/>
+      <c r="F12" s="620"/>
       <c r="G12" s="337" t="s">
         <v>400</v>
       </c>
@@ -7662,16 +7657,16 @@
       </c>
       <c r="I12" s="605"/>
       <c r="J12" s="605"/>
-      <c r="K12" s="683"/>
+      <c r="K12" s="627"/>
       <c r="L12" s="203"/>
       <c r="M12" s="203"/>
       <c r="N12" s="203"/>
-      <c r="O12" s="679"/>
-      <c r="P12" s="648"/>
+      <c r="O12" s="623"/>
+      <c r="P12" s="653"/>
       <c r="R12" s="122" t="s">
         <v>180</v>
       </c>
-      <c r="S12" s="658"/>
+      <c r="S12" s="636"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -7681,7 +7676,7 @@
       <c r="X12" s="431" t="s">
         <v>166</v>
       </c>
-      <c r="Y12" s="654"/>
+      <c r="Y12" s="658"/>
       <c r="Z12" s="407">
         <v>1</v>
       </c>
@@ -7692,16 +7687,16 @@
       <c r="AC12" s="100" t="s">
         <v>481</v>
       </c>
-      <c r="AD12" s="668" t="s">
+      <c r="AD12" s="639" t="s">
         <v>240</v>
       </c>
       <c r="AE12" s="441" t="s">
         <v>239</v>
       </c>
-      <c r="AF12" s="656" t="s">
+      <c r="AF12" s="631" t="s">
         <v>228</v>
       </c>
-      <c r="AG12" s="656"/>
+      <c r="AG12" s="631"/>
       <c r="AH12" s="238" t="s">
         <v>259</v>
       </c>
@@ -7711,10 +7706,10 @@
       <c r="AJ12" s="257"/>
       <c r="AK12" s="257"/>
       <c r="AL12" s="257"/>
-      <c r="AM12" s="651" t="s">
+      <c r="AM12" s="655" t="s">
         <v>249</v>
       </c>
-      <c r="AN12" s="636"/>
+      <c r="AN12" s="641"/>
       <c r="AO12" s="338" t="s">
         <v>96</v>
       </c>
@@ -7726,17 +7721,17 @@
       <c r="E13" s="448">
         <v>-3</v>
       </c>
-      <c r="F13" s="641"/>
+      <c r="F13" s="620"/>
       <c r="G13" s="605" t="s">
         <v>430</v>
       </c>
       <c r="H13" s="605"/>
       <c r="I13" s="605"/>
-      <c r="J13" s="683"/>
+      <c r="J13" s="627"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="679"/>
-      <c r="P13" s="649"/>
+      <c r="O13" s="623"/>
+      <c r="P13" s="654"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
       </c>
@@ -7746,7 +7741,7 @@
       <c r="X13" s="431" t="s">
         <v>167</v>
       </c>
-      <c r="Y13" s="654"/>
+      <c r="Y13" s="658"/>
       <c r="Z13" s="407">
         <v>1</v>
       </c>
@@ -7757,8 +7752,8 @@
         <v>500</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="668"/>
-      <c r="AF13" s="656"/>
+      <c r="AD13" s="639"/>
+      <c r="AF13" s="631"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="238" t="s">
         <v>308</v>
@@ -7769,8 +7764,8 @@
       <c r="AJ13" s="80"/>
       <c r="AK13" s="257"/>
       <c r="AL13" s="257"/>
-      <c r="AM13" s="651"/>
-      <c r="AN13" s="636"/>
+      <c r="AM13" s="655"/>
+      <c r="AN13" s="641"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="450"/>
@@ -7778,18 +7773,18 @@
       <c r="C14" s="459"/>
       <c r="D14" s="452"/>
       <c r="E14" s="453"/>
-      <c r="F14" s="641"/>
+      <c r="F14" s="620"/>
       <c r="G14" s="605" t="s">
         <v>429</v>
       </c>
       <c r="H14" s="605"/>
       <c r="I14" s="605"/>
-      <c r="J14" s="683"/>
+      <c r="J14" s="627"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="679"/>
+      <c r="O14" s="623"/>
       <c r="Q14" s="61" t="s">
         <v>532</v>
       </c>
@@ -7803,24 +7798,24 @@
       <c r="X14" s="431" t="s">
         <v>168</v>
       </c>
-      <c r="Y14" s="654"/>
+      <c r="Y14" s="658"/>
       <c r="Z14" s="407">
         <v>1</v>
       </c>
       <c r="AA14" s="307"/>
       <c r="AB14" s="209"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="668"/>
+      <c r="AD14" s="639"/>
       <c r="AE14" s="257"/>
-      <c r="AF14" s="656"/>
+      <c r="AF14" s="631"/>
       <c r="AG14" s="257"/>
       <c r="AH14" s="257"/>
       <c r="AI14" s="70"/>
       <c r="AJ14" s="257"/>
       <c r="AK14" s="257"/>
       <c r="AL14" s="257"/>
-      <c r="AM14" s="651"/>
-      <c r="AN14" s="636"/>
+      <c r="AM14" s="655"/>
+      <c r="AN14" s="641"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="449" t="s">
@@ -7829,8 +7824,8 @@
       <c r="C15" s="598" t="s">
         <v>373</v>
       </c>
-      <c r="F15" s="641"/>
-      <c r="O15" s="679"/>
+      <c r="F15" s="620"/>
+      <c r="O15" s="623"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -7843,7 +7838,7 @@
       <c r="X15" s="431" t="s">
         <v>169</v>
       </c>
-      <c r="Y15" s="654"/>
+      <c r="Y15" s="658"/>
       <c r="Z15" s="409">
         <v>1</v>
       </c>
@@ -7852,8 +7847,8 @@
       <c r="AC15" s="76" t="s">
         <v>479</v>
       </c>
-      <c r="AD15" s="668"/>
-      <c r="AF15" s="656"/>
+      <c r="AD15" s="639"/>
+      <c r="AF15" s="631"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="238" t="s">
         <v>448</v>
@@ -7866,8 +7861,8 @@
       </c>
       <c r="AK15" s="257"/>
       <c r="AL15" s="257"/>
-      <c r="AM15" s="651"/>
-      <c r="AN15" s="636"/>
+      <c r="AM15" s="655"/>
+      <c r="AN15" s="641"/>
       <c r="AP15" s="76" t="s">
         <v>73</v>
       </c>
@@ -7889,13 +7884,13 @@
       <c r="E16" s="224">
         <v>1</v>
       </c>
-      <c r="F16" s="641"/>
+      <c r="F16" s="620"/>
       <c r="G16" s="337" t="s">
         <v>488</v>
       </c>
       <c r="I16" s="469"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="679"/>
+      <c r="O16" s="623"/>
       <c r="R16" s="435" t="s">
         <v>184</v>
       </c>
@@ -7906,7 +7901,7 @@
       <c r="X16" s="431" t="s">
         <v>170</v>
       </c>
-      <c r="Y16" s="654"/>
+      <c r="Y16" s="658"/>
       <c r="Z16" s="407">
         <v>1</v>
       </c>
@@ -7927,18 +7922,18 @@
       <c r="AM16" s="428" t="s">
         <v>317</v>
       </c>
-      <c r="AN16" s="636"/>
+      <c r="AN16" s="641"/>
       <c r="AP16" s="76" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="641"/>
+      <c r="F17" s="620"/>
       <c r="I17" s="470"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="679"/>
+      <c r="O17" s="623"/>
       <c r="Q17" s="21" t="s">
         <v>530</v>
       </c>
@@ -7958,7 +7953,7 @@
       <c r="X17" s="431" t="s">
         <v>171</v>
       </c>
-      <c r="Y17" s="654"/>
+      <c r="Y17" s="658"/>
       <c r="Z17" s="409"/>
       <c r="AA17" s="307"/>
       <c r="AB17" s="209"/>
@@ -7983,7 +7978,7 @@
       <c r="AK17" s="257"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="428"/>
-      <c r="AN17" s="636"/>
+      <c r="AN17" s="641"/>
       <c r="AO17" s="204" t="s">
         <v>497</v>
       </c>
@@ -8007,21 +8002,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="641"/>
+      <c r="F18" s="620"/>
       <c r="G18" s="337" t="s">
         <v>527</v>
       </c>
       <c r="I18" s="24"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="679"/>
+      <c r="O18" s="623"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="673" t="s">
+      <c r="R18" s="615" t="s">
         <v>535</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="612" t="s">
+      <c r="U18" s="663" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -8031,7 +8026,7 @@
       <c r="X18" s="431" t="s">
         <v>172</v>
       </c>
-      <c r="Y18" s="654"/>
+      <c r="Y18" s="658"/>
       <c r="Z18" s="409">
         <v>1</v>
       </c>
@@ -8042,38 +8037,38 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="257"/>
-      <c r="AF18" s="650" t="s">
+      <c r="AF18" s="630" t="s">
         <v>475</v>
       </c>
       <c r="AG18" s="257"/>
       <c r="AH18" s="70"/>
       <c r="AI18" s="70"/>
-      <c r="AJ18" s="652" t="s">
+      <c r="AJ18" s="656" t="s">
         <v>315</v>
       </c>
       <c r="AK18" s="257"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="428"/>
-      <c r="AN18" s="636"/>
+      <c r="AN18" s="641"/>
       <c r="AP18" s="76" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="641"/>
+      <c r="F19" s="620"/>
       <c r="I19" s="219"/>
-      <c r="O19" s="679"/>
-      <c r="R19" s="674"/>
+      <c r="O19" s="623"/>
+      <c r="R19" s="616"/>
       <c r="S19" s="30" t="s">
         <v>533</v>
       </c>
-      <c r="U19" s="613"/>
+      <c r="U19" s="664"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="431" t="s">
         <v>173</v>
       </c>
-      <c r="Y19" s="654"/>
+      <c r="Y19" s="658"/>
       <c r="Z19" s="407">
         <v>1</v>
       </c>
@@ -8082,17 +8077,17 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="257"/>
-      <c r="AF19" s="650"/>
+      <c r="AF19" s="630"/>
       <c r="AG19" s="257"/>
       <c r="AH19" s="257"/>
       <c r="AI19" s="70"/>
-      <c r="AJ19" s="652"/>
+      <c r="AJ19" s="656"/>
       <c r="AK19" s="460" t="s">
         <v>251</v>
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="428"/>
-      <c r="AN19" s="636"/>
+      <c r="AN19" s="641"/>
       <c r="AP19" s="76" t="s">
         <v>468</v>
       </c>
@@ -8113,24 +8108,24 @@
       <c r="E20" s="437">
         <v>-1</v>
       </c>
-      <c r="F20" s="641"/>
+      <c r="F20" s="620"/>
       <c r="G20" s="337" t="s">
         <v>491</v>
       </c>
       <c r="I20" s="219"/>
-      <c r="O20" s="679"/>
-      <c r="Q20" s="681" t="s">
+      <c r="O20" s="623"/>
+      <c r="Q20" s="625" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="404" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="614"/>
+      <c r="U20" s="665"/>
       <c r="W20" s="405"/>
       <c r="X20" s="432" t="s">
         <v>174</v>
       </c>
-      <c r="Y20" s="654"/>
+      <c r="Y20" s="658"/>
       <c r="Z20" s="411">
         <v>1</v>
       </c>
@@ -8155,7 +8150,7 @@
       <c r="AM20" s="381" t="s">
         <v>249</v>
       </c>
-      <c r="AN20" s="636"/>
+      <c r="AN20" s="641"/>
       <c r="AO20" s="338" t="s">
         <v>460</v>
       </c>
@@ -8176,20 +8171,20 @@
       <c r="E21" s="265">
         <v>0</v>
       </c>
-      <c r="F21" s="641"/>
+      <c r="F21" s="620"/>
       <c r="I21" s="219"/>
-      <c r="O21" s="679"/>
-      <c r="Q21" s="682"/>
+      <c r="O21" s="623"/>
+      <c r="Q21" s="626"/>
       <c r="T21" s="422"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="609"/>
+      <c r="V21" s="660"/>
       <c r="W21" s="426" t="s">
         <v>175</v>
       </c>
       <c r="X21" s="429" t="s">
         <v>186</v>
       </c>
-      <c r="Y21" s="654"/>
+      <c r="Y21" s="658"/>
       <c r="Z21" s="445">
         <v>3</v>
       </c>
@@ -8220,15 +8215,15 @@
       <c r="AM21" s="428" t="s">
         <v>544</v>
       </c>
-      <c r="AN21" s="636"/>
+      <c r="AN21" s="641"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="641"/>
+      <c r="F22" s="620"/>
       <c r="G22" s="337" t="s">
         <v>489</v>
       </c>
       <c r="I22" s="219"/>
-      <c r="O22" s="679"/>
+      <c r="O22" s="623"/>
       <c r="R22" s="434" t="s">
         <v>44</v>
       </c>
@@ -8236,14 +8231,14 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="610"/>
+      <c r="V22" s="661"/>
       <c r="W22" s="426" t="s">
         <v>175</v>
       </c>
       <c r="X22" s="429" t="s">
         <v>187</v>
       </c>
-      <c r="Y22" s="654"/>
+      <c r="Y22" s="658"/>
       <c r="Z22" s="415"/>
       <c r="AA22" s="10"/>
       <c r="AB22" s="415"/>
@@ -8254,7 +8249,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="650" t="s">
+      <c r="AJ22" s="630" t="s">
         <v>472</v>
       </c>
       <c r="AK22" s="257"/>
@@ -8262,7 +8257,7 @@
         <v>478</v>
       </c>
       <c r="AM22" s="300"/>
-      <c r="AN22" s="636"/>
+      <c r="AN22" s="641"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="231" t="s">
@@ -8280,22 +8275,22 @@
       <c r="E23" s="225">
         <v>1</v>
       </c>
-      <c r="F23" s="641"/>
+      <c r="F23" s="620"/>
       <c r="I23" s="219"/>
-      <c r="O23" s="679"/>
-      <c r="Q23" s="681" t="s">
+      <c r="O23" s="623"/>
+      <c r="Q23" s="625" t="s">
         <v>144</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="420" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="610"/>
+      <c r="V23" s="661"/>
       <c r="W23" s="148"/>
       <c r="X23" s="429" t="s">
         <v>188</v>
       </c>
-      <c r="Y23" s="654"/>
+      <c r="Y23" s="658"/>
       <c r="Z23" s="17"/>
       <c r="AA23" s="10"/>
       <c r="AB23" s="415"/>
@@ -8306,13 +8301,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="650"/>
+      <c r="AJ23" s="630"/>
       <c r="AK23" s="257"/>
       <c r="AL23" s="80" t="s">
         <v>507</v>
       </c>
       <c r="AM23" s="300"/>
-      <c r="AN23" s="636"/>
+      <c r="AN23" s="641"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="440" t="s">
@@ -8330,23 +8325,23 @@
       <c r="E24" s="436">
         <v>1</v>
       </c>
-      <c r="F24" s="641"/>
+      <c r="F24" s="620"/>
       <c r="G24" s="61" t="s">
         <v>490</v>
       </c>
       <c r="I24" s="219"/>
-      <c r="O24" s="679"/>
-      <c r="Q24" s="682"/>
+      <c r="O24" s="623"/>
+      <c r="Q24" s="626"/>
       <c r="T24" s="17"/>
       <c r="U24" s="227" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="610"/>
+      <c r="V24" s="661"/>
       <c r="W24" s="148"/>
       <c r="X24" s="429" t="s">
         <v>185</v>
       </c>
-      <c r="Y24" s="654"/>
+      <c r="Y24" s="658"/>
       <c r="Z24" s="17"/>
       <c r="AA24" s="10"/>
       <c r="AB24" s="415"/>
@@ -8365,12 +8360,12 @@
         <v>463</v>
       </c>
       <c r="AM24" s="300"/>
-      <c r="AN24" s="636"/>
+      <c r="AN24" s="641"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="641"/>
+      <c r="F25" s="620"/>
       <c r="I25" s="219"/>
-      <c r="O25" s="679"/>
+      <c r="O25" s="623"/>
       <c r="P25" s="204" t="s">
         <v>280</v>
       </c>
@@ -8383,12 +8378,12 @@
       <c r="U25" s="400" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="611"/>
+      <c r="V25" s="662"/>
       <c r="W25" s="148"/>
       <c r="X25" s="429" t="s">
         <v>189</v>
       </c>
-      <c r="Y25" s="654"/>
+      <c r="Y25" s="658"/>
       <c r="Z25" s="17"/>
       <c r="AA25" s="10"/>
       <c r="AB25" s="415"/>
@@ -8405,7 +8400,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="300"/>
-      <c r="AN25" s="636"/>
+      <c r="AN25" s="641"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="231" t="s">
@@ -8423,17 +8418,17 @@
       <c r="E26" s="380">
         <v>1</v>
       </c>
-      <c r="F26" s="641"/>
+      <c r="F26" s="620"/>
       <c r="G26" s="337" t="s">
         <v>487</v>
       </c>
       <c r="I26" s="219"/>
-      <c r="O26" s="679"/>
-      <c r="P26" s="638" t="s">
+      <c r="O26" s="623"/>
+      <c r="P26" s="643" t="s">
         <v>525</v>
       </c>
-      <c r="Q26" s="639"/>
-      <c r="R26" s="675" t="s">
+      <c r="Q26" s="644"/>
+      <c r="R26" s="617" t="s">
         <v>534</v>
       </c>
       <c r="T26" s="178"/>
@@ -8445,7 +8440,7 @@
       <c r="X26" s="429" t="s">
         <v>181</v>
       </c>
-      <c r="Y26" s="654"/>
+      <c r="Y26" s="658"/>
       <c r="Z26" s="17"/>
       <c r="AA26" s="10"/>
       <c r="AB26" s="415"/>
@@ -8472,7 +8467,7 @@
       <c r="AM26" s="442" t="s">
         <v>456</v>
       </c>
-      <c r="AN26" s="636"/>
+      <c r="AN26" s="641"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -8484,13 +8479,13 @@
       <c r="E27" s="265" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="677"/>
+      <c r="F27" s="621"/>
       <c r="G27" s="61" t="s">
         <v>543</v>
       </c>
       <c r="I27" s="220"/>
-      <c r="O27" s="680"/>
-      <c r="R27" s="676"/>
+      <c r="O27" s="624"/>
+      <c r="R27" s="618"/>
       <c r="S27" s="421" t="s">
         <v>54</v>
       </c>
@@ -8503,7 +8498,7 @@
       <c r="X27" s="429" t="s">
         <v>529</v>
       </c>
-      <c r="Y27" s="655"/>
+      <c r="Y27" s="659"/>
       <c r="Z27" s="161"/>
       <c r="AA27" s="13"/>
       <c r="AB27" s="416"/>
@@ -8520,32 +8515,26 @@
       <c r="AM27" s="381" t="s">
         <v>319</v>
       </c>
-      <c r="AN27" s="637"/>
+      <c r="AN27" s="642"/>
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="F2:F27"/>
-    <mergeCell ref="O10:O27"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AI6:AI10"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AG7:AG12"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="V21:V25"/>
+    <mergeCell ref="U18:U20"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="G5:L6"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B4:B5"/>
     <mergeCell ref="AN1:AN27"/>
     <mergeCell ref="P26:Q26"/>
     <mergeCell ref="Q2:Q3"/>
@@ -8562,22 +8551,28 @@
     <mergeCell ref="AD3:AD4"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="R2:R3"/>
-    <mergeCell ref="V21:V25"/>
-    <mergeCell ref="U18:U20"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="G5:L6"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="AI6:AI10"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AG7:AG12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="O10:O27"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8614,12 +8609,12 @@
       <c r="B1" s="603" t="s">
         <v>310</v>
       </c>
-      <c r="C1" s="683"/>
+      <c r="C1" s="627"/>
       <c r="D1" s="204"/>
       <c r="J1" s="603" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="683"/>
+      <c r="K1" s="627"/>
       <c r="L1" s="195" t="s">
         <v>330</v>
       </c>
@@ -9022,7 +9017,7 @@
       <c r="P1" s="398" t="s">
         <v>397</v>
       </c>
-      <c r="Q1" s="714" t="s">
+      <c r="Q1" s="701" t="s">
         <v>180</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -9046,7 +9041,7 @@
       <c r="AA1" s="517" t="s">
         <v>437</v>
       </c>
-      <c r="AB1" s="708" t="s">
+      <c r="AB1" s="695" t="s">
         <v>593</v>
       </c>
       <c r="AC1" s="99" t="s">
@@ -9068,32 +9063,32 @@
       </c>
     </row>
     <row r="2" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="693">
+      <c r="A2" s="706">
         <f ca="1">TODAY()</f>
-        <v>45290</v>
-      </c>
-      <c r="B2" s="695" t="s">
+        <v>45291</v>
+      </c>
+      <c r="B2" s="708" t="s">
         <v>379</v>
       </c>
-      <c r="C2" s="615" t="s">
+      <c r="C2" s="645" t="s">
         <v>357</v>
       </c>
-      <c r="D2" s="697" t="s">
+      <c r="D2" s="710" t="s">
         <v>102</v>
       </c>
-      <c r="E2" s="699" t="s">
+      <c r="E2" s="712" t="s">
         <v>64</v>
       </c>
       <c r="F2" s="191" t="s">
         <v>218</v>
       </c>
-      <c r="G2" s="659" t="s">
+      <c r="G2" s="613" t="s">
         <v>372</v>
       </c>
       <c r="H2" s="206" t="s">
         <v>218</v>
       </c>
-      <c r="I2" s="705" t="s">
+      <c r="I2" s="692" t="s">
         <v>102</v>
       </c>
       <c r="J2" s="396" t="s">
@@ -9117,7 +9112,7 @@
       <c r="P2" s="399">
         <v>40</v>
       </c>
-      <c r="Q2" s="715"/>
+      <c r="Q2" s="702"/>
       <c r="R2" s="21">
         <f>R7+R20</f>
         <v>2</v>
@@ -9142,7 +9137,7 @@
         <f>IF((Z2+T2)&gt;0,0,-1)</f>
         <v>0</v>
       </c>
-      <c r="AB2" s="709"/>
+      <c r="AB2" s="696"/>
       <c r="AC2" s="35"/>
       <c r="AH2" s="6" t="s">
         <v>344</v>
@@ -9157,14 +9152,14 @@
       </c>
     </row>
     <row r="3" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="694"/>
-      <c r="B3" s="696"/>
-      <c r="C3" s="616"/>
-      <c r="D3" s="698"/>
-      <c r="E3" s="700"/>
-      <c r="G3" s="660"/>
+      <c r="A3" s="707"/>
+      <c r="B3" s="709"/>
+      <c r="C3" s="646"/>
+      <c r="D3" s="711"/>
+      <c r="E3" s="713"/>
+      <c r="G3" s="614"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="706"/>
+      <c r="I3" s="693"/>
       <c r="K3" s="24">
         <v>2</v>
       </c>
@@ -9179,7 +9174,7 @@
       <c r="V3" s="470"/>
       <c r="W3" s="6"/>
       <c r="X3" s="470"/>
-      <c r="AB3" s="709"/>
+      <c r="AB3" s="696"/>
       <c r="AC3" s="35"/>
       <c r="AE3" s="100" t="s">
         <v>588</v>
@@ -9208,10 +9203,10 @@
         <v>380</v>
       </c>
       <c r="B4" s="243"/>
-      <c r="C4" s="701" t="s">
+      <c r="C4" s="714" t="s">
         <v>177</v>
       </c>
-      <c r="I4" s="706"/>
+      <c r="I4" s="693"/>
       <c r="R4" s="471" t="s">
         <v>588</v>
       </c>
@@ -9223,7 +9218,7 @@
       <c r="V4" s="470"/>
       <c r="W4" s="6"/>
       <c r="X4" s="470"/>
-      <c r="AB4" s="709"/>
+      <c r="AB4" s="696"/>
       <c r="AC4" s="35"/>
       <c r="AE4" s="20"/>
       <c r="AF4" s="100" t="s">
@@ -9239,7 +9234,7 @@
       <c r="AI4" s="470"/>
       <c r="AJ4" s="552"/>
       <c r="AK4" s="6" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="AL4" s="24">
         <v>1</v>
@@ -9252,7 +9247,7 @@
       <c r="B5" s="100" t="s">
         <v>357</v>
       </c>
-      <c r="C5" s="702"/>
+      <c r="C5" s="715"/>
       <c r="D5" s="222" t="s">
         <v>102</v>
       </c>
@@ -9268,7 +9263,7 @@
       <c r="H5" s="206" t="s">
         <v>218</v>
       </c>
-      <c r="I5" s="706"/>
+      <c r="I5" s="693"/>
       <c r="J5" s="397" t="s">
         <v>268</v>
       </c>
@@ -9295,7 +9290,7 @@
       <c r="V5" s="468"/>
       <c r="W5" s="6"/>
       <c r="X5" s="468"/>
-      <c r="AB5" s="709"/>
+      <c r="AB5" s="696"/>
       <c r="AC5" s="2" t="s">
         <v>591</v>
       </c>
@@ -9315,19 +9310,19 @@
       <c r="AL5" s="468"/>
     </row>
     <row r="6" spans="1:38" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="690" t="s">
+      <c r="A6" s="703" t="s">
         <v>285</v>
       </c>
       <c r="B6" s="105" t="s">
         <v>198</v>
       </c>
-      <c r="C6" s="661"/>
-      <c r="D6" s="662"/>
+      <c r="C6" s="628"/>
+      <c r="D6" s="629"/>
       <c r="E6" s="96">
         <v>1</v>
       </c>
       <c r="G6" s="599"/>
-      <c r="I6" s="706"/>
+      <c r="I6" s="693"/>
       <c r="P6" s="61" t="s">
         <v>591</v>
       </c>
@@ -9339,7 +9334,7 @@
         <f>S7+S11-SUM(V2:V10)</f>
         <v>3</v>
       </c>
-      <c r="AB6" s="709"/>
+      <c r="AB6" s="696"/>
       <c r="AC6" s="35"/>
       <c r="AE6" s="64">
         <f>AE7-SUM(AL2:AL10)+AE11</f>
@@ -9355,7 +9350,7 @@
       <c r="AL6" s="112"/>
     </row>
     <row r="7" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="691"/>
+      <c r="A7" s="704"/>
       <c r="B7" s="100" t="s">
         <v>154</v>
       </c>
@@ -9366,7 +9361,7 @@
         <v>135</v>
       </c>
       <c r="G7" s="599"/>
-      <c r="I7" s="706"/>
+      <c r="I7" s="693"/>
       <c r="M7" s="16" t="s">
         <v>347</v>
       </c>
@@ -9396,7 +9391,7 @@
         <v>249</v>
       </c>
       <c r="X7" s="469"/>
-      <c r="AB7" s="709"/>
+      <c r="AB7" s="696"/>
       <c r="AC7" s="99" t="s">
         <v>592</v>
       </c>
@@ -9424,7 +9419,7 @@
       <c r="AL7" s="24"/>
     </row>
     <row r="8" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="692"/>
+      <c r="A8" s="705"/>
       <c r="B8" s="212" t="s">
         <v>28</v>
       </c>
@@ -9433,7 +9428,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="599"/>
-      <c r="I8" s="706"/>
+      <c r="I8" s="693"/>
       <c r="N8" s="80"/>
       <c r="U8" s="6"/>
       <c r="V8" s="24"/>
@@ -9441,7 +9436,7 @@
         <v>611</v>
       </c>
       <c r="X8" s="470"/>
-      <c r="AB8" s="709"/>
+      <c r="AB8" s="696"/>
       <c r="AC8" s="515"/>
       <c r="AH8" s="6" t="s">
         <v>610</v>
@@ -9472,7 +9467,7 @@
       </c>
       <c r="G9" s="599"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="706"/>
+      <c r="I9" s="693"/>
       <c r="M9" s="19" t="s">
         <v>524</v>
       </c>
@@ -9483,7 +9478,7 @@
         <v>603</v>
       </c>
       <c r="X9" s="470"/>
-      <c r="AB9" s="709"/>
+      <c r="AB9" s="696"/>
       <c r="AC9" s="515"/>
       <c r="AE9" s="20"/>
       <c r="AF9" s="20"/>
@@ -9491,7 +9486,7 @@
       <c r="AI9" s="470"/>
       <c r="AJ9" s="552"/>
       <c r="AK9" s="6" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="AL9" s="469">
         <v>1</v>
@@ -9511,7 +9506,7 @@
         <v>37</v>
       </c>
       <c r="G10" s="599"/>
-      <c r="I10" s="706"/>
+      <c r="I10" s="693"/>
       <c r="J10" s="24" t="s">
         <v>372</v>
       </c>
@@ -9526,7 +9521,7 @@
       <c r="V10" s="470"/>
       <c r="W10" s="6"/>
       <c r="X10" s="470"/>
-      <c r="AB10" s="709"/>
+      <c r="AB10" s="696"/>
       <c r="AC10" s="515"/>
       <c r="AE10" s="20"/>
       <c r="AF10" s="20"/>
@@ -9554,7 +9549,7 @@
         <v>265</v>
       </c>
       <c r="G11" s="599"/>
-      <c r="I11" s="706"/>
+      <c r="I11" s="693"/>
       <c r="J11" s="24" t="s">
         <v>194</v>
       </c>
@@ -9580,13 +9575,13 @@
       <c r="S11" s="24">
         <v>3</v>
       </c>
-      <c r="U11" s="711" t="s">
+      <c r="U11" s="698" t="s">
         <v>557</v>
       </c>
-      <c r="V11" s="712"/>
-      <c r="W11" s="712"/>
-      <c r="X11" s="713"/>
-      <c r="AB11" s="710"/>
+      <c r="V11" s="699"/>
+      <c r="W11" s="699"/>
+      <c r="X11" s="700"/>
+      <c r="AB11" s="697"/>
       <c r="AC11" s="99" t="s">
         <v>594</v>
       </c>
@@ -9600,13 +9595,13 @@
         <v>3</v>
       </c>
       <c r="AG11" s="414"/>
-      <c r="AH11" s="711" t="s">
+      <c r="AH11" s="698" t="s">
         <v>602</v>
       </c>
-      <c r="AI11" s="712"/>
-      <c r="AJ11" s="712"/>
-      <c r="AK11" s="712"/>
-      <c r="AL11" s="713"/>
+      <c r="AI11" s="699"/>
+      <c r="AJ11" s="699"/>
+      <c r="AK11" s="699"/>
+      <c r="AL11" s="700"/>
     </row>
     <row r="12" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="227" t="s">
@@ -9617,7 +9612,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="599"/>
-      <c r="I12" s="706"/>
+      <c r="I12" s="693"/>
       <c r="J12" s="24" t="s">
         <v>515</v>
       </c>
@@ -9650,7 +9645,7 @@
       </c>
       <c r="D13" s="20"/>
       <c r="G13" s="599"/>
-      <c r="I13" s="706"/>
+      <c r="I13" s="693"/>
       <c r="J13" s="108" t="s">
         <v>547</v>
       </c>
@@ -9694,7 +9689,7 @@
       <c r="H14" s="206" t="s">
         <v>218</v>
       </c>
-      <c r="I14" s="706"/>
+      <c r="I14" s="693"/>
       <c r="U14" s="67" t="s">
         <v>80</v>
       </c>
@@ -9721,7 +9716,7 @@
       <c r="H15" s="271">
         <v>0</v>
       </c>
-      <c r="I15" s="706"/>
+      <c r="I15" s="693"/>
       <c r="J15" s="108" t="s">
         <v>153</v>
       </c>
@@ -9752,7 +9747,7 @@
       <c r="D16" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="I16" s="706"/>
+      <c r="I16" s="693"/>
       <c r="K16" s="100" t="s">
         <v>44</v>
       </c>
@@ -9796,7 +9791,7 @@
       <c r="G17" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="I17" s="706"/>
+      <c r="I17" s="693"/>
       <c r="L17" s="2" t="s">
         <v>426</v>
       </c>
@@ -9810,13 +9805,13 @@
     </row>
     <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
-      <c r="I18" s="706"/>
+      <c r="I18" s="693"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="703" t="s">
+      <c r="O18" s="690" t="s">
         <v>516</v>
       </c>
-      <c r="P18" s="704"/>
+      <c r="P18" s="691"/>
       <c r="Q18" s="127" t="s">
         <v>44</v>
       </c>
@@ -9831,14 +9826,14 @@
       <c r="U18" s="19"/>
       <c r="V18" s="24"/>
       <c r="W18" s="19" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="X18" s="24">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="706"/>
+      <c r="I19" s="693"/>
       <c r="M19" s="21" t="s">
         <v>425</v>
       </c>
@@ -9870,7 +9865,7 @@
       <c r="G20" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="I20" s="706"/>
+      <c r="I20" s="693"/>
       <c r="K20" s="19" t="s">
         <v>422</v>
       </c>
@@ -9899,7 +9894,7 @@
       <c r="X20" s="468"/>
     </row>
     <row r="21" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="706"/>
+      <c r="I21" s="693"/>
       <c r="M21" s="216" t="s">
         <v>411</v>
       </c>
@@ -9929,7 +9924,7 @@
       <c r="G22" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="I22" s="706"/>
+      <c r="I22" s="693"/>
       <c r="P22" s="99" t="s">
         <v>590</v>
       </c>
@@ -9944,7 +9939,7 @@
       <c r="E23" s="283" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="706"/>
+      <c r="I23" s="693"/>
       <c r="Q23" s="24">
         <f>SUM(V23:V31)</f>
         <v>7</v>
@@ -9961,7 +9956,7 @@
       </c>
     </row>
     <row r="24" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="706"/>
+      <c r="I24" s="693"/>
       <c r="U24" s="35"/>
       <c r="V24" s="509">
         <v>1</v>
@@ -9989,7 +9984,7 @@
       <c r="H25" s="191" t="s">
         <v>266</v>
       </c>
-      <c r="I25" s="706"/>
+      <c r="I25" s="693"/>
       <c r="J25" s="397" t="s">
         <v>269</v>
       </c>
@@ -10034,7 +10029,7 @@
       <c r="H26" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="I26" s="706"/>
+      <c r="I26" s="693"/>
       <c r="K26" s="24">
         <v>15</v>
       </c>
@@ -10069,7 +10064,7 @@
       </c>
     </row>
     <row r="27" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="706"/>
+      <c r="I27" s="693"/>
       <c r="O27" s="2" t="s">
         <v>98</v>
       </c>
@@ -10096,7 +10091,7 @@
       <c r="E28" s="215">
         <v>2</v>
       </c>
-      <c r="I28" s="706"/>
+      <c r="I28" s="693"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="142"/>
@@ -10118,7 +10113,7 @@
       <c r="H29" s="191" t="s">
         <v>267</v>
       </c>
-      <c r="I29" s="707"/>
+      <c r="I29" s="694"/>
       <c r="J29" s="324"/>
       <c r="L29" s="96" t="s">
         <v>273</v>
@@ -10176,13 +10171,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I2:I29"/>
-    <mergeCell ref="AB1:AB11"/>
-    <mergeCell ref="AH11:AL11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="U11:X11"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="G5:G14"/>
     <mergeCell ref="A2:A3"/>
@@ -10194,6 +10182,13 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C2:C3"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I2:I29"/>
+    <mergeCell ref="AB1:AB11"/>
+    <mergeCell ref="AH11:AL11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="U11:X11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10204,8 +10199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AT37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" topLeftCell="T18" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10303,16 +10298,16 @@
       </c>
       <c r="S1" s="151">
         <f ca="1">TODAY()</f>
-        <v>45290</v>
-      </c>
-      <c r="T1" s="742"/>
+        <v>45291</v>
+      </c>
+      <c r="T1" s="735"/>
       <c r="U1" s="142"/>
       <c r="V1" s="6"/>
       <c r="W1" s="6"/>
-      <c r="X1" s="726" t="s">
+      <c r="X1" s="719" t="s">
         <v>441</v>
       </c>
-      <c r="Y1" s="727"/>
+      <c r="Y1" s="720"/>
       <c r="Z1" s="306">
         <f>68-(W8+Y3+X3+U3)</f>
         <v>0</v>
@@ -10328,27 +10323,27 @@
       <c r="AD1" s="302" t="s">
         <v>44</v>
       </c>
-      <c r="AE1" s="728" t="s">
+      <c r="AE1" s="721" t="s">
         <v>190</v>
       </c>
-      <c r="AF1" s="729"/>
-      <c r="AG1" s="730"/>
-      <c r="AH1" s="731" t="s">
+      <c r="AF1" s="722"/>
+      <c r="AG1" s="723"/>
+      <c r="AH1" s="724" t="s">
         <v>293</v>
       </c>
-      <c r="AI1" s="732"/>
-      <c r="AJ1" s="733"/>
-      <c r="AK1" s="659" t="s">
+      <c r="AI1" s="725"/>
+      <c r="AJ1" s="726"/>
+      <c r="AK1" s="613" t="s">
         <v>613</v>
       </c>
       <c r="AL1" s="550" t="s">
         <v>614</v>
       </c>
-      <c r="AM1" s="723" t="s">
+      <c r="AM1" s="716" t="s">
         <v>444</v>
       </c>
-      <c r="AN1" s="724"/>
-      <c r="AO1" s="725"/>
+      <c r="AN1" s="717"/>
+      <c r="AO1" s="718"/>
       <c r="AR1" s="142"/>
     </row>
     <row r="2" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10363,27 +10358,27 @@
         <f>K2+L2</f>
         <v>26</v>
       </c>
-      <c r="K2" s="721">
+      <c r="K2" s="743">
         <f>SUM(K4:K37)</f>
         <v>6</v>
       </c>
-      <c r="L2" s="719">
+      <c r="L2" s="741">
         <f>SUM(L4:L37)</f>
         <v>20</v>
       </c>
-      <c r="M2" s="734">
+      <c r="M2" s="727">
         <f>SUM(M5:M30)</f>
         <v>0</v>
       </c>
-      <c r="N2" s="736">
+      <c r="N2" s="729">
         <f>SUM(N4:N29)</f>
         <v>8</v>
       </c>
-      <c r="O2" s="738">
+      <c r="O2" s="731">
         <f>SUM(O4:O29)</f>
         <v>11</v>
       </c>
-      <c r="P2" s="666">
+      <c r="P2" s="637">
         <f>SUM(N30:N37)* (-1)</f>
         <v>-1</v>
       </c>
@@ -10396,14 +10391,14 @@
       <c r="S2" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="T2" s="743"/>
+      <c r="T2" s="736"/>
       <c r="U2" s="537" t="s">
         <v>262</v>
       </c>
       <c r="V2" s="482" t="s">
         <v>219</v>
       </c>
-      <c r="W2" s="740" t="s">
+      <c r="W2" s="733" t="s">
         <v>234</v>
       </c>
       <c r="X2" s="483" t="s">
@@ -10445,7 +10440,7 @@
       <c r="AJ2" s="150" t="s">
         <v>288</v>
       </c>
-      <c r="AK2" s="660"/>
+      <c r="AK2" s="614"/>
       <c r="AL2" s="591" t="s">
         <v>288</v>
       </c>
@@ -10473,12 +10468,12 @@
         <f>V3+X3+Y3+U3</f>
         <v>68</v>
       </c>
-      <c r="K3" s="722"/>
-      <c r="L3" s="720"/>
-      <c r="M3" s="735"/>
-      <c r="N3" s="737"/>
-      <c r="O3" s="739"/>
-      <c r="P3" s="667"/>
+      <c r="K3" s="744"/>
+      <c r="L3" s="742"/>
+      <c r="M3" s="728"/>
+      <c r="N3" s="730"/>
+      <c r="O3" s="732"/>
+      <c r="P3" s="638"/>
       <c r="Q3" s="172">
         <f>(M2+N2)-Y3</f>
         <v>0</v>
@@ -10486,7 +10481,7 @@
       <c r="S3" s="159" t="s">
         <v>244</v>
       </c>
-      <c r="T3" s="744"/>
+      <c r="T3" s="737"/>
       <c r="U3" s="538">
         <f>SUM(U4:U29)</f>
         <v>14</v>
@@ -10495,7 +10490,7 @@
         <f>SUM(V4:V29)</f>
         <v>37</v>
       </c>
-      <c r="W3" s="741"/>
+      <c r="W3" s="734"/>
       <c r="X3" s="485">
         <f t="shared" ref="X3:AC3" si="0">SUM(X4:X29)</f>
         <v>9</v>
@@ -10601,7 +10596,7 @@
         <f>AC4</f>
         <v>0</v>
       </c>
-      <c r="P4" s="716"/>
+      <c r="P4" s="738"/>
       <c r="Q4" s="20"/>
       <c r="R4" s="2" t="s">
         <v>334</v>
@@ -10685,7 +10680,7 @@
         <f>AC5</f>
         <v>0</v>
       </c>
-      <c r="P5" s="717"/>
+      <c r="P5" s="739"/>
       <c r="Q5" s="20"/>
       <c r="R5" s="2" t="s">
         <v>340</v>
@@ -10779,7 +10774,7 @@
         <f>AC6</f>
         <v>1</v>
       </c>
-      <c r="P6" s="717"/>
+      <c r="P6" s="739"/>
       <c r="Q6" s="54" t="s">
         <v>335</v>
       </c>
@@ -10884,7 +10879,7 @@
         <f>AC7</f>
         <v>1</v>
       </c>
-      <c r="P7" s="717"/>
+      <c r="P7" s="739"/>
       <c r="Q7" s="20"/>
       <c r="R7" s="2" t="s">
         <v>335</v>
@@ -11000,7 +10995,7 @@
         <f t="shared" ref="O8:O37" si="10">AC8</f>
         <v>0</v>
       </c>
-      <c r="P8" s="717"/>
+      <c r="P8" s="739"/>
       <c r="Q8" s="108" t="s">
         <v>233</v>
       </c>
@@ -11091,7 +11086,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P9" s="717"/>
+      <c r="P9" s="739"/>
       <c r="Q9" s="108" t="s">
         <v>335</v>
       </c>
@@ -11196,7 +11191,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P10" s="717"/>
+      <c r="P10" s="739"/>
       <c r="Q10" s="20"/>
       <c r="R10" s="2" t="s">
         <v>340</v>
@@ -11286,7 +11281,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P11" s="717"/>
+      <c r="P11" s="739"/>
       <c r="Q11" s="108" t="s">
         <v>335</v>
       </c>
@@ -11351,14 +11346,14 @@
       <c r="AR11" s="508"/>
     </row>
     <row r="12" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="626" t="s">
+      <c r="A12" s="675" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
         <v>13</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="E12" s="681" t="s">
+      <c r="E12" s="625" t="s">
         <v>56</v>
       </c>
       <c r="G12" s="262"/>
@@ -11383,7 +11378,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P12" s="717"/>
+      <c r="P12" s="739"/>
       <c r="Q12" s="108" t="s">
         <v>335</v>
       </c>
@@ -11460,14 +11455,14 @@
       </c>
     </row>
     <row r="13" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="628"/>
+      <c r="A13" s="677"/>
       <c r="B13" s="583">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="682"/>
+      <c r="E13" s="626"/>
       <c r="F13" s="172">
         <v>0</v>
       </c>
@@ -11491,7 +11486,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P13" s="717"/>
+      <c r="P13" s="739"/>
       <c r="Q13" s="108" t="s">
         <v>335</v>
       </c>
@@ -11573,7 +11568,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P14" s="717"/>
+      <c r="P14" s="739"/>
       <c r="Q14" s="20"/>
       <c r="R14" s="200" t="s">
         <v>339</v>
@@ -11676,7 +11671,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P15" s="717"/>
+      <c r="P15" s="739"/>
       <c r="Q15" s="20"/>
       <c r="R15" s="200" t="s">
         <v>339</v>
@@ -11770,7 +11765,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P16" s="717"/>
+      <c r="P16" s="739"/>
       <c r="Q16" s="108" t="s">
         <v>335</v>
       </c>
@@ -11871,7 +11866,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P17" s="717"/>
+      <c r="P17" s="739"/>
       <c r="Q17" s="20"/>
       <c r="R17" s="2" t="s">
         <v>341</v>
@@ -11971,7 +11966,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P18" s="717"/>
+      <c r="P18" s="739"/>
       <c r="Q18" s="108" t="s">
         <v>335</v>
       </c>
@@ -12061,7 +12056,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P19" s="717"/>
+      <c r="P19" s="739"/>
       <c r="Q19" s="20"/>
       <c r="R19" s="2" t="s">
         <v>334</v>
@@ -12169,11 +12164,11 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P20" s="718"/>
+      <c r="P20" s="740"/>
       <c r="Q20" s="605" t="s">
         <v>335</v>
       </c>
-      <c r="R20" s="683"/>
+      <c r="R20" s="627"/>
       <c r="S20" s="534" t="s">
         <v>85</v>
       </c>
@@ -12435,7 +12430,7 @@
     </row>
     <row r="23" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="24"/>
-      <c r="E23" s="633" t="s">
+      <c r="E23" s="682" t="s">
         <v>289</v>
       </c>
       <c r="F23" s="180"/>
@@ -12540,7 +12535,7 @@
       <c r="C24" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="E24" s="634"/>
+      <c r="E24" s="683"/>
       <c r="F24" s="172"/>
       <c r="H24" s="42"/>
       <c r="J24" s="570" t="s">
@@ -12566,7 +12561,7 @@
       <c r="Q24" s="605" t="s">
         <v>335</v>
       </c>
-      <c r="R24" s="683"/>
+      <c r="R24" s="627"/>
       <c r="S24" s="534" t="s">
         <v>249</v>
       </c>
@@ -13234,8 +13229,8 @@
       <c r="AR31" s="508"/>
     </row>
     <row r="32" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="650"/>
-      <c r="B32" s="650"/>
+      <c r="A32" s="630"/>
+      <c r="B32" s="630"/>
       <c r="J32" s="571"/>
       <c r="K32" s="586"/>
       <c r="L32" s="580">
@@ -13432,9 +13427,7 @@
       </c>
     </row>
     <row r="34" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="21">
-        <v>6</v>
-      </c>
+      <c r="B34" s="21"/>
       <c r="C34" s="2" t="s">
         <v>257</v>
       </c>
@@ -13715,7 +13708,7 @@
     </row>
     <row r="37" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="21">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D37" s="382">
         <v>1</v>
@@ -13816,11 +13809,20 @@
         <v>563</v>
       </c>
       <c r="AR37" s="540" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="P4:P20"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="Q20:R20"/>
     <mergeCell ref="AM1:AO1"/>
     <mergeCell ref="X1:Y1"/>
     <mergeCell ref="AE1:AG1"/>
@@ -13832,15 +13834,6 @@
     <mergeCell ref="W2:W3"/>
     <mergeCell ref="T1:T3"/>
     <mergeCell ref="AK1:AK2"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="P4:P20"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="Q20:R20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13903,12 +13896,12 @@
       <c r="P1" s="38"/>
       <c r="S1" s="58">
         <f ca="1">TODAY()</f>
-        <v>45290</v>
+        <v>45291</v>
       </c>
       <c r="V1" s="603" t="s">
         <v>70</v>
       </c>
-      <c r="W1" s="683"/>
+      <c r="W1" s="627"/>
       <c r="X1" s="62" t="s">
         <v>101</v>
       </c>
@@ -13927,7 +13920,7 @@
       <c r="AC1" s="116" t="s">
         <v>190</v>
       </c>
-      <c r="AD1" s="759" t="s">
+      <c r="AD1" s="752" t="s">
         <v>211</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -13944,10 +13937,10 @@
       <c r="E2" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="790" t="s">
+      <c r="F2" s="751" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="747" t="s">
+      <c r="G2" s="779" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -13975,10 +13968,10 @@
       <c r="U2" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="V2" s="726" t="s">
+      <c r="V2" s="719" t="s">
         <v>120</v>
       </c>
-      <c r="W2" s="727"/>
+      <c r="W2" s="720"/>
       <c r="X2" s="64" t="s">
         <v>109</v>
       </c>
@@ -13997,7 +13990,7 @@
       <c r="AC2" s="117" t="s">
         <v>98</v>
       </c>
-      <c r="AD2" s="760"/>
+      <c r="AD2" s="753"/>
       <c r="AE2" s="64" t="s">
         <v>98</v>
       </c>
@@ -14016,8 +14009,8 @@
       <c r="E3" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="F3" s="630"/>
-      <c r="G3" s="748"/>
+      <c r="F3" s="679"/>
+      <c r="G3" s="780"/>
       <c r="H3" s="40" t="s">
         <v>80</v>
       </c>
@@ -14028,13 +14021,13 @@
         <v>81</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="757" t="s">
+      <c r="O3" s="789" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="778" t="s">
+      <c r="P3" s="771" t="s">
         <v>217</v>
       </c>
-      <c r="Q3" s="779"/>
+      <c r="Q3" s="772"/>
       <c r="S3" s="57" t="s">
         <v>218</v>
       </c>
@@ -14044,15 +14037,15 @@
       <c r="W3" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="AD3" s="760"/>
+      <c r="AD3" s="753"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="748"/>
+      <c r="G4" s="780"/>
       <c r="H4" s="6"/>
       <c r="L4" s="687" t="s">
         <v>82</v>
       </c>
-      <c r="O4" s="758"/>
+      <c r="O4" s="790"/>
       <c r="T4" s="55" t="s">
         <v>97</v>
       </c>
@@ -14066,8 +14059,8 @@
         <v>194</v>
       </c>
       <c r="Z4" s="605"/>
-      <c r="AA4" s="683"/>
-      <c r="AD4" s="760"/>
+      <c r="AA4" s="627"/>
+      <c r="AD4" s="753"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -14082,21 +14075,21 @@
       <c r="F5" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="G5" s="748"/>
+      <c r="G5" s="780"/>
       <c r="H5" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="K5" s="765" t="s">
+      <c r="K5" s="758" t="s">
         <v>215</v>
       </c>
-      <c r="L5" s="780"/>
+      <c r="L5" s="773"/>
       <c r="M5" s="2" t="s">
         <v>213</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>212</v>
       </c>
-      <c r="O5" s="758"/>
+      <c r="O5" s="790"/>
       <c r="P5" s="108" t="s">
         <v>214</v>
       </c>
@@ -14112,11 +14105,11 @@
       <c r="U5" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="Y5" s="768" t="s">
+      <c r="Y5" s="761" t="s">
         <v>282</v>
       </c>
-      <c r="Z5" s="769"/>
-      <c r="AD5" s="760"/>
+      <c r="Z5" s="762"/>
+      <c r="AD5" s="753"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -14126,16 +14119,16 @@
       <c r="E6" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="G6" s="748"/>
+      <c r="G6" s="780"/>
       <c r="H6" s="46" t="s">
         <v>80</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="766"/>
-      <c r="L6" s="780"/>
-      <c r="O6" s="758"/>
+      <c r="K6" s="759"/>
+      <c r="L6" s="773"/>
+      <c r="O6" s="790"/>
       <c r="T6" s="2" t="s">
         <v>100</v>
       </c>
@@ -14145,23 +14138,23 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="760"/>
+      <c r="AD6" s="753"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="748"/>
+      <c r="G7" s="780"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="766"/>
-      <c r="L7" s="780"/>
+      <c r="K7" s="759"/>
+      <c r="L7" s="773"/>
       <c r="N7" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="O7" s="758"/>
+      <c r="O7" s="790"/>
       <c r="P7" s="73"/>
       <c r="U7" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="760"/>
+      <c r="AD7" s="753"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -14174,7 +14167,7 @@
       <c r="F8" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="G8" s="748"/>
+      <c r="G8" s="780"/>
       <c r="H8" s="50" t="s">
         <v>75</v>
       </c>
@@ -14184,41 +14177,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="766"/>
-      <c r="L8" s="780"/>
-      <c r="O8" s="758"/>
+      <c r="K8" s="759"/>
+      <c r="L8" s="773"/>
+      <c r="O8" s="790"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="762" t="s">
+      <c r="S8" s="755" t="s">
         <v>210</v>
       </c>
-      <c r="T8" s="763"/>
-      <c r="U8" s="763"/>
-      <c r="V8" s="763"/>
-      <c r="W8" s="763"/>
-      <c r="X8" s="763"/>
-      <c r="Y8" s="763"/>
-      <c r="Z8" s="763"/>
-      <c r="AA8" s="763"/>
-      <c r="AB8" s="763"/>
-      <c r="AC8" s="764"/>
-      <c r="AD8" s="760"/>
+      <c r="T8" s="756"/>
+      <c r="U8" s="756"/>
+      <c r="V8" s="756"/>
+      <c r="W8" s="756"/>
+      <c r="X8" s="756"/>
+      <c r="Y8" s="756"/>
+      <c r="Z8" s="756"/>
+      <c r="AA8" s="756"/>
+      <c r="AB8" s="756"/>
+      <c r="AC8" s="757"/>
+      <c r="AD8" s="753"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="784"/>
-      <c r="G9" s="748"/>
+      <c r="C9" s="745"/>
+      <c r="G9" s="780"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="766"/>
-      <c r="L9" s="751" t="s">
+      <c r="K9" s="759"/>
+      <c r="L9" s="783" t="s">
         <v>216</v>
       </c>
-      <c r="M9" s="752"/>
-      <c r="N9" s="753"/>
-      <c r="O9" s="758"/>
+      <c r="M9" s="784"/>
+      <c r="N9" s="785"/>
+      <c r="O9" s="790"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="760"/>
+      <c r="AD9" s="753"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="785"/>
+      <c r="C10" s="746"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>87</v>
@@ -14226,7 +14219,7 @@
       <c r="F10" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="G10" s="748"/>
+      <c r="G10" s="780"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>80</v>
@@ -14234,33 +14227,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="766"/>
-      <c r="M10" s="787" t="s">
+      <c r="K10" s="759"/>
+      <c r="M10" s="748" t="s">
         <v>89</v>
       </c>
-      <c r="N10" s="788"/>
-      <c r="O10" s="788"/>
-      <c r="P10" s="788"/>
-      <c r="Q10" s="788"/>
-      <c r="R10" s="788"/>
-      <c r="S10" s="788"/>
-      <c r="T10" s="788"/>
-      <c r="U10" s="788"/>
-      <c r="V10" s="788"/>
-      <c r="W10" s="788"/>
-      <c r="X10" s="788"/>
-      <c r="Y10" s="788"/>
-      <c r="Z10" s="788"/>
-      <c r="AA10" s="788"/>
-      <c r="AB10" s="788"/>
-      <c r="AC10" s="789"/>
-      <c r="AD10" s="760"/>
+      <c r="N10" s="749"/>
+      <c r="O10" s="749"/>
+      <c r="P10" s="749"/>
+      <c r="Q10" s="749"/>
+      <c r="R10" s="749"/>
+      <c r="S10" s="749"/>
+      <c r="T10" s="749"/>
+      <c r="U10" s="749"/>
+      <c r="V10" s="749"/>
+      <c r="W10" s="749"/>
+      <c r="X10" s="749"/>
+      <c r="Y10" s="749"/>
+      <c r="Z10" s="749"/>
+      <c r="AA10" s="749"/>
+      <c r="AB10" s="749"/>
+      <c r="AC10" s="750"/>
+      <c r="AD10" s="753"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="786"/>
-      <c r="G11" s="748"/>
+      <c r="C11" s="747"/>
+      <c r="G11" s="780"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="766"/>
+      <c r="K11" s="759"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -14268,17 +14261,17 @@
       <c r="Y11" s="68" t="s">
         <v>120</v>
       </c>
-      <c r="Z11" s="776" t="s">
+      <c r="Z11" s="769" t="s">
         <v>120</v>
       </c>
-      <c r="AA11" s="777"/>
+      <c r="AA11" s="770"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>120</v>
       </c>
-      <c r="AD11" s="760"/>
+      <c r="AD11" s="753"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -14291,7 +14284,7 @@
       <c r="F12" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="G12" s="748"/>
+      <c r="G12" s="780"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>80</v>
@@ -14299,8 +14292,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="766"/>
-      <c r="L12" s="781" t="s">
+      <c r="K12" s="759"/>
+      <c r="L12" s="774" t="s">
         <v>92</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -14331,25 +14324,25 @@
         <v>115</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="770" t="s">
+      <c r="AA12" s="763" t="s">
         <v>125</v>
       </c>
-      <c r="AB12" s="771"/>
+      <c r="AB12" s="764"/>
       <c r="AC12" s="21" t="s">
         <v>230</v>
       </c>
-      <c r="AD12" s="760"/>
+      <c r="AD12" s="753"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="784"/>
-      <c r="G13" s="748"/>
-      <c r="K13" s="766"/>
-      <c r="L13" s="782"/>
+      <c r="C13" s="745"/>
+      <c r="G13" s="780"/>
+      <c r="K13" s="759"/>
+      <c r="L13" s="775"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="750" t="s">
+      <c r="Q13" s="782" t="s">
         <v>208</v>
       </c>
-      <c r="R13" s="639"/>
+      <c r="R13" s="644"/>
       <c r="S13" s="599"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
@@ -14358,17 +14351,17 @@
       <c r="X13" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="AA13" s="772"/>
-      <c r="AB13" s="773"/>
-      <c r="AD13" s="760"/>
+      <c r="AA13" s="765"/>
+      <c r="AB13" s="766"/>
+      <c r="AD13" s="753"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="C14" s="786"/>
+      <c r="C14" s="747"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="748"/>
+      <c r="G14" s="780"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -14376,8 +14369,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="766"/>
-      <c r="L14" s="782"/>
+      <c r="K14" s="759"/>
+      <c r="L14" s="775"/>
       <c r="M14" s="21" t="s">
         <v>110</v>
       </c>
@@ -14398,9 +14391,9 @@
       <c r="Y14" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="AA14" s="772"/>
-      <c r="AB14" s="773"/>
-      <c r="AD14" s="760"/>
+      <c r="AA14" s="765"/>
+      <c r="AB14" s="766"/>
+      <c r="AD14" s="753"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -14415,19 +14408,19 @@
       <c r="F15" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="G15" s="748"/>
+      <c r="G15" s="780"/>
       <c r="H15" s="2" t="s">
         <v>80</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="K15" s="766"/>
-      <c r="L15" s="783"/>
-      <c r="Q15" s="750" t="s">
+      <c r="K15" s="759"/>
+      <c r="L15" s="776"/>
+      <c r="Q15" s="782" t="s">
         <v>209</v>
       </c>
-      <c r="R15" s="639"/>
+      <c r="R15" s="644"/>
       <c r="S15" s="599"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
@@ -14436,14 +14429,14 @@
       <c r="X15" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="AA15" s="772"/>
-      <c r="AB15" s="773"/>
-      <c r="AD15" s="760"/>
+      <c r="AA15" s="765"/>
+      <c r="AB15" s="766"/>
+      <c r="AD15" s="753"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="748"/>
-      <c r="K16" s="766"/>
+      <c r="G16" s="780"/>
+      <c r="K16" s="759"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>108</v>
@@ -14462,24 +14455,24 @@
       <c r="Z16" s="76" t="s">
         <v>126</v>
       </c>
-      <c r="AA16" s="772"/>
-      <c r="AB16" s="773"/>
-      <c r="AD16" s="760"/>
+      <c r="AA16" s="765"/>
+      <c r="AB16" s="766"/>
+      <c r="AD16" s="753"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F17" s="745" t="s">
+      <c r="F17" s="777" t="s">
         <v>95</v>
       </c>
-      <c r="G17" s="748"/>
+      <c r="G17" s="780"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>80</v>
       </c>
-      <c r="K17" s="766"/>
+      <c r="K17" s="759"/>
       <c r="S17" s="599"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
@@ -14487,9 +14480,9 @@
       <c r="X17" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA17" s="772"/>
-      <c r="AB17" s="773"/>
-      <c r="AD17" s="760"/>
+      <c r="AA17" s="765"/>
+      <c r="AB17" s="766"/>
+      <c r="AD17" s="753"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -14499,15 +14492,15 @@
       <c r="E18" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F18" s="746"/>
-      <c r="G18" s="748"/>
+      <c r="F18" s="778"/>
+      <c r="G18" s="780"/>
       <c r="H18" s="108" t="s">
         <v>75</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="K18" s="766"/>
+      <c r="K18" s="759"/>
       <c r="O18" s="64" t="s">
         <v>114</v>
       </c>
@@ -14518,39 +14511,42 @@
       <c r="X18" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AA18" s="774"/>
-      <c r="AB18" s="775"/>
-      <c r="AD18" s="760"/>
+      <c r="AA18" s="767"/>
+      <c r="AB18" s="768"/>
+      <c r="AD18" s="753"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>207</v>
       </c>
-      <c r="G19" s="749"/>
-      <c r="K19" s="767"/>
+      <c r="G19" s="781"/>
+      <c r="K19" s="760"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="754" t="s">
+      <c r="R19" s="786" t="s">
         <v>123</v>
       </c>
-      <c r="S19" s="755"/>
-      <c r="T19" s="756"/>
+      <c r="S19" s="787"/>
+      <c r="T19" s="788"/>
       <c r="V19" s="77" t="s">
         <v>114</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="AD19" s="761"/>
+      <c r="AD19" s="754"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="M10:AC10"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="S12:S18"/>
+    <mergeCell ref="O3:O9"/>
     <mergeCell ref="AD1:AD19"/>
     <mergeCell ref="S8:AC8"/>
     <mergeCell ref="K5:K19"/>
@@ -14562,14 +14558,11 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L12:L15"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G19"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="S12:S18"/>
-    <mergeCell ref="O3:O9"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="M10:AC10"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rw Usage Updates S.1.0.0.5 _3:00PM
Boat Enabled -
InCapacity - [0] , NodeW - [-3] , BirdW - [6] , FuelW - [20] , OnHost - [8+1]
VillageW=[5]
Rw - Local(Left Running With Cost ) - [For Business/Shop/Market only] -
</commit_message>
<xml_diff>
--- a/System_2.2.1.xlsx
+++ b/System_2.2.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4B3DBD-6C41-4908-BAC9-276AA5D93695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CB210D-0CCB-4866-957F-AC8ED217F24F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5027,6 +5027,186 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5039,12 +5219,6 @@
     <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5056,12 +5230,6 @@
     </xf>
     <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
@@ -5084,190 +5252,61 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5309,43 +5348,25 @@
     <xf numFmtId="0" fontId="39" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5414,46 +5435,46 @@
     <xf numFmtId="14" fontId="5" fillId="14" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5531,46 +5552,25 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -6903,7 +6903,7 @@
       <c r="H1" s="97" t="s">
         <v>343</v>
       </c>
-      <c r="I1" s="613" t="s">
+      <c r="I1" s="659" t="s">
         <v>369</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -6939,7 +6939,7 @@
       <c r="X1" s="430" t="s">
         <v>155</v>
       </c>
-      <c r="Y1" s="657" t="s">
+      <c r="Y1" s="653" t="s">
         <v>528</v>
       </c>
       <c r="Z1" s="406">
@@ -6964,7 +6964,7 @@
         <v>498</v>
       </c>
       <c r="AM1" s="402"/>
-      <c r="AN1" s="640"/>
+      <c r="AN1" s="635"/>
       <c r="AO1" s="338" t="s">
         <v>469</v>
       </c>
@@ -6973,23 +6973,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="666">
+      <c r="A2" s="617">
         <f ca="1">TODAY()</f>
         <v>45291</v>
       </c>
-      <c r="B2" s="668" t="s">
+      <c r="B2" s="619" t="s">
         <v>370</v>
       </c>
-      <c r="C2" s="645" t="s">
+      <c r="C2" s="615" t="s">
         <v>357</v>
       </c>
-      <c r="D2" s="670" t="s">
+      <c r="D2" s="621" t="s">
         <v>355</v>
       </c>
-      <c r="E2" s="609" t="s">
+      <c r="E2" s="669" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="619" t="s">
+      <c r="F2" s="640" t="s">
         <v>102</v>
       </c>
       <c r="G2" s="393" t="s">
@@ -6998,31 +6998,31 @@
       <c r="H2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="614"/>
+      <c r="I2" s="660"/>
       <c r="J2" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="611" t="s">
+      <c r="K2" s="671" t="s">
         <v>342</v>
       </c>
-      <c r="L2" s="612"/>
-      <c r="M2" s="619" t="s">
+      <c r="L2" s="672"/>
+      <c r="M2" s="640" t="s">
         <v>102</v>
       </c>
       <c r="N2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="649" t="s">
+      <c r="O2" s="644" t="s">
         <v>102</v>
       </c>
       <c r="P2" s="85" t="s">
         <v>147</v>
       </c>
-      <c r="Q2" s="645" t="s">
+      <c r="Q2" s="615" t="s">
         <v>143</v>
       </c>
       <c r="R2" s="598"/>
-      <c r="S2" s="634" t="s">
+      <c r="S2" s="657" t="s">
         <v>148</v>
       </c>
       <c r="T2" s="89"/>
@@ -7032,7 +7032,7 @@
       <c r="X2" s="431" t="s">
         <v>156</v>
       </c>
-      <c r="Y2" s="658"/>
+      <c r="Y2" s="654"/>
       <c r="Z2" s="407">
         <v>1</v>
       </c>
@@ -7055,15 +7055,15 @@
         <v>463</v>
       </c>
       <c r="AM2" s="428"/>
-      <c r="AN2" s="641"/>
+      <c r="AN2" s="636"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="667"/>
-      <c r="B3" s="669"/>
-      <c r="C3" s="646"/>
-      <c r="D3" s="671"/>
-      <c r="E3" s="610"/>
-      <c r="F3" s="620"/>
+      <c r="A3" s="618"/>
+      <c r="B3" s="620"/>
+      <c r="C3" s="616"/>
+      <c r="D3" s="622"/>
+      <c r="E3" s="670"/>
+      <c r="F3" s="641"/>
       <c r="G3" s="394" t="s">
         <v>28</v>
       </c>
@@ -7082,17 +7082,17 @@
       <c r="L3" s="201" t="s">
         <v>107</v>
       </c>
-      <c r="M3" s="620"/>
+      <c r="M3" s="641"/>
       <c r="N3" s="69" t="s">
         <v>146</v>
       </c>
-      <c r="O3" s="650"/>
+      <c r="O3" s="645"/>
       <c r="P3" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="Q3" s="646"/>
+      <c r="Q3" s="616"/>
       <c r="R3" s="600"/>
-      <c r="S3" s="636"/>
+      <c r="S3" s="658"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -7100,7 +7100,7 @@
       <c r="X3" s="431" t="s">
         <v>157</v>
       </c>
-      <c r="Y3" s="658"/>
+      <c r="Y3" s="654"/>
       <c r="Z3" s="408">
         <v>1</v>
       </c>
@@ -7109,7 +7109,7 @@
       <c r="AC3" s="100" t="s">
         <v>480</v>
       </c>
-      <c r="AD3" s="631" t="s">
+      <c r="AD3" s="656" t="s">
         <v>455</v>
       </c>
       <c r="AE3" s="257"/>
@@ -7121,16 +7121,16 @@
       <c r="AK3" s="257"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="428"/>
-      <c r="AN3" s="641"/>
+      <c r="AN3" s="636"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="238" t="s">
         <v>183</v>
       </c>
-      <c r="B4" s="682" t="s">
+      <c r="B4" s="633" t="s">
         <v>373</v>
       </c>
-      <c r="C4" s="645" t="s">
+      <c r="C4" s="615" t="s">
         <v>154</v>
       </c>
       <c r="D4" s="347" t="s">
@@ -7139,7 +7139,7 @@
       <c r="E4" s="378">
         <v>2</v>
       </c>
-      <c r="F4" s="620"/>
+      <c r="F4" s="641"/>
       <c r="G4" s="381" t="s">
         <v>201</v>
       </c>
@@ -7156,11 +7156,11 @@
         <v>150</v>
       </c>
       <c r="L4" s="204"/>
-      <c r="M4" s="620"/>
+      <c r="M4" s="641"/>
       <c r="N4" s="174" t="s">
         <v>69</v>
       </c>
-      <c r="O4" s="650"/>
+      <c r="O4" s="645"/>
       <c r="P4" s="2" t="s">
         <v>191</v>
       </c>
@@ -7182,12 +7182,12 @@
       <c r="X4" s="431" t="s">
         <v>158</v>
       </c>
-      <c r="Y4" s="658"/>
+      <c r="Y4" s="654"/>
       <c r="Z4" s="409"/>
       <c r="AA4" s="307"/>
       <c r="AB4" s="209"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="631"/>
+      <c r="AD4" s="656"/>
       <c r="AE4" s="257"/>
       <c r="AF4" s="257"/>
       <c r="AG4" s="16"/>
@@ -7197,37 +7197,37 @@
       <c r="AK4" s="257"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="428"/>
-      <c r="AN4" s="641"/>
+      <c r="AN4" s="636"/>
       <c r="AO4" s="338" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="613" t="s">
+      <c r="A5" s="659" t="s">
         <v>418</v>
       </c>
-      <c r="B5" s="683"/>
-      <c r="C5" s="646"/>
+      <c r="B5" s="634"/>
+      <c r="C5" s="616"/>
       <c r="D5" s="61" t="s">
         <v>153</v>
       </c>
       <c r="E5" s="379">
         <v>1</v>
       </c>
-      <c r="F5" s="620"/>
-      <c r="G5" s="674" t="s">
+      <c r="F5" s="641"/>
+      <c r="G5" s="625" t="s">
         <v>192</v>
       </c>
-      <c r="H5" s="674"/>
-      <c r="I5" s="674"/>
-      <c r="J5" s="674"/>
-      <c r="K5" s="674"/>
-      <c r="L5" s="675"/>
-      <c r="M5" s="620"/>
+      <c r="H5" s="625"/>
+      <c r="I5" s="625"/>
+      <c r="J5" s="625"/>
+      <c r="K5" s="625"/>
+      <c r="L5" s="626"/>
+      <c r="M5" s="641"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
-      <c r="O5" s="650"/>
+      <c r="O5" s="645"/>
       <c r="T5" s="89"/>
       <c r="U5" s="124"/>
       <c r="V5" s="120"/>
@@ -7235,7 +7235,7 @@
       <c r="X5" s="431" t="s">
         <v>159</v>
       </c>
-      <c r="Y5" s="658"/>
+      <c r="Y5" s="654"/>
       <c r="Z5" s="409">
         <v>1</v>
       </c>
@@ -7258,24 +7258,24 @@
       <c r="AK5" s="257"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="428"/>
-      <c r="AN5" s="641"/>
+      <c r="AN5" s="636"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="614"/>
-      <c r="B6" s="680" t="s">
+      <c r="A6" s="660"/>
+      <c r="B6" s="631" t="s">
         <v>177</v>
       </c>
-      <c r="C6" s="628"/>
-      <c r="D6" s="629"/>
-      <c r="F6" s="620"/>
-      <c r="G6" s="676"/>
-      <c r="H6" s="676"/>
-      <c r="I6" s="676"/>
-      <c r="J6" s="676"/>
-      <c r="K6" s="676"/>
-      <c r="L6" s="677"/>
-      <c r="M6" s="620"/>
-      <c r="O6" s="650"/>
+      <c r="C6" s="661"/>
+      <c r="D6" s="662"/>
+      <c r="F6" s="641"/>
+      <c r="G6" s="627"/>
+      <c r="H6" s="627"/>
+      <c r="I6" s="627"/>
+      <c r="J6" s="627"/>
+      <c r="K6" s="627"/>
+      <c r="L6" s="628"/>
+      <c r="M6" s="641"/>
+      <c r="O6" s="645"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
       <c r="V6" s="98" t="s">
@@ -7285,7 +7285,7 @@
       <c r="X6" s="431" t="s">
         <v>160</v>
       </c>
-      <c r="Y6" s="658"/>
+      <c r="Y6" s="654"/>
       <c r="Z6" s="407">
         <v>1</v>
       </c>
@@ -7299,16 +7299,16 @@
       <c r="AF6" s="257"/>
       <c r="AG6" s="257"/>
       <c r="AH6" s="257"/>
-      <c r="AI6" s="630"/>
+      <c r="AI6" s="650"/>
       <c r="AJ6" s="441" t="s">
         <v>458</v>
       </c>
-      <c r="AK6" s="630" t="s">
+      <c r="AK6" s="650" t="s">
         <v>251</v>
       </c>
       <c r="AL6" s="257"/>
       <c r="AM6" s="428"/>
-      <c r="AN6" s="641"/>
+      <c r="AN6" s="636"/>
       <c r="AO6" s="338" t="s">
         <v>470</v>
       </c>
@@ -7317,7 +7317,7 @@
       <c r="A7" s="232" t="s">
         <v>571</v>
       </c>
-      <c r="B7" s="681"/>
+      <c r="B7" s="632"/>
       <c r="C7" s="202" t="s">
         <v>374</v>
       </c>
@@ -7327,7 +7327,7 @@
       <c r="E7" s="265">
         <v>3</v>
       </c>
-      <c r="F7" s="620"/>
+      <c r="F7" s="641"/>
       <c r="G7" s="395">
         <v>0</v>
       </c>
@@ -7346,8 +7346,8 @@
       <c r="L7" s="212">
         <v>0</v>
       </c>
-      <c r="M7" s="620"/>
-      <c r="O7" s="650"/>
+      <c r="M7" s="641"/>
+      <c r="O7" s="645"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
       </c>
@@ -7361,7 +7361,7 @@
       <c r="X7" s="431" t="s">
         <v>161</v>
       </c>
-      <c r="Y7" s="658"/>
+      <c r="Y7" s="654"/>
       <c r="Z7" s="407">
         <v>1</v>
       </c>
@@ -7371,18 +7371,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="257"/>
       <c r="AF7" s="257"/>
-      <c r="AG7" s="631" t="s">
+      <c r="AG7" s="656" t="s">
         <v>454</v>
       </c>
       <c r="AH7" s="257"/>
-      <c r="AI7" s="630"/>
+      <c r="AI7" s="650"/>
       <c r="AJ7" s="257"/>
-      <c r="AK7" s="630"/>
+      <c r="AK7" s="650"/>
       <c r="AL7" s="80" t="s">
         <v>496</v>
       </c>
       <c r="AM7" s="428"/>
-      <c r="AN7" s="641"/>
+      <c r="AN7" s="636"/>
       <c r="AP7" s="76" t="s">
         <v>471</v>
       </c>
@@ -7399,27 +7399,27 @@
         <f>SUM(G7:N9)</f>
         <v>15</v>
       </c>
-      <c r="F8" s="620"/>
-      <c r="G8" s="675">
-        <v>0</v>
-      </c>
-      <c r="H8" s="672" t="s">
+      <c r="F8" s="641"/>
+      <c r="G8" s="626">
+        <v>0</v>
+      </c>
+      <c r="H8" s="623" t="s">
         <v>104</v>
       </c>
       <c r="I8" s="598">
         <v>0</v>
       </c>
-      <c r="J8" s="672" t="s">
+      <c r="J8" s="623" t="s">
         <v>104</v>
       </c>
-      <c r="K8" s="678"/>
-      <c r="L8" s="632"/>
-      <c r="M8" s="647"/>
-      <c r="N8" s="637">
+      <c r="K8" s="629"/>
+      <c r="L8" s="663"/>
+      <c r="M8" s="642"/>
+      <c r="N8" s="666">
         <f>N5+N11</f>
         <v>15</v>
       </c>
-      <c r="O8" s="650"/>
+      <c r="O8" s="645"/>
       <c r="T8" s="103" t="s">
         <v>44</v>
       </c>
@@ -7429,7 +7429,7 @@
       <c r="X8" s="431" t="s">
         <v>162</v>
       </c>
-      <c r="Y8" s="658"/>
+      <c r="Y8" s="654"/>
       <c r="Z8" s="409"/>
       <c r="AA8" s="307"/>
       <c r="AB8" s="209"/>
@@ -7437,14 +7437,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="257"/>
       <c r="AF8" s="257"/>
-      <c r="AG8" s="631"/>
+      <c r="AG8" s="656"/>
       <c r="AH8" s="257"/>
-      <c r="AI8" s="630"/>
+      <c r="AI8" s="650"/>
       <c r="AJ8" s="257"/>
       <c r="AK8" s="257"/>
       <c r="AL8" s="257"/>
       <c r="AM8" s="428"/>
-      <c r="AN8" s="641"/>
+      <c r="AN8" s="636"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="232" t="s">
@@ -7459,17 +7459,17 @@
       <c r="D9" s="348" t="s">
         <v>281</v>
       </c>
-      <c r="F9" s="620"/>
-      <c r="G9" s="677"/>
-      <c r="H9" s="673"/>
+      <c r="F9" s="641"/>
+      <c r="G9" s="628"/>
+      <c r="H9" s="624"/>
       <c r="I9" s="600"/>
-      <c r="J9" s="673"/>
-      <c r="K9" s="679"/>
-      <c r="L9" s="633"/>
-      <c r="M9" s="648"/>
-      <c r="N9" s="638"/>
-      <c r="O9" s="651"/>
-      <c r="S9" s="634" t="s">
+      <c r="J9" s="624"/>
+      <c r="K9" s="630"/>
+      <c r="L9" s="664"/>
+      <c r="M9" s="643"/>
+      <c r="N9" s="667"/>
+      <c r="O9" s="646"/>
+      <c r="S9" s="657" t="s">
         <v>61</v>
       </c>
       <c r="T9" s="89"/>
@@ -7481,7 +7481,7 @@
       <c r="X9" s="431" t="s">
         <v>163</v>
       </c>
-      <c r="Y9" s="658"/>
+      <c r="Y9" s="654"/>
       <c r="Z9" s="410"/>
       <c r="AA9" s="307"/>
       <c r="AB9" s="209"/>
@@ -7491,16 +7491,16 @@
       </c>
       <c r="AE9" s="257"/>
       <c r="AF9" s="257"/>
-      <c r="AG9" s="631"/>
+      <c r="AG9" s="656"/>
       <c r="AH9" s="257"/>
-      <c r="AI9" s="630"/>
+      <c r="AI9" s="650"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="630" t="s">
+      <c r="AK9" s="650" t="s">
         <v>251</v>
       </c>
       <c r="AL9" s="257"/>
       <c r="AM9" s="428"/>
-      <c r="AN9" s="641"/>
+      <c r="AN9" s="636"/>
       <c r="AP9" s="2" t="s">
         <v>508</v>
       </c>
@@ -7517,20 +7517,20 @@
         <f>Boat!W8</f>
         <v>37</v>
       </c>
-      <c r="F10" s="620"/>
+      <c r="F10" s="641"/>
       <c r="N10" s="418" t="s">
         <v>396</v>
       </c>
-      <c r="O10" s="622" t="s">
+      <c r="O10" s="678" t="s">
         <v>102</v>
       </c>
-      <c r="P10" s="652" t="s">
+      <c r="P10" s="647" t="s">
         <v>400</v>
       </c>
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="635"/>
+      <c r="S10" s="665"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>176</v>
@@ -7542,7 +7542,7 @@
       <c r="X10" s="431" t="s">
         <v>164</v>
       </c>
-      <c r="Y10" s="658"/>
+      <c r="Y10" s="654"/>
       <c r="Z10" s="409">
         <v>0</v>
       </c>
@@ -7560,16 +7560,16 @@
       <c r="AF10" s="238" t="s">
         <v>311</v>
       </c>
-      <c r="AG10" s="631"/>
+      <c r="AG10" s="656"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="630"/>
+      <c r="AI10" s="650"/>
       <c r="AJ10" s="257"/>
-      <c r="AK10" s="630"/>
+      <c r="AK10" s="650"/>
       <c r="AL10" s="257"/>
       <c r="AM10" s="442" t="s">
         <v>318</v>
       </c>
-      <c r="AN10" s="641"/>
+      <c r="AN10" s="636"/>
       <c r="AO10" s="204" t="s">
         <v>94</v>
       </c>
@@ -7587,18 +7587,18 @@
       <c r="D11" s="170" t="s">
         <v>355</v>
       </c>
-      <c r="F11" s="620"/>
+      <c r="F11" s="641"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="623"/>
-      <c r="P11" s="653"/>
+      <c r="O11" s="679"/>
+      <c r="P11" s="648"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>220</v>
       </c>
-      <c r="S11" s="635"/>
+      <c r="S11" s="665"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -7608,7 +7608,7 @@
       <c r="X11" s="431" t="s">
         <v>165</v>
       </c>
-      <c r="Y11" s="658"/>
+      <c r="Y11" s="654"/>
       <c r="Z11" s="409"/>
       <c r="AA11" s="307">
         <v>1</v>
@@ -7622,14 +7622,14 @@
       <c r="AF11" s="257" t="s">
         <v>476</v>
       </c>
-      <c r="AG11" s="631"/>
+      <c r="AG11" s="656"/>
       <c r="AH11" s="257"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="257"/>
       <c r="AK11" s="257"/>
       <c r="AL11" s="257"/>
       <c r="AM11" s="428"/>
-      <c r="AN11" s="641"/>
+      <c r="AN11" s="636"/>
       <c r="AP11" s="76" t="s">
         <v>484</v>
       </c>
@@ -7648,7 +7648,7 @@
       <c r="E12" s="224">
         <v>3</v>
       </c>
-      <c r="F12" s="620"/>
+      <c r="F12" s="641"/>
       <c r="G12" s="337" t="s">
         <v>400</v>
       </c>
@@ -7657,16 +7657,16 @@
       </c>
       <c r="I12" s="605"/>
       <c r="J12" s="605"/>
-      <c r="K12" s="627"/>
+      <c r="K12" s="683"/>
       <c r="L12" s="203"/>
       <c r="M12" s="203"/>
       <c r="N12" s="203"/>
-      <c r="O12" s="623"/>
-      <c r="P12" s="653"/>
+      <c r="O12" s="679"/>
+      <c r="P12" s="648"/>
       <c r="R12" s="122" t="s">
         <v>180</v>
       </c>
-      <c r="S12" s="636"/>
+      <c r="S12" s="658"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -7676,7 +7676,7 @@
       <c r="X12" s="431" t="s">
         <v>166</v>
       </c>
-      <c r="Y12" s="658"/>
+      <c r="Y12" s="654"/>
       <c r="Z12" s="407">
         <v>1</v>
       </c>
@@ -7687,16 +7687,16 @@
       <c r="AC12" s="100" t="s">
         <v>481</v>
       </c>
-      <c r="AD12" s="639" t="s">
+      <c r="AD12" s="668" t="s">
         <v>240</v>
       </c>
       <c r="AE12" s="441" t="s">
         <v>239</v>
       </c>
-      <c r="AF12" s="631" t="s">
+      <c r="AF12" s="656" t="s">
         <v>228</v>
       </c>
-      <c r="AG12" s="631"/>
+      <c r="AG12" s="656"/>
       <c r="AH12" s="238" t="s">
         <v>259</v>
       </c>
@@ -7706,10 +7706,10 @@
       <c r="AJ12" s="257"/>
       <c r="AK12" s="257"/>
       <c r="AL12" s="257"/>
-      <c r="AM12" s="655" t="s">
+      <c r="AM12" s="651" t="s">
         <v>249</v>
       </c>
-      <c r="AN12" s="641"/>
+      <c r="AN12" s="636"/>
       <c r="AO12" s="338" t="s">
         <v>96</v>
       </c>
@@ -7721,17 +7721,17 @@
       <c r="E13" s="448">
         <v>-3</v>
       </c>
-      <c r="F13" s="620"/>
+      <c r="F13" s="641"/>
       <c r="G13" s="605" t="s">
         <v>430</v>
       </c>
       <c r="H13" s="605"/>
       <c r="I13" s="605"/>
-      <c r="J13" s="627"/>
+      <c r="J13" s="683"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="623"/>
-      <c r="P13" s="654"/>
+      <c r="O13" s="679"/>
+      <c r="P13" s="649"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
       </c>
@@ -7741,7 +7741,7 @@
       <c r="X13" s="431" t="s">
         <v>167</v>
       </c>
-      <c r="Y13" s="658"/>
+      <c r="Y13" s="654"/>
       <c r="Z13" s="407">
         <v>1</v>
       </c>
@@ -7752,8 +7752,8 @@
         <v>500</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="639"/>
-      <c r="AF13" s="631"/>
+      <c r="AD13" s="668"/>
+      <c r="AF13" s="656"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="238" t="s">
         <v>308</v>
@@ -7764,8 +7764,8 @@
       <c r="AJ13" s="80"/>
       <c r="AK13" s="257"/>
       <c r="AL13" s="257"/>
-      <c r="AM13" s="655"/>
-      <c r="AN13" s="641"/>
+      <c r="AM13" s="651"/>
+      <c r="AN13" s="636"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="450"/>
@@ -7773,18 +7773,18 @@
       <c r="C14" s="459"/>
       <c r="D14" s="452"/>
       <c r="E14" s="453"/>
-      <c r="F14" s="620"/>
+      <c r="F14" s="641"/>
       <c r="G14" s="605" t="s">
         <v>429</v>
       </c>
       <c r="H14" s="605"/>
       <c r="I14" s="605"/>
-      <c r="J14" s="627"/>
+      <c r="J14" s="683"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="623"/>
+      <c r="O14" s="679"/>
       <c r="Q14" s="61" t="s">
         <v>532</v>
       </c>
@@ -7798,24 +7798,24 @@
       <c r="X14" s="431" t="s">
         <v>168</v>
       </c>
-      <c r="Y14" s="658"/>
+      <c r="Y14" s="654"/>
       <c r="Z14" s="407">
         <v>1</v>
       </c>
       <c r="AA14" s="307"/>
       <c r="AB14" s="209"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="639"/>
+      <c r="AD14" s="668"/>
       <c r="AE14" s="257"/>
-      <c r="AF14" s="631"/>
+      <c r="AF14" s="656"/>
       <c r="AG14" s="257"/>
       <c r="AH14" s="257"/>
       <c r="AI14" s="70"/>
       <c r="AJ14" s="257"/>
       <c r="AK14" s="257"/>
       <c r="AL14" s="257"/>
-      <c r="AM14" s="655"/>
-      <c r="AN14" s="641"/>
+      <c r="AM14" s="651"/>
+      <c r="AN14" s="636"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="449" t="s">
@@ -7824,8 +7824,8 @@
       <c r="C15" s="598" t="s">
         <v>373</v>
       </c>
-      <c r="F15" s="620"/>
-      <c r="O15" s="623"/>
+      <c r="F15" s="641"/>
+      <c r="O15" s="679"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -7838,7 +7838,7 @@
       <c r="X15" s="431" t="s">
         <v>169</v>
       </c>
-      <c r="Y15" s="658"/>
+      <c r="Y15" s="654"/>
       <c r="Z15" s="409">
         <v>1</v>
       </c>
@@ -7847,8 +7847,8 @@
       <c r="AC15" s="76" t="s">
         <v>479</v>
       </c>
-      <c r="AD15" s="639"/>
-      <c r="AF15" s="631"/>
+      <c r="AD15" s="668"/>
+      <c r="AF15" s="656"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="238" t="s">
         <v>448</v>
@@ -7861,8 +7861,8 @@
       </c>
       <c r="AK15" s="257"/>
       <c r="AL15" s="257"/>
-      <c r="AM15" s="655"/>
-      <c r="AN15" s="641"/>
+      <c r="AM15" s="651"/>
+      <c r="AN15" s="636"/>
       <c r="AP15" s="76" t="s">
         <v>73</v>
       </c>
@@ -7884,13 +7884,13 @@
       <c r="E16" s="224">
         <v>1</v>
       </c>
-      <c r="F16" s="620"/>
+      <c r="F16" s="641"/>
       <c r="G16" s="337" t="s">
         <v>488</v>
       </c>
       <c r="I16" s="469"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="623"/>
+      <c r="O16" s="679"/>
       <c r="R16" s="435" t="s">
         <v>184</v>
       </c>
@@ -7901,7 +7901,7 @@
       <c r="X16" s="431" t="s">
         <v>170</v>
       </c>
-      <c r="Y16" s="658"/>
+      <c r="Y16" s="654"/>
       <c r="Z16" s="407">
         <v>1</v>
       </c>
@@ -7922,18 +7922,18 @@
       <c r="AM16" s="428" t="s">
         <v>317</v>
       </c>
-      <c r="AN16" s="641"/>
+      <c r="AN16" s="636"/>
       <c r="AP16" s="76" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="620"/>
+      <c r="F17" s="641"/>
       <c r="I17" s="470"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="623"/>
+      <c r="O17" s="679"/>
       <c r="Q17" s="21" t="s">
         <v>530</v>
       </c>
@@ -7953,7 +7953,7 @@
       <c r="X17" s="431" t="s">
         <v>171</v>
       </c>
-      <c r="Y17" s="658"/>
+      <c r="Y17" s="654"/>
       <c r="Z17" s="409"/>
       <c r="AA17" s="307"/>
       <c r="AB17" s="209"/>
@@ -7978,7 +7978,7 @@
       <c r="AK17" s="257"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="428"/>
-      <c r="AN17" s="641"/>
+      <c r="AN17" s="636"/>
       <c r="AO17" s="204" t="s">
         <v>497</v>
       </c>
@@ -8002,21 +8002,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="620"/>
+      <c r="F18" s="641"/>
       <c r="G18" s="337" t="s">
         <v>527</v>
       </c>
       <c r="I18" s="24"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="623"/>
+      <c r="O18" s="679"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="615" t="s">
+      <c r="R18" s="673" t="s">
         <v>535</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="663" t="s">
+      <c r="U18" s="612" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -8026,7 +8026,7 @@
       <c r="X18" s="431" t="s">
         <v>172</v>
       </c>
-      <c r="Y18" s="658"/>
+      <c r="Y18" s="654"/>
       <c r="Z18" s="409">
         <v>1</v>
       </c>
@@ -8037,38 +8037,38 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="257"/>
-      <c r="AF18" s="630" t="s">
+      <c r="AF18" s="650" t="s">
         <v>475</v>
       </c>
       <c r="AG18" s="257"/>
       <c r="AH18" s="70"/>
       <c r="AI18" s="70"/>
-      <c r="AJ18" s="656" t="s">
+      <c r="AJ18" s="652" t="s">
         <v>315</v>
       </c>
       <c r="AK18" s="257"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="428"/>
-      <c r="AN18" s="641"/>
+      <c r="AN18" s="636"/>
       <c r="AP18" s="76" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="620"/>
+      <c r="F19" s="641"/>
       <c r="I19" s="219"/>
-      <c r="O19" s="623"/>
-      <c r="R19" s="616"/>
+      <c r="O19" s="679"/>
+      <c r="R19" s="674"/>
       <c r="S19" s="30" t="s">
         <v>533</v>
       </c>
-      <c r="U19" s="664"/>
+      <c r="U19" s="613"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="431" t="s">
         <v>173</v>
       </c>
-      <c r="Y19" s="658"/>
+      <c r="Y19" s="654"/>
       <c r="Z19" s="407">
         <v>1</v>
       </c>
@@ -8077,17 +8077,17 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="257"/>
-      <c r="AF19" s="630"/>
+      <c r="AF19" s="650"/>
       <c r="AG19" s="257"/>
       <c r="AH19" s="257"/>
       <c r="AI19" s="70"/>
-      <c r="AJ19" s="656"/>
+      <c r="AJ19" s="652"/>
       <c r="AK19" s="460" t="s">
         <v>251</v>
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="428"/>
-      <c r="AN19" s="641"/>
+      <c r="AN19" s="636"/>
       <c r="AP19" s="76" t="s">
         <v>468</v>
       </c>
@@ -8108,24 +8108,24 @@
       <c r="E20" s="437">
         <v>-1</v>
       </c>
-      <c r="F20" s="620"/>
+      <c r="F20" s="641"/>
       <c r="G20" s="337" t="s">
         <v>491</v>
       </c>
       <c r="I20" s="219"/>
-      <c r="O20" s="623"/>
-      <c r="Q20" s="625" t="s">
+      <c r="O20" s="679"/>
+      <c r="Q20" s="681" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="404" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="665"/>
+      <c r="U20" s="614"/>
       <c r="W20" s="405"/>
       <c r="X20" s="432" t="s">
         <v>174</v>
       </c>
-      <c r="Y20" s="658"/>
+      <c r="Y20" s="654"/>
       <c r="Z20" s="411">
         <v>1</v>
       </c>
@@ -8150,7 +8150,7 @@
       <c r="AM20" s="381" t="s">
         <v>249</v>
       </c>
-      <c r="AN20" s="641"/>
+      <c r="AN20" s="636"/>
       <c r="AO20" s="338" t="s">
         <v>460</v>
       </c>
@@ -8171,20 +8171,20 @@
       <c r="E21" s="265">
         <v>0</v>
       </c>
-      <c r="F21" s="620"/>
+      <c r="F21" s="641"/>
       <c r="I21" s="219"/>
-      <c r="O21" s="623"/>
-      <c r="Q21" s="626"/>
+      <c r="O21" s="679"/>
+      <c r="Q21" s="682"/>
       <c r="T21" s="422"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="660"/>
+      <c r="V21" s="609"/>
       <c r="W21" s="426" t="s">
         <v>175</v>
       </c>
       <c r="X21" s="429" t="s">
         <v>186</v>
       </c>
-      <c r="Y21" s="658"/>
+      <c r="Y21" s="654"/>
       <c r="Z21" s="445">
         <v>3</v>
       </c>
@@ -8215,15 +8215,15 @@
       <c r="AM21" s="428" t="s">
         <v>544</v>
       </c>
-      <c r="AN21" s="641"/>
+      <c r="AN21" s="636"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="620"/>
+      <c r="F22" s="641"/>
       <c r="G22" s="337" t="s">
         <v>489</v>
       </c>
       <c r="I22" s="219"/>
-      <c r="O22" s="623"/>
+      <c r="O22" s="679"/>
       <c r="R22" s="434" t="s">
         <v>44</v>
       </c>
@@ -8231,14 +8231,14 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="661"/>
+      <c r="V22" s="610"/>
       <c r="W22" s="426" t="s">
         <v>175</v>
       </c>
       <c r="X22" s="429" t="s">
         <v>187</v>
       </c>
-      <c r="Y22" s="658"/>
+      <c r="Y22" s="654"/>
       <c r="Z22" s="415"/>
       <c r="AA22" s="10"/>
       <c r="AB22" s="415"/>
@@ -8249,7 +8249,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="630" t="s">
+      <c r="AJ22" s="650" t="s">
         <v>472</v>
       </c>
       <c r="AK22" s="257"/>
@@ -8257,7 +8257,7 @@
         <v>478</v>
       </c>
       <c r="AM22" s="300"/>
-      <c r="AN22" s="641"/>
+      <c r="AN22" s="636"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="231" t="s">
@@ -8275,22 +8275,22 @@
       <c r="E23" s="225">
         <v>1</v>
       </c>
-      <c r="F23" s="620"/>
+      <c r="F23" s="641"/>
       <c r="I23" s="219"/>
-      <c r="O23" s="623"/>
-      <c r="Q23" s="625" t="s">
+      <c r="O23" s="679"/>
+      <c r="Q23" s="681" t="s">
         <v>144</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="420" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="661"/>
+      <c r="V23" s="610"/>
       <c r="W23" s="148"/>
       <c r="X23" s="429" t="s">
         <v>188</v>
       </c>
-      <c r="Y23" s="658"/>
+      <c r="Y23" s="654"/>
       <c r="Z23" s="17"/>
       <c r="AA23" s="10"/>
       <c r="AB23" s="415"/>
@@ -8301,13 +8301,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="630"/>
+      <c r="AJ23" s="650"/>
       <c r="AK23" s="257"/>
       <c r="AL23" s="80" t="s">
         <v>507</v>
       </c>
       <c r="AM23" s="300"/>
-      <c r="AN23" s="641"/>
+      <c r="AN23" s="636"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="440" t="s">
@@ -8325,23 +8325,23 @@
       <c r="E24" s="436">
         <v>1</v>
       </c>
-      <c r="F24" s="620"/>
+      <c r="F24" s="641"/>
       <c r="G24" s="61" t="s">
         <v>490</v>
       </c>
       <c r="I24" s="219"/>
-      <c r="O24" s="623"/>
-      <c r="Q24" s="626"/>
+      <c r="O24" s="679"/>
+      <c r="Q24" s="682"/>
       <c r="T24" s="17"/>
       <c r="U24" s="227" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="661"/>
+      <c r="V24" s="610"/>
       <c r="W24" s="148"/>
       <c r="X24" s="429" t="s">
         <v>185</v>
       </c>
-      <c r="Y24" s="658"/>
+      <c r="Y24" s="654"/>
       <c r="Z24" s="17"/>
       <c r="AA24" s="10"/>
       <c r="AB24" s="415"/>
@@ -8360,12 +8360,12 @@
         <v>463</v>
       </c>
       <c r="AM24" s="300"/>
-      <c r="AN24" s="641"/>
+      <c r="AN24" s="636"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="620"/>
+      <c r="F25" s="641"/>
       <c r="I25" s="219"/>
-      <c r="O25" s="623"/>
+      <c r="O25" s="679"/>
       <c r="P25" s="204" t="s">
         <v>280</v>
       </c>
@@ -8378,12 +8378,12 @@
       <c r="U25" s="400" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="662"/>
+      <c r="V25" s="611"/>
       <c r="W25" s="148"/>
       <c r="X25" s="429" t="s">
         <v>189</v>
       </c>
-      <c r="Y25" s="658"/>
+      <c r="Y25" s="654"/>
       <c r="Z25" s="17"/>
       <c r="AA25" s="10"/>
       <c r="AB25" s="415"/>
@@ -8400,7 +8400,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="300"/>
-      <c r="AN25" s="641"/>
+      <c r="AN25" s="636"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="231" t="s">
@@ -8418,17 +8418,17 @@
       <c r="E26" s="380">
         <v>1</v>
       </c>
-      <c r="F26" s="620"/>
+      <c r="F26" s="641"/>
       <c r="G26" s="337" t="s">
         <v>487</v>
       </c>
       <c r="I26" s="219"/>
-      <c r="O26" s="623"/>
-      <c r="P26" s="643" t="s">
+      <c r="O26" s="679"/>
+      <c r="P26" s="638" t="s">
         <v>525</v>
       </c>
-      <c r="Q26" s="644"/>
-      <c r="R26" s="617" t="s">
+      <c r="Q26" s="639"/>
+      <c r="R26" s="675" t="s">
         <v>534</v>
       </c>
       <c r="T26" s="178"/>
@@ -8440,7 +8440,7 @@
       <c r="X26" s="429" t="s">
         <v>181</v>
       </c>
-      <c r="Y26" s="658"/>
+      <c r="Y26" s="654"/>
       <c r="Z26" s="17"/>
       <c r="AA26" s="10"/>
       <c r="AB26" s="415"/>
@@ -8467,7 +8467,7 @@
       <c r="AM26" s="442" t="s">
         <v>456</v>
       </c>
-      <c r="AN26" s="641"/>
+      <c r="AN26" s="636"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -8479,13 +8479,13 @@
       <c r="E27" s="265" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="621"/>
+      <c r="F27" s="677"/>
       <c r="G27" s="61" t="s">
         <v>543</v>
       </c>
       <c r="I27" s="220"/>
-      <c r="O27" s="624"/>
-      <c r="R27" s="618"/>
+      <c r="O27" s="680"/>
+      <c r="R27" s="676"/>
       <c r="S27" s="421" t="s">
         <v>54</v>
       </c>
@@ -8498,7 +8498,7 @@
       <c r="X27" s="429" t="s">
         <v>529</v>
       </c>
-      <c r="Y27" s="659"/>
+      <c r="Y27" s="655"/>
       <c r="Z27" s="161"/>
       <c r="AA27" s="13"/>
       <c r="AB27" s="416"/>
@@ -8515,10 +8515,48 @@
       <c r="AM27" s="381" t="s">
         <v>319</v>
       </c>
-      <c r="AN27" s="642"/>
+      <c r="AN27" s="637"/>
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="O10:O27"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="AI6:AI10"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AG7:AG12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="AN1:AN27"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="M2:M9"/>
+    <mergeCell ref="O2:O9"/>
+    <mergeCell ref="P10:P13"/>
+    <mergeCell ref="AK6:AK7"/>
+    <mergeCell ref="AM12:AM15"/>
+    <mergeCell ref="AF18:AF19"/>
+    <mergeCell ref="AJ18:AJ19"/>
+    <mergeCell ref="Y1:Y27"/>
+    <mergeCell ref="AJ22:AJ23"/>
+    <mergeCell ref="AK9:AK10"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="R2:R3"/>
     <mergeCell ref="V21:V25"/>
     <mergeCell ref="U18:U20"/>
     <mergeCell ref="C2:C3"/>
@@ -8535,44 +8573,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="AN1:AN27"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="M2:M9"/>
-    <mergeCell ref="O2:O9"/>
-    <mergeCell ref="P10:P13"/>
-    <mergeCell ref="AK6:AK7"/>
-    <mergeCell ref="AM12:AM15"/>
-    <mergeCell ref="AF18:AF19"/>
-    <mergeCell ref="AJ18:AJ19"/>
-    <mergeCell ref="Y1:Y27"/>
-    <mergeCell ref="AJ22:AJ23"/>
-    <mergeCell ref="AK9:AK10"/>
-    <mergeCell ref="AD3:AD4"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AI6:AI10"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AG7:AG12"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="F2:F27"/>
-    <mergeCell ref="O10:O27"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8609,12 +8609,12 @@
       <c r="B1" s="603" t="s">
         <v>310</v>
       </c>
-      <c r="C1" s="627"/>
+      <c r="C1" s="683"/>
       <c r="D1" s="204"/>
       <c r="J1" s="603" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="627"/>
+      <c r="K1" s="683"/>
       <c r="L1" s="195" t="s">
         <v>330</v>
       </c>
@@ -9017,7 +9017,7 @@
       <c r="P1" s="398" t="s">
         <v>397</v>
       </c>
-      <c r="Q1" s="701" t="s">
+      <c r="Q1" s="714" t="s">
         <v>180</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -9041,7 +9041,7 @@
       <c r="AA1" s="517" t="s">
         <v>437</v>
       </c>
-      <c r="AB1" s="695" t="s">
+      <c r="AB1" s="708" t="s">
         <v>593</v>
       </c>
       <c r="AC1" s="99" t="s">
@@ -9063,32 +9063,32 @@
       </c>
     </row>
     <row r="2" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="706">
+      <c r="A2" s="693">
         <f ca="1">TODAY()</f>
         <v>45291</v>
       </c>
-      <c r="B2" s="708" t="s">
+      <c r="B2" s="695" t="s">
         <v>379</v>
       </c>
-      <c r="C2" s="645" t="s">
+      <c r="C2" s="615" t="s">
         <v>357</v>
       </c>
-      <c r="D2" s="710" t="s">
+      <c r="D2" s="697" t="s">
         <v>102</v>
       </c>
-      <c r="E2" s="712" t="s">
+      <c r="E2" s="699" t="s">
         <v>64</v>
       </c>
       <c r="F2" s="191" t="s">
         <v>218</v>
       </c>
-      <c r="G2" s="613" t="s">
+      <c r="G2" s="659" t="s">
         <v>372</v>
       </c>
       <c r="H2" s="206" t="s">
         <v>218</v>
       </c>
-      <c r="I2" s="692" t="s">
+      <c r="I2" s="705" t="s">
         <v>102</v>
       </c>
       <c r="J2" s="396" t="s">
@@ -9112,7 +9112,7 @@
       <c r="P2" s="399">
         <v>40</v>
       </c>
-      <c r="Q2" s="702"/>
+      <c r="Q2" s="715"/>
       <c r="R2" s="21">
         <f>R7+R20</f>
         <v>2</v>
@@ -9137,7 +9137,7 @@
         <f>IF((Z2+T2)&gt;0,0,-1)</f>
         <v>0</v>
       </c>
-      <c r="AB2" s="696"/>
+      <c r="AB2" s="709"/>
       <c r="AC2" s="35"/>
       <c r="AH2" s="6" t="s">
         <v>344</v>
@@ -9152,14 +9152,14 @@
       </c>
     </row>
     <row r="3" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="707"/>
-      <c r="B3" s="709"/>
-      <c r="C3" s="646"/>
-      <c r="D3" s="711"/>
-      <c r="E3" s="713"/>
-      <c r="G3" s="614"/>
+      <c r="A3" s="694"/>
+      <c r="B3" s="696"/>
+      <c r="C3" s="616"/>
+      <c r="D3" s="698"/>
+      <c r="E3" s="700"/>
+      <c r="G3" s="660"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="693"/>
+      <c r="I3" s="706"/>
       <c r="K3" s="24">
         <v>2</v>
       </c>
@@ -9174,7 +9174,7 @@
       <c r="V3" s="470"/>
       <c r="W3" s="6"/>
       <c r="X3" s="470"/>
-      <c r="AB3" s="696"/>
+      <c r="AB3" s="709"/>
       <c r="AC3" s="35"/>
       <c r="AE3" s="100" t="s">
         <v>588</v>
@@ -9203,10 +9203,10 @@
         <v>380</v>
       </c>
       <c r="B4" s="243"/>
-      <c r="C4" s="714" t="s">
+      <c r="C4" s="701" t="s">
         <v>177</v>
       </c>
-      <c r="I4" s="693"/>
+      <c r="I4" s="706"/>
       <c r="R4" s="471" t="s">
         <v>588</v>
       </c>
@@ -9218,7 +9218,7 @@
       <c r="V4" s="470"/>
       <c r="W4" s="6"/>
       <c r="X4" s="470"/>
-      <c r="AB4" s="696"/>
+      <c r="AB4" s="709"/>
       <c r="AC4" s="35"/>
       <c r="AE4" s="20"/>
       <c r="AF4" s="100" t="s">
@@ -9247,7 +9247,7 @@
       <c r="B5" s="100" t="s">
         <v>357</v>
       </c>
-      <c r="C5" s="715"/>
+      <c r="C5" s="702"/>
       <c r="D5" s="222" t="s">
         <v>102</v>
       </c>
@@ -9263,7 +9263,7 @@
       <c r="H5" s="206" t="s">
         <v>218</v>
       </c>
-      <c r="I5" s="693"/>
+      <c r="I5" s="706"/>
       <c r="J5" s="397" t="s">
         <v>268</v>
       </c>
@@ -9290,7 +9290,7 @@
       <c r="V5" s="468"/>
       <c r="W5" s="6"/>
       <c r="X5" s="468"/>
-      <c r="AB5" s="696"/>
+      <c r="AB5" s="709"/>
       <c r="AC5" s="2" t="s">
         <v>591</v>
       </c>
@@ -9310,19 +9310,19 @@
       <c r="AL5" s="468"/>
     </row>
     <row r="6" spans="1:38" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="703" t="s">
+      <c r="A6" s="690" t="s">
         <v>285</v>
       </c>
       <c r="B6" s="105" t="s">
         <v>198</v>
       </c>
-      <c r="C6" s="628"/>
-      <c r="D6" s="629"/>
+      <c r="C6" s="661"/>
+      <c r="D6" s="662"/>
       <c r="E6" s="96">
         <v>1</v>
       </c>
       <c r="G6" s="599"/>
-      <c r="I6" s="693"/>
+      <c r="I6" s="706"/>
       <c r="P6" s="61" t="s">
         <v>591</v>
       </c>
@@ -9334,7 +9334,7 @@
         <f>S7+S11-SUM(V2:V10)</f>
         <v>3</v>
       </c>
-      <c r="AB6" s="696"/>
+      <c r="AB6" s="709"/>
       <c r="AC6" s="35"/>
       <c r="AE6" s="64">
         <f>AE7-SUM(AL2:AL10)+AE11</f>
@@ -9350,7 +9350,7 @@
       <c r="AL6" s="112"/>
     </row>
     <row r="7" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="704"/>
+      <c r="A7" s="691"/>
       <c r="B7" s="100" t="s">
         <v>154</v>
       </c>
@@ -9361,7 +9361,7 @@
         <v>135</v>
       </c>
       <c r="G7" s="599"/>
-      <c r="I7" s="693"/>
+      <c r="I7" s="706"/>
       <c r="M7" s="16" t="s">
         <v>347</v>
       </c>
@@ -9391,7 +9391,7 @@
         <v>249</v>
       </c>
       <c r="X7" s="469"/>
-      <c r="AB7" s="696"/>
+      <c r="AB7" s="709"/>
       <c r="AC7" s="99" t="s">
         <v>592</v>
       </c>
@@ -9419,7 +9419,7 @@
       <c r="AL7" s="24"/>
     </row>
     <row r="8" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="705"/>
+      <c r="A8" s="692"/>
       <c r="B8" s="212" t="s">
         <v>28</v>
       </c>
@@ -9428,7 +9428,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="599"/>
-      <c r="I8" s="693"/>
+      <c r="I8" s="706"/>
       <c r="N8" s="80"/>
       <c r="U8" s="6"/>
       <c r="V8" s="24"/>
@@ -9436,7 +9436,7 @@
         <v>611</v>
       </c>
       <c r="X8" s="470"/>
-      <c r="AB8" s="696"/>
+      <c r="AB8" s="709"/>
       <c r="AC8" s="515"/>
       <c r="AH8" s="6" t="s">
         <v>610</v>
@@ -9467,7 +9467,7 @@
       </c>
       <c r="G9" s="599"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="693"/>
+      <c r="I9" s="706"/>
       <c r="M9" s="19" t="s">
         <v>524</v>
       </c>
@@ -9478,7 +9478,7 @@
         <v>603</v>
       </c>
       <c r="X9" s="470"/>
-      <c r="AB9" s="696"/>
+      <c r="AB9" s="709"/>
       <c r="AC9" s="515"/>
       <c r="AE9" s="20"/>
       <c r="AF9" s="20"/>
@@ -9506,7 +9506,7 @@
         <v>37</v>
       </c>
       <c r="G10" s="599"/>
-      <c r="I10" s="693"/>
+      <c r="I10" s="706"/>
       <c r="J10" s="24" t="s">
         <v>372</v>
       </c>
@@ -9521,7 +9521,7 @@
       <c r="V10" s="470"/>
       <c r="W10" s="6"/>
       <c r="X10" s="470"/>
-      <c r="AB10" s="696"/>
+      <c r="AB10" s="709"/>
       <c r="AC10" s="515"/>
       <c r="AE10" s="20"/>
       <c r="AF10" s="20"/>
@@ -9549,7 +9549,7 @@
         <v>265</v>
       </c>
       <c r="G11" s="599"/>
-      <c r="I11" s="693"/>
+      <c r="I11" s="706"/>
       <c r="J11" s="24" t="s">
         <v>194</v>
       </c>
@@ -9575,13 +9575,13 @@
       <c r="S11" s="24">
         <v>3</v>
       </c>
-      <c r="U11" s="698" t="s">
+      <c r="U11" s="711" t="s">
         <v>557</v>
       </c>
-      <c r="V11" s="699"/>
-      <c r="W11" s="699"/>
-      <c r="X11" s="700"/>
-      <c r="AB11" s="697"/>
+      <c r="V11" s="712"/>
+      <c r="W11" s="712"/>
+      <c r="X11" s="713"/>
+      <c r="AB11" s="710"/>
       <c r="AC11" s="99" t="s">
         <v>594</v>
       </c>
@@ -9595,13 +9595,13 @@
         <v>3</v>
       </c>
       <c r="AG11" s="414"/>
-      <c r="AH11" s="698" t="s">
+      <c r="AH11" s="711" t="s">
         <v>602</v>
       </c>
-      <c r="AI11" s="699"/>
-      <c r="AJ11" s="699"/>
-      <c r="AK11" s="699"/>
-      <c r="AL11" s="700"/>
+      <c r="AI11" s="712"/>
+      <c r="AJ11" s="712"/>
+      <c r="AK11" s="712"/>
+      <c r="AL11" s="713"/>
     </row>
     <row r="12" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="227" t="s">
@@ -9612,7 +9612,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="599"/>
-      <c r="I12" s="693"/>
+      <c r="I12" s="706"/>
       <c r="J12" s="24" t="s">
         <v>515</v>
       </c>
@@ -9645,7 +9645,7 @@
       </c>
       <c r="D13" s="20"/>
       <c r="G13" s="599"/>
-      <c r="I13" s="693"/>
+      <c r="I13" s="706"/>
       <c r="J13" s="108" t="s">
         <v>547</v>
       </c>
@@ -9689,7 +9689,7 @@
       <c r="H14" s="206" t="s">
         <v>218</v>
       </c>
-      <c r="I14" s="693"/>
+      <c r="I14" s="706"/>
       <c r="U14" s="67" t="s">
         <v>80</v>
       </c>
@@ -9716,7 +9716,7 @@
       <c r="H15" s="271">
         <v>0</v>
       </c>
-      <c r="I15" s="693"/>
+      <c r="I15" s="706"/>
       <c r="J15" s="108" t="s">
         <v>153</v>
       </c>
@@ -9747,7 +9747,7 @@
       <c r="D16" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="I16" s="693"/>
+      <c r="I16" s="706"/>
       <c r="K16" s="100" t="s">
         <v>44</v>
       </c>
@@ -9791,7 +9791,7 @@
       <c r="G17" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="I17" s="693"/>
+      <c r="I17" s="706"/>
       <c r="L17" s="2" t="s">
         <v>426</v>
       </c>
@@ -9805,13 +9805,13 @@
     </row>
     <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
-      <c r="I18" s="693"/>
+      <c r="I18" s="706"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="690" t="s">
+      <c r="O18" s="703" t="s">
         <v>516</v>
       </c>
-      <c r="P18" s="691"/>
+      <c r="P18" s="704"/>
       <c r="Q18" s="127" t="s">
         <v>44</v>
       </c>
@@ -9833,7 +9833,7 @@
       </c>
     </row>
     <row r="19" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="693"/>
+      <c r="I19" s="706"/>
       <c r="M19" s="21" t="s">
         <v>425</v>
       </c>
@@ -9865,7 +9865,7 @@
       <c r="G20" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="I20" s="693"/>
+      <c r="I20" s="706"/>
       <c r="K20" s="19" t="s">
         <v>422</v>
       </c>
@@ -9894,7 +9894,7 @@
       <c r="X20" s="468"/>
     </row>
     <row r="21" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="693"/>
+      <c r="I21" s="706"/>
       <c r="M21" s="216" t="s">
         <v>411</v>
       </c>
@@ -9924,7 +9924,7 @@
       <c r="G22" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="I22" s="693"/>
+      <c r="I22" s="706"/>
       <c r="P22" s="99" t="s">
         <v>590</v>
       </c>
@@ -9939,7 +9939,7 @@
       <c r="E23" s="283" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="693"/>
+      <c r="I23" s="706"/>
       <c r="Q23" s="24">
         <f>SUM(V23:V31)</f>
         <v>7</v>
@@ -9956,7 +9956,7 @@
       </c>
     </row>
     <row r="24" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="693"/>
+      <c r="I24" s="706"/>
       <c r="U24" s="35"/>
       <c r="V24" s="509">
         <v>1</v>
@@ -9984,7 +9984,7 @@
       <c r="H25" s="191" t="s">
         <v>266</v>
       </c>
-      <c r="I25" s="693"/>
+      <c r="I25" s="706"/>
       <c r="J25" s="397" t="s">
         <v>269</v>
       </c>
@@ -10029,7 +10029,7 @@
       <c r="H26" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="I26" s="693"/>
+      <c r="I26" s="706"/>
       <c r="K26" s="24">
         <v>15</v>
       </c>
@@ -10064,7 +10064,7 @@
       </c>
     </row>
     <row r="27" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="693"/>
+      <c r="I27" s="706"/>
       <c r="O27" s="2" t="s">
         <v>98</v>
       </c>
@@ -10091,7 +10091,7 @@
       <c r="E28" s="215">
         <v>2</v>
       </c>
-      <c r="I28" s="693"/>
+      <c r="I28" s="706"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="142"/>
@@ -10113,7 +10113,7 @@
       <c r="H29" s="191" t="s">
         <v>267</v>
       </c>
-      <c r="I29" s="694"/>
+      <c r="I29" s="707"/>
       <c r="J29" s="324"/>
       <c r="L29" s="96" t="s">
         <v>273</v>
@@ -10171,6 +10171,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I2:I29"/>
+    <mergeCell ref="AB1:AB11"/>
+    <mergeCell ref="AH11:AL11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="U11:X11"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="G5:G14"/>
     <mergeCell ref="A2:A3"/>
@@ -10182,13 +10189,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I2:I29"/>
-    <mergeCell ref="AB1:AB11"/>
-    <mergeCell ref="AH11:AL11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="U11:X11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10199,8 +10199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AT37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T18" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10300,14 +10300,14 @@
         <f ca="1">TODAY()</f>
         <v>45291</v>
       </c>
-      <c r="T1" s="735"/>
+      <c r="T1" s="742"/>
       <c r="U1" s="142"/>
       <c r="V1" s="6"/>
       <c r="W1" s="6"/>
-      <c r="X1" s="719" t="s">
+      <c r="X1" s="726" t="s">
         <v>441</v>
       </c>
-      <c r="Y1" s="720"/>
+      <c r="Y1" s="727"/>
       <c r="Z1" s="306">
         <f>68-(W8+Y3+X3+U3)</f>
         <v>0</v>
@@ -10323,27 +10323,27 @@
       <c r="AD1" s="302" t="s">
         <v>44</v>
       </c>
-      <c r="AE1" s="721" t="s">
+      <c r="AE1" s="728" t="s">
         <v>190</v>
       </c>
-      <c r="AF1" s="722"/>
-      <c r="AG1" s="723"/>
-      <c r="AH1" s="724" t="s">
+      <c r="AF1" s="729"/>
+      <c r="AG1" s="730"/>
+      <c r="AH1" s="731" t="s">
         <v>293</v>
       </c>
-      <c r="AI1" s="725"/>
-      <c r="AJ1" s="726"/>
-      <c r="AK1" s="613" t="s">
+      <c r="AI1" s="732"/>
+      <c r="AJ1" s="733"/>
+      <c r="AK1" s="659" t="s">
         <v>613</v>
       </c>
       <c r="AL1" s="550" t="s">
         <v>614</v>
       </c>
-      <c r="AM1" s="716" t="s">
+      <c r="AM1" s="723" t="s">
         <v>444</v>
       </c>
-      <c r="AN1" s="717"/>
-      <c r="AO1" s="718"/>
+      <c r="AN1" s="724"/>
+      <c r="AO1" s="725"/>
       <c r="AR1" s="142"/>
     </row>
     <row r="2" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10358,27 +10358,27 @@
         <f>K2+L2</f>
         <v>26</v>
       </c>
-      <c r="K2" s="743">
+      <c r="K2" s="721">
         <f>SUM(K4:K37)</f>
         <v>6</v>
       </c>
-      <c r="L2" s="741">
+      <c r="L2" s="719">
         <f>SUM(L4:L37)</f>
         <v>20</v>
       </c>
-      <c r="M2" s="727">
+      <c r="M2" s="734">
         <f>SUM(M5:M30)</f>
         <v>0</v>
       </c>
-      <c r="N2" s="729">
+      <c r="N2" s="736">
         <f>SUM(N4:N29)</f>
         <v>8</v>
       </c>
-      <c r="O2" s="731">
+      <c r="O2" s="738">
         <f>SUM(O4:O29)</f>
         <v>11</v>
       </c>
-      <c r="P2" s="637">
+      <c r="P2" s="666">
         <f>SUM(N30:N37)* (-1)</f>
         <v>-1</v>
       </c>
@@ -10391,14 +10391,14 @@
       <c r="S2" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="T2" s="736"/>
+      <c r="T2" s="743"/>
       <c r="U2" s="537" t="s">
         <v>262</v>
       </c>
       <c r="V2" s="482" t="s">
         <v>219</v>
       </c>
-      <c r="W2" s="733" t="s">
+      <c r="W2" s="740" t="s">
         <v>234</v>
       </c>
       <c r="X2" s="483" t="s">
@@ -10440,7 +10440,7 @@
       <c r="AJ2" s="150" t="s">
         <v>288</v>
       </c>
-      <c r="AK2" s="614"/>
+      <c r="AK2" s="660"/>
       <c r="AL2" s="591" t="s">
         <v>288</v>
       </c>
@@ -10468,12 +10468,12 @@
         <f>V3+X3+Y3+U3</f>
         <v>68</v>
       </c>
-      <c r="K3" s="744"/>
-      <c r="L3" s="742"/>
-      <c r="M3" s="728"/>
-      <c r="N3" s="730"/>
-      <c r="O3" s="732"/>
-      <c r="P3" s="638"/>
+      <c r="K3" s="722"/>
+      <c r="L3" s="720"/>
+      <c r="M3" s="735"/>
+      <c r="N3" s="737"/>
+      <c r="O3" s="739"/>
+      <c r="P3" s="667"/>
       <c r="Q3" s="172">
         <f>(M2+N2)-Y3</f>
         <v>0</v>
@@ -10481,7 +10481,7 @@
       <c r="S3" s="159" t="s">
         <v>244</v>
       </c>
-      <c r="T3" s="737"/>
+      <c r="T3" s="744"/>
       <c r="U3" s="538">
         <f>SUM(U4:U29)</f>
         <v>14</v>
@@ -10490,7 +10490,7 @@
         <f>SUM(V4:V29)</f>
         <v>37</v>
       </c>
-      <c r="W3" s="734"/>
+      <c r="W3" s="741"/>
       <c r="X3" s="485">
         <f t="shared" ref="X3:AC3" si="0">SUM(X4:X29)</f>
         <v>9</v>
@@ -10596,7 +10596,7 @@
         <f>AC4</f>
         <v>0</v>
       </c>
-      <c r="P4" s="738"/>
+      <c r="P4" s="716"/>
       <c r="Q4" s="20"/>
       <c r="R4" s="2" t="s">
         <v>334</v>
@@ -10680,7 +10680,7 @@
         <f>AC5</f>
         <v>0</v>
       </c>
-      <c r="P5" s="739"/>
+      <c r="P5" s="717"/>
       <c r="Q5" s="20"/>
       <c r="R5" s="2" t="s">
         <v>340</v>
@@ -10774,7 +10774,7 @@
         <f>AC6</f>
         <v>1</v>
       </c>
-      <c r="P6" s="739"/>
+      <c r="P6" s="717"/>
       <c r="Q6" s="54" t="s">
         <v>335</v>
       </c>
@@ -10879,7 +10879,7 @@
         <f>AC7</f>
         <v>1</v>
       </c>
-      <c r="P7" s="739"/>
+      <c r="P7" s="717"/>
       <c r="Q7" s="20"/>
       <c r="R7" s="2" t="s">
         <v>335</v>
@@ -10995,7 +10995,7 @@
         <f t="shared" ref="O8:O37" si="10">AC8</f>
         <v>0</v>
       </c>
-      <c r="P8" s="739"/>
+      <c r="P8" s="717"/>
       <c r="Q8" s="108" t="s">
         <v>233</v>
       </c>
@@ -11086,7 +11086,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P9" s="739"/>
+      <c r="P9" s="717"/>
       <c r="Q9" s="108" t="s">
         <v>335</v>
       </c>
@@ -11191,7 +11191,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P10" s="739"/>
+      <c r="P10" s="717"/>
       <c r="Q10" s="20"/>
       <c r="R10" s="2" t="s">
         <v>340</v>
@@ -11281,7 +11281,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P11" s="739"/>
+      <c r="P11" s="717"/>
       <c r="Q11" s="108" t="s">
         <v>335</v>
       </c>
@@ -11346,14 +11346,14 @@
       <c r="AR11" s="508"/>
     </row>
     <row r="12" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="675" t="s">
+      <c r="A12" s="626" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
         <v>13</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="E12" s="625" t="s">
+      <c r="E12" s="681" t="s">
         <v>56</v>
       </c>
       <c r="G12" s="262"/>
@@ -11378,7 +11378,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P12" s="739"/>
+      <c r="P12" s="717"/>
       <c r="Q12" s="108" t="s">
         <v>335</v>
       </c>
@@ -11455,14 +11455,14 @@
       </c>
     </row>
     <row r="13" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="677"/>
+      <c r="A13" s="628"/>
       <c r="B13" s="583">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="626"/>
+      <c r="E13" s="682"/>
       <c r="F13" s="172">
         <v>0</v>
       </c>
@@ -11486,7 +11486,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P13" s="739"/>
+      <c r="P13" s="717"/>
       <c r="Q13" s="108" t="s">
         <v>335</v>
       </c>
@@ -11568,7 +11568,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P14" s="739"/>
+      <c r="P14" s="717"/>
       <c r="Q14" s="20"/>
       <c r="R14" s="200" t="s">
         <v>339</v>
@@ -11671,7 +11671,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P15" s="739"/>
+      <c r="P15" s="717"/>
       <c r="Q15" s="20"/>
       <c r="R15" s="200" t="s">
         <v>339</v>
@@ -11765,7 +11765,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P16" s="739"/>
+      <c r="P16" s="717"/>
       <c r="Q16" s="108" t="s">
         <v>335</v>
       </c>
@@ -11866,7 +11866,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P17" s="739"/>
+      <c r="P17" s="717"/>
       <c r="Q17" s="20"/>
       <c r="R17" s="2" t="s">
         <v>341</v>
@@ -11966,7 +11966,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P18" s="739"/>
+      <c r="P18" s="717"/>
       <c r="Q18" s="108" t="s">
         <v>335</v>
       </c>
@@ -12056,7 +12056,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P19" s="739"/>
+      <c r="P19" s="717"/>
       <c r="Q19" s="20"/>
       <c r="R19" s="2" t="s">
         <v>334</v>
@@ -12164,11 +12164,11 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P20" s="740"/>
+      <c r="P20" s="718"/>
       <c r="Q20" s="605" t="s">
         <v>335</v>
       </c>
-      <c r="R20" s="627"/>
+      <c r="R20" s="683"/>
       <c r="S20" s="534" t="s">
         <v>85</v>
       </c>
@@ -12430,7 +12430,7 @@
     </row>
     <row r="23" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="24"/>
-      <c r="E23" s="682" t="s">
+      <c r="E23" s="633" t="s">
         <v>289</v>
       </c>
       <c r="F23" s="180"/>
@@ -12535,7 +12535,7 @@
       <c r="C24" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="E24" s="683"/>
+      <c r="E24" s="634"/>
       <c r="F24" s="172"/>
       <c r="H24" s="42"/>
       <c r="J24" s="570" t="s">
@@ -12561,7 +12561,7 @@
       <c r="Q24" s="605" t="s">
         <v>335</v>
       </c>
-      <c r="R24" s="627"/>
+      <c r="R24" s="683"/>
       <c r="S24" s="534" t="s">
         <v>249</v>
       </c>
@@ -13229,8 +13229,8 @@
       <c r="AR31" s="508"/>
     </row>
     <row r="32" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="630"/>
-      <c r="B32" s="630"/>
+      <c r="A32" s="650"/>
+      <c r="B32" s="650"/>
       <c r="J32" s="571"/>
       <c r="K32" s="586"/>
       <c r="L32" s="580">
@@ -13708,7 +13708,7 @@
     </row>
     <row r="37" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="21">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D37" s="382">
         <v>1</v>
@@ -13814,15 +13814,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="P4:P20"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="Q20:R20"/>
     <mergeCell ref="AM1:AO1"/>
     <mergeCell ref="X1:Y1"/>
     <mergeCell ref="AE1:AG1"/>
@@ -13834,6 +13825,15 @@
     <mergeCell ref="W2:W3"/>
     <mergeCell ref="T1:T3"/>
     <mergeCell ref="AK1:AK2"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="P4:P20"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="Q20:R20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13901,7 +13901,7 @@
       <c r="V1" s="603" t="s">
         <v>70</v>
       </c>
-      <c r="W1" s="627"/>
+      <c r="W1" s="683"/>
       <c r="X1" s="62" t="s">
         <v>101</v>
       </c>
@@ -13920,7 +13920,7 @@
       <c r="AC1" s="116" t="s">
         <v>190</v>
       </c>
-      <c r="AD1" s="752" t="s">
+      <c r="AD1" s="759" t="s">
         <v>211</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -13937,10 +13937,10 @@
       <c r="E2" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="751" t="s">
+      <c r="F2" s="790" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="779" t="s">
+      <c r="G2" s="747" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -13968,10 +13968,10 @@
       <c r="U2" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="V2" s="719" t="s">
+      <c r="V2" s="726" t="s">
         <v>120</v>
       </c>
-      <c r="W2" s="720"/>
+      <c r="W2" s="727"/>
       <c r="X2" s="64" t="s">
         <v>109</v>
       </c>
@@ -13990,7 +13990,7 @@
       <c r="AC2" s="117" t="s">
         <v>98</v>
       </c>
-      <c r="AD2" s="753"/>
+      <c r="AD2" s="760"/>
       <c r="AE2" s="64" t="s">
         <v>98</v>
       </c>
@@ -14009,8 +14009,8 @@
       <c r="E3" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="F3" s="679"/>
-      <c r="G3" s="780"/>
+      <c r="F3" s="630"/>
+      <c r="G3" s="748"/>
       <c r="H3" s="40" t="s">
         <v>80</v>
       </c>
@@ -14021,13 +14021,13 @@
         <v>81</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="789" t="s">
+      <c r="O3" s="757" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="771" t="s">
+      <c r="P3" s="778" t="s">
         <v>217</v>
       </c>
-      <c r="Q3" s="772"/>
+      <c r="Q3" s="779"/>
       <c r="S3" s="57" t="s">
         <v>218</v>
       </c>
@@ -14037,15 +14037,15 @@
       <c r="W3" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="AD3" s="753"/>
+      <c r="AD3" s="760"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="780"/>
+      <c r="G4" s="748"/>
       <c r="H4" s="6"/>
       <c r="L4" s="687" t="s">
         <v>82</v>
       </c>
-      <c r="O4" s="790"/>
+      <c r="O4" s="758"/>
       <c r="T4" s="55" t="s">
         <v>97</v>
       </c>
@@ -14059,8 +14059,8 @@
         <v>194</v>
       </c>
       <c r="Z4" s="605"/>
-      <c r="AA4" s="627"/>
-      <c r="AD4" s="753"/>
+      <c r="AA4" s="683"/>
+      <c r="AD4" s="760"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -14075,21 +14075,21 @@
       <c r="F5" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="G5" s="780"/>
+      <c r="G5" s="748"/>
       <c r="H5" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="K5" s="758" t="s">
+      <c r="K5" s="765" t="s">
         <v>215</v>
       </c>
-      <c r="L5" s="773"/>
+      <c r="L5" s="780"/>
       <c r="M5" s="2" t="s">
         <v>213</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>212</v>
       </c>
-      <c r="O5" s="790"/>
+      <c r="O5" s="758"/>
       <c r="P5" s="108" t="s">
         <v>214</v>
       </c>
@@ -14105,11 +14105,11 @@
       <c r="U5" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="Y5" s="761" t="s">
+      <c r="Y5" s="768" t="s">
         <v>282</v>
       </c>
-      <c r="Z5" s="762"/>
-      <c r="AD5" s="753"/>
+      <c r="Z5" s="769"/>
+      <c r="AD5" s="760"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -14119,16 +14119,16 @@
       <c r="E6" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="G6" s="780"/>
+      <c r="G6" s="748"/>
       <c r="H6" s="46" t="s">
         <v>80</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="759"/>
-      <c r="L6" s="773"/>
-      <c r="O6" s="790"/>
+      <c r="K6" s="766"/>
+      <c r="L6" s="780"/>
+      <c r="O6" s="758"/>
       <c r="T6" s="2" t="s">
         <v>100</v>
       </c>
@@ -14138,23 +14138,23 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="753"/>
+      <c r="AD6" s="760"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="780"/>
+      <c r="G7" s="748"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="759"/>
-      <c r="L7" s="773"/>
+      <c r="K7" s="766"/>
+      <c r="L7" s="780"/>
       <c r="N7" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="O7" s="790"/>
+      <c r="O7" s="758"/>
       <c r="P7" s="73"/>
       <c r="U7" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="753"/>
+      <c r="AD7" s="760"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -14167,7 +14167,7 @@
       <c r="F8" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="G8" s="780"/>
+      <c r="G8" s="748"/>
       <c r="H8" s="50" t="s">
         <v>75</v>
       </c>
@@ -14177,41 +14177,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="759"/>
-      <c r="L8" s="773"/>
-      <c r="O8" s="790"/>
+      <c r="K8" s="766"/>
+      <c r="L8" s="780"/>
+      <c r="O8" s="758"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="755" t="s">
+      <c r="S8" s="762" t="s">
         <v>210</v>
       </c>
-      <c r="T8" s="756"/>
-      <c r="U8" s="756"/>
-      <c r="V8" s="756"/>
-      <c r="W8" s="756"/>
-      <c r="X8" s="756"/>
-      <c r="Y8" s="756"/>
-      <c r="Z8" s="756"/>
-      <c r="AA8" s="756"/>
-      <c r="AB8" s="756"/>
-      <c r="AC8" s="757"/>
-      <c r="AD8" s="753"/>
+      <c r="T8" s="763"/>
+      <c r="U8" s="763"/>
+      <c r="V8" s="763"/>
+      <c r="W8" s="763"/>
+      <c r="X8" s="763"/>
+      <c r="Y8" s="763"/>
+      <c r="Z8" s="763"/>
+      <c r="AA8" s="763"/>
+      <c r="AB8" s="763"/>
+      <c r="AC8" s="764"/>
+      <c r="AD8" s="760"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="745"/>
-      <c r="G9" s="780"/>
+      <c r="C9" s="784"/>
+      <c r="G9" s="748"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="759"/>
-      <c r="L9" s="783" t="s">
+      <c r="K9" s="766"/>
+      <c r="L9" s="751" t="s">
         <v>216</v>
       </c>
-      <c r="M9" s="784"/>
-      <c r="N9" s="785"/>
-      <c r="O9" s="790"/>
+      <c r="M9" s="752"/>
+      <c r="N9" s="753"/>
+      <c r="O9" s="758"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="753"/>
+      <c r="AD9" s="760"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="746"/>
+      <c r="C10" s="785"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>87</v>
@@ -14219,7 +14219,7 @@
       <c r="F10" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="G10" s="780"/>
+      <c r="G10" s="748"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>80</v>
@@ -14227,33 +14227,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="759"/>
-      <c r="M10" s="748" t="s">
+      <c r="K10" s="766"/>
+      <c r="M10" s="787" t="s">
         <v>89</v>
       </c>
-      <c r="N10" s="749"/>
-      <c r="O10" s="749"/>
-      <c r="P10" s="749"/>
-      <c r="Q10" s="749"/>
-      <c r="R10" s="749"/>
-      <c r="S10" s="749"/>
-      <c r="T10" s="749"/>
-      <c r="U10" s="749"/>
-      <c r="V10" s="749"/>
-      <c r="W10" s="749"/>
-      <c r="X10" s="749"/>
-      <c r="Y10" s="749"/>
-      <c r="Z10" s="749"/>
-      <c r="AA10" s="749"/>
-      <c r="AB10" s="749"/>
-      <c r="AC10" s="750"/>
-      <c r="AD10" s="753"/>
+      <c r="N10" s="788"/>
+      <c r="O10" s="788"/>
+      <c r="P10" s="788"/>
+      <c r="Q10" s="788"/>
+      <c r="R10" s="788"/>
+      <c r="S10" s="788"/>
+      <c r="T10" s="788"/>
+      <c r="U10" s="788"/>
+      <c r="V10" s="788"/>
+      <c r="W10" s="788"/>
+      <c r="X10" s="788"/>
+      <c r="Y10" s="788"/>
+      <c r="Z10" s="788"/>
+      <c r="AA10" s="788"/>
+      <c r="AB10" s="788"/>
+      <c r="AC10" s="789"/>
+      <c r="AD10" s="760"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="747"/>
-      <c r="G11" s="780"/>
+      <c r="C11" s="786"/>
+      <c r="G11" s="748"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="759"/>
+      <c r="K11" s="766"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -14261,17 +14261,17 @@
       <c r="Y11" s="68" t="s">
         <v>120</v>
       </c>
-      <c r="Z11" s="769" t="s">
+      <c r="Z11" s="776" t="s">
         <v>120</v>
       </c>
-      <c r="AA11" s="770"/>
+      <c r="AA11" s="777"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>120</v>
       </c>
-      <c r="AD11" s="753"/>
+      <c r="AD11" s="760"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -14284,7 +14284,7 @@
       <c r="F12" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="G12" s="780"/>
+      <c r="G12" s="748"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>80</v>
@@ -14292,8 +14292,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="759"/>
-      <c r="L12" s="774" t="s">
+      <c r="K12" s="766"/>
+      <c r="L12" s="781" t="s">
         <v>92</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -14324,25 +14324,25 @@
         <v>115</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="763" t="s">
+      <c r="AA12" s="770" t="s">
         <v>125</v>
       </c>
-      <c r="AB12" s="764"/>
+      <c r="AB12" s="771"/>
       <c r="AC12" s="21" t="s">
         <v>230</v>
       </c>
-      <c r="AD12" s="753"/>
+      <c r="AD12" s="760"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="745"/>
-      <c r="G13" s="780"/>
-      <c r="K13" s="759"/>
-      <c r="L13" s="775"/>
+      <c r="C13" s="784"/>
+      <c r="G13" s="748"/>
+      <c r="K13" s="766"/>
+      <c r="L13" s="782"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="782" t="s">
+      <c r="Q13" s="750" t="s">
         <v>208</v>
       </c>
-      <c r="R13" s="644"/>
+      <c r="R13" s="639"/>
       <c r="S13" s="599"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
@@ -14351,17 +14351,17 @@
       <c r="X13" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="AA13" s="765"/>
-      <c r="AB13" s="766"/>
-      <c r="AD13" s="753"/>
+      <c r="AA13" s="772"/>
+      <c r="AB13" s="773"/>
+      <c r="AD13" s="760"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="C14" s="747"/>
+      <c r="C14" s="786"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="780"/>
+      <c r="G14" s="748"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -14369,8 +14369,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="759"/>
-      <c r="L14" s="775"/>
+      <c r="K14" s="766"/>
+      <c r="L14" s="782"/>
       <c r="M14" s="21" t="s">
         <v>110</v>
       </c>
@@ -14391,9 +14391,9 @@
       <c r="Y14" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="AA14" s="765"/>
-      <c r="AB14" s="766"/>
-      <c r="AD14" s="753"/>
+      <c r="AA14" s="772"/>
+      <c r="AB14" s="773"/>
+      <c r="AD14" s="760"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -14408,19 +14408,19 @@
       <c r="F15" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="G15" s="780"/>
+      <c r="G15" s="748"/>
       <c r="H15" s="2" t="s">
         <v>80</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="K15" s="759"/>
-      <c r="L15" s="776"/>
-      <c r="Q15" s="782" t="s">
+      <c r="K15" s="766"/>
+      <c r="L15" s="783"/>
+      <c r="Q15" s="750" t="s">
         <v>209</v>
       </c>
-      <c r="R15" s="644"/>
+      <c r="R15" s="639"/>
       <c r="S15" s="599"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
@@ -14429,14 +14429,14 @@
       <c r="X15" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="AA15" s="765"/>
-      <c r="AB15" s="766"/>
-      <c r="AD15" s="753"/>
+      <c r="AA15" s="772"/>
+      <c r="AB15" s="773"/>
+      <c r="AD15" s="760"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="780"/>
-      <c r="K16" s="759"/>
+      <c r="G16" s="748"/>
+      <c r="K16" s="766"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>108</v>
@@ -14455,24 +14455,24 @@
       <c r="Z16" s="76" t="s">
         <v>126</v>
       </c>
-      <c r="AA16" s="765"/>
-      <c r="AB16" s="766"/>
-      <c r="AD16" s="753"/>
+      <c r="AA16" s="772"/>
+      <c r="AB16" s="773"/>
+      <c r="AD16" s="760"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F17" s="777" t="s">
+      <c r="F17" s="745" t="s">
         <v>95</v>
       </c>
-      <c r="G17" s="780"/>
+      <c r="G17" s="748"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>80</v>
       </c>
-      <c r="K17" s="759"/>
+      <c r="K17" s="766"/>
       <c r="S17" s="599"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
@@ -14480,9 +14480,9 @@
       <c r="X17" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA17" s="765"/>
-      <c r="AB17" s="766"/>
-      <c r="AD17" s="753"/>
+      <c r="AA17" s="772"/>
+      <c r="AB17" s="773"/>
+      <c r="AD17" s="760"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -14492,15 +14492,15 @@
       <c r="E18" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F18" s="778"/>
-      <c r="G18" s="780"/>
+      <c r="F18" s="746"/>
+      <c r="G18" s="748"/>
       <c r="H18" s="108" t="s">
         <v>75</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="K18" s="759"/>
+      <c r="K18" s="766"/>
       <c r="O18" s="64" t="s">
         <v>114</v>
       </c>
@@ -14511,42 +14511,39 @@
       <c r="X18" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AA18" s="767"/>
-      <c r="AB18" s="768"/>
-      <c r="AD18" s="753"/>
+      <c r="AA18" s="774"/>
+      <c r="AB18" s="775"/>
+      <c r="AD18" s="760"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>207</v>
       </c>
-      <c r="G19" s="781"/>
-      <c r="K19" s="760"/>
+      <c r="G19" s="749"/>
+      <c r="K19" s="767"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="786" t="s">
+      <c r="R19" s="754" t="s">
         <v>123</v>
       </c>
-      <c r="S19" s="787"/>
-      <c r="T19" s="788"/>
+      <c r="S19" s="755"/>
+      <c r="T19" s="756"/>
       <c r="V19" s="77" t="s">
         <v>114</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="AD19" s="754"/>
+      <c r="AD19" s="761"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G19"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="S12:S18"/>
-    <mergeCell ref="O3:O9"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="M10:AC10"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="AD1:AD19"/>
     <mergeCell ref="S8:AC8"/>
     <mergeCell ref="K5:K19"/>
@@ -14558,11 +14555,14 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L12:L15"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="M10:AC10"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="S12:S18"/>
+    <mergeCell ref="O3:O9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rw Usage Updates S.1.0.0.6 _9:25PM
Boat Enabled -
InCapacity - [0] , NodeW - [-3] , BirdW - [6] , FuelW - [20] , OnHost - [8+1]
VillageW=[5]
Rw - Local(Left Running With Cost ) - [For Business/Shop/Market only] -
</commit_message>
<xml_diff>
--- a/System_2.2.1.xlsx
+++ b/System_2.2.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CB210D-0CCB-4866-957F-AC8ED217F24F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C266F1AC-FDBA-48C9-95C8-E99486AF06F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BoardRW" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="623">
   <si>
     <t>Zone</t>
   </si>
@@ -1905,9 +1905,6 @@
   </si>
   <si>
     <t>TaiwanNews</t>
-  </si>
-  <si>
-    <t>7F in Capacity</t>
   </si>
   <si>
     <t>bharat24</t>
@@ -5027,6 +5024,159 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5045,12 +5195,6 @@
     <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5105,169 +5249,61 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5309,43 +5345,70 @@
     <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="52" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="52" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="14" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5369,112 +5432,25 @@
     <xf numFmtId="0" fontId="29" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="52" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="52" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="14" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5552,25 +5528,46 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5868,8 +5865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:X28"/>
   <sheetViews>
-    <sheetView topLeftCell="C9" workbookViewId="0">
-      <selection activeCell="V26" sqref="V26"/>
+    <sheetView tabSelected="1" topLeftCell="C9" workbookViewId="0">
+      <selection activeCell="X13" sqref="X13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6592,9 +6589,7 @@
       </c>
       <c r="P22" s="313"/>
       <c r="T22" s="607"/>
-      <c r="X22" s="2" t="s">
-        <v>622</v>
-      </c>
+      <c r="X22" s="2"/>
     </row>
     <row r="23" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
@@ -6903,7 +6898,7 @@
       <c r="H1" s="97" t="s">
         <v>343</v>
       </c>
-      <c r="I1" s="659" t="s">
+      <c r="I1" s="613" t="s">
         <v>369</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -6939,7 +6934,7 @@
       <c r="X1" s="430" t="s">
         <v>155</v>
       </c>
-      <c r="Y1" s="653" t="s">
+      <c r="Y1" s="657" t="s">
         <v>528</v>
       </c>
       <c r="Z1" s="406">
@@ -6964,7 +6959,7 @@
         <v>498</v>
       </c>
       <c r="AM1" s="402"/>
-      <c r="AN1" s="635"/>
+      <c r="AN1" s="640"/>
       <c r="AO1" s="338" t="s">
         <v>469</v>
       </c>
@@ -6973,23 +6968,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="617">
+      <c r="A2" s="666">
         <f ca="1">TODAY()</f>
         <v>45291</v>
       </c>
-      <c r="B2" s="619" t="s">
+      <c r="B2" s="668" t="s">
         <v>370</v>
       </c>
-      <c r="C2" s="615" t="s">
+      <c r="C2" s="645" t="s">
         <v>357</v>
       </c>
-      <c r="D2" s="621" t="s">
+      <c r="D2" s="670" t="s">
         <v>355</v>
       </c>
-      <c r="E2" s="669" t="s">
+      <c r="E2" s="609" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="640" t="s">
+      <c r="F2" s="619" t="s">
         <v>102</v>
       </c>
       <c r="G2" s="393" t="s">
@@ -6998,31 +6993,31 @@
       <c r="H2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="660"/>
+      <c r="I2" s="614"/>
       <c r="J2" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="671" t="s">
+      <c r="K2" s="611" t="s">
         <v>342</v>
       </c>
-      <c r="L2" s="672"/>
-      <c r="M2" s="640" t="s">
+      <c r="L2" s="612"/>
+      <c r="M2" s="619" t="s">
         <v>102</v>
       </c>
       <c r="N2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="644" t="s">
+      <c r="O2" s="649" t="s">
         <v>102</v>
       </c>
       <c r="P2" s="85" t="s">
         <v>147</v>
       </c>
-      <c r="Q2" s="615" t="s">
+      <c r="Q2" s="645" t="s">
         <v>143</v>
       </c>
       <c r="R2" s="598"/>
-      <c r="S2" s="657" t="s">
+      <c r="S2" s="634" t="s">
         <v>148</v>
       </c>
       <c r="T2" s="89"/>
@@ -7032,7 +7027,7 @@
       <c r="X2" s="431" t="s">
         <v>156</v>
       </c>
-      <c r="Y2" s="654"/>
+      <c r="Y2" s="658"/>
       <c r="Z2" s="407">
         <v>1</v>
       </c>
@@ -7055,15 +7050,15 @@
         <v>463</v>
       </c>
       <c r="AM2" s="428"/>
-      <c r="AN2" s="636"/>
+      <c r="AN2" s="641"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="618"/>
-      <c r="B3" s="620"/>
-      <c r="C3" s="616"/>
-      <c r="D3" s="622"/>
-      <c r="E3" s="670"/>
-      <c r="F3" s="641"/>
+      <c r="A3" s="667"/>
+      <c r="B3" s="669"/>
+      <c r="C3" s="646"/>
+      <c r="D3" s="671"/>
+      <c r="E3" s="610"/>
+      <c r="F3" s="620"/>
       <c r="G3" s="394" t="s">
         <v>28</v>
       </c>
@@ -7082,17 +7077,17 @@
       <c r="L3" s="201" t="s">
         <v>107</v>
       </c>
-      <c r="M3" s="641"/>
+      <c r="M3" s="620"/>
       <c r="N3" s="69" t="s">
         <v>146</v>
       </c>
-      <c r="O3" s="645"/>
+      <c r="O3" s="650"/>
       <c r="P3" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="Q3" s="616"/>
+      <c r="Q3" s="646"/>
       <c r="R3" s="600"/>
-      <c r="S3" s="658"/>
+      <c r="S3" s="636"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -7100,7 +7095,7 @@
       <c r="X3" s="431" t="s">
         <v>157</v>
       </c>
-      <c r="Y3" s="654"/>
+      <c r="Y3" s="658"/>
       <c r="Z3" s="408">
         <v>1</v>
       </c>
@@ -7109,7 +7104,7 @@
       <c r="AC3" s="100" t="s">
         <v>480</v>
       </c>
-      <c r="AD3" s="656" t="s">
+      <c r="AD3" s="631" t="s">
         <v>455</v>
       </c>
       <c r="AE3" s="257"/>
@@ -7121,16 +7116,16 @@
       <c r="AK3" s="257"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="428"/>
-      <c r="AN3" s="636"/>
+      <c r="AN3" s="641"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="238" t="s">
         <v>183</v>
       </c>
-      <c r="B4" s="633" t="s">
+      <c r="B4" s="682" t="s">
         <v>373</v>
       </c>
-      <c r="C4" s="615" t="s">
+      <c r="C4" s="645" t="s">
         <v>154</v>
       </c>
       <c r="D4" s="347" t="s">
@@ -7139,7 +7134,7 @@
       <c r="E4" s="378">
         <v>2</v>
       </c>
-      <c r="F4" s="641"/>
+      <c r="F4" s="620"/>
       <c r="G4" s="381" t="s">
         <v>201</v>
       </c>
@@ -7156,11 +7151,11 @@
         <v>150</v>
       </c>
       <c r="L4" s="204"/>
-      <c r="M4" s="641"/>
+      <c r="M4" s="620"/>
       <c r="N4" s="174" t="s">
         <v>69</v>
       </c>
-      <c r="O4" s="645"/>
+      <c r="O4" s="650"/>
       <c r="P4" s="2" t="s">
         <v>191</v>
       </c>
@@ -7182,12 +7177,12 @@
       <c r="X4" s="431" t="s">
         <v>158</v>
       </c>
-      <c r="Y4" s="654"/>
+      <c r="Y4" s="658"/>
       <c r="Z4" s="409"/>
       <c r="AA4" s="307"/>
       <c r="AB4" s="209"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="656"/>
+      <c r="AD4" s="631"/>
       <c r="AE4" s="257"/>
       <c r="AF4" s="257"/>
       <c r="AG4" s="16"/>
@@ -7197,37 +7192,37 @@
       <c r="AK4" s="257"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="428"/>
-      <c r="AN4" s="636"/>
+      <c r="AN4" s="641"/>
       <c r="AO4" s="338" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="659" t="s">
+      <c r="A5" s="613" t="s">
         <v>418</v>
       </c>
-      <c r="B5" s="634"/>
-      <c r="C5" s="616"/>
+      <c r="B5" s="683"/>
+      <c r="C5" s="646"/>
       <c r="D5" s="61" t="s">
         <v>153</v>
       </c>
       <c r="E5" s="379">
         <v>1</v>
       </c>
-      <c r="F5" s="641"/>
-      <c r="G5" s="625" t="s">
+      <c r="F5" s="620"/>
+      <c r="G5" s="674" t="s">
         <v>192</v>
       </c>
-      <c r="H5" s="625"/>
-      <c r="I5" s="625"/>
-      <c r="J5" s="625"/>
-      <c r="K5" s="625"/>
-      <c r="L5" s="626"/>
-      <c r="M5" s="641"/>
+      <c r="H5" s="674"/>
+      <c r="I5" s="674"/>
+      <c r="J5" s="674"/>
+      <c r="K5" s="674"/>
+      <c r="L5" s="675"/>
+      <c r="M5" s="620"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
-      <c r="O5" s="645"/>
+      <c r="O5" s="650"/>
       <c r="T5" s="89"/>
       <c r="U5" s="124"/>
       <c r="V5" s="120"/>
@@ -7235,7 +7230,7 @@
       <c r="X5" s="431" t="s">
         <v>159</v>
       </c>
-      <c r="Y5" s="654"/>
+      <c r="Y5" s="658"/>
       <c r="Z5" s="409">
         <v>1</v>
       </c>
@@ -7258,24 +7253,24 @@
       <c r="AK5" s="257"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="428"/>
-      <c r="AN5" s="636"/>
+      <c r="AN5" s="641"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="660"/>
-      <c r="B6" s="631" t="s">
+      <c r="A6" s="614"/>
+      <c r="B6" s="680" t="s">
         <v>177</v>
       </c>
-      <c r="C6" s="661"/>
-      <c r="D6" s="662"/>
-      <c r="F6" s="641"/>
-      <c r="G6" s="627"/>
-      <c r="H6" s="627"/>
-      <c r="I6" s="627"/>
-      <c r="J6" s="627"/>
-      <c r="K6" s="627"/>
-      <c r="L6" s="628"/>
-      <c r="M6" s="641"/>
-      <c r="O6" s="645"/>
+      <c r="C6" s="628"/>
+      <c r="D6" s="629"/>
+      <c r="F6" s="620"/>
+      <c r="G6" s="676"/>
+      <c r="H6" s="676"/>
+      <c r="I6" s="676"/>
+      <c r="J6" s="676"/>
+      <c r="K6" s="676"/>
+      <c r="L6" s="677"/>
+      <c r="M6" s="620"/>
+      <c r="O6" s="650"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
       <c r="V6" s="98" t="s">
@@ -7285,7 +7280,7 @@
       <c r="X6" s="431" t="s">
         <v>160</v>
       </c>
-      <c r="Y6" s="654"/>
+      <c r="Y6" s="658"/>
       <c r="Z6" s="407">
         <v>1</v>
       </c>
@@ -7299,16 +7294,16 @@
       <c r="AF6" s="257"/>
       <c r="AG6" s="257"/>
       <c r="AH6" s="257"/>
-      <c r="AI6" s="650"/>
+      <c r="AI6" s="630"/>
       <c r="AJ6" s="441" t="s">
         <v>458</v>
       </c>
-      <c r="AK6" s="650" t="s">
+      <c r="AK6" s="630" t="s">
         <v>251</v>
       </c>
       <c r="AL6" s="257"/>
       <c r="AM6" s="428"/>
-      <c r="AN6" s="636"/>
+      <c r="AN6" s="641"/>
       <c r="AO6" s="338" t="s">
         <v>470</v>
       </c>
@@ -7317,7 +7312,7 @@
       <c r="A7" s="232" t="s">
         <v>571</v>
       </c>
-      <c r="B7" s="632"/>
+      <c r="B7" s="681"/>
       <c r="C7" s="202" t="s">
         <v>374</v>
       </c>
@@ -7327,7 +7322,7 @@
       <c r="E7" s="265">
         <v>3</v>
       </c>
-      <c r="F7" s="641"/>
+      <c r="F7" s="620"/>
       <c r="G7" s="395">
         <v>0</v>
       </c>
@@ -7346,8 +7341,8 @@
       <c r="L7" s="212">
         <v>0</v>
       </c>
-      <c r="M7" s="641"/>
-      <c r="O7" s="645"/>
+      <c r="M7" s="620"/>
+      <c r="O7" s="650"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
       </c>
@@ -7361,7 +7356,7 @@
       <c r="X7" s="431" t="s">
         <v>161</v>
       </c>
-      <c r="Y7" s="654"/>
+      <c r="Y7" s="658"/>
       <c r="Z7" s="407">
         <v>1</v>
       </c>
@@ -7371,18 +7366,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="257"/>
       <c r="AF7" s="257"/>
-      <c r="AG7" s="656" t="s">
+      <c r="AG7" s="631" t="s">
         <v>454</v>
       </c>
       <c r="AH7" s="257"/>
-      <c r="AI7" s="650"/>
+      <c r="AI7" s="630"/>
       <c r="AJ7" s="257"/>
-      <c r="AK7" s="650"/>
+      <c r="AK7" s="630"/>
       <c r="AL7" s="80" t="s">
         <v>496</v>
       </c>
       <c r="AM7" s="428"/>
-      <c r="AN7" s="636"/>
+      <c r="AN7" s="641"/>
       <c r="AP7" s="76" t="s">
         <v>471</v>
       </c>
@@ -7399,27 +7394,27 @@
         <f>SUM(G7:N9)</f>
         <v>15</v>
       </c>
-      <c r="F8" s="641"/>
-      <c r="G8" s="626">
-        <v>0</v>
-      </c>
-      <c r="H8" s="623" t="s">
+      <c r="F8" s="620"/>
+      <c r="G8" s="675">
+        <v>0</v>
+      </c>
+      <c r="H8" s="672" t="s">
         <v>104</v>
       </c>
       <c r="I8" s="598">
         <v>0</v>
       </c>
-      <c r="J8" s="623" t="s">
+      <c r="J8" s="672" t="s">
         <v>104</v>
       </c>
-      <c r="K8" s="629"/>
-      <c r="L8" s="663"/>
-      <c r="M8" s="642"/>
-      <c r="N8" s="666">
+      <c r="K8" s="678"/>
+      <c r="L8" s="632"/>
+      <c r="M8" s="647"/>
+      <c r="N8" s="637">
         <f>N5+N11</f>
         <v>15</v>
       </c>
-      <c r="O8" s="645"/>
+      <c r="O8" s="650"/>
       <c r="T8" s="103" t="s">
         <v>44</v>
       </c>
@@ -7429,7 +7424,7 @@
       <c r="X8" s="431" t="s">
         <v>162</v>
       </c>
-      <c r="Y8" s="654"/>
+      <c r="Y8" s="658"/>
       <c r="Z8" s="409"/>
       <c r="AA8" s="307"/>
       <c r="AB8" s="209"/>
@@ -7437,14 +7432,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="257"/>
       <c r="AF8" s="257"/>
-      <c r="AG8" s="656"/>
+      <c r="AG8" s="631"/>
       <c r="AH8" s="257"/>
-      <c r="AI8" s="650"/>
+      <c r="AI8" s="630"/>
       <c r="AJ8" s="257"/>
       <c r="AK8" s="257"/>
       <c r="AL8" s="257"/>
       <c r="AM8" s="428"/>
-      <c r="AN8" s="636"/>
+      <c r="AN8" s="641"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="232" t="s">
@@ -7459,17 +7454,17 @@
       <c r="D9" s="348" t="s">
         <v>281</v>
       </c>
-      <c r="F9" s="641"/>
-      <c r="G9" s="628"/>
-      <c r="H9" s="624"/>
+      <c r="F9" s="620"/>
+      <c r="G9" s="677"/>
+      <c r="H9" s="673"/>
       <c r="I9" s="600"/>
-      <c r="J9" s="624"/>
-      <c r="K9" s="630"/>
-      <c r="L9" s="664"/>
-      <c r="M9" s="643"/>
-      <c r="N9" s="667"/>
-      <c r="O9" s="646"/>
-      <c r="S9" s="657" t="s">
+      <c r="J9" s="673"/>
+      <c r="K9" s="679"/>
+      <c r="L9" s="633"/>
+      <c r="M9" s="648"/>
+      <c r="N9" s="638"/>
+      <c r="O9" s="651"/>
+      <c r="S9" s="634" t="s">
         <v>61</v>
       </c>
       <c r="T9" s="89"/>
@@ -7481,7 +7476,7 @@
       <c r="X9" s="431" t="s">
         <v>163</v>
       </c>
-      <c r="Y9" s="654"/>
+      <c r="Y9" s="658"/>
       <c r="Z9" s="410"/>
       <c r="AA9" s="307"/>
       <c r="AB9" s="209"/>
@@ -7491,16 +7486,16 @@
       </c>
       <c r="AE9" s="257"/>
       <c r="AF9" s="257"/>
-      <c r="AG9" s="656"/>
+      <c r="AG9" s="631"/>
       <c r="AH9" s="257"/>
-      <c r="AI9" s="650"/>
+      <c r="AI9" s="630"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="650" t="s">
+      <c r="AK9" s="630" t="s">
         <v>251</v>
       </c>
       <c r="AL9" s="257"/>
       <c r="AM9" s="428"/>
-      <c r="AN9" s="636"/>
+      <c r="AN9" s="641"/>
       <c r="AP9" s="2" t="s">
         <v>508</v>
       </c>
@@ -7517,20 +7512,20 @@
         <f>Boat!W8</f>
         <v>37</v>
       </c>
-      <c r="F10" s="641"/>
+      <c r="F10" s="620"/>
       <c r="N10" s="418" t="s">
         <v>396</v>
       </c>
-      <c r="O10" s="678" t="s">
+      <c r="O10" s="622" t="s">
         <v>102</v>
       </c>
-      <c r="P10" s="647" t="s">
+      <c r="P10" s="652" t="s">
         <v>400</v>
       </c>
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="665"/>
+      <c r="S10" s="635"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>176</v>
@@ -7542,7 +7537,7 @@
       <c r="X10" s="431" t="s">
         <v>164</v>
       </c>
-      <c r="Y10" s="654"/>
+      <c r="Y10" s="658"/>
       <c r="Z10" s="409">
         <v>0</v>
       </c>
@@ -7560,16 +7555,16 @@
       <c r="AF10" s="238" t="s">
         <v>311</v>
       </c>
-      <c r="AG10" s="656"/>
+      <c r="AG10" s="631"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="650"/>
+      <c r="AI10" s="630"/>
       <c r="AJ10" s="257"/>
-      <c r="AK10" s="650"/>
+      <c r="AK10" s="630"/>
       <c r="AL10" s="257"/>
       <c r="AM10" s="442" t="s">
         <v>318</v>
       </c>
-      <c r="AN10" s="636"/>
+      <c r="AN10" s="641"/>
       <c r="AO10" s="204" t="s">
         <v>94</v>
       </c>
@@ -7587,18 +7582,18 @@
       <c r="D11" s="170" t="s">
         <v>355</v>
       </c>
-      <c r="F11" s="641"/>
+      <c r="F11" s="620"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="679"/>
-      <c r="P11" s="648"/>
+      <c r="O11" s="623"/>
+      <c r="P11" s="653"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>220</v>
       </c>
-      <c r="S11" s="665"/>
+      <c r="S11" s="635"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -7608,7 +7603,7 @@
       <c r="X11" s="431" t="s">
         <v>165</v>
       </c>
-      <c r="Y11" s="654"/>
+      <c r="Y11" s="658"/>
       <c r="Z11" s="409"/>
       <c r="AA11" s="307">
         <v>1</v>
@@ -7622,14 +7617,14 @@
       <c r="AF11" s="257" t="s">
         <v>476</v>
       </c>
-      <c r="AG11" s="656"/>
+      <c r="AG11" s="631"/>
       <c r="AH11" s="257"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="257"/>
       <c r="AK11" s="257"/>
       <c r="AL11" s="257"/>
       <c r="AM11" s="428"/>
-      <c r="AN11" s="636"/>
+      <c r="AN11" s="641"/>
       <c r="AP11" s="76" t="s">
         <v>484</v>
       </c>
@@ -7648,7 +7643,7 @@
       <c r="E12" s="224">
         <v>3</v>
       </c>
-      <c r="F12" s="641"/>
+      <c r="F12" s="620"/>
       <c r="G12" s="337" t="s">
         <v>400</v>
       </c>
@@ -7657,16 +7652,16 @@
       </c>
       <c r="I12" s="605"/>
       <c r="J12" s="605"/>
-      <c r="K12" s="683"/>
+      <c r="K12" s="627"/>
       <c r="L12" s="203"/>
       <c r="M12" s="203"/>
       <c r="N12" s="203"/>
-      <c r="O12" s="679"/>
-      <c r="P12" s="648"/>
+      <c r="O12" s="623"/>
+      <c r="P12" s="653"/>
       <c r="R12" s="122" t="s">
         <v>180</v>
       </c>
-      <c r="S12" s="658"/>
+      <c r="S12" s="636"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -7676,7 +7671,7 @@
       <c r="X12" s="431" t="s">
         <v>166</v>
       </c>
-      <c r="Y12" s="654"/>
+      <c r="Y12" s="658"/>
       <c r="Z12" s="407">
         <v>1</v>
       </c>
@@ -7687,16 +7682,16 @@
       <c r="AC12" s="100" t="s">
         <v>481</v>
       </c>
-      <c r="AD12" s="668" t="s">
+      <c r="AD12" s="639" t="s">
         <v>240</v>
       </c>
       <c r="AE12" s="441" t="s">
         <v>239</v>
       </c>
-      <c r="AF12" s="656" t="s">
+      <c r="AF12" s="631" t="s">
         <v>228</v>
       </c>
-      <c r="AG12" s="656"/>
+      <c r="AG12" s="631"/>
       <c r="AH12" s="238" t="s">
         <v>259</v>
       </c>
@@ -7706,10 +7701,10 @@
       <c r="AJ12" s="257"/>
       <c r="AK12" s="257"/>
       <c r="AL12" s="257"/>
-      <c r="AM12" s="651" t="s">
+      <c r="AM12" s="655" t="s">
         <v>249</v>
       </c>
-      <c r="AN12" s="636"/>
+      <c r="AN12" s="641"/>
       <c r="AO12" s="338" t="s">
         <v>96</v>
       </c>
@@ -7721,17 +7716,17 @@
       <c r="E13" s="448">
         <v>-3</v>
       </c>
-      <c r="F13" s="641"/>
+      <c r="F13" s="620"/>
       <c r="G13" s="605" t="s">
         <v>430</v>
       </c>
       <c r="H13" s="605"/>
       <c r="I13" s="605"/>
-      <c r="J13" s="683"/>
+      <c r="J13" s="627"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="679"/>
-      <c r="P13" s="649"/>
+      <c r="O13" s="623"/>
+      <c r="P13" s="654"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
       </c>
@@ -7741,7 +7736,7 @@
       <c r="X13" s="431" t="s">
         <v>167</v>
       </c>
-      <c r="Y13" s="654"/>
+      <c r="Y13" s="658"/>
       <c r="Z13" s="407">
         <v>1</v>
       </c>
@@ -7752,8 +7747,8 @@
         <v>500</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="668"/>
-      <c r="AF13" s="656"/>
+      <c r="AD13" s="639"/>
+      <c r="AF13" s="631"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="238" t="s">
         <v>308</v>
@@ -7764,8 +7759,8 @@
       <c r="AJ13" s="80"/>
       <c r="AK13" s="257"/>
       <c r="AL13" s="257"/>
-      <c r="AM13" s="651"/>
-      <c r="AN13" s="636"/>
+      <c r="AM13" s="655"/>
+      <c r="AN13" s="641"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="450"/>
@@ -7773,18 +7768,18 @@
       <c r="C14" s="459"/>
       <c r="D14" s="452"/>
       <c r="E14" s="453"/>
-      <c r="F14" s="641"/>
+      <c r="F14" s="620"/>
       <c r="G14" s="605" t="s">
         <v>429</v>
       </c>
       <c r="H14" s="605"/>
       <c r="I14" s="605"/>
-      <c r="J14" s="683"/>
+      <c r="J14" s="627"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="679"/>
+      <c r="O14" s="623"/>
       <c r="Q14" s="61" t="s">
         <v>532</v>
       </c>
@@ -7798,24 +7793,24 @@
       <c r="X14" s="431" t="s">
         <v>168</v>
       </c>
-      <c r="Y14" s="654"/>
+      <c r="Y14" s="658"/>
       <c r="Z14" s="407">
         <v>1</v>
       </c>
       <c r="AA14" s="307"/>
       <c r="AB14" s="209"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="668"/>
+      <c r="AD14" s="639"/>
       <c r="AE14" s="257"/>
-      <c r="AF14" s="656"/>
+      <c r="AF14" s="631"/>
       <c r="AG14" s="257"/>
       <c r="AH14" s="257"/>
       <c r="AI14" s="70"/>
       <c r="AJ14" s="257"/>
       <c r="AK14" s="257"/>
       <c r="AL14" s="257"/>
-      <c r="AM14" s="651"/>
-      <c r="AN14" s="636"/>
+      <c r="AM14" s="655"/>
+      <c r="AN14" s="641"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="449" t="s">
@@ -7824,8 +7819,8 @@
       <c r="C15" s="598" t="s">
         <v>373</v>
       </c>
-      <c r="F15" s="641"/>
-      <c r="O15" s="679"/>
+      <c r="F15" s="620"/>
+      <c r="O15" s="623"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -7838,7 +7833,7 @@
       <c r="X15" s="431" t="s">
         <v>169</v>
       </c>
-      <c r="Y15" s="654"/>
+      <c r="Y15" s="658"/>
       <c r="Z15" s="409">
         <v>1</v>
       </c>
@@ -7847,8 +7842,8 @@
       <c r="AC15" s="76" t="s">
         <v>479</v>
       </c>
-      <c r="AD15" s="668"/>
-      <c r="AF15" s="656"/>
+      <c r="AD15" s="639"/>
+      <c r="AF15" s="631"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="238" t="s">
         <v>448</v>
@@ -7861,8 +7856,8 @@
       </c>
       <c r="AK15" s="257"/>
       <c r="AL15" s="257"/>
-      <c r="AM15" s="651"/>
-      <c r="AN15" s="636"/>
+      <c r="AM15" s="655"/>
+      <c r="AN15" s="641"/>
       <c r="AP15" s="76" t="s">
         <v>73</v>
       </c>
@@ -7884,13 +7879,13 @@
       <c r="E16" s="224">
         <v>1</v>
       </c>
-      <c r="F16" s="641"/>
+      <c r="F16" s="620"/>
       <c r="G16" s="337" t="s">
         <v>488</v>
       </c>
       <c r="I16" s="469"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="679"/>
+      <c r="O16" s="623"/>
       <c r="R16" s="435" t="s">
         <v>184</v>
       </c>
@@ -7901,7 +7896,7 @@
       <c r="X16" s="431" t="s">
         <v>170</v>
       </c>
-      <c r="Y16" s="654"/>
+      <c r="Y16" s="658"/>
       <c r="Z16" s="407">
         <v>1</v>
       </c>
@@ -7922,18 +7917,18 @@
       <c r="AM16" s="428" t="s">
         <v>317</v>
       </c>
-      <c r="AN16" s="636"/>
+      <c r="AN16" s="641"/>
       <c r="AP16" s="76" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="641"/>
+      <c r="F17" s="620"/>
       <c r="I17" s="470"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="679"/>
+      <c r="O17" s="623"/>
       <c r="Q17" s="21" t="s">
         <v>530</v>
       </c>
@@ -7953,7 +7948,7 @@
       <c r="X17" s="431" t="s">
         <v>171</v>
       </c>
-      <c r="Y17" s="654"/>
+      <c r="Y17" s="658"/>
       <c r="Z17" s="409"/>
       <c r="AA17" s="307"/>
       <c r="AB17" s="209"/>
@@ -7978,7 +7973,7 @@
       <c r="AK17" s="257"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="428"/>
-      <c r="AN17" s="636"/>
+      <c r="AN17" s="641"/>
       <c r="AO17" s="204" t="s">
         <v>497</v>
       </c>
@@ -8002,21 +7997,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="641"/>
+      <c r="F18" s="620"/>
       <c r="G18" s="337" t="s">
         <v>527</v>
       </c>
       <c r="I18" s="24"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="679"/>
+      <c r="O18" s="623"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="673" t="s">
+      <c r="R18" s="615" t="s">
         <v>535</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="612" t="s">
+      <c r="U18" s="663" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -8026,7 +8021,7 @@
       <c r="X18" s="431" t="s">
         <v>172</v>
       </c>
-      <c r="Y18" s="654"/>
+      <c r="Y18" s="658"/>
       <c r="Z18" s="409">
         <v>1</v>
       </c>
@@ -8037,38 +8032,38 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="257"/>
-      <c r="AF18" s="650" t="s">
+      <c r="AF18" s="630" t="s">
         <v>475</v>
       </c>
       <c r="AG18" s="257"/>
       <c r="AH18" s="70"/>
       <c r="AI18" s="70"/>
-      <c r="AJ18" s="652" t="s">
+      <c r="AJ18" s="656" t="s">
         <v>315</v>
       </c>
       <c r="AK18" s="257"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="428"/>
-      <c r="AN18" s="636"/>
+      <c r="AN18" s="641"/>
       <c r="AP18" s="76" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="641"/>
+      <c r="F19" s="620"/>
       <c r="I19" s="219"/>
-      <c r="O19" s="679"/>
-      <c r="R19" s="674"/>
+      <c r="O19" s="623"/>
+      <c r="R19" s="616"/>
       <c r="S19" s="30" t="s">
         <v>533</v>
       </c>
-      <c r="U19" s="613"/>
+      <c r="U19" s="664"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="431" t="s">
         <v>173</v>
       </c>
-      <c r="Y19" s="654"/>
+      <c r="Y19" s="658"/>
       <c r="Z19" s="407">
         <v>1</v>
       </c>
@@ -8077,17 +8072,17 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="257"/>
-      <c r="AF19" s="650"/>
+      <c r="AF19" s="630"/>
       <c r="AG19" s="257"/>
       <c r="AH19" s="257"/>
       <c r="AI19" s="70"/>
-      <c r="AJ19" s="652"/>
+      <c r="AJ19" s="656"/>
       <c r="AK19" s="460" t="s">
         <v>251</v>
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="428"/>
-      <c r="AN19" s="636"/>
+      <c r="AN19" s="641"/>
       <c r="AP19" s="76" t="s">
         <v>468</v>
       </c>
@@ -8108,24 +8103,24 @@
       <c r="E20" s="437">
         <v>-1</v>
       </c>
-      <c r="F20" s="641"/>
+      <c r="F20" s="620"/>
       <c r="G20" s="337" t="s">
         <v>491</v>
       </c>
       <c r="I20" s="219"/>
-      <c r="O20" s="679"/>
-      <c r="Q20" s="681" t="s">
+      <c r="O20" s="623"/>
+      <c r="Q20" s="625" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="404" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="614"/>
+      <c r="U20" s="665"/>
       <c r="W20" s="405"/>
       <c r="X20" s="432" t="s">
         <v>174</v>
       </c>
-      <c r="Y20" s="654"/>
+      <c r="Y20" s="658"/>
       <c r="Z20" s="411">
         <v>1</v>
       </c>
@@ -8150,7 +8145,7 @@
       <c r="AM20" s="381" t="s">
         <v>249</v>
       </c>
-      <c r="AN20" s="636"/>
+      <c r="AN20" s="641"/>
       <c r="AO20" s="338" t="s">
         <v>460</v>
       </c>
@@ -8171,20 +8166,20 @@
       <c r="E21" s="265">
         <v>0</v>
       </c>
-      <c r="F21" s="641"/>
+      <c r="F21" s="620"/>
       <c r="I21" s="219"/>
-      <c r="O21" s="679"/>
-      <c r="Q21" s="682"/>
+      <c r="O21" s="623"/>
+      <c r="Q21" s="626"/>
       <c r="T21" s="422"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="609"/>
+      <c r="V21" s="660"/>
       <c r="W21" s="426" t="s">
         <v>175</v>
       </c>
       <c r="X21" s="429" t="s">
         <v>186</v>
       </c>
-      <c r="Y21" s="654"/>
+      <c r="Y21" s="658"/>
       <c r="Z21" s="445">
         <v>3</v>
       </c>
@@ -8215,15 +8210,15 @@
       <c r="AM21" s="428" t="s">
         <v>544</v>
       </c>
-      <c r="AN21" s="636"/>
+      <c r="AN21" s="641"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="641"/>
+      <c r="F22" s="620"/>
       <c r="G22" s="337" t="s">
         <v>489</v>
       </c>
       <c r="I22" s="219"/>
-      <c r="O22" s="679"/>
+      <c r="O22" s="623"/>
       <c r="R22" s="434" t="s">
         <v>44</v>
       </c>
@@ -8231,14 +8226,14 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="610"/>
+      <c r="V22" s="661"/>
       <c r="W22" s="426" t="s">
         <v>175</v>
       </c>
       <c r="X22" s="429" t="s">
         <v>187</v>
       </c>
-      <c r="Y22" s="654"/>
+      <c r="Y22" s="658"/>
       <c r="Z22" s="415"/>
       <c r="AA22" s="10"/>
       <c r="AB22" s="415"/>
@@ -8249,7 +8244,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="650" t="s">
+      <c r="AJ22" s="630" t="s">
         <v>472</v>
       </c>
       <c r="AK22" s="257"/>
@@ -8257,7 +8252,7 @@
         <v>478</v>
       </c>
       <c r="AM22" s="300"/>
-      <c r="AN22" s="636"/>
+      <c r="AN22" s="641"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="231" t="s">
@@ -8275,22 +8270,22 @@
       <c r="E23" s="225">
         <v>1</v>
       </c>
-      <c r="F23" s="641"/>
+      <c r="F23" s="620"/>
       <c r="I23" s="219"/>
-      <c r="O23" s="679"/>
-      <c r="Q23" s="681" t="s">
+      <c r="O23" s="623"/>
+      <c r="Q23" s="625" t="s">
         <v>144</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="420" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="610"/>
+      <c r="V23" s="661"/>
       <c r="W23" s="148"/>
       <c r="X23" s="429" t="s">
         <v>188</v>
       </c>
-      <c r="Y23" s="654"/>
+      <c r="Y23" s="658"/>
       <c r="Z23" s="17"/>
       <c r="AA23" s="10"/>
       <c r="AB23" s="415"/>
@@ -8301,13 +8296,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="650"/>
+      <c r="AJ23" s="630"/>
       <c r="AK23" s="257"/>
       <c r="AL23" s="80" t="s">
         <v>507</v>
       </c>
       <c r="AM23" s="300"/>
-      <c r="AN23" s="636"/>
+      <c r="AN23" s="641"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="440" t="s">
@@ -8325,23 +8320,23 @@
       <c r="E24" s="436">
         <v>1</v>
       </c>
-      <c r="F24" s="641"/>
+      <c r="F24" s="620"/>
       <c r="G24" s="61" t="s">
         <v>490</v>
       </c>
       <c r="I24" s="219"/>
-      <c r="O24" s="679"/>
-      <c r="Q24" s="682"/>
+      <c r="O24" s="623"/>
+      <c r="Q24" s="626"/>
       <c r="T24" s="17"/>
       <c r="U24" s="227" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="610"/>
+      <c r="V24" s="661"/>
       <c r="W24" s="148"/>
       <c r="X24" s="429" t="s">
         <v>185</v>
       </c>
-      <c r="Y24" s="654"/>
+      <c r="Y24" s="658"/>
       <c r="Z24" s="17"/>
       <c r="AA24" s="10"/>
       <c r="AB24" s="415"/>
@@ -8360,12 +8355,12 @@
         <v>463</v>
       </c>
       <c r="AM24" s="300"/>
-      <c r="AN24" s="636"/>
+      <c r="AN24" s="641"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="641"/>
+      <c r="F25" s="620"/>
       <c r="I25" s="219"/>
-      <c r="O25" s="679"/>
+      <c r="O25" s="623"/>
       <c r="P25" s="204" t="s">
         <v>280</v>
       </c>
@@ -8378,12 +8373,12 @@
       <c r="U25" s="400" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="611"/>
+      <c r="V25" s="662"/>
       <c r="W25" s="148"/>
       <c r="X25" s="429" t="s">
         <v>189</v>
       </c>
-      <c r="Y25" s="654"/>
+      <c r="Y25" s="658"/>
       <c r="Z25" s="17"/>
       <c r="AA25" s="10"/>
       <c r="AB25" s="415"/>
@@ -8400,7 +8395,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="300"/>
-      <c r="AN25" s="636"/>
+      <c r="AN25" s="641"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="231" t="s">
@@ -8418,17 +8413,17 @@
       <c r="E26" s="380">
         <v>1</v>
       </c>
-      <c r="F26" s="641"/>
+      <c r="F26" s="620"/>
       <c r="G26" s="337" t="s">
         <v>487</v>
       </c>
       <c r="I26" s="219"/>
-      <c r="O26" s="679"/>
-      <c r="P26" s="638" t="s">
+      <c r="O26" s="623"/>
+      <c r="P26" s="643" t="s">
         <v>525</v>
       </c>
-      <c r="Q26" s="639"/>
-      <c r="R26" s="675" t="s">
+      <c r="Q26" s="644"/>
+      <c r="R26" s="617" t="s">
         <v>534</v>
       </c>
       <c r="T26" s="178"/>
@@ -8440,7 +8435,7 @@
       <c r="X26" s="429" t="s">
         <v>181</v>
       </c>
-      <c r="Y26" s="654"/>
+      <c r="Y26" s="658"/>
       <c r="Z26" s="17"/>
       <c r="AA26" s="10"/>
       <c r="AB26" s="415"/>
@@ -8467,7 +8462,7 @@
       <c r="AM26" s="442" t="s">
         <v>456</v>
       </c>
-      <c r="AN26" s="636"/>
+      <c r="AN26" s="641"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -8479,13 +8474,13 @@
       <c r="E27" s="265" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="677"/>
+      <c r="F27" s="621"/>
       <c r="G27" s="61" t="s">
         <v>543</v>
       </c>
       <c r="I27" s="220"/>
-      <c r="O27" s="680"/>
-      <c r="R27" s="676"/>
+      <c r="O27" s="624"/>
+      <c r="R27" s="618"/>
       <c r="S27" s="421" t="s">
         <v>54</v>
       </c>
@@ -8498,7 +8493,7 @@
       <c r="X27" s="429" t="s">
         <v>529</v>
       </c>
-      <c r="Y27" s="655"/>
+      <c r="Y27" s="659"/>
       <c r="Z27" s="161"/>
       <c r="AA27" s="13"/>
       <c r="AB27" s="416"/>
@@ -8515,32 +8510,26 @@
       <c r="AM27" s="381" t="s">
         <v>319</v>
       </c>
-      <c r="AN27" s="637"/>
+      <c r="AN27" s="642"/>
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="F2:F27"/>
-    <mergeCell ref="O10:O27"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AI6:AI10"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AG7:AG12"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="V21:V25"/>
+    <mergeCell ref="U18:U20"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="G5:L6"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B4:B5"/>
     <mergeCell ref="AN1:AN27"/>
     <mergeCell ref="P26:Q26"/>
     <mergeCell ref="Q2:Q3"/>
@@ -8557,22 +8546,28 @@
     <mergeCell ref="AD3:AD4"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="R2:R3"/>
-    <mergeCell ref="V21:V25"/>
-    <mergeCell ref="U18:U20"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="G5:L6"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="AI6:AI10"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AG7:AG12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="O10:O27"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8583,7 +8578,7 @@
   <dimension ref="B1:R20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8609,12 +8604,12 @@
       <c r="B1" s="603" t="s">
         <v>310</v>
       </c>
-      <c r="C1" s="683"/>
+      <c r="C1" s="627"/>
       <c r="D1" s="204"/>
       <c r="J1" s="603" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="683"/>
+      <c r="K1" s="627"/>
       <c r="L1" s="195" t="s">
         <v>330</v>
       </c>
@@ -9017,7 +9012,7 @@
       <c r="P1" s="398" t="s">
         <v>397</v>
       </c>
-      <c r="Q1" s="714" t="s">
+      <c r="Q1" s="701" t="s">
         <v>180</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -9041,7 +9036,7 @@
       <c r="AA1" s="517" t="s">
         <v>437</v>
       </c>
-      <c r="AB1" s="708" t="s">
+      <c r="AB1" s="695" t="s">
         <v>593</v>
       </c>
       <c r="AC1" s="99" t="s">
@@ -9063,32 +9058,32 @@
       </c>
     </row>
     <row r="2" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="693">
+      <c r="A2" s="706">
         <f ca="1">TODAY()</f>
         <v>45291</v>
       </c>
-      <c r="B2" s="695" t="s">
+      <c r="B2" s="708" t="s">
         <v>379</v>
       </c>
-      <c r="C2" s="615" t="s">
+      <c r="C2" s="645" t="s">
         <v>357</v>
       </c>
-      <c r="D2" s="697" t="s">
+      <c r="D2" s="710" t="s">
         <v>102</v>
       </c>
-      <c r="E2" s="699" t="s">
+      <c r="E2" s="712" t="s">
         <v>64</v>
       </c>
       <c r="F2" s="191" t="s">
         <v>218</v>
       </c>
-      <c r="G2" s="659" t="s">
+      <c r="G2" s="613" t="s">
         <v>372</v>
       </c>
       <c r="H2" s="206" t="s">
         <v>218</v>
       </c>
-      <c r="I2" s="705" t="s">
+      <c r="I2" s="692" t="s">
         <v>102</v>
       </c>
       <c r="J2" s="396" t="s">
@@ -9112,7 +9107,7 @@
       <c r="P2" s="399">
         <v>40</v>
       </c>
-      <c r="Q2" s="715"/>
+      <c r="Q2" s="702"/>
       <c r="R2" s="21">
         <f>R7+R20</f>
         <v>2</v>
@@ -9137,7 +9132,7 @@
         <f>IF((Z2+T2)&gt;0,0,-1)</f>
         <v>0</v>
       </c>
-      <c r="AB2" s="709"/>
+      <c r="AB2" s="696"/>
       <c r="AC2" s="35"/>
       <c r="AH2" s="6" t="s">
         <v>344</v>
@@ -9152,14 +9147,14 @@
       </c>
     </row>
     <row r="3" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="694"/>
-      <c r="B3" s="696"/>
-      <c r="C3" s="616"/>
-      <c r="D3" s="698"/>
-      <c r="E3" s="700"/>
-      <c r="G3" s="660"/>
+      <c r="A3" s="707"/>
+      <c r="B3" s="709"/>
+      <c r="C3" s="646"/>
+      <c r="D3" s="711"/>
+      <c r="E3" s="713"/>
+      <c r="G3" s="614"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="706"/>
+      <c r="I3" s="693"/>
       <c r="K3" s="24">
         <v>2</v>
       </c>
@@ -9174,7 +9169,7 @@
       <c r="V3" s="470"/>
       <c r="W3" s="6"/>
       <c r="X3" s="470"/>
-      <c r="AB3" s="709"/>
+      <c r="AB3" s="696"/>
       <c r="AC3" s="35"/>
       <c r="AE3" s="100" t="s">
         <v>588</v>
@@ -9203,10 +9198,10 @@
         <v>380</v>
       </c>
       <c r="B4" s="243"/>
-      <c r="C4" s="701" t="s">
+      <c r="C4" s="714" t="s">
         <v>177</v>
       </c>
-      <c r="I4" s="706"/>
+      <c r="I4" s="693"/>
       <c r="R4" s="471" t="s">
         <v>588</v>
       </c>
@@ -9218,7 +9213,7 @@
       <c r="V4" s="470"/>
       <c r="W4" s="6"/>
       <c r="X4" s="470"/>
-      <c r="AB4" s="709"/>
+      <c r="AB4" s="696"/>
       <c r="AC4" s="35"/>
       <c r="AE4" s="20"/>
       <c r="AF4" s="100" t="s">
@@ -9234,7 +9229,7 @@
       <c r="AI4" s="470"/>
       <c r="AJ4" s="552"/>
       <c r="AK4" s="6" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="AL4" s="24">
         <v>1</v>
@@ -9247,7 +9242,7 @@
       <c r="B5" s="100" t="s">
         <v>357</v>
       </c>
-      <c r="C5" s="702"/>
+      <c r="C5" s="715"/>
       <c r="D5" s="222" t="s">
         <v>102</v>
       </c>
@@ -9263,7 +9258,7 @@
       <c r="H5" s="206" t="s">
         <v>218</v>
       </c>
-      <c r="I5" s="706"/>
+      <c r="I5" s="693"/>
       <c r="J5" s="397" t="s">
         <v>268</v>
       </c>
@@ -9290,7 +9285,7 @@
       <c r="V5" s="468"/>
       <c r="W5" s="6"/>
       <c r="X5" s="468"/>
-      <c r="AB5" s="709"/>
+      <c r="AB5" s="696"/>
       <c r="AC5" s="2" t="s">
         <v>591</v>
       </c>
@@ -9310,19 +9305,19 @@
       <c r="AL5" s="468"/>
     </row>
     <row r="6" spans="1:38" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="690" t="s">
+      <c r="A6" s="703" t="s">
         <v>285</v>
       </c>
       <c r="B6" s="105" t="s">
         <v>198</v>
       </c>
-      <c r="C6" s="661"/>
-      <c r="D6" s="662"/>
+      <c r="C6" s="628"/>
+      <c r="D6" s="629"/>
       <c r="E6" s="96">
         <v>1</v>
       </c>
       <c r="G6" s="599"/>
-      <c r="I6" s="706"/>
+      <c r="I6" s="693"/>
       <c r="P6" s="61" t="s">
         <v>591</v>
       </c>
@@ -9334,7 +9329,7 @@
         <f>S7+S11-SUM(V2:V10)</f>
         <v>3</v>
       </c>
-      <c r="AB6" s="709"/>
+      <c r="AB6" s="696"/>
       <c r="AC6" s="35"/>
       <c r="AE6" s="64">
         <f>AE7-SUM(AL2:AL10)+AE11</f>
@@ -9350,7 +9345,7 @@
       <c r="AL6" s="112"/>
     </row>
     <row r="7" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="691"/>
+      <c r="A7" s="704"/>
       <c r="B7" s="100" t="s">
         <v>154</v>
       </c>
@@ -9361,7 +9356,7 @@
         <v>135</v>
       </c>
       <c r="G7" s="599"/>
-      <c r="I7" s="706"/>
+      <c r="I7" s="693"/>
       <c r="M7" s="16" t="s">
         <v>347</v>
       </c>
@@ -9391,7 +9386,7 @@
         <v>249</v>
       </c>
       <c r="X7" s="469"/>
-      <c r="AB7" s="709"/>
+      <c r="AB7" s="696"/>
       <c r="AC7" s="99" t="s">
         <v>592</v>
       </c>
@@ -9419,7 +9414,7 @@
       <c r="AL7" s="24"/>
     </row>
     <row r="8" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="692"/>
+      <c r="A8" s="705"/>
       <c r="B8" s="212" t="s">
         <v>28</v>
       </c>
@@ -9428,7 +9423,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="599"/>
-      <c r="I8" s="706"/>
+      <c r="I8" s="693"/>
       <c r="N8" s="80"/>
       <c r="U8" s="6"/>
       <c r="V8" s="24"/>
@@ -9436,7 +9431,7 @@
         <v>611</v>
       </c>
       <c r="X8" s="470"/>
-      <c r="AB8" s="709"/>
+      <c r="AB8" s="696"/>
       <c r="AC8" s="515"/>
       <c r="AH8" s="6" t="s">
         <v>610</v>
@@ -9467,7 +9462,7 @@
       </c>
       <c r="G9" s="599"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="706"/>
+      <c r="I9" s="693"/>
       <c r="M9" s="19" t="s">
         <v>524</v>
       </c>
@@ -9478,7 +9473,7 @@
         <v>603</v>
       </c>
       <c r="X9" s="470"/>
-      <c r="AB9" s="709"/>
+      <c r="AB9" s="696"/>
       <c r="AC9" s="515"/>
       <c r="AE9" s="20"/>
       <c r="AF9" s="20"/>
@@ -9506,7 +9501,7 @@
         <v>37</v>
       </c>
       <c r="G10" s="599"/>
-      <c r="I10" s="706"/>
+      <c r="I10" s="693"/>
       <c r="J10" s="24" t="s">
         <v>372</v>
       </c>
@@ -9521,7 +9516,7 @@
       <c r="V10" s="470"/>
       <c r="W10" s="6"/>
       <c r="X10" s="470"/>
-      <c r="AB10" s="709"/>
+      <c r="AB10" s="696"/>
       <c r="AC10" s="515"/>
       <c r="AE10" s="20"/>
       <c r="AF10" s="20"/>
@@ -9549,7 +9544,7 @@
         <v>265</v>
       </c>
       <c r="G11" s="599"/>
-      <c r="I11" s="706"/>
+      <c r="I11" s="693"/>
       <c r="J11" s="24" t="s">
         <v>194</v>
       </c>
@@ -9575,13 +9570,13 @@
       <c r="S11" s="24">
         <v>3</v>
       </c>
-      <c r="U11" s="711" t="s">
+      <c r="U11" s="698" t="s">
         <v>557</v>
       </c>
-      <c r="V11" s="712"/>
-      <c r="W11" s="712"/>
-      <c r="X11" s="713"/>
-      <c r="AB11" s="710"/>
+      <c r="V11" s="699"/>
+      <c r="W11" s="699"/>
+      <c r="X11" s="700"/>
+      <c r="AB11" s="697"/>
       <c r="AC11" s="99" t="s">
         <v>594</v>
       </c>
@@ -9595,13 +9590,13 @@
         <v>3</v>
       </c>
       <c r="AG11" s="414"/>
-      <c r="AH11" s="711" t="s">
+      <c r="AH11" s="698" t="s">
         <v>602</v>
       </c>
-      <c r="AI11" s="712"/>
-      <c r="AJ11" s="712"/>
-      <c r="AK11" s="712"/>
-      <c r="AL11" s="713"/>
+      <c r="AI11" s="699"/>
+      <c r="AJ11" s="699"/>
+      <c r="AK11" s="699"/>
+      <c r="AL11" s="700"/>
     </row>
     <row r="12" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="227" t="s">
@@ -9612,7 +9607,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="599"/>
-      <c r="I12" s="706"/>
+      <c r="I12" s="693"/>
       <c r="J12" s="24" t="s">
         <v>515</v>
       </c>
@@ -9645,7 +9640,7 @@
       </c>
       <c r="D13" s="20"/>
       <c r="G13" s="599"/>
-      <c r="I13" s="706"/>
+      <c r="I13" s="693"/>
       <c r="J13" s="108" t="s">
         <v>547</v>
       </c>
@@ -9689,7 +9684,7 @@
       <c r="H14" s="206" t="s">
         <v>218</v>
       </c>
-      <c r="I14" s="706"/>
+      <c r="I14" s="693"/>
       <c r="U14" s="67" t="s">
         <v>80</v>
       </c>
@@ -9716,7 +9711,7 @@
       <c r="H15" s="271">
         <v>0</v>
       </c>
-      <c r="I15" s="706"/>
+      <c r="I15" s="693"/>
       <c r="J15" s="108" t="s">
         <v>153</v>
       </c>
@@ -9747,7 +9742,7 @@
       <c r="D16" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="I16" s="706"/>
+      <c r="I16" s="693"/>
       <c r="K16" s="100" t="s">
         <v>44</v>
       </c>
@@ -9791,7 +9786,7 @@
       <c r="G17" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="I17" s="706"/>
+      <c r="I17" s="693"/>
       <c r="L17" s="2" t="s">
         <v>426</v>
       </c>
@@ -9805,13 +9800,13 @@
     </row>
     <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
-      <c r="I18" s="706"/>
+      <c r="I18" s="693"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="703" t="s">
+      <c r="O18" s="690" t="s">
         <v>516</v>
       </c>
-      <c r="P18" s="704"/>
+      <c r="P18" s="691"/>
       <c r="Q18" s="127" t="s">
         <v>44</v>
       </c>
@@ -9833,7 +9828,7 @@
       </c>
     </row>
     <row r="19" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="706"/>
+      <c r="I19" s="693"/>
       <c r="M19" s="21" t="s">
         <v>425</v>
       </c>
@@ -9865,7 +9860,7 @@
       <c r="G20" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="I20" s="706"/>
+      <c r="I20" s="693"/>
       <c r="K20" s="19" t="s">
         <v>422</v>
       </c>
@@ -9894,7 +9889,7 @@
       <c r="X20" s="468"/>
     </row>
     <row r="21" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="706"/>
+      <c r="I21" s="693"/>
       <c r="M21" s="216" t="s">
         <v>411</v>
       </c>
@@ -9924,7 +9919,7 @@
       <c r="G22" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="I22" s="706"/>
+      <c r="I22" s="693"/>
       <c r="P22" s="99" t="s">
         <v>590</v>
       </c>
@@ -9939,7 +9934,7 @@
       <c r="E23" s="283" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="706"/>
+      <c r="I23" s="693"/>
       <c r="Q23" s="24">
         <f>SUM(V23:V31)</f>
         <v>7</v>
@@ -9956,7 +9951,7 @@
       </c>
     </row>
     <row r="24" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="706"/>
+      <c r="I24" s="693"/>
       <c r="U24" s="35"/>
       <c r="V24" s="509">
         <v>1</v>
@@ -9984,7 +9979,7 @@
       <c r="H25" s="191" t="s">
         <v>266</v>
       </c>
-      <c r="I25" s="706"/>
+      <c r="I25" s="693"/>
       <c r="J25" s="397" t="s">
         <v>269</v>
       </c>
@@ -10029,7 +10024,7 @@
       <c r="H26" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="I26" s="706"/>
+      <c r="I26" s="693"/>
       <c r="K26" s="24">
         <v>15</v>
       </c>
@@ -10064,7 +10059,7 @@
       </c>
     </row>
     <row r="27" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="706"/>
+      <c r="I27" s="693"/>
       <c r="O27" s="2" t="s">
         <v>98</v>
       </c>
@@ -10091,7 +10086,7 @@
       <c r="E28" s="215">
         <v>2</v>
       </c>
-      <c r="I28" s="706"/>
+      <c r="I28" s="693"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="142"/>
@@ -10113,7 +10108,7 @@
       <c r="H29" s="191" t="s">
         <v>267</v>
       </c>
-      <c r="I29" s="707"/>
+      <c r="I29" s="694"/>
       <c r="J29" s="324"/>
       <c r="L29" s="96" t="s">
         <v>273</v>
@@ -10171,13 +10166,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I2:I29"/>
-    <mergeCell ref="AB1:AB11"/>
-    <mergeCell ref="AH11:AL11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="U11:X11"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="G5:G14"/>
     <mergeCell ref="A2:A3"/>
@@ -10189,6 +10177,13 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C2:C3"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I2:I29"/>
+    <mergeCell ref="AB1:AB11"/>
+    <mergeCell ref="AH11:AL11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="U11:X11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10199,8 +10194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AT37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10300,14 +10295,14 @@
         <f ca="1">TODAY()</f>
         <v>45291</v>
       </c>
-      <c r="T1" s="742"/>
+      <c r="T1" s="735"/>
       <c r="U1" s="142"/>
       <c r="V1" s="6"/>
       <c r="W1" s="6"/>
-      <c r="X1" s="726" t="s">
+      <c r="X1" s="719" t="s">
         <v>441</v>
       </c>
-      <c r="Y1" s="727"/>
+      <c r="Y1" s="720"/>
       <c r="Z1" s="306">
         <f>68-(W8+Y3+X3+U3)</f>
         <v>0</v>
@@ -10323,27 +10318,27 @@
       <c r="AD1" s="302" t="s">
         <v>44</v>
       </c>
-      <c r="AE1" s="728" t="s">
+      <c r="AE1" s="721" t="s">
         <v>190</v>
       </c>
-      <c r="AF1" s="729"/>
-      <c r="AG1" s="730"/>
-      <c r="AH1" s="731" t="s">
+      <c r="AF1" s="722"/>
+      <c r="AG1" s="723"/>
+      <c r="AH1" s="724" t="s">
         <v>293</v>
       </c>
-      <c r="AI1" s="732"/>
-      <c r="AJ1" s="733"/>
-      <c r="AK1" s="659" t="s">
+      <c r="AI1" s="725"/>
+      <c r="AJ1" s="726"/>
+      <c r="AK1" s="613" t="s">
         <v>613</v>
       </c>
       <c r="AL1" s="550" t="s">
         <v>614</v>
       </c>
-      <c r="AM1" s="723" t="s">
+      <c r="AM1" s="716" t="s">
         <v>444</v>
       </c>
-      <c r="AN1" s="724"/>
-      <c r="AO1" s="725"/>
+      <c r="AN1" s="717"/>
+      <c r="AO1" s="718"/>
       <c r="AR1" s="142"/>
     </row>
     <row r="2" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10358,27 +10353,27 @@
         <f>K2+L2</f>
         <v>26</v>
       </c>
-      <c r="K2" s="721">
+      <c r="K2" s="743">
         <f>SUM(K4:K37)</f>
         <v>6</v>
       </c>
-      <c r="L2" s="719">
+      <c r="L2" s="741">
         <f>SUM(L4:L37)</f>
         <v>20</v>
       </c>
-      <c r="M2" s="734">
+      <c r="M2" s="727">
         <f>SUM(M5:M30)</f>
         <v>0</v>
       </c>
-      <c r="N2" s="736">
+      <c r="N2" s="729">
         <f>SUM(N4:N29)</f>
         <v>8</v>
       </c>
-      <c r="O2" s="738">
+      <c r="O2" s="731">
         <f>SUM(O4:O29)</f>
         <v>11</v>
       </c>
-      <c r="P2" s="666">
+      <c r="P2" s="637">
         <f>SUM(N30:N37)* (-1)</f>
         <v>-1</v>
       </c>
@@ -10391,14 +10386,14 @@
       <c r="S2" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="T2" s="743"/>
+      <c r="T2" s="736"/>
       <c r="U2" s="537" t="s">
         <v>262</v>
       </c>
       <c r="V2" s="482" t="s">
         <v>219</v>
       </c>
-      <c r="W2" s="740" t="s">
+      <c r="W2" s="733" t="s">
         <v>234</v>
       </c>
       <c r="X2" s="483" t="s">
@@ -10440,7 +10435,7 @@
       <c r="AJ2" s="150" t="s">
         <v>288</v>
       </c>
-      <c r="AK2" s="660"/>
+      <c r="AK2" s="614"/>
       <c r="AL2" s="591" t="s">
         <v>288</v>
       </c>
@@ -10468,12 +10463,12 @@
         <f>V3+X3+Y3+U3</f>
         <v>68</v>
       </c>
-      <c r="K3" s="722"/>
-      <c r="L3" s="720"/>
-      <c r="M3" s="735"/>
-      <c r="N3" s="737"/>
-      <c r="O3" s="739"/>
-      <c r="P3" s="667"/>
+      <c r="K3" s="744"/>
+      <c r="L3" s="742"/>
+      <c r="M3" s="728"/>
+      <c r="N3" s="730"/>
+      <c r="O3" s="732"/>
+      <c r="P3" s="638"/>
       <c r="Q3" s="172">
         <f>(M2+N2)-Y3</f>
         <v>0</v>
@@ -10481,7 +10476,7 @@
       <c r="S3" s="159" t="s">
         <v>244</v>
       </c>
-      <c r="T3" s="744"/>
+      <c r="T3" s="737"/>
       <c r="U3" s="538">
         <f>SUM(U4:U29)</f>
         <v>14</v>
@@ -10490,7 +10485,7 @@
         <f>SUM(V4:V29)</f>
         <v>37</v>
       </c>
-      <c r="W3" s="741"/>
+      <c r="W3" s="734"/>
       <c r="X3" s="485">
         <f t="shared" ref="X3:AC3" si="0">SUM(X4:X29)</f>
         <v>9</v>
@@ -10596,7 +10591,7 @@
         <f>AC4</f>
         <v>0</v>
       </c>
-      <c r="P4" s="716"/>
+      <c r="P4" s="738"/>
       <c r="Q4" s="20"/>
       <c r="R4" s="2" t="s">
         <v>334</v>
@@ -10680,7 +10675,7 @@
         <f>AC5</f>
         <v>0</v>
       </c>
-      <c r="P5" s="717"/>
+      <c r="P5" s="739"/>
       <c r="Q5" s="20"/>
       <c r="R5" s="2" t="s">
         <v>340</v>
@@ -10774,7 +10769,7 @@
         <f>AC6</f>
         <v>1</v>
       </c>
-      <c r="P6" s="717"/>
+      <c r="P6" s="739"/>
       <c r="Q6" s="54" t="s">
         <v>335</v>
       </c>
@@ -10879,7 +10874,7 @@
         <f>AC7</f>
         <v>1</v>
       </c>
-      <c r="P7" s="717"/>
+      <c r="P7" s="739"/>
       <c r="Q7" s="20"/>
       <c r="R7" s="2" t="s">
         <v>335</v>
@@ -10995,7 +10990,7 @@
         <f t="shared" ref="O8:O37" si="10">AC8</f>
         <v>0</v>
       </c>
-      <c r="P8" s="717"/>
+      <c r="P8" s="739"/>
       <c r="Q8" s="108" t="s">
         <v>233</v>
       </c>
@@ -11086,7 +11081,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P9" s="717"/>
+      <c r="P9" s="739"/>
       <c r="Q9" s="108" t="s">
         <v>335</v>
       </c>
@@ -11191,7 +11186,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P10" s="717"/>
+      <c r="P10" s="739"/>
       <c r="Q10" s="20"/>
       <c r="R10" s="2" t="s">
         <v>340</v>
@@ -11281,7 +11276,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P11" s="717"/>
+      <c r="P11" s="739"/>
       <c r="Q11" s="108" t="s">
         <v>335</v>
       </c>
@@ -11346,14 +11341,14 @@
       <c r="AR11" s="508"/>
     </row>
     <row r="12" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="626" t="s">
+      <c r="A12" s="675" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
         <v>13</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="E12" s="681" t="s">
+      <c r="E12" s="625" t="s">
         <v>56</v>
       </c>
       <c r="G12" s="262"/>
@@ -11378,7 +11373,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P12" s="717"/>
+      <c r="P12" s="739"/>
       <c r="Q12" s="108" t="s">
         <v>335</v>
       </c>
@@ -11455,14 +11450,14 @@
       </c>
     </row>
     <row r="13" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="628"/>
+      <c r="A13" s="677"/>
       <c r="B13" s="583">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="682"/>
+      <c r="E13" s="626"/>
       <c r="F13" s="172">
         <v>0</v>
       </c>
@@ -11486,7 +11481,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P13" s="717"/>
+      <c r="P13" s="739"/>
       <c r="Q13" s="108" t="s">
         <v>335</v>
       </c>
@@ -11568,7 +11563,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P14" s="717"/>
+      <c r="P14" s="739"/>
       <c r="Q14" s="20"/>
       <c r="R14" s="200" t="s">
         <v>339</v>
@@ -11671,7 +11666,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P15" s="717"/>
+      <c r="P15" s="739"/>
       <c r="Q15" s="20"/>
       <c r="R15" s="200" t="s">
         <v>339</v>
@@ -11765,7 +11760,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P16" s="717"/>
+      <c r="P16" s="739"/>
       <c r="Q16" s="108" t="s">
         <v>335</v>
       </c>
@@ -11866,7 +11861,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P17" s="717"/>
+      <c r="P17" s="739"/>
       <c r="Q17" s="20"/>
       <c r="R17" s="2" t="s">
         <v>341</v>
@@ -11966,7 +11961,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P18" s="717"/>
+      <c r="P18" s="739"/>
       <c r="Q18" s="108" t="s">
         <v>335</v>
       </c>
@@ -12056,7 +12051,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P19" s="717"/>
+      <c r="P19" s="739"/>
       <c r="Q19" s="20"/>
       <c r="R19" s="2" t="s">
         <v>334</v>
@@ -12164,11 +12159,11 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P20" s="718"/>
+      <c r="P20" s="740"/>
       <c r="Q20" s="605" t="s">
         <v>335</v>
       </c>
-      <c r="R20" s="683"/>
+      <c r="R20" s="627"/>
       <c r="S20" s="534" t="s">
         <v>85</v>
       </c>
@@ -12430,7 +12425,7 @@
     </row>
     <row r="23" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="24"/>
-      <c r="E23" s="633" t="s">
+      <c r="E23" s="682" t="s">
         <v>289</v>
       </c>
       <c r="F23" s="180"/>
@@ -12535,7 +12530,7 @@
       <c r="C24" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="E24" s="634"/>
+      <c r="E24" s="683"/>
       <c r="F24" s="172"/>
       <c r="H24" s="42"/>
       <c r="J24" s="570" t="s">
@@ -12561,7 +12556,7 @@
       <c r="Q24" s="605" t="s">
         <v>335</v>
       </c>
-      <c r="R24" s="683"/>
+      <c r="R24" s="627"/>
       <c r="S24" s="534" t="s">
         <v>249</v>
       </c>
@@ -13229,8 +13224,8 @@
       <c r="AR31" s="508"/>
     </row>
     <row r="32" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="650"/>
-      <c r="B32" s="650"/>
+      <c r="A32" s="630"/>
+      <c r="B32" s="630"/>
       <c r="J32" s="571"/>
       <c r="K32" s="586"/>
       <c r="L32" s="580">
@@ -13707,9 +13702,7 @@
       </c>
     </row>
     <row r="37" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="21">
-        <v>0</v>
-      </c>
+      <c r="B37" s="21"/>
       <c r="D37" s="382">
         <v>1</v>
       </c>
@@ -13814,6 +13807,15 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="P4:P20"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="Q20:R20"/>
     <mergeCell ref="AM1:AO1"/>
     <mergeCell ref="X1:Y1"/>
     <mergeCell ref="AE1:AG1"/>
@@ -13825,15 +13827,6 @@
     <mergeCell ref="W2:W3"/>
     <mergeCell ref="T1:T3"/>
     <mergeCell ref="AK1:AK2"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="P4:P20"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="Q20:R20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13901,7 +13894,7 @@
       <c r="V1" s="603" t="s">
         <v>70</v>
       </c>
-      <c r="W1" s="683"/>
+      <c r="W1" s="627"/>
       <c r="X1" s="62" t="s">
         <v>101</v>
       </c>
@@ -13920,7 +13913,7 @@
       <c r="AC1" s="116" t="s">
         <v>190</v>
       </c>
-      <c r="AD1" s="759" t="s">
+      <c r="AD1" s="752" t="s">
         <v>211</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -13937,10 +13930,10 @@
       <c r="E2" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="790" t="s">
+      <c r="F2" s="751" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="747" t="s">
+      <c r="G2" s="779" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -13968,10 +13961,10 @@
       <c r="U2" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="V2" s="726" t="s">
+      <c r="V2" s="719" t="s">
         <v>120</v>
       </c>
-      <c r="W2" s="727"/>
+      <c r="W2" s="720"/>
       <c r="X2" s="64" t="s">
         <v>109</v>
       </c>
@@ -13990,7 +13983,7 @@
       <c r="AC2" s="117" t="s">
         <v>98</v>
       </c>
-      <c r="AD2" s="760"/>
+      <c r="AD2" s="753"/>
       <c r="AE2" s="64" t="s">
         <v>98</v>
       </c>
@@ -14009,8 +14002,8 @@
       <c r="E3" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="F3" s="630"/>
-      <c r="G3" s="748"/>
+      <c r="F3" s="679"/>
+      <c r="G3" s="780"/>
       <c r="H3" s="40" t="s">
         <v>80</v>
       </c>
@@ -14021,13 +14014,13 @@
         <v>81</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="757" t="s">
+      <c r="O3" s="789" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="778" t="s">
+      <c r="P3" s="771" t="s">
         <v>217</v>
       </c>
-      <c r="Q3" s="779"/>
+      <c r="Q3" s="772"/>
       <c r="S3" s="57" t="s">
         <v>218</v>
       </c>
@@ -14037,15 +14030,15 @@
       <c r="W3" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="AD3" s="760"/>
+      <c r="AD3" s="753"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="748"/>
+      <c r="G4" s="780"/>
       <c r="H4" s="6"/>
       <c r="L4" s="687" t="s">
         <v>82</v>
       </c>
-      <c r="O4" s="758"/>
+      <c r="O4" s="790"/>
       <c r="T4" s="55" t="s">
         <v>97</v>
       </c>
@@ -14059,8 +14052,8 @@
         <v>194</v>
       </c>
       <c r="Z4" s="605"/>
-      <c r="AA4" s="683"/>
-      <c r="AD4" s="760"/>
+      <c r="AA4" s="627"/>
+      <c r="AD4" s="753"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -14075,21 +14068,21 @@
       <c r="F5" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="G5" s="748"/>
+      <c r="G5" s="780"/>
       <c r="H5" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="K5" s="765" t="s">
+      <c r="K5" s="758" t="s">
         <v>215</v>
       </c>
-      <c r="L5" s="780"/>
+      <c r="L5" s="773"/>
       <c r="M5" s="2" t="s">
         <v>213</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>212</v>
       </c>
-      <c r="O5" s="758"/>
+      <c r="O5" s="790"/>
       <c r="P5" s="108" t="s">
         <v>214</v>
       </c>
@@ -14105,11 +14098,11 @@
       <c r="U5" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="Y5" s="768" t="s">
+      <c r="Y5" s="761" t="s">
         <v>282</v>
       </c>
-      <c r="Z5" s="769"/>
-      <c r="AD5" s="760"/>
+      <c r="Z5" s="762"/>
+      <c r="AD5" s="753"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -14119,16 +14112,16 @@
       <c r="E6" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="G6" s="748"/>
+      <c r="G6" s="780"/>
       <c r="H6" s="46" t="s">
         <v>80</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="766"/>
-      <c r="L6" s="780"/>
-      <c r="O6" s="758"/>
+      <c r="K6" s="759"/>
+      <c r="L6" s="773"/>
+      <c r="O6" s="790"/>
       <c r="T6" s="2" t="s">
         <v>100</v>
       </c>
@@ -14138,23 +14131,23 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="760"/>
+      <c r="AD6" s="753"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="748"/>
+      <c r="G7" s="780"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="766"/>
-      <c r="L7" s="780"/>
+      <c r="K7" s="759"/>
+      <c r="L7" s="773"/>
       <c r="N7" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="O7" s="758"/>
+      <c r="O7" s="790"/>
       <c r="P7" s="73"/>
       <c r="U7" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="760"/>
+      <c r="AD7" s="753"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -14167,7 +14160,7 @@
       <c r="F8" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="G8" s="748"/>
+      <c r="G8" s="780"/>
       <c r="H8" s="50" t="s">
         <v>75</v>
       </c>
@@ -14177,41 +14170,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="766"/>
-      <c r="L8" s="780"/>
-      <c r="O8" s="758"/>
+      <c r="K8" s="759"/>
+      <c r="L8" s="773"/>
+      <c r="O8" s="790"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="762" t="s">
+      <c r="S8" s="755" t="s">
         <v>210</v>
       </c>
-      <c r="T8" s="763"/>
-      <c r="U8" s="763"/>
-      <c r="V8" s="763"/>
-      <c r="W8" s="763"/>
-      <c r="X8" s="763"/>
-      <c r="Y8" s="763"/>
-      <c r="Z8" s="763"/>
-      <c r="AA8" s="763"/>
-      <c r="AB8" s="763"/>
-      <c r="AC8" s="764"/>
-      <c r="AD8" s="760"/>
+      <c r="T8" s="756"/>
+      <c r="U8" s="756"/>
+      <c r="V8" s="756"/>
+      <c r="W8" s="756"/>
+      <c r="X8" s="756"/>
+      <c r="Y8" s="756"/>
+      <c r="Z8" s="756"/>
+      <c r="AA8" s="756"/>
+      <c r="AB8" s="756"/>
+      <c r="AC8" s="757"/>
+      <c r="AD8" s="753"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="784"/>
-      <c r="G9" s="748"/>
+      <c r="C9" s="745"/>
+      <c r="G9" s="780"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="766"/>
-      <c r="L9" s="751" t="s">
+      <c r="K9" s="759"/>
+      <c r="L9" s="783" t="s">
         <v>216</v>
       </c>
-      <c r="M9" s="752"/>
-      <c r="N9" s="753"/>
-      <c r="O9" s="758"/>
+      <c r="M9" s="784"/>
+      <c r="N9" s="785"/>
+      <c r="O9" s="790"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="760"/>
+      <c r="AD9" s="753"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="785"/>
+      <c r="C10" s="746"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>87</v>
@@ -14219,7 +14212,7 @@
       <c r="F10" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="G10" s="748"/>
+      <c r="G10" s="780"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>80</v>
@@ -14227,33 +14220,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="766"/>
-      <c r="M10" s="787" t="s">
+      <c r="K10" s="759"/>
+      <c r="M10" s="748" t="s">
         <v>89</v>
       </c>
-      <c r="N10" s="788"/>
-      <c r="O10" s="788"/>
-      <c r="P10" s="788"/>
-      <c r="Q10" s="788"/>
-      <c r="R10" s="788"/>
-      <c r="S10" s="788"/>
-      <c r="T10" s="788"/>
-      <c r="U10" s="788"/>
-      <c r="V10" s="788"/>
-      <c r="W10" s="788"/>
-      <c r="X10" s="788"/>
-      <c r="Y10" s="788"/>
-      <c r="Z10" s="788"/>
-      <c r="AA10" s="788"/>
-      <c r="AB10" s="788"/>
-      <c r="AC10" s="789"/>
-      <c r="AD10" s="760"/>
+      <c r="N10" s="749"/>
+      <c r="O10" s="749"/>
+      <c r="P10" s="749"/>
+      <c r="Q10" s="749"/>
+      <c r="R10" s="749"/>
+      <c r="S10" s="749"/>
+      <c r="T10" s="749"/>
+      <c r="U10" s="749"/>
+      <c r="V10" s="749"/>
+      <c r="W10" s="749"/>
+      <c r="X10" s="749"/>
+      <c r="Y10" s="749"/>
+      <c r="Z10" s="749"/>
+      <c r="AA10" s="749"/>
+      <c r="AB10" s="749"/>
+      <c r="AC10" s="750"/>
+      <c r="AD10" s="753"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="786"/>
-      <c r="G11" s="748"/>
+      <c r="C11" s="747"/>
+      <c r="G11" s="780"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="766"/>
+      <c r="K11" s="759"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -14261,17 +14254,17 @@
       <c r="Y11" s="68" t="s">
         <v>120</v>
       </c>
-      <c r="Z11" s="776" t="s">
+      <c r="Z11" s="769" t="s">
         <v>120</v>
       </c>
-      <c r="AA11" s="777"/>
+      <c r="AA11" s="770"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>120</v>
       </c>
-      <c r="AD11" s="760"/>
+      <c r="AD11" s="753"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -14284,7 +14277,7 @@
       <c r="F12" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="G12" s="748"/>
+      <c r="G12" s="780"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>80</v>
@@ -14292,8 +14285,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="766"/>
-      <c r="L12" s="781" t="s">
+      <c r="K12" s="759"/>
+      <c r="L12" s="774" t="s">
         <v>92</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -14324,25 +14317,25 @@
         <v>115</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="770" t="s">
+      <c r="AA12" s="763" t="s">
         <v>125</v>
       </c>
-      <c r="AB12" s="771"/>
+      <c r="AB12" s="764"/>
       <c r="AC12" s="21" t="s">
         <v>230</v>
       </c>
-      <c r="AD12" s="760"/>
+      <c r="AD12" s="753"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="784"/>
-      <c r="G13" s="748"/>
-      <c r="K13" s="766"/>
-      <c r="L13" s="782"/>
+      <c r="C13" s="745"/>
+      <c r="G13" s="780"/>
+      <c r="K13" s="759"/>
+      <c r="L13" s="775"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="750" t="s">
+      <c r="Q13" s="782" t="s">
         <v>208</v>
       </c>
-      <c r="R13" s="639"/>
+      <c r="R13" s="644"/>
       <c r="S13" s="599"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
@@ -14351,17 +14344,17 @@
       <c r="X13" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="AA13" s="772"/>
-      <c r="AB13" s="773"/>
-      <c r="AD13" s="760"/>
+      <c r="AA13" s="765"/>
+      <c r="AB13" s="766"/>
+      <c r="AD13" s="753"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="C14" s="786"/>
+      <c r="C14" s="747"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="748"/>
+      <c r="G14" s="780"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -14369,8 +14362,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="766"/>
-      <c r="L14" s="782"/>
+      <c r="K14" s="759"/>
+      <c r="L14" s="775"/>
       <c r="M14" s="21" t="s">
         <v>110</v>
       </c>
@@ -14391,9 +14384,9 @@
       <c r="Y14" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="AA14" s="772"/>
-      <c r="AB14" s="773"/>
-      <c r="AD14" s="760"/>
+      <c r="AA14" s="765"/>
+      <c r="AB14" s="766"/>
+      <c r="AD14" s="753"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -14408,19 +14401,19 @@
       <c r="F15" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="G15" s="748"/>
+      <c r="G15" s="780"/>
       <c r="H15" s="2" t="s">
         <v>80</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="K15" s="766"/>
-      <c r="L15" s="783"/>
-      <c r="Q15" s="750" t="s">
+      <c r="K15" s="759"/>
+      <c r="L15" s="776"/>
+      <c r="Q15" s="782" t="s">
         <v>209</v>
       </c>
-      <c r="R15" s="639"/>
+      <c r="R15" s="644"/>
       <c r="S15" s="599"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
@@ -14429,14 +14422,14 @@
       <c r="X15" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="AA15" s="772"/>
-      <c r="AB15" s="773"/>
-      <c r="AD15" s="760"/>
+      <c r="AA15" s="765"/>
+      <c r="AB15" s="766"/>
+      <c r="AD15" s="753"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="748"/>
-      <c r="K16" s="766"/>
+      <c r="G16" s="780"/>
+      <c r="K16" s="759"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>108</v>
@@ -14455,24 +14448,24 @@
       <c r="Z16" s="76" t="s">
         <v>126</v>
       </c>
-      <c r="AA16" s="772"/>
-      <c r="AB16" s="773"/>
-      <c r="AD16" s="760"/>
+      <c r="AA16" s="765"/>
+      <c r="AB16" s="766"/>
+      <c r="AD16" s="753"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F17" s="745" t="s">
+      <c r="F17" s="777" t="s">
         <v>95</v>
       </c>
-      <c r="G17" s="748"/>
+      <c r="G17" s="780"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>80</v>
       </c>
-      <c r="K17" s="766"/>
+      <c r="K17" s="759"/>
       <c r="S17" s="599"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
@@ -14480,9 +14473,9 @@
       <c r="X17" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA17" s="772"/>
-      <c r="AB17" s="773"/>
-      <c r="AD17" s="760"/>
+      <c r="AA17" s="765"/>
+      <c r="AB17" s="766"/>
+      <c r="AD17" s="753"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -14492,15 +14485,15 @@
       <c r="E18" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F18" s="746"/>
-      <c r="G18" s="748"/>
+      <c r="F18" s="778"/>
+      <c r="G18" s="780"/>
       <c r="H18" s="108" t="s">
         <v>75</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="K18" s="766"/>
+      <c r="K18" s="759"/>
       <c r="O18" s="64" t="s">
         <v>114</v>
       </c>
@@ -14511,39 +14504,42 @@
       <c r="X18" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AA18" s="774"/>
-      <c r="AB18" s="775"/>
-      <c r="AD18" s="760"/>
+      <c r="AA18" s="767"/>
+      <c r="AB18" s="768"/>
+      <c r="AD18" s="753"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>207</v>
       </c>
-      <c r="G19" s="749"/>
-      <c r="K19" s="767"/>
+      <c r="G19" s="781"/>
+      <c r="K19" s="760"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="754" t="s">
+      <c r="R19" s="786" t="s">
         <v>123</v>
       </c>
-      <c r="S19" s="755"/>
-      <c r="T19" s="756"/>
+      <c r="S19" s="787"/>
+      <c r="T19" s="788"/>
       <c r="V19" s="77" t="s">
         <v>114</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="AD19" s="761"/>
+      <c r="AD19" s="754"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="M10:AC10"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="S12:S18"/>
+    <mergeCell ref="O3:O9"/>
     <mergeCell ref="AD1:AD19"/>
     <mergeCell ref="S8:AC8"/>
     <mergeCell ref="K5:K19"/>
@@ -14555,14 +14551,11 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L12:L15"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G19"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="S12:S18"/>
-    <mergeCell ref="O3:O9"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="M10:AC10"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rw Usage Updates S.1.0.1.2 _12:45PM
Boat Enabled -
InCapacity - [0] , NodeW - [-3] , BirdW - [7] , FuelW - [22] , OnHost - [8+1]
VillageW=[0] ,  [X-MarketShieldMatrix-X] = [5,24,10,9]
Rw - Local(Left Running With Cost ) - [For Business/Shop/Market only] -
</commit_message>
<xml_diff>
--- a/System_2.2.1.xlsx
+++ b/System_2.2.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F2FA74-8462-48FB-82E3-759EE57F4002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0454AF1-9F38-4911-9B2D-03FDCD3E9BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="624">
   <si>
     <t>Zone</t>
   </si>
@@ -1908,6 +1908,9 @@
   </si>
   <si>
     <t>bharat24</t>
+  </si>
+  <si>
+    <t>X-MSM-X</t>
   </si>
 </sst>
 </file>
@@ -5024,6 +5027,159 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5042,12 +5198,6 @@
     <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5102,169 +5252,61 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5306,43 +5348,70 @@
     <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="52" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="52" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="14" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5366,112 +5435,25 @@
     <xf numFmtId="0" fontId="29" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="52" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="52" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="14" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5549,25 +5531,46 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5866,7 +5869,7 @@
   <dimension ref="B1:X28"/>
   <sheetViews>
     <sheetView topLeftCell="C9" workbookViewId="0">
-      <selection activeCell="X13" sqref="X13"/>
+      <selection activeCell="W14" sqref="W14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6589,7 +6592,9 @@
       </c>
       <c r="P22" s="313"/>
       <c r="T22" s="607"/>
-      <c r="X22" s="2"/>
+      <c r="X22" s="2" t="s">
+        <v>623</v>
+      </c>
     </row>
     <row r="23" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
@@ -6898,7 +6903,7 @@
       <c r="H1" s="97" t="s">
         <v>343</v>
       </c>
-      <c r="I1" s="659" t="s">
+      <c r="I1" s="613" t="s">
         <v>369</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -6934,7 +6939,7 @@
       <c r="X1" s="430" t="s">
         <v>155</v>
       </c>
-      <c r="Y1" s="653" t="s">
+      <c r="Y1" s="657" t="s">
         <v>528</v>
       </c>
       <c r="Z1" s="406">
@@ -6959,7 +6964,7 @@
         <v>498</v>
       </c>
       <c r="AM1" s="402"/>
-      <c r="AN1" s="635"/>
+      <c r="AN1" s="640"/>
       <c r="AO1" s="338" t="s">
         <v>469</v>
       </c>
@@ -6968,23 +6973,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="617">
+      <c r="A2" s="666">
         <f ca="1">TODAY()</f>
         <v>45293</v>
       </c>
-      <c r="B2" s="619" t="s">
+      <c r="B2" s="668" t="s">
         <v>370</v>
       </c>
-      <c r="C2" s="615" t="s">
+      <c r="C2" s="645" t="s">
         <v>357</v>
       </c>
-      <c r="D2" s="621" t="s">
+      <c r="D2" s="670" t="s">
         <v>355</v>
       </c>
-      <c r="E2" s="669" t="s">
+      <c r="E2" s="609" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="640" t="s">
+      <c r="F2" s="619" t="s">
         <v>102</v>
       </c>
       <c r="G2" s="393" t="s">
@@ -6993,31 +6998,31 @@
       <c r="H2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="660"/>
+      <c r="I2" s="614"/>
       <c r="J2" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="671" t="s">
+      <c r="K2" s="611" t="s">
         <v>342</v>
       </c>
-      <c r="L2" s="672"/>
-      <c r="M2" s="640" t="s">
+      <c r="L2" s="612"/>
+      <c r="M2" s="619" t="s">
         <v>102</v>
       </c>
       <c r="N2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="644" t="s">
+      <c r="O2" s="649" t="s">
         <v>102</v>
       </c>
       <c r="P2" s="85" t="s">
         <v>147</v>
       </c>
-      <c r="Q2" s="615" t="s">
+      <c r="Q2" s="645" t="s">
         <v>143</v>
       </c>
       <c r="R2" s="598"/>
-      <c r="S2" s="657" t="s">
+      <c r="S2" s="634" t="s">
         <v>148</v>
       </c>
       <c r="T2" s="89"/>
@@ -7027,7 +7032,7 @@
       <c r="X2" s="431" t="s">
         <v>156</v>
       </c>
-      <c r="Y2" s="654"/>
+      <c r="Y2" s="658"/>
       <c r="Z2" s="407">
         <v>1</v>
       </c>
@@ -7050,15 +7055,15 @@
         <v>463</v>
       </c>
       <c r="AM2" s="428"/>
-      <c r="AN2" s="636"/>
+      <c r="AN2" s="641"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="618"/>
-      <c r="B3" s="620"/>
-      <c r="C3" s="616"/>
-      <c r="D3" s="622"/>
-      <c r="E3" s="670"/>
-      <c r="F3" s="641"/>
+      <c r="A3" s="667"/>
+      <c r="B3" s="669"/>
+      <c r="C3" s="646"/>
+      <c r="D3" s="671"/>
+      <c r="E3" s="610"/>
+      <c r="F3" s="620"/>
       <c r="G3" s="394" t="s">
         <v>28</v>
       </c>
@@ -7077,17 +7082,17 @@
       <c r="L3" s="201" t="s">
         <v>107</v>
       </c>
-      <c r="M3" s="641"/>
+      <c r="M3" s="620"/>
       <c r="N3" s="69" t="s">
         <v>146</v>
       </c>
-      <c r="O3" s="645"/>
+      <c r="O3" s="650"/>
       <c r="P3" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="Q3" s="616"/>
+      <c r="Q3" s="646"/>
       <c r="R3" s="600"/>
-      <c r="S3" s="658"/>
+      <c r="S3" s="636"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -7095,7 +7100,7 @@
       <c r="X3" s="431" t="s">
         <v>157</v>
       </c>
-      <c r="Y3" s="654"/>
+      <c r="Y3" s="658"/>
       <c r="Z3" s="408">
         <v>1</v>
       </c>
@@ -7104,7 +7109,7 @@
       <c r="AC3" s="100" t="s">
         <v>480</v>
       </c>
-      <c r="AD3" s="656" t="s">
+      <c r="AD3" s="631" t="s">
         <v>455</v>
       </c>
       <c r="AE3" s="257"/>
@@ -7116,16 +7121,16 @@
       <c r="AK3" s="257"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="428"/>
-      <c r="AN3" s="636"/>
+      <c r="AN3" s="641"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="238" t="s">
         <v>183</v>
       </c>
-      <c r="B4" s="633" t="s">
+      <c r="B4" s="682" t="s">
         <v>373</v>
       </c>
-      <c r="C4" s="615" t="s">
+      <c r="C4" s="645" t="s">
         <v>154</v>
       </c>
       <c r="D4" s="347" t="s">
@@ -7134,7 +7139,7 @@
       <c r="E4" s="378">
         <v>2</v>
       </c>
-      <c r="F4" s="641"/>
+      <c r="F4" s="620"/>
       <c r="G4" s="381" t="s">
         <v>201</v>
       </c>
@@ -7151,11 +7156,11 @@
         <v>150</v>
       </c>
       <c r="L4" s="204"/>
-      <c r="M4" s="641"/>
+      <c r="M4" s="620"/>
       <c r="N4" s="174" t="s">
         <v>69</v>
       </c>
-      <c r="O4" s="645"/>
+      <c r="O4" s="650"/>
       <c r="P4" s="2" t="s">
         <v>191</v>
       </c>
@@ -7177,12 +7182,12 @@
       <c r="X4" s="431" t="s">
         <v>158</v>
       </c>
-      <c r="Y4" s="654"/>
+      <c r="Y4" s="658"/>
       <c r="Z4" s="409"/>
       <c r="AA4" s="307"/>
       <c r="AB4" s="209"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="656"/>
+      <c r="AD4" s="631"/>
       <c r="AE4" s="257"/>
       <c r="AF4" s="257"/>
       <c r="AG4" s="16"/>
@@ -7192,37 +7197,37 @@
       <c r="AK4" s="257"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="428"/>
-      <c r="AN4" s="636"/>
+      <c r="AN4" s="641"/>
       <c r="AO4" s="338" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="659" t="s">
+      <c r="A5" s="613" t="s">
         <v>418</v>
       </c>
-      <c r="B5" s="634"/>
-      <c r="C5" s="616"/>
+      <c r="B5" s="683"/>
+      <c r="C5" s="646"/>
       <c r="D5" s="61" t="s">
         <v>153</v>
       </c>
       <c r="E5" s="379">
         <v>1</v>
       </c>
-      <c r="F5" s="641"/>
-      <c r="G5" s="625" t="s">
+      <c r="F5" s="620"/>
+      <c r="G5" s="674" t="s">
         <v>192</v>
       </c>
-      <c r="H5" s="625"/>
-      <c r="I5" s="625"/>
-      <c r="J5" s="625"/>
-      <c r="K5" s="625"/>
-      <c r="L5" s="626"/>
-      <c r="M5" s="641"/>
+      <c r="H5" s="674"/>
+      <c r="I5" s="674"/>
+      <c r="J5" s="674"/>
+      <c r="K5" s="674"/>
+      <c r="L5" s="675"/>
+      <c r="M5" s="620"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
-      <c r="O5" s="645"/>
+      <c r="O5" s="650"/>
       <c r="T5" s="89"/>
       <c r="U5" s="124"/>
       <c r="V5" s="120"/>
@@ -7230,7 +7235,7 @@
       <c r="X5" s="431" t="s">
         <v>159</v>
       </c>
-      <c r="Y5" s="654"/>
+      <c r="Y5" s="658"/>
       <c r="Z5" s="409">
         <v>1</v>
       </c>
@@ -7253,24 +7258,24 @@
       <c r="AK5" s="257"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="428"/>
-      <c r="AN5" s="636"/>
+      <c r="AN5" s="641"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="660"/>
-      <c r="B6" s="631" t="s">
+      <c r="A6" s="614"/>
+      <c r="B6" s="680" t="s">
         <v>177</v>
       </c>
-      <c r="C6" s="661"/>
-      <c r="D6" s="662"/>
-      <c r="F6" s="641"/>
-      <c r="G6" s="627"/>
-      <c r="H6" s="627"/>
-      <c r="I6" s="627"/>
-      <c r="J6" s="627"/>
-      <c r="K6" s="627"/>
-      <c r="L6" s="628"/>
-      <c r="M6" s="641"/>
-      <c r="O6" s="645"/>
+      <c r="C6" s="628"/>
+      <c r="D6" s="629"/>
+      <c r="F6" s="620"/>
+      <c r="G6" s="676"/>
+      <c r="H6" s="676"/>
+      <c r="I6" s="676"/>
+      <c r="J6" s="676"/>
+      <c r="K6" s="676"/>
+      <c r="L6" s="677"/>
+      <c r="M6" s="620"/>
+      <c r="O6" s="650"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
       <c r="V6" s="98" t="s">
@@ -7280,7 +7285,7 @@
       <c r="X6" s="431" t="s">
         <v>160</v>
       </c>
-      <c r="Y6" s="654"/>
+      <c r="Y6" s="658"/>
       <c r="Z6" s="407">
         <v>1</v>
       </c>
@@ -7294,16 +7299,16 @@
       <c r="AF6" s="257"/>
       <c r="AG6" s="257"/>
       <c r="AH6" s="257"/>
-      <c r="AI6" s="650"/>
+      <c r="AI6" s="630"/>
       <c r="AJ6" s="441" t="s">
         <v>458</v>
       </c>
-      <c r="AK6" s="650" t="s">
+      <c r="AK6" s="630" t="s">
         <v>251</v>
       </c>
       <c r="AL6" s="257"/>
       <c r="AM6" s="428"/>
-      <c r="AN6" s="636"/>
+      <c r="AN6" s="641"/>
       <c r="AO6" s="338" t="s">
         <v>470</v>
       </c>
@@ -7312,7 +7317,7 @@
       <c r="A7" s="232" t="s">
         <v>571</v>
       </c>
-      <c r="B7" s="632"/>
+      <c r="B7" s="681"/>
       <c r="C7" s="202" t="s">
         <v>374</v>
       </c>
@@ -7322,7 +7327,7 @@
       <c r="E7" s="265">
         <v>3</v>
       </c>
-      <c r="F7" s="641"/>
+      <c r="F7" s="620"/>
       <c r="G7" s="395">
         <v>0</v>
       </c>
@@ -7341,8 +7346,8 @@
       <c r="L7" s="212">
         <v>0</v>
       </c>
-      <c r="M7" s="641"/>
-      <c r="O7" s="645"/>
+      <c r="M7" s="620"/>
+      <c r="O7" s="650"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
       </c>
@@ -7356,7 +7361,7 @@
       <c r="X7" s="431" t="s">
         <v>161</v>
       </c>
-      <c r="Y7" s="654"/>
+      <c r="Y7" s="658"/>
       <c r="Z7" s="407">
         <v>1</v>
       </c>
@@ -7366,18 +7371,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="257"/>
       <c r="AF7" s="257"/>
-      <c r="AG7" s="656" t="s">
+      <c r="AG7" s="631" t="s">
         <v>454</v>
       </c>
       <c r="AH7" s="257"/>
-      <c r="AI7" s="650"/>
+      <c r="AI7" s="630"/>
       <c r="AJ7" s="257"/>
-      <c r="AK7" s="650"/>
+      <c r="AK7" s="630"/>
       <c r="AL7" s="80" t="s">
         <v>496</v>
       </c>
       <c r="AM7" s="428"/>
-      <c r="AN7" s="636"/>
+      <c r="AN7" s="641"/>
       <c r="AP7" s="76" t="s">
         <v>471</v>
       </c>
@@ -7394,27 +7399,27 @@
         <f>SUM(G7:N9)</f>
         <v>15</v>
       </c>
-      <c r="F8" s="641"/>
-      <c r="G8" s="626">
-        <v>0</v>
-      </c>
-      <c r="H8" s="623" t="s">
+      <c r="F8" s="620"/>
+      <c r="G8" s="675">
+        <v>0</v>
+      </c>
+      <c r="H8" s="672" t="s">
         <v>104</v>
       </c>
       <c r="I8" s="598">
         <v>0</v>
       </c>
-      <c r="J8" s="623" t="s">
+      <c r="J8" s="672" t="s">
         <v>104</v>
       </c>
-      <c r="K8" s="629"/>
-      <c r="L8" s="663"/>
-      <c r="M8" s="642"/>
-      <c r="N8" s="666">
+      <c r="K8" s="678"/>
+      <c r="L8" s="632"/>
+      <c r="M8" s="647"/>
+      <c r="N8" s="637">
         <f>N5+N11</f>
         <v>15</v>
       </c>
-      <c r="O8" s="645"/>
+      <c r="O8" s="650"/>
       <c r="T8" s="103" t="s">
         <v>44</v>
       </c>
@@ -7424,7 +7429,7 @@
       <c r="X8" s="431" t="s">
         <v>162</v>
       </c>
-      <c r="Y8" s="654"/>
+      <c r="Y8" s="658"/>
       <c r="Z8" s="409"/>
       <c r="AA8" s="307"/>
       <c r="AB8" s="209"/>
@@ -7432,14 +7437,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="257"/>
       <c r="AF8" s="257"/>
-      <c r="AG8" s="656"/>
+      <c r="AG8" s="631"/>
       <c r="AH8" s="257"/>
-      <c r="AI8" s="650"/>
+      <c r="AI8" s="630"/>
       <c r="AJ8" s="257"/>
       <c r="AK8" s="257"/>
       <c r="AL8" s="257"/>
       <c r="AM8" s="428"/>
-      <c r="AN8" s="636"/>
+      <c r="AN8" s="641"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="232" t="s">
@@ -7454,17 +7459,17 @@
       <c r="D9" s="348" t="s">
         <v>281</v>
       </c>
-      <c r="F9" s="641"/>
-      <c r="G9" s="628"/>
-      <c r="H9" s="624"/>
+      <c r="F9" s="620"/>
+      <c r="G9" s="677"/>
+      <c r="H9" s="673"/>
       <c r="I9" s="600"/>
-      <c r="J9" s="624"/>
-      <c r="K9" s="630"/>
-      <c r="L9" s="664"/>
-      <c r="M9" s="643"/>
-      <c r="N9" s="667"/>
-      <c r="O9" s="646"/>
-      <c r="S9" s="657" t="s">
+      <c r="J9" s="673"/>
+      <c r="K9" s="679"/>
+      <c r="L9" s="633"/>
+      <c r="M9" s="648"/>
+      <c r="N9" s="638"/>
+      <c r="O9" s="651"/>
+      <c r="S9" s="634" t="s">
         <v>61</v>
       </c>
       <c r="T9" s="89"/>
@@ -7476,7 +7481,7 @@
       <c r="X9" s="431" t="s">
         <v>163</v>
       </c>
-      <c r="Y9" s="654"/>
+      <c r="Y9" s="658"/>
       <c r="Z9" s="410"/>
       <c r="AA9" s="307"/>
       <c r="AB9" s="209"/>
@@ -7486,16 +7491,16 @@
       </c>
       <c r="AE9" s="257"/>
       <c r="AF9" s="257"/>
-      <c r="AG9" s="656"/>
+      <c r="AG9" s="631"/>
       <c r="AH9" s="257"/>
-      <c r="AI9" s="650"/>
+      <c r="AI9" s="630"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="650" t="s">
+      <c r="AK9" s="630" t="s">
         <v>251</v>
       </c>
       <c r="AL9" s="257"/>
       <c r="AM9" s="428"/>
-      <c r="AN9" s="636"/>
+      <c r="AN9" s="641"/>
       <c r="AP9" s="2" t="s">
         <v>508</v>
       </c>
@@ -7512,20 +7517,20 @@
         <f>Boat!W8</f>
         <v>37</v>
       </c>
-      <c r="F10" s="641"/>
+      <c r="F10" s="620"/>
       <c r="N10" s="418" t="s">
         <v>396</v>
       </c>
-      <c r="O10" s="678" t="s">
+      <c r="O10" s="622" t="s">
         <v>102</v>
       </c>
-      <c r="P10" s="647" t="s">
+      <c r="P10" s="652" t="s">
         <v>400</v>
       </c>
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="665"/>
+      <c r="S10" s="635"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>176</v>
@@ -7537,7 +7542,7 @@
       <c r="X10" s="431" t="s">
         <v>164</v>
       </c>
-      <c r="Y10" s="654"/>
+      <c r="Y10" s="658"/>
       <c r="Z10" s="409">
         <v>0</v>
       </c>
@@ -7555,16 +7560,16 @@
       <c r="AF10" s="238" t="s">
         <v>311</v>
       </c>
-      <c r="AG10" s="656"/>
+      <c r="AG10" s="631"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="650"/>
+      <c r="AI10" s="630"/>
       <c r="AJ10" s="257"/>
-      <c r="AK10" s="650"/>
+      <c r="AK10" s="630"/>
       <c r="AL10" s="257"/>
       <c r="AM10" s="442" t="s">
         <v>318</v>
       </c>
-      <c r="AN10" s="636"/>
+      <c r="AN10" s="641"/>
       <c r="AO10" s="204" t="s">
         <v>94</v>
       </c>
@@ -7582,18 +7587,18 @@
       <c r="D11" s="170" t="s">
         <v>355</v>
       </c>
-      <c r="F11" s="641"/>
+      <c r="F11" s="620"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="679"/>
-      <c r="P11" s="648"/>
+      <c r="O11" s="623"/>
+      <c r="P11" s="653"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>220</v>
       </c>
-      <c r="S11" s="665"/>
+      <c r="S11" s="635"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -7603,7 +7608,7 @@
       <c r="X11" s="431" t="s">
         <v>165</v>
       </c>
-      <c r="Y11" s="654"/>
+      <c r="Y11" s="658"/>
       <c r="Z11" s="409"/>
       <c r="AA11" s="307">
         <v>1</v>
@@ -7617,14 +7622,14 @@
       <c r="AF11" s="257" t="s">
         <v>476</v>
       </c>
-      <c r="AG11" s="656"/>
+      <c r="AG11" s="631"/>
       <c r="AH11" s="257"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="257"/>
       <c r="AK11" s="257"/>
       <c r="AL11" s="257"/>
       <c r="AM11" s="428"/>
-      <c r="AN11" s="636"/>
+      <c r="AN11" s="641"/>
       <c r="AP11" s="76" t="s">
         <v>484</v>
       </c>
@@ -7643,7 +7648,7 @@
       <c r="E12" s="224">
         <v>3</v>
       </c>
-      <c r="F12" s="641"/>
+      <c r="F12" s="620"/>
       <c r="G12" s="337" t="s">
         <v>400</v>
       </c>
@@ -7652,16 +7657,16 @@
       </c>
       <c r="I12" s="605"/>
       <c r="J12" s="605"/>
-      <c r="K12" s="683"/>
+      <c r="K12" s="627"/>
       <c r="L12" s="203"/>
       <c r="M12" s="203"/>
       <c r="N12" s="203"/>
-      <c r="O12" s="679"/>
-      <c r="P12" s="648"/>
+      <c r="O12" s="623"/>
+      <c r="P12" s="653"/>
       <c r="R12" s="122" t="s">
         <v>180</v>
       </c>
-      <c r="S12" s="658"/>
+      <c r="S12" s="636"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -7671,7 +7676,7 @@
       <c r="X12" s="431" t="s">
         <v>166</v>
       </c>
-      <c r="Y12" s="654"/>
+      <c r="Y12" s="658"/>
       <c r="Z12" s="407">
         <v>1</v>
       </c>
@@ -7682,16 +7687,16 @@
       <c r="AC12" s="100" t="s">
         <v>481</v>
       </c>
-      <c r="AD12" s="668" t="s">
+      <c r="AD12" s="639" t="s">
         <v>240</v>
       </c>
       <c r="AE12" s="441" t="s">
         <v>239</v>
       </c>
-      <c r="AF12" s="656" t="s">
+      <c r="AF12" s="631" t="s">
         <v>228</v>
       </c>
-      <c r="AG12" s="656"/>
+      <c r="AG12" s="631"/>
       <c r="AH12" s="238" t="s">
         <v>259</v>
       </c>
@@ -7701,10 +7706,10 @@
       <c r="AJ12" s="257"/>
       <c r="AK12" s="257"/>
       <c r="AL12" s="257"/>
-      <c r="AM12" s="651" t="s">
+      <c r="AM12" s="655" t="s">
         <v>249</v>
       </c>
-      <c r="AN12" s="636"/>
+      <c r="AN12" s="641"/>
       <c r="AO12" s="338" t="s">
         <v>96</v>
       </c>
@@ -7716,17 +7721,17 @@
       <c r="E13" s="448">
         <v>-3</v>
       </c>
-      <c r="F13" s="641"/>
+      <c r="F13" s="620"/>
       <c r="G13" s="605" t="s">
         <v>430</v>
       </c>
       <c r="H13" s="605"/>
       <c r="I13" s="605"/>
-      <c r="J13" s="683"/>
+      <c r="J13" s="627"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="679"/>
-      <c r="P13" s="649"/>
+      <c r="O13" s="623"/>
+      <c r="P13" s="654"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
       </c>
@@ -7736,7 +7741,7 @@
       <c r="X13" s="431" t="s">
         <v>167</v>
       </c>
-      <c r="Y13" s="654"/>
+      <c r="Y13" s="658"/>
       <c r="Z13" s="407">
         <v>1</v>
       </c>
@@ -7747,8 +7752,8 @@
         <v>500</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="668"/>
-      <c r="AF13" s="656"/>
+      <c r="AD13" s="639"/>
+      <c r="AF13" s="631"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="238" t="s">
         <v>308</v>
@@ -7759,8 +7764,8 @@
       <c r="AJ13" s="80"/>
       <c r="AK13" s="257"/>
       <c r="AL13" s="257"/>
-      <c r="AM13" s="651"/>
-      <c r="AN13" s="636"/>
+      <c r="AM13" s="655"/>
+      <c r="AN13" s="641"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="450"/>
@@ -7768,18 +7773,18 @@
       <c r="C14" s="459"/>
       <c r="D14" s="452"/>
       <c r="E14" s="453"/>
-      <c r="F14" s="641"/>
+      <c r="F14" s="620"/>
       <c r="G14" s="605" t="s">
         <v>429</v>
       </c>
       <c r="H14" s="605"/>
       <c r="I14" s="605"/>
-      <c r="J14" s="683"/>
+      <c r="J14" s="627"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="679"/>
+      <c r="O14" s="623"/>
       <c r="Q14" s="61" t="s">
         <v>532</v>
       </c>
@@ -7793,24 +7798,24 @@
       <c r="X14" s="431" t="s">
         <v>168</v>
       </c>
-      <c r="Y14" s="654"/>
+      <c r="Y14" s="658"/>
       <c r="Z14" s="407">
         <v>1</v>
       </c>
       <c r="AA14" s="307"/>
       <c r="AB14" s="209"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="668"/>
+      <c r="AD14" s="639"/>
       <c r="AE14" s="257"/>
-      <c r="AF14" s="656"/>
+      <c r="AF14" s="631"/>
       <c r="AG14" s="257"/>
       <c r="AH14" s="257"/>
       <c r="AI14" s="70"/>
       <c r="AJ14" s="257"/>
       <c r="AK14" s="257"/>
       <c r="AL14" s="257"/>
-      <c r="AM14" s="651"/>
-      <c r="AN14" s="636"/>
+      <c r="AM14" s="655"/>
+      <c r="AN14" s="641"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="449" t="s">
@@ -7819,8 +7824,8 @@
       <c r="C15" s="598" t="s">
         <v>373</v>
       </c>
-      <c r="F15" s="641"/>
-      <c r="O15" s="679"/>
+      <c r="F15" s="620"/>
+      <c r="O15" s="623"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -7833,7 +7838,7 @@
       <c r="X15" s="431" t="s">
         <v>169</v>
       </c>
-      <c r="Y15" s="654"/>
+      <c r="Y15" s="658"/>
       <c r="Z15" s="409">
         <v>1</v>
       </c>
@@ -7842,8 +7847,8 @@
       <c r="AC15" s="76" t="s">
         <v>479</v>
       </c>
-      <c r="AD15" s="668"/>
-      <c r="AF15" s="656"/>
+      <c r="AD15" s="639"/>
+      <c r="AF15" s="631"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="238" t="s">
         <v>448</v>
@@ -7856,8 +7861,8 @@
       </c>
       <c r="AK15" s="257"/>
       <c r="AL15" s="257"/>
-      <c r="AM15" s="651"/>
-      <c r="AN15" s="636"/>
+      <c r="AM15" s="655"/>
+      <c r="AN15" s="641"/>
       <c r="AP15" s="76" t="s">
         <v>73</v>
       </c>
@@ -7879,13 +7884,13 @@
       <c r="E16" s="224">
         <v>1</v>
       </c>
-      <c r="F16" s="641"/>
+      <c r="F16" s="620"/>
       <c r="G16" s="337" t="s">
         <v>488</v>
       </c>
       <c r="I16" s="469"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="679"/>
+      <c r="O16" s="623"/>
       <c r="R16" s="435" t="s">
         <v>184</v>
       </c>
@@ -7896,7 +7901,7 @@
       <c r="X16" s="431" t="s">
         <v>170</v>
       </c>
-      <c r="Y16" s="654"/>
+      <c r="Y16" s="658"/>
       <c r="Z16" s="407">
         <v>1</v>
       </c>
@@ -7917,18 +7922,18 @@
       <c r="AM16" s="428" t="s">
         <v>317</v>
       </c>
-      <c r="AN16" s="636"/>
+      <c r="AN16" s="641"/>
       <c r="AP16" s="76" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="641"/>
+      <c r="F17" s="620"/>
       <c r="I17" s="470"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="679"/>
+      <c r="O17" s="623"/>
       <c r="Q17" s="21" t="s">
         <v>530</v>
       </c>
@@ -7948,7 +7953,7 @@
       <c r="X17" s="431" t="s">
         <v>171</v>
       </c>
-      <c r="Y17" s="654"/>
+      <c r="Y17" s="658"/>
       <c r="Z17" s="409"/>
       <c r="AA17" s="307"/>
       <c r="AB17" s="209"/>
@@ -7973,7 +7978,7 @@
       <c r="AK17" s="257"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="428"/>
-      <c r="AN17" s="636"/>
+      <c r="AN17" s="641"/>
       <c r="AO17" s="204" t="s">
         <v>497</v>
       </c>
@@ -7997,21 +8002,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="641"/>
+      <c r="F18" s="620"/>
       <c r="G18" s="337" t="s">
         <v>527</v>
       </c>
       <c r="I18" s="24"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="679"/>
+      <c r="O18" s="623"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="673" t="s">
+      <c r="R18" s="615" t="s">
         <v>535</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="612" t="s">
+      <c r="U18" s="663" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -8021,7 +8026,7 @@
       <c r="X18" s="431" t="s">
         <v>172</v>
       </c>
-      <c r="Y18" s="654"/>
+      <c r="Y18" s="658"/>
       <c r="Z18" s="409">
         <v>1</v>
       </c>
@@ -8032,38 +8037,38 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="257"/>
-      <c r="AF18" s="650" t="s">
+      <c r="AF18" s="630" t="s">
         <v>475</v>
       </c>
       <c r="AG18" s="257"/>
       <c r="AH18" s="70"/>
       <c r="AI18" s="70"/>
-      <c r="AJ18" s="652" t="s">
+      <c r="AJ18" s="656" t="s">
         <v>315</v>
       </c>
       <c r="AK18" s="257"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="428"/>
-      <c r="AN18" s="636"/>
+      <c r="AN18" s="641"/>
       <c r="AP18" s="76" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="641"/>
+      <c r="F19" s="620"/>
       <c r="I19" s="219"/>
-      <c r="O19" s="679"/>
-      <c r="R19" s="674"/>
+      <c r="O19" s="623"/>
+      <c r="R19" s="616"/>
       <c r="S19" s="30" t="s">
         <v>533</v>
       </c>
-      <c r="U19" s="613"/>
+      <c r="U19" s="664"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="431" t="s">
         <v>173</v>
       </c>
-      <c r="Y19" s="654"/>
+      <c r="Y19" s="658"/>
       <c r="Z19" s="407">
         <v>1</v>
       </c>
@@ -8072,17 +8077,17 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="257"/>
-      <c r="AF19" s="650"/>
+      <c r="AF19" s="630"/>
       <c r="AG19" s="257"/>
       <c r="AH19" s="257"/>
       <c r="AI19" s="70"/>
-      <c r="AJ19" s="652"/>
+      <c r="AJ19" s="656"/>
       <c r="AK19" s="460" t="s">
         <v>251</v>
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="428"/>
-      <c r="AN19" s="636"/>
+      <c r="AN19" s="641"/>
       <c r="AP19" s="76" t="s">
         <v>468</v>
       </c>
@@ -8103,24 +8108,24 @@
       <c r="E20" s="437">
         <v>-1</v>
       </c>
-      <c r="F20" s="641"/>
+      <c r="F20" s="620"/>
       <c r="G20" s="337" t="s">
         <v>491</v>
       </c>
       <c r="I20" s="219"/>
-      <c r="O20" s="679"/>
-      <c r="Q20" s="681" t="s">
+      <c r="O20" s="623"/>
+      <c r="Q20" s="625" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="404" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="614"/>
+      <c r="U20" s="665"/>
       <c r="W20" s="405"/>
       <c r="X20" s="432" t="s">
         <v>174</v>
       </c>
-      <c r="Y20" s="654"/>
+      <c r="Y20" s="658"/>
       <c r="Z20" s="411">
         <v>1</v>
       </c>
@@ -8145,7 +8150,7 @@
       <c r="AM20" s="381" t="s">
         <v>249</v>
       </c>
-      <c r="AN20" s="636"/>
+      <c r="AN20" s="641"/>
       <c r="AO20" s="338" t="s">
         <v>460</v>
       </c>
@@ -8166,20 +8171,20 @@
       <c r="E21" s="265">
         <v>0</v>
       </c>
-      <c r="F21" s="641"/>
+      <c r="F21" s="620"/>
       <c r="I21" s="219"/>
-      <c r="O21" s="679"/>
-      <c r="Q21" s="682"/>
+      <c r="O21" s="623"/>
+      <c r="Q21" s="626"/>
       <c r="T21" s="422"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="609"/>
+      <c r="V21" s="660"/>
       <c r="W21" s="426" t="s">
         <v>175</v>
       </c>
       <c r="X21" s="429" t="s">
         <v>186</v>
       </c>
-      <c r="Y21" s="654"/>
+      <c r="Y21" s="658"/>
       <c r="Z21" s="445">
         <v>3</v>
       </c>
@@ -8210,15 +8215,15 @@
       <c r="AM21" s="428" t="s">
         <v>544</v>
       </c>
-      <c r="AN21" s="636"/>
+      <c r="AN21" s="641"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="641"/>
+      <c r="F22" s="620"/>
       <c r="G22" s="337" t="s">
         <v>489</v>
       </c>
       <c r="I22" s="219"/>
-      <c r="O22" s="679"/>
+      <c r="O22" s="623"/>
       <c r="R22" s="434" t="s">
         <v>44</v>
       </c>
@@ -8226,14 +8231,14 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="610"/>
+      <c r="V22" s="661"/>
       <c r="W22" s="426" t="s">
         <v>175</v>
       </c>
       <c r="X22" s="429" t="s">
         <v>187</v>
       </c>
-      <c r="Y22" s="654"/>
+      <c r="Y22" s="658"/>
       <c r="Z22" s="415"/>
       <c r="AA22" s="10"/>
       <c r="AB22" s="415"/>
@@ -8244,7 +8249,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="650" t="s">
+      <c r="AJ22" s="630" t="s">
         <v>472</v>
       </c>
       <c r="AK22" s="257"/>
@@ -8252,7 +8257,7 @@
         <v>478</v>
       </c>
       <c r="AM22" s="300"/>
-      <c r="AN22" s="636"/>
+      <c r="AN22" s="641"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="231" t="s">
@@ -8270,22 +8275,22 @@
       <c r="E23" s="225">
         <v>1</v>
       </c>
-      <c r="F23" s="641"/>
+      <c r="F23" s="620"/>
       <c r="I23" s="219"/>
-      <c r="O23" s="679"/>
-      <c r="Q23" s="681" t="s">
+      <c r="O23" s="623"/>
+      <c r="Q23" s="625" t="s">
         <v>144</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="420" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="610"/>
+      <c r="V23" s="661"/>
       <c r="W23" s="148"/>
       <c r="X23" s="429" t="s">
         <v>188</v>
       </c>
-      <c r="Y23" s="654"/>
+      <c r="Y23" s="658"/>
       <c r="Z23" s="17"/>
       <c r="AA23" s="10"/>
       <c r="AB23" s="415"/>
@@ -8296,13 +8301,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="650"/>
+      <c r="AJ23" s="630"/>
       <c r="AK23" s="257"/>
       <c r="AL23" s="80" t="s">
         <v>507</v>
       </c>
       <c r="AM23" s="300"/>
-      <c r="AN23" s="636"/>
+      <c r="AN23" s="641"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="440" t="s">
@@ -8320,23 +8325,23 @@
       <c r="E24" s="436">
         <v>1</v>
       </c>
-      <c r="F24" s="641"/>
+      <c r="F24" s="620"/>
       <c r="G24" s="61" t="s">
         <v>490</v>
       </c>
       <c r="I24" s="219"/>
-      <c r="O24" s="679"/>
-      <c r="Q24" s="682"/>
+      <c r="O24" s="623"/>
+      <c r="Q24" s="626"/>
       <c r="T24" s="17"/>
       <c r="U24" s="227" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="610"/>
+      <c r="V24" s="661"/>
       <c r="W24" s="148"/>
       <c r="X24" s="429" t="s">
         <v>185</v>
       </c>
-      <c r="Y24" s="654"/>
+      <c r="Y24" s="658"/>
       <c r="Z24" s="17"/>
       <c r="AA24" s="10"/>
       <c r="AB24" s="415"/>
@@ -8355,12 +8360,12 @@
         <v>463</v>
       </c>
       <c r="AM24" s="300"/>
-      <c r="AN24" s="636"/>
+      <c r="AN24" s="641"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="641"/>
+      <c r="F25" s="620"/>
       <c r="I25" s="219"/>
-      <c r="O25" s="679"/>
+      <c r="O25" s="623"/>
       <c r="P25" s="204" t="s">
         <v>280</v>
       </c>
@@ -8373,12 +8378,12 @@
       <c r="U25" s="400" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="611"/>
+      <c r="V25" s="662"/>
       <c r="W25" s="148"/>
       <c r="X25" s="429" t="s">
         <v>189</v>
       </c>
-      <c r="Y25" s="654"/>
+      <c r="Y25" s="658"/>
       <c r="Z25" s="17"/>
       <c r="AA25" s="10"/>
       <c r="AB25" s="415"/>
@@ -8395,7 +8400,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="300"/>
-      <c r="AN25" s="636"/>
+      <c r="AN25" s="641"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="231" t="s">
@@ -8413,17 +8418,17 @@
       <c r="E26" s="380">
         <v>1</v>
       </c>
-      <c r="F26" s="641"/>
+      <c r="F26" s="620"/>
       <c r="G26" s="337" t="s">
         <v>487</v>
       </c>
       <c r="I26" s="219"/>
-      <c r="O26" s="679"/>
-      <c r="P26" s="638" t="s">
+      <c r="O26" s="623"/>
+      <c r="P26" s="643" t="s">
         <v>525</v>
       </c>
-      <c r="Q26" s="639"/>
-      <c r="R26" s="675" t="s">
+      <c r="Q26" s="644"/>
+      <c r="R26" s="617" t="s">
         <v>534</v>
       </c>
       <c r="T26" s="178"/>
@@ -8435,7 +8440,7 @@
       <c r="X26" s="429" t="s">
         <v>181</v>
       </c>
-      <c r="Y26" s="654"/>
+      <c r="Y26" s="658"/>
       <c r="Z26" s="17"/>
       <c r="AA26" s="10"/>
       <c r="AB26" s="415"/>
@@ -8462,7 +8467,7 @@
       <c r="AM26" s="442" t="s">
         <v>456</v>
       </c>
-      <c r="AN26" s="636"/>
+      <c r="AN26" s="641"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -8474,13 +8479,13 @@
       <c r="E27" s="265" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="677"/>
+      <c r="F27" s="621"/>
       <c r="G27" s="61" t="s">
         <v>543</v>
       </c>
       <c r="I27" s="220"/>
-      <c r="O27" s="680"/>
-      <c r="R27" s="676"/>
+      <c r="O27" s="624"/>
+      <c r="R27" s="618"/>
       <c r="S27" s="421" t="s">
         <v>54</v>
       </c>
@@ -8493,7 +8498,7 @@
       <c r="X27" s="429" t="s">
         <v>529</v>
       </c>
-      <c r="Y27" s="655"/>
+      <c r="Y27" s="659"/>
       <c r="Z27" s="161"/>
       <c r="AA27" s="13"/>
       <c r="AB27" s="416"/>
@@ -8510,32 +8515,26 @@
       <c r="AM27" s="381" t="s">
         <v>319</v>
       </c>
-      <c r="AN27" s="637"/>
+      <c r="AN27" s="642"/>
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="F2:F27"/>
-    <mergeCell ref="O10:O27"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AI6:AI10"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AG7:AG12"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="V21:V25"/>
+    <mergeCell ref="U18:U20"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="G5:L6"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B4:B5"/>
     <mergeCell ref="AN1:AN27"/>
     <mergeCell ref="P26:Q26"/>
     <mergeCell ref="Q2:Q3"/>
@@ -8552,22 +8551,28 @@
     <mergeCell ref="AD3:AD4"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="R2:R3"/>
-    <mergeCell ref="V21:V25"/>
-    <mergeCell ref="U18:U20"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="G5:L6"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="AI6:AI10"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AG7:AG12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="O10:O27"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8604,12 +8609,12 @@
       <c r="B1" s="603" t="s">
         <v>310</v>
       </c>
-      <c r="C1" s="683"/>
+      <c r="C1" s="627"/>
       <c r="D1" s="204"/>
       <c r="J1" s="603" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="683"/>
+      <c r="K1" s="627"/>
       <c r="L1" s="195" t="s">
         <v>330</v>
       </c>
@@ -9012,7 +9017,7 @@
       <c r="P1" s="398" t="s">
         <v>397</v>
       </c>
-      <c r="Q1" s="714" t="s">
+      <c r="Q1" s="701" t="s">
         <v>180</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -9036,7 +9041,7 @@
       <c r="AA1" s="517" t="s">
         <v>437</v>
       </c>
-      <c r="AB1" s="708" t="s">
+      <c r="AB1" s="695" t="s">
         <v>593</v>
       </c>
       <c r="AC1" s="99" t="s">
@@ -9058,32 +9063,32 @@
       </c>
     </row>
     <row r="2" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="693">
+      <c r="A2" s="706">
         <f ca="1">TODAY()</f>
         <v>45293</v>
       </c>
-      <c r="B2" s="695" t="s">
+      <c r="B2" s="708" t="s">
         <v>379</v>
       </c>
-      <c r="C2" s="615" t="s">
+      <c r="C2" s="645" t="s">
         <v>357</v>
       </c>
-      <c r="D2" s="697" t="s">
+      <c r="D2" s="710" t="s">
         <v>102</v>
       </c>
-      <c r="E2" s="699" t="s">
+      <c r="E2" s="712" t="s">
         <v>64</v>
       </c>
       <c r="F2" s="191" t="s">
         <v>218</v>
       </c>
-      <c r="G2" s="659" t="s">
+      <c r="G2" s="613" t="s">
         <v>372</v>
       </c>
       <c r="H2" s="206" t="s">
         <v>218</v>
       </c>
-      <c r="I2" s="705" t="s">
+      <c r="I2" s="692" t="s">
         <v>102</v>
       </c>
       <c r="J2" s="396" t="s">
@@ -9107,7 +9112,7 @@
       <c r="P2" s="399">
         <v>40</v>
       </c>
-      <c r="Q2" s="715"/>
+      <c r="Q2" s="702"/>
       <c r="R2" s="21">
         <f>R7+R20</f>
         <v>2</v>
@@ -9132,7 +9137,7 @@
         <f>IF((Z2+T2)&gt;0,0,-1)</f>
         <v>0</v>
       </c>
-      <c r="AB2" s="709"/>
+      <c r="AB2" s="696"/>
       <c r="AC2" s="35"/>
       <c r="AH2" s="6" t="s">
         <v>344</v>
@@ -9147,14 +9152,14 @@
       </c>
     </row>
     <row r="3" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="694"/>
-      <c r="B3" s="696"/>
-      <c r="C3" s="616"/>
-      <c r="D3" s="698"/>
-      <c r="E3" s="700"/>
-      <c r="G3" s="660"/>
+      <c r="A3" s="707"/>
+      <c r="B3" s="709"/>
+      <c r="C3" s="646"/>
+      <c r="D3" s="711"/>
+      <c r="E3" s="713"/>
+      <c r="G3" s="614"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="706"/>
+      <c r="I3" s="693"/>
       <c r="K3" s="24">
         <v>2</v>
       </c>
@@ -9169,7 +9174,7 @@
       <c r="V3" s="470"/>
       <c r="W3" s="6"/>
       <c r="X3" s="470"/>
-      <c r="AB3" s="709"/>
+      <c r="AB3" s="696"/>
       <c r="AC3" s="35"/>
       <c r="AE3" s="100" t="s">
         <v>588</v>
@@ -9198,10 +9203,10 @@
         <v>380</v>
       </c>
       <c r="B4" s="243"/>
-      <c r="C4" s="701" t="s">
+      <c r="C4" s="714" t="s">
         <v>177</v>
       </c>
-      <c r="I4" s="706"/>
+      <c r="I4" s="693"/>
       <c r="R4" s="471" t="s">
         <v>588</v>
       </c>
@@ -9213,7 +9218,7 @@
       <c r="V4" s="470"/>
       <c r="W4" s="6"/>
       <c r="X4" s="470"/>
-      <c r="AB4" s="709"/>
+      <c r="AB4" s="696"/>
       <c r="AC4" s="35"/>
       <c r="AE4" s="20"/>
       <c r="AF4" s="100" t="s">
@@ -9242,7 +9247,7 @@
       <c r="B5" s="100" t="s">
         <v>357</v>
       </c>
-      <c r="C5" s="702"/>
+      <c r="C5" s="715"/>
       <c r="D5" s="222" t="s">
         <v>102</v>
       </c>
@@ -9258,7 +9263,7 @@
       <c r="H5" s="206" t="s">
         <v>218</v>
       </c>
-      <c r="I5" s="706"/>
+      <c r="I5" s="693"/>
       <c r="J5" s="397" t="s">
         <v>268</v>
       </c>
@@ -9285,7 +9290,7 @@
       <c r="V5" s="468"/>
       <c r="W5" s="6"/>
       <c r="X5" s="468"/>
-      <c r="AB5" s="709"/>
+      <c r="AB5" s="696"/>
       <c r="AC5" s="2" t="s">
         <v>591</v>
       </c>
@@ -9305,19 +9310,19 @@
       <c r="AL5" s="468"/>
     </row>
     <row r="6" spans="1:38" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="690" t="s">
+      <c r="A6" s="703" t="s">
         <v>285</v>
       </c>
       <c r="B6" s="105" t="s">
         <v>198</v>
       </c>
-      <c r="C6" s="661"/>
-      <c r="D6" s="662"/>
+      <c r="C6" s="628"/>
+      <c r="D6" s="629"/>
       <c r="E6" s="96">
         <v>1</v>
       </c>
       <c r="G6" s="599"/>
-      <c r="I6" s="706"/>
+      <c r="I6" s="693"/>
       <c r="P6" s="61" t="s">
         <v>591</v>
       </c>
@@ -9329,7 +9334,7 @@
         <f>S7+S11-SUM(V2:V10)</f>
         <v>3</v>
       </c>
-      <c r="AB6" s="709"/>
+      <c r="AB6" s="696"/>
       <c r="AC6" s="35"/>
       <c r="AE6" s="64">
         <f>AE7-SUM(AL2:AL10)+AE11</f>
@@ -9345,7 +9350,7 @@
       <c r="AL6" s="112"/>
     </row>
     <row r="7" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="691"/>
+      <c r="A7" s="704"/>
       <c r="B7" s="100" t="s">
         <v>154</v>
       </c>
@@ -9356,7 +9361,7 @@
         <v>135</v>
       </c>
       <c r="G7" s="599"/>
-      <c r="I7" s="706"/>
+      <c r="I7" s="693"/>
       <c r="M7" s="16" t="s">
         <v>347</v>
       </c>
@@ -9386,7 +9391,7 @@
         <v>249</v>
       </c>
       <c r="X7" s="469"/>
-      <c r="AB7" s="709"/>
+      <c r="AB7" s="696"/>
       <c r="AC7" s="99" t="s">
         <v>592</v>
       </c>
@@ -9414,7 +9419,7 @@
       <c r="AL7" s="24"/>
     </row>
     <row r="8" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="692"/>
+      <c r="A8" s="705"/>
       <c r="B8" s="212" t="s">
         <v>28</v>
       </c>
@@ -9423,7 +9428,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="599"/>
-      <c r="I8" s="706"/>
+      <c r="I8" s="693"/>
       <c r="N8" s="80"/>
       <c r="U8" s="6"/>
       <c r="V8" s="24"/>
@@ -9431,7 +9436,7 @@
         <v>611</v>
       </c>
       <c r="X8" s="470"/>
-      <c r="AB8" s="709"/>
+      <c r="AB8" s="696"/>
       <c r="AC8" s="515"/>
       <c r="AH8" s="6" t="s">
         <v>610</v>
@@ -9462,7 +9467,7 @@
       </c>
       <c r="G9" s="599"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="706"/>
+      <c r="I9" s="693"/>
       <c r="M9" s="19" t="s">
         <v>524</v>
       </c>
@@ -9473,7 +9478,7 @@
         <v>603</v>
       </c>
       <c r="X9" s="470"/>
-      <c r="AB9" s="709"/>
+      <c r="AB9" s="696"/>
       <c r="AC9" s="515"/>
       <c r="AE9" s="20"/>
       <c r="AF9" s="20"/>
@@ -9501,7 +9506,7 @@
         <v>37</v>
       </c>
       <c r="G10" s="599"/>
-      <c r="I10" s="706"/>
+      <c r="I10" s="693"/>
       <c r="J10" s="24" t="s">
         <v>372</v>
       </c>
@@ -9516,7 +9521,7 @@
       <c r="V10" s="470"/>
       <c r="W10" s="6"/>
       <c r="X10" s="470"/>
-      <c r="AB10" s="709"/>
+      <c r="AB10" s="696"/>
       <c r="AC10" s="515"/>
       <c r="AE10" s="20"/>
       <c r="AF10" s="20"/>
@@ -9544,7 +9549,7 @@
         <v>265</v>
       </c>
       <c r="G11" s="599"/>
-      <c r="I11" s="706"/>
+      <c r="I11" s="693"/>
       <c r="J11" s="24" t="s">
         <v>194</v>
       </c>
@@ -9570,13 +9575,13 @@
       <c r="S11" s="24">
         <v>3</v>
       </c>
-      <c r="U11" s="711" t="s">
+      <c r="U11" s="698" t="s">
         <v>557</v>
       </c>
-      <c r="V11" s="712"/>
-      <c r="W11" s="712"/>
-      <c r="X11" s="713"/>
-      <c r="AB11" s="710"/>
+      <c r="V11" s="699"/>
+      <c r="W11" s="699"/>
+      <c r="X11" s="700"/>
+      <c r="AB11" s="697"/>
       <c r="AC11" s="99" t="s">
         <v>594</v>
       </c>
@@ -9590,13 +9595,13 @@
         <v>3</v>
       </c>
       <c r="AG11" s="414"/>
-      <c r="AH11" s="711" t="s">
+      <c r="AH11" s="698" t="s">
         <v>602</v>
       </c>
-      <c r="AI11" s="712"/>
-      <c r="AJ11" s="712"/>
-      <c r="AK11" s="712"/>
-      <c r="AL11" s="713"/>
+      <c r="AI11" s="699"/>
+      <c r="AJ11" s="699"/>
+      <c r="AK11" s="699"/>
+      <c r="AL11" s="700"/>
     </row>
     <row r="12" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="227" t="s">
@@ -9607,7 +9612,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="599"/>
-      <c r="I12" s="706"/>
+      <c r="I12" s="693"/>
       <c r="J12" s="24" t="s">
         <v>515</v>
       </c>
@@ -9640,7 +9645,7 @@
       </c>
       <c r="D13" s="20"/>
       <c r="G13" s="599"/>
-      <c r="I13" s="706"/>
+      <c r="I13" s="693"/>
       <c r="J13" s="108" t="s">
         <v>547</v>
       </c>
@@ -9684,7 +9689,7 @@
       <c r="H14" s="206" t="s">
         <v>218</v>
       </c>
-      <c r="I14" s="706"/>
+      <c r="I14" s="693"/>
       <c r="U14" s="67" t="s">
         <v>80</v>
       </c>
@@ -9711,7 +9716,7 @@
       <c r="H15" s="271">
         <v>0</v>
       </c>
-      <c r="I15" s="706"/>
+      <c r="I15" s="693"/>
       <c r="J15" s="108" t="s">
         <v>153</v>
       </c>
@@ -9742,7 +9747,7 @@
       <c r="D16" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="I16" s="706"/>
+      <c r="I16" s="693"/>
       <c r="K16" s="100" t="s">
         <v>44</v>
       </c>
@@ -9786,7 +9791,7 @@
       <c r="G17" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="I17" s="706"/>
+      <c r="I17" s="693"/>
       <c r="L17" s="2" t="s">
         <v>426</v>
       </c>
@@ -9800,13 +9805,13 @@
     </row>
     <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
-      <c r="I18" s="706"/>
+      <c r="I18" s="693"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="703" t="s">
+      <c r="O18" s="690" t="s">
         <v>516</v>
       </c>
-      <c r="P18" s="704"/>
+      <c r="P18" s="691"/>
       <c r="Q18" s="127" t="s">
         <v>44</v>
       </c>
@@ -9828,7 +9833,7 @@
       </c>
     </row>
     <row r="19" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="706"/>
+      <c r="I19" s="693"/>
       <c r="M19" s="21" t="s">
         <v>425</v>
       </c>
@@ -9860,7 +9865,7 @@
       <c r="G20" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="I20" s="706"/>
+      <c r="I20" s="693"/>
       <c r="K20" s="19" t="s">
         <v>422</v>
       </c>
@@ -9889,7 +9894,7 @@
       <c r="X20" s="468"/>
     </row>
     <row r="21" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="706"/>
+      <c r="I21" s="693"/>
       <c r="M21" s="216" t="s">
         <v>411</v>
       </c>
@@ -9919,7 +9924,7 @@
       <c r="G22" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="I22" s="706"/>
+      <c r="I22" s="693"/>
       <c r="P22" s="99" t="s">
         <v>590</v>
       </c>
@@ -9934,7 +9939,7 @@
       <c r="E23" s="283" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="706"/>
+      <c r="I23" s="693"/>
       <c r="Q23" s="24">
         <f>SUM(V23:V31)</f>
         <v>7</v>
@@ -9951,7 +9956,7 @@
       </c>
     </row>
     <row r="24" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="706"/>
+      <c r="I24" s="693"/>
       <c r="U24" s="35"/>
       <c r="V24" s="509">
         <v>1</v>
@@ -9979,7 +9984,7 @@
       <c r="H25" s="191" t="s">
         <v>266</v>
       </c>
-      <c r="I25" s="706"/>
+      <c r="I25" s="693"/>
       <c r="J25" s="397" t="s">
         <v>269</v>
       </c>
@@ -10024,7 +10029,7 @@
       <c r="H26" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="I26" s="706"/>
+      <c r="I26" s="693"/>
       <c r="K26" s="24">
         <v>15</v>
       </c>
@@ -10059,7 +10064,7 @@
       </c>
     </row>
     <row r="27" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="706"/>
+      <c r="I27" s="693"/>
       <c r="O27" s="2" t="s">
         <v>98</v>
       </c>
@@ -10086,7 +10091,7 @@
       <c r="E28" s="215">
         <v>2</v>
       </c>
-      <c r="I28" s="706"/>
+      <c r="I28" s="693"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="142"/>
@@ -10108,7 +10113,7 @@
       <c r="H29" s="191" t="s">
         <v>267</v>
       </c>
-      <c r="I29" s="707"/>
+      <c r="I29" s="694"/>
       <c r="J29" s="324"/>
       <c r="L29" s="96" t="s">
         <v>273</v>
@@ -10166,13 +10171,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I2:I29"/>
-    <mergeCell ref="AB1:AB11"/>
-    <mergeCell ref="AH11:AL11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="U11:X11"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="G5:G14"/>
     <mergeCell ref="A2:A3"/>
@@ -10184,6 +10182,13 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C2:C3"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I2:I29"/>
+    <mergeCell ref="AB1:AB11"/>
+    <mergeCell ref="AH11:AL11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="U11:X11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10194,8 +10199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AT37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10295,14 +10300,14 @@
         <f ca="1">TODAY()</f>
         <v>45293</v>
       </c>
-      <c r="T1" s="742"/>
+      <c r="T1" s="735"/>
       <c r="U1" s="142"/>
       <c r="V1" s="6"/>
       <c r="W1" s="6"/>
-      <c r="X1" s="726" t="s">
+      <c r="X1" s="719" t="s">
         <v>441</v>
       </c>
-      <c r="Y1" s="727"/>
+      <c r="Y1" s="720"/>
       <c r="Z1" s="306">
         <f>68-(W8+Y3+X3+U3)</f>
         <v>0</v>
@@ -10318,27 +10323,27 @@
       <c r="AD1" s="302" t="s">
         <v>44</v>
       </c>
-      <c r="AE1" s="728" t="s">
+      <c r="AE1" s="721" t="s">
         <v>190</v>
       </c>
-      <c r="AF1" s="729"/>
-      <c r="AG1" s="730"/>
-      <c r="AH1" s="731" t="s">
+      <c r="AF1" s="722"/>
+      <c r="AG1" s="723"/>
+      <c r="AH1" s="724" t="s">
         <v>293</v>
       </c>
-      <c r="AI1" s="732"/>
-      <c r="AJ1" s="733"/>
-      <c r="AK1" s="659" t="s">
+      <c r="AI1" s="725"/>
+      <c r="AJ1" s="726"/>
+      <c r="AK1" s="613" t="s">
         <v>613</v>
       </c>
       <c r="AL1" s="550" t="s">
         <v>614</v>
       </c>
-      <c r="AM1" s="723" t="s">
+      <c r="AM1" s="716" t="s">
         <v>444</v>
       </c>
-      <c r="AN1" s="724"/>
-      <c r="AO1" s="725"/>
+      <c r="AN1" s="717"/>
+      <c r="AO1" s="718"/>
       <c r="AR1" s="142"/>
     </row>
     <row r="2" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10351,29 +10356,29 @@
       </c>
       <c r="J2" s="318">
         <f>K2+L2</f>
-        <v>26</v>
-      </c>
-      <c r="K2" s="721">
+        <v>29</v>
+      </c>
+      <c r="K2" s="743">
         <f>SUM(K4:K37)</f>
-        <v>6</v>
-      </c>
-      <c r="L2" s="719">
+        <v>7</v>
+      </c>
+      <c r="L2" s="741">
         <f>SUM(L4:L37)</f>
-        <v>20</v>
-      </c>
-      <c r="M2" s="734">
+        <v>22</v>
+      </c>
+      <c r="M2" s="727">
         <f>SUM(M5:M30)</f>
         <v>0</v>
       </c>
-      <c r="N2" s="736">
+      <c r="N2" s="729">
         <f>SUM(N4:N29)</f>
         <v>8</v>
       </c>
-      <c r="O2" s="738">
+      <c r="O2" s="731">
         <f>SUM(O4:O29)</f>
         <v>11</v>
       </c>
-      <c r="P2" s="666">
+      <c r="P2" s="637">
         <f>SUM(N30:N37)* (-1)</f>
         <v>-1</v>
       </c>
@@ -10386,14 +10391,14 @@
       <c r="S2" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="T2" s="743"/>
+      <c r="T2" s="736"/>
       <c r="U2" s="537" t="s">
         <v>262</v>
       </c>
       <c r="V2" s="482" t="s">
         <v>219</v>
       </c>
-      <c r="W2" s="740" t="s">
+      <c r="W2" s="733" t="s">
         <v>234</v>
       </c>
       <c r="X2" s="483" t="s">
@@ -10435,7 +10440,7 @@
       <c r="AJ2" s="150" t="s">
         <v>288</v>
       </c>
-      <c r="AK2" s="660"/>
+      <c r="AK2" s="614"/>
       <c r="AL2" s="591" t="s">
         <v>288</v>
       </c>
@@ -10463,12 +10468,12 @@
         <f>V3+X3+Y3+U3</f>
         <v>68</v>
       </c>
-      <c r="K3" s="722"/>
-      <c r="L3" s="720"/>
-      <c r="M3" s="735"/>
-      <c r="N3" s="737"/>
-      <c r="O3" s="739"/>
-      <c r="P3" s="667"/>
+      <c r="K3" s="744"/>
+      <c r="L3" s="742"/>
+      <c r="M3" s="728"/>
+      <c r="N3" s="730"/>
+      <c r="O3" s="732"/>
+      <c r="P3" s="638"/>
       <c r="Q3" s="172">
         <f>(M2+N2)-Y3</f>
         <v>0</v>
@@ -10476,7 +10481,7 @@
       <c r="S3" s="159" t="s">
         <v>244</v>
       </c>
-      <c r="T3" s="744"/>
+      <c r="T3" s="737"/>
       <c r="U3" s="538">
         <f>SUM(U4:U29)</f>
         <v>14</v>
@@ -10485,7 +10490,7 @@
         <f>SUM(V4:V29)</f>
         <v>37</v>
       </c>
-      <c r="W3" s="741"/>
+      <c r="W3" s="734"/>
       <c r="X3" s="485">
         <f t="shared" ref="X3:AC3" si="0">SUM(X4:X29)</f>
         <v>9</v>
@@ -10579,7 +10584,9 @@
       <c r="H4" s="271"/>
       <c r="I4" s="271"/>
       <c r="J4" s="569"/>
-      <c r="K4" s="573"/>
+      <c r="K4" s="573">
+        <v>1</v>
+      </c>
       <c r="L4" s="579">
         <v>1</v>
       </c>
@@ -10591,7 +10598,7 @@
         <f>AC4</f>
         <v>0</v>
       </c>
-      <c r="P4" s="716"/>
+      <c r="P4" s="738"/>
       <c r="Q4" s="20"/>
       <c r="R4" s="2" t="s">
         <v>334</v>
@@ -10675,7 +10682,7 @@
         <f>AC5</f>
         <v>0</v>
       </c>
-      <c r="P5" s="717"/>
+      <c r="P5" s="739"/>
       <c r="Q5" s="20"/>
       <c r="R5" s="2" t="s">
         <v>340</v>
@@ -10769,7 +10776,7 @@
         <f>AC6</f>
         <v>1</v>
       </c>
-      <c r="P6" s="717"/>
+      <c r="P6" s="739"/>
       <c r="Q6" s="54" t="s">
         <v>335</v>
       </c>
@@ -10874,7 +10881,7 @@
         <f>AC7</f>
         <v>1</v>
       </c>
-      <c r="P7" s="717"/>
+      <c r="P7" s="739"/>
       <c r="Q7" s="20"/>
       <c r="R7" s="2" t="s">
         <v>335</v>
@@ -10990,7 +10997,7 @@
         <f t="shared" ref="O8:O37" si="10">AC8</f>
         <v>0</v>
       </c>
-      <c r="P8" s="717"/>
+      <c r="P8" s="739"/>
       <c r="Q8" s="108" t="s">
         <v>233</v>
       </c>
@@ -11072,7 +11079,9 @@
         <v>352</v>
       </c>
       <c r="K9" s="574"/>
-      <c r="L9" s="580"/>
+      <c r="L9" s="580">
+        <v>1</v>
+      </c>
       <c r="M9" s="327"/>
       <c r="N9" s="107">
         <v>0</v>
@@ -11081,7 +11090,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P9" s="717"/>
+      <c r="P9" s="739"/>
       <c r="Q9" s="108" t="s">
         <v>335</v>
       </c>
@@ -11186,7 +11195,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P10" s="717"/>
+      <c r="P10" s="739"/>
       <c r="Q10" s="20"/>
       <c r="R10" s="2" t="s">
         <v>340</v>
@@ -11267,7 +11276,9 @@
         <v>305</v>
       </c>
       <c r="K11" s="574"/>
-      <c r="L11" s="580"/>
+      <c r="L11" s="580">
+        <v>1</v>
+      </c>
       <c r="M11" s="328"/>
       <c r="N11" s="107">
         <v>0</v>
@@ -11276,7 +11287,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P11" s="717"/>
+      <c r="P11" s="739"/>
       <c r="Q11" s="108" t="s">
         <v>335</v>
       </c>
@@ -11341,14 +11352,14 @@
       <c r="AR11" s="508"/>
     </row>
     <row r="12" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="626" t="s">
+      <c r="A12" s="675" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
         <v>13</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="E12" s="681" t="s">
+      <c r="E12" s="625" t="s">
         <v>56</v>
       </c>
       <c r="G12" s="262"/>
@@ -11373,7 +11384,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P12" s="717"/>
+      <c r="P12" s="739"/>
       <c r="Q12" s="108" t="s">
         <v>335</v>
       </c>
@@ -11450,14 +11461,14 @@
       </c>
     </row>
     <row r="13" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="628"/>
+      <c r="A13" s="677"/>
       <c r="B13" s="583">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="682"/>
+      <c r="E13" s="626"/>
       <c r="F13" s="172">
         <v>0</v>
       </c>
@@ -11481,7 +11492,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P13" s="717"/>
+      <c r="P13" s="739"/>
       <c r="Q13" s="108" t="s">
         <v>335</v>
       </c>
@@ -11563,7 +11574,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P14" s="717"/>
+      <c r="P14" s="739"/>
       <c r="Q14" s="20"/>
       <c r="R14" s="200" t="s">
         <v>339</v>
@@ -11666,7 +11677,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P15" s="717"/>
+      <c r="P15" s="739"/>
       <c r="Q15" s="20"/>
       <c r="R15" s="200" t="s">
         <v>339</v>
@@ -11760,7 +11771,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P16" s="717"/>
+      <c r="P16" s="739"/>
       <c r="Q16" s="108" t="s">
         <v>335</v>
       </c>
@@ -11861,7 +11872,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P17" s="717"/>
+      <c r="P17" s="739"/>
       <c r="Q17" s="20"/>
       <c r="R17" s="2" t="s">
         <v>341</v>
@@ -11961,7 +11972,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P18" s="717"/>
+      <c r="P18" s="739"/>
       <c r="Q18" s="108" t="s">
         <v>335</v>
       </c>
@@ -12040,9 +12051,7 @@
       <c r="K19" s="575">
         <v>2</v>
       </c>
-      <c r="L19" s="581">
-        <v>0</v>
-      </c>
+      <c r="L19" s="581"/>
       <c r="M19" s="118"/>
       <c r="N19" s="107">
         <v>1</v>
@@ -12051,7 +12060,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P19" s="717"/>
+      <c r="P19" s="739"/>
       <c r="Q19" s="20"/>
       <c r="R19" s="2" t="s">
         <v>334</v>
@@ -12159,11 +12168,11 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P20" s="718"/>
+      <c r="P20" s="740"/>
       <c r="Q20" s="605" t="s">
         <v>335</v>
       </c>
-      <c r="R20" s="683"/>
+      <c r="R20" s="627"/>
       <c r="S20" s="534" t="s">
         <v>85</v>
       </c>
@@ -12425,7 +12434,7 @@
     </row>
     <row r="23" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="24"/>
-      <c r="E23" s="633" t="s">
+      <c r="E23" s="682" t="s">
         <v>289</v>
       </c>
       <c r="F23" s="180"/>
@@ -12530,7 +12539,7 @@
       <c r="C24" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="E24" s="634"/>
+      <c r="E24" s="683"/>
       <c r="F24" s="172"/>
       <c r="H24" s="42"/>
       <c r="J24" s="570" t="s">
@@ -12539,9 +12548,7 @@
       <c r="K24" s="574">
         <v>1</v>
       </c>
-      <c r="L24" s="580">
-        <v>0</v>
-      </c>
+      <c r="L24" s="580"/>
       <c r="M24" s="326">
         <v>0</v>
       </c>
@@ -12556,7 +12563,7 @@
       <c r="Q24" s="605" t="s">
         <v>335</v>
       </c>
-      <c r="R24" s="683"/>
+      <c r="R24" s="627"/>
       <c r="S24" s="534" t="s">
         <v>249</v>
       </c>
@@ -12743,9 +12750,7 @@
       <c r="K26" s="574">
         <v>1</v>
       </c>
-      <c r="L26" s="580">
-        <v>0</v>
-      </c>
+      <c r="L26" s="580"/>
       <c r="M26" s="326">
         <v>0</v>
       </c>
@@ -13224,8 +13229,8 @@
       <c r="AR31" s="508"/>
     </row>
     <row r="32" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="650"/>
-      <c r="B32" s="650"/>
+      <c r="A32" s="630"/>
+      <c r="B32" s="630"/>
       <c r="J32" s="571"/>
       <c r="K32" s="586"/>
       <c r="L32" s="580">
@@ -13322,9 +13327,7 @@
     </row>
     <row r="33" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="80"/>
-      <c r="B33" s="21">
-        <v>-6</v>
-      </c>
+      <c r="B33" s="21"/>
       <c r="G33" s="382">
         <v>-1</v>
       </c>
@@ -13424,7 +13427,9 @@
       </c>
     </row>
     <row r="34" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="21"/>
+      <c r="B34" s="21">
+        <v>5</v>
+      </c>
       <c r="C34" s="2" t="s">
         <v>257</v>
       </c>
@@ -13704,9 +13709,7 @@
       </c>
     </row>
     <row r="37" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="21">
-        <v>-20</v>
-      </c>
+      <c r="B37" s="21"/>
       <c r="D37" s="382">
         <v>1</v>
       </c>
@@ -13811,6 +13814,15 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="P4:P20"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="Q20:R20"/>
     <mergeCell ref="AM1:AO1"/>
     <mergeCell ref="X1:Y1"/>
     <mergeCell ref="AE1:AG1"/>
@@ -13822,15 +13834,6 @@
     <mergeCell ref="W2:W3"/>
     <mergeCell ref="T1:T3"/>
     <mergeCell ref="AK1:AK2"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="P4:P20"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="Q20:R20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13898,7 +13901,7 @@
       <c r="V1" s="603" t="s">
         <v>70</v>
       </c>
-      <c r="W1" s="683"/>
+      <c r="W1" s="627"/>
       <c r="X1" s="62" t="s">
         <v>101</v>
       </c>
@@ -13917,7 +13920,7 @@
       <c r="AC1" s="116" t="s">
         <v>190</v>
       </c>
-      <c r="AD1" s="759" t="s">
+      <c r="AD1" s="752" t="s">
         <v>211</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -13934,10 +13937,10 @@
       <c r="E2" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="790" t="s">
+      <c r="F2" s="751" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="747" t="s">
+      <c r="G2" s="779" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -13965,10 +13968,10 @@
       <c r="U2" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="V2" s="726" t="s">
+      <c r="V2" s="719" t="s">
         <v>120</v>
       </c>
-      <c r="W2" s="727"/>
+      <c r="W2" s="720"/>
       <c r="X2" s="64" t="s">
         <v>109</v>
       </c>
@@ -13987,7 +13990,7 @@
       <c r="AC2" s="117" t="s">
         <v>98</v>
       </c>
-      <c r="AD2" s="760"/>
+      <c r="AD2" s="753"/>
       <c r="AE2" s="64" t="s">
         <v>98</v>
       </c>
@@ -14006,8 +14009,8 @@
       <c r="E3" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="F3" s="630"/>
-      <c r="G3" s="748"/>
+      <c r="F3" s="679"/>
+      <c r="G3" s="780"/>
       <c r="H3" s="40" t="s">
         <v>80</v>
       </c>
@@ -14018,13 +14021,13 @@
         <v>81</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="757" t="s">
+      <c r="O3" s="789" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="778" t="s">
+      <c r="P3" s="771" t="s">
         <v>217</v>
       </c>
-      <c r="Q3" s="779"/>
+      <c r="Q3" s="772"/>
       <c r="S3" s="57" t="s">
         <v>218</v>
       </c>
@@ -14034,15 +14037,15 @@
       <c r="W3" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="AD3" s="760"/>
+      <c r="AD3" s="753"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="748"/>
+      <c r="G4" s="780"/>
       <c r="H4" s="6"/>
       <c r="L4" s="687" t="s">
         <v>82</v>
       </c>
-      <c r="O4" s="758"/>
+      <c r="O4" s="790"/>
       <c r="T4" s="55" t="s">
         <v>97</v>
       </c>
@@ -14056,8 +14059,8 @@
         <v>194</v>
       </c>
       <c r="Z4" s="605"/>
-      <c r="AA4" s="683"/>
-      <c r="AD4" s="760"/>
+      <c r="AA4" s="627"/>
+      <c r="AD4" s="753"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -14072,21 +14075,21 @@
       <c r="F5" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="G5" s="748"/>
+      <c r="G5" s="780"/>
       <c r="H5" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="K5" s="765" t="s">
+      <c r="K5" s="758" t="s">
         <v>215</v>
       </c>
-      <c r="L5" s="780"/>
+      <c r="L5" s="773"/>
       <c r="M5" s="2" t="s">
         <v>213</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>212</v>
       </c>
-      <c r="O5" s="758"/>
+      <c r="O5" s="790"/>
       <c r="P5" s="108" t="s">
         <v>214</v>
       </c>
@@ -14102,11 +14105,11 @@
       <c r="U5" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="Y5" s="768" t="s">
+      <c r="Y5" s="761" t="s">
         <v>282</v>
       </c>
-      <c r="Z5" s="769"/>
-      <c r="AD5" s="760"/>
+      <c r="Z5" s="762"/>
+      <c r="AD5" s="753"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -14116,16 +14119,16 @@
       <c r="E6" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="G6" s="748"/>
+      <c r="G6" s="780"/>
       <c r="H6" s="46" t="s">
         <v>80</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="766"/>
-      <c r="L6" s="780"/>
-      <c r="O6" s="758"/>
+      <c r="K6" s="759"/>
+      <c r="L6" s="773"/>
+      <c r="O6" s="790"/>
       <c r="T6" s="2" t="s">
         <v>100</v>
       </c>
@@ -14135,23 +14138,23 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="760"/>
+      <c r="AD6" s="753"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="748"/>
+      <c r="G7" s="780"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="766"/>
-      <c r="L7" s="780"/>
+      <c r="K7" s="759"/>
+      <c r="L7" s="773"/>
       <c r="N7" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="O7" s="758"/>
+      <c r="O7" s="790"/>
       <c r="P7" s="73"/>
       <c r="U7" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="760"/>
+      <c r="AD7" s="753"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -14164,7 +14167,7 @@
       <c r="F8" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="G8" s="748"/>
+      <c r="G8" s="780"/>
       <c r="H8" s="50" t="s">
         <v>75</v>
       </c>
@@ -14174,41 +14177,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="766"/>
-      <c r="L8" s="780"/>
-      <c r="O8" s="758"/>
+      <c r="K8" s="759"/>
+      <c r="L8" s="773"/>
+      <c r="O8" s="790"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="762" t="s">
+      <c r="S8" s="755" t="s">
         <v>210</v>
       </c>
-      <c r="T8" s="763"/>
-      <c r="U8" s="763"/>
-      <c r="V8" s="763"/>
-      <c r="W8" s="763"/>
-      <c r="X8" s="763"/>
-      <c r="Y8" s="763"/>
-      <c r="Z8" s="763"/>
-      <c r="AA8" s="763"/>
-      <c r="AB8" s="763"/>
-      <c r="AC8" s="764"/>
-      <c r="AD8" s="760"/>
+      <c r="T8" s="756"/>
+      <c r="U8" s="756"/>
+      <c r="V8" s="756"/>
+      <c r="W8" s="756"/>
+      <c r="X8" s="756"/>
+      <c r="Y8" s="756"/>
+      <c r="Z8" s="756"/>
+      <c r="AA8" s="756"/>
+      <c r="AB8" s="756"/>
+      <c r="AC8" s="757"/>
+      <c r="AD8" s="753"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="784"/>
-      <c r="G9" s="748"/>
+      <c r="C9" s="745"/>
+      <c r="G9" s="780"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="766"/>
-      <c r="L9" s="751" t="s">
+      <c r="K9" s="759"/>
+      <c r="L9" s="783" t="s">
         <v>216</v>
       </c>
-      <c r="M9" s="752"/>
-      <c r="N9" s="753"/>
-      <c r="O9" s="758"/>
+      <c r="M9" s="784"/>
+      <c r="N9" s="785"/>
+      <c r="O9" s="790"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="760"/>
+      <c r="AD9" s="753"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="785"/>
+      <c r="C10" s="746"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>87</v>
@@ -14216,7 +14219,7 @@
       <c r="F10" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="G10" s="748"/>
+      <c r="G10" s="780"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>80</v>
@@ -14224,33 +14227,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="766"/>
-      <c r="M10" s="787" t="s">
+      <c r="K10" s="759"/>
+      <c r="M10" s="748" t="s">
         <v>89</v>
       </c>
-      <c r="N10" s="788"/>
-      <c r="O10" s="788"/>
-      <c r="P10" s="788"/>
-      <c r="Q10" s="788"/>
-      <c r="R10" s="788"/>
-      <c r="S10" s="788"/>
-      <c r="T10" s="788"/>
-      <c r="U10" s="788"/>
-      <c r="V10" s="788"/>
-      <c r="W10" s="788"/>
-      <c r="X10" s="788"/>
-      <c r="Y10" s="788"/>
-      <c r="Z10" s="788"/>
-      <c r="AA10" s="788"/>
-      <c r="AB10" s="788"/>
-      <c r="AC10" s="789"/>
-      <c r="AD10" s="760"/>
+      <c r="N10" s="749"/>
+      <c r="O10" s="749"/>
+      <c r="P10" s="749"/>
+      <c r="Q10" s="749"/>
+      <c r="R10" s="749"/>
+      <c r="S10" s="749"/>
+      <c r="T10" s="749"/>
+      <c r="U10" s="749"/>
+      <c r="V10" s="749"/>
+      <c r="W10" s="749"/>
+      <c r="X10" s="749"/>
+      <c r="Y10" s="749"/>
+      <c r="Z10" s="749"/>
+      <c r="AA10" s="749"/>
+      <c r="AB10" s="749"/>
+      <c r="AC10" s="750"/>
+      <c r="AD10" s="753"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="786"/>
-      <c r="G11" s="748"/>
+      <c r="C11" s="747"/>
+      <c r="G11" s="780"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="766"/>
+      <c r="K11" s="759"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -14258,17 +14261,17 @@
       <c r="Y11" s="68" t="s">
         <v>120</v>
       </c>
-      <c r="Z11" s="776" t="s">
+      <c r="Z11" s="769" t="s">
         <v>120</v>
       </c>
-      <c r="AA11" s="777"/>
+      <c r="AA11" s="770"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>120</v>
       </c>
-      <c r="AD11" s="760"/>
+      <c r="AD11" s="753"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -14281,7 +14284,7 @@
       <c r="F12" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="G12" s="748"/>
+      <c r="G12" s="780"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>80</v>
@@ -14289,8 +14292,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="766"/>
-      <c r="L12" s="781" t="s">
+      <c r="K12" s="759"/>
+      <c r="L12" s="774" t="s">
         <v>92</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -14321,25 +14324,25 @@
         <v>115</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="770" t="s">
+      <c r="AA12" s="763" t="s">
         <v>125</v>
       </c>
-      <c r="AB12" s="771"/>
+      <c r="AB12" s="764"/>
       <c r="AC12" s="21" t="s">
         <v>230</v>
       </c>
-      <c r="AD12" s="760"/>
+      <c r="AD12" s="753"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="784"/>
-      <c r="G13" s="748"/>
-      <c r="K13" s="766"/>
-      <c r="L13" s="782"/>
+      <c r="C13" s="745"/>
+      <c r="G13" s="780"/>
+      <c r="K13" s="759"/>
+      <c r="L13" s="775"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="750" t="s">
+      <c r="Q13" s="782" t="s">
         <v>208</v>
       </c>
-      <c r="R13" s="639"/>
+      <c r="R13" s="644"/>
       <c r="S13" s="599"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
@@ -14348,17 +14351,17 @@
       <c r="X13" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="AA13" s="772"/>
-      <c r="AB13" s="773"/>
-      <c r="AD13" s="760"/>
+      <c r="AA13" s="765"/>
+      <c r="AB13" s="766"/>
+      <c r="AD13" s="753"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="C14" s="786"/>
+      <c r="C14" s="747"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="748"/>
+      <c r="G14" s="780"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -14366,8 +14369,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="766"/>
-      <c r="L14" s="782"/>
+      <c r="K14" s="759"/>
+      <c r="L14" s="775"/>
       <c r="M14" s="21" t="s">
         <v>110</v>
       </c>
@@ -14388,9 +14391,9 @@
       <c r="Y14" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="AA14" s="772"/>
-      <c r="AB14" s="773"/>
-      <c r="AD14" s="760"/>
+      <c r="AA14" s="765"/>
+      <c r="AB14" s="766"/>
+      <c r="AD14" s="753"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -14405,19 +14408,19 @@
       <c r="F15" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="G15" s="748"/>
+      <c r="G15" s="780"/>
       <c r="H15" s="2" t="s">
         <v>80</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="K15" s="766"/>
-      <c r="L15" s="783"/>
-      <c r="Q15" s="750" t="s">
+      <c r="K15" s="759"/>
+      <c r="L15" s="776"/>
+      <c r="Q15" s="782" t="s">
         <v>209</v>
       </c>
-      <c r="R15" s="639"/>
+      <c r="R15" s="644"/>
       <c r="S15" s="599"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
@@ -14426,14 +14429,14 @@
       <c r="X15" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="AA15" s="772"/>
-      <c r="AB15" s="773"/>
-      <c r="AD15" s="760"/>
+      <c r="AA15" s="765"/>
+      <c r="AB15" s="766"/>
+      <c r="AD15" s="753"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="748"/>
-      <c r="K16" s="766"/>
+      <c r="G16" s="780"/>
+      <c r="K16" s="759"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>108</v>
@@ -14452,24 +14455,24 @@
       <c r="Z16" s="76" t="s">
         <v>126</v>
       </c>
-      <c r="AA16" s="772"/>
-      <c r="AB16" s="773"/>
-      <c r="AD16" s="760"/>
+      <c r="AA16" s="765"/>
+      <c r="AB16" s="766"/>
+      <c r="AD16" s="753"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F17" s="745" t="s">
+      <c r="F17" s="777" t="s">
         <v>95</v>
       </c>
-      <c r="G17" s="748"/>
+      <c r="G17" s="780"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>80</v>
       </c>
-      <c r="K17" s="766"/>
+      <c r="K17" s="759"/>
       <c r="S17" s="599"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
@@ -14477,9 +14480,9 @@
       <c r="X17" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA17" s="772"/>
-      <c r="AB17" s="773"/>
-      <c r="AD17" s="760"/>
+      <c r="AA17" s="765"/>
+      <c r="AB17" s="766"/>
+      <c r="AD17" s="753"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -14489,15 +14492,15 @@
       <c r="E18" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F18" s="746"/>
-      <c r="G18" s="748"/>
+      <c r="F18" s="778"/>
+      <c r="G18" s="780"/>
       <c r="H18" s="108" t="s">
         <v>75</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="K18" s="766"/>
+      <c r="K18" s="759"/>
       <c r="O18" s="64" t="s">
         <v>114</v>
       </c>
@@ -14508,39 +14511,42 @@
       <c r="X18" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AA18" s="774"/>
-      <c r="AB18" s="775"/>
-      <c r="AD18" s="760"/>
+      <c r="AA18" s="767"/>
+      <c r="AB18" s="768"/>
+      <c r="AD18" s="753"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>207</v>
       </c>
-      <c r="G19" s="749"/>
-      <c r="K19" s="767"/>
+      <c r="G19" s="781"/>
+      <c r="K19" s="760"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="754" t="s">
+      <c r="R19" s="786" t="s">
         <v>123</v>
       </c>
-      <c r="S19" s="755"/>
-      <c r="T19" s="756"/>
+      <c r="S19" s="787"/>
+      <c r="T19" s="788"/>
       <c r="V19" s="77" t="s">
         <v>114</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="AD19" s="761"/>
+      <c r="AD19" s="754"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="M10:AC10"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="S12:S18"/>
+    <mergeCell ref="O3:O9"/>
     <mergeCell ref="AD1:AD19"/>
     <mergeCell ref="S8:AC8"/>
     <mergeCell ref="K5:K19"/>
@@ -14552,14 +14558,11 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L12:L15"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G19"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="S12:S18"/>
-    <mergeCell ref="O3:O9"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="M10:AC10"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rw Usage Updates S.1.0.1.6 _11:45PM
Boat Enabled -
InCapacity - [17,8,Cnt] ,
NodeW - [-3] ,
BirdW - [7][CityW-MundiaSahi] ,
FuelW_Day - ['22][CityW-CM Nagar] ,
OnHost - [8+1]
VillageW=[0],
CityW=[2] ,
[X-MarketShieldMatrix-X] = [5,1,2,1] = [Lx -2 , Bx - 4 ]

Rw - Local(Left Running With Cost ) - [For Business/Shop/Market only] -
</commit_message>
<xml_diff>
--- a/System_2.2.1.xlsx
+++ b/System_2.2.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0454AF1-9F38-4911-9B2D-03FDCD3E9BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F44BD5-193B-4ECD-A817-B7BD7EA528F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5027,6 +5027,186 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5039,12 +5219,6 @@
     <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5056,12 +5230,6 @@
     </xf>
     <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
@@ -5084,190 +5252,61 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5309,43 +5348,25 @@
     <xf numFmtId="0" fontId="39" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5414,46 +5435,46 @@
     <xf numFmtId="14" fontId="5" fillId="14" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5531,46 +5552,25 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -6903,7 +6903,7 @@
       <c r="H1" s="97" t="s">
         <v>343</v>
       </c>
-      <c r="I1" s="613" t="s">
+      <c r="I1" s="659" t="s">
         <v>369</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -6939,7 +6939,7 @@
       <c r="X1" s="430" t="s">
         <v>155</v>
       </c>
-      <c r="Y1" s="657" t="s">
+      <c r="Y1" s="653" t="s">
         <v>528</v>
       </c>
       <c r="Z1" s="406">
@@ -6964,7 +6964,7 @@
         <v>498</v>
       </c>
       <c r="AM1" s="402"/>
-      <c r="AN1" s="640"/>
+      <c r="AN1" s="635"/>
       <c r="AO1" s="338" t="s">
         <v>469</v>
       </c>
@@ -6973,23 +6973,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="666">
+      <c r="A2" s="617">
         <f ca="1">TODAY()</f>
-        <v>45293</v>
-      </c>
-      <c r="B2" s="668" t="s">
+        <v>45294</v>
+      </c>
+      <c r="B2" s="619" t="s">
         <v>370</v>
       </c>
-      <c r="C2" s="645" t="s">
+      <c r="C2" s="615" t="s">
         <v>357</v>
       </c>
-      <c r="D2" s="670" t="s">
+      <c r="D2" s="621" t="s">
         <v>355</v>
       </c>
-      <c r="E2" s="609" t="s">
+      <c r="E2" s="669" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="619" t="s">
+      <c r="F2" s="640" t="s">
         <v>102</v>
       </c>
       <c r="G2" s="393" t="s">
@@ -6998,31 +6998,31 @@
       <c r="H2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="614"/>
+      <c r="I2" s="660"/>
       <c r="J2" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="611" t="s">
+      <c r="K2" s="671" t="s">
         <v>342</v>
       </c>
-      <c r="L2" s="612"/>
-      <c r="M2" s="619" t="s">
+      <c r="L2" s="672"/>
+      <c r="M2" s="640" t="s">
         <v>102</v>
       </c>
       <c r="N2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="649" t="s">
+      <c r="O2" s="644" t="s">
         <v>102</v>
       </c>
       <c r="P2" s="85" t="s">
         <v>147</v>
       </c>
-      <c r="Q2" s="645" t="s">
+      <c r="Q2" s="615" t="s">
         <v>143</v>
       </c>
       <c r="R2" s="598"/>
-      <c r="S2" s="634" t="s">
+      <c r="S2" s="657" t="s">
         <v>148</v>
       </c>
       <c r="T2" s="89"/>
@@ -7032,7 +7032,7 @@
       <c r="X2" s="431" t="s">
         <v>156</v>
       </c>
-      <c r="Y2" s="658"/>
+      <c r="Y2" s="654"/>
       <c r="Z2" s="407">
         <v>1</v>
       </c>
@@ -7055,15 +7055,15 @@
         <v>463</v>
       </c>
       <c r="AM2" s="428"/>
-      <c r="AN2" s="641"/>
+      <c r="AN2" s="636"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="667"/>
-      <c r="B3" s="669"/>
-      <c r="C3" s="646"/>
-      <c r="D3" s="671"/>
-      <c r="E3" s="610"/>
-      <c r="F3" s="620"/>
+      <c r="A3" s="618"/>
+      <c r="B3" s="620"/>
+      <c r="C3" s="616"/>
+      <c r="D3" s="622"/>
+      <c r="E3" s="670"/>
+      <c r="F3" s="641"/>
       <c r="G3" s="394" t="s">
         <v>28</v>
       </c>
@@ -7082,17 +7082,17 @@
       <c r="L3" s="201" t="s">
         <v>107</v>
       </c>
-      <c r="M3" s="620"/>
+      <c r="M3" s="641"/>
       <c r="N3" s="69" t="s">
         <v>146</v>
       </c>
-      <c r="O3" s="650"/>
+      <c r="O3" s="645"/>
       <c r="P3" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="Q3" s="646"/>
+      <c r="Q3" s="616"/>
       <c r="R3" s="600"/>
-      <c r="S3" s="636"/>
+      <c r="S3" s="658"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -7100,7 +7100,7 @@
       <c r="X3" s="431" t="s">
         <v>157</v>
       </c>
-      <c r="Y3" s="658"/>
+      <c r="Y3" s="654"/>
       <c r="Z3" s="408">
         <v>1</v>
       </c>
@@ -7109,7 +7109,7 @@
       <c r="AC3" s="100" t="s">
         <v>480</v>
       </c>
-      <c r="AD3" s="631" t="s">
+      <c r="AD3" s="656" t="s">
         <v>455</v>
       </c>
       <c r="AE3" s="257"/>
@@ -7121,16 +7121,16 @@
       <c r="AK3" s="257"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="428"/>
-      <c r="AN3" s="641"/>
+      <c r="AN3" s="636"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="238" t="s">
         <v>183</v>
       </c>
-      <c r="B4" s="682" t="s">
+      <c r="B4" s="633" t="s">
         <v>373</v>
       </c>
-      <c r="C4" s="645" t="s">
+      <c r="C4" s="615" t="s">
         <v>154</v>
       </c>
       <c r="D4" s="347" t="s">
@@ -7139,7 +7139,7 @@
       <c r="E4" s="378">
         <v>2</v>
       </c>
-      <c r="F4" s="620"/>
+      <c r="F4" s="641"/>
       <c r="G4" s="381" t="s">
         <v>201</v>
       </c>
@@ -7156,11 +7156,11 @@
         <v>150</v>
       </c>
       <c r="L4" s="204"/>
-      <c r="M4" s="620"/>
+      <c r="M4" s="641"/>
       <c r="N4" s="174" t="s">
         <v>69</v>
       </c>
-      <c r="O4" s="650"/>
+      <c r="O4" s="645"/>
       <c r="P4" s="2" t="s">
         <v>191</v>
       </c>
@@ -7182,12 +7182,12 @@
       <c r="X4" s="431" t="s">
         <v>158</v>
       </c>
-      <c r="Y4" s="658"/>
+      <c r="Y4" s="654"/>
       <c r="Z4" s="409"/>
       <c r="AA4" s="307"/>
       <c r="AB4" s="209"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="631"/>
+      <c r="AD4" s="656"/>
       <c r="AE4" s="257"/>
       <c r="AF4" s="257"/>
       <c r="AG4" s="16"/>
@@ -7197,37 +7197,37 @@
       <c r="AK4" s="257"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="428"/>
-      <c r="AN4" s="641"/>
+      <c r="AN4" s="636"/>
       <c r="AO4" s="338" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="613" t="s">
+      <c r="A5" s="659" t="s">
         <v>418</v>
       </c>
-      <c r="B5" s="683"/>
-      <c r="C5" s="646"/>
+      <c r="B5" s="634"/>
+      <c r="C5" s="616"/>
       <c r="D5" s="61" t="s">
         <v>153</v>
       </c>
       <c r="E5" s="379">
         <v>1</v>
       </c>
-      <c r="F5" s="620"/>
-      <c r="G5" s="674" t="s">
+      <c r="F5" s="641"/>
+      <c r="G5" s="625" t="s">
         <v>192</v>
       </c>
-      <c r="H5" s="674"/>
-      <c r="I5" s="674"/>
-      <c r="J5" s="674"/>
-      <c r="K5" s="674"/>
-      <c r="L5" s="675"/>
-      <c r="M5" s="620"/>
+      <c r="H5" s="625"/>
+      <c r="I5" s="625"/>
+      <c r="J5" s="625"/>
+      <c r="K5" s="625"/>
+      <c r="L5" s="626"/>
+      <c r="M5" s="641"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
-      <c r="O5" s="650"/>
+      <c r="O5" s="645"/>
       <c r="T5" s="89"/>
       <c r="U5" s="124"/>
       <c r="V5" s="120"/>
@@ -7235,7 +7235,7 @@
       <c r="X5" s="431" t="s">
         <v>159</v>
       </c>
-      <c r="Y5" s="658"/>
+      <c r="Y5" s="654"/>
       <c r="Z5" s="409">
         <v>1</v>
       </c>
@@ -7258,24 +7258,24 @@
       <c r="AK5" s="257"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="428"/>
-      <c r="AN5" s="641"/>
+      <c r="AN5" s="636"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="614"/>
-      <c r="B6" s="680" t="s">
+      <c r="A6" s="660"/>
+      <c r="B6" s="631" t="s">
         <v>177</v>
       </c>
-      <c r="C6" s="628"/>
-      <c r="D6" s="629"/>
-      <c r="F6" s="620"/>
-      <c r="G6" s="676"/>
-      <c r="H6" s="676"/>
-      <c r="I6" s="676"/>
-      <c r="J6" s="676"/>
-      <c r="K6" s="676"/>
-      <c r="L6" s="677"/>
-      <c r="M6" s="620"/>
-      <c r="O6" s="650"/>
+      <c r="C6" s="661"/>
+      <c r="D6" s="662"/>
+      <c r="F6" s="641"/>
+      <c r="G6" s="627"/>
+      <c r="H6" s="627"/>
+      <c r="I6" s="627"/>
+      <c r="J6" s="627"/>
+      <c r="K6" s="627"/>
+      <c r="L6" s="628"/>
+      <c r="M6" s="641"/>
+      <c r="O6" s="645"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
       <c r="V6" s="98" t="s">
@@ -7285,7 +7285,7 @@
       <c r="X6" s="431" t="s">
         <v>160</v>
       </c>
-      <c r="Y6" s="658"/>
+      <c r="Y6" s="654"/>
       <c r="Z6" s="407">
         <v>1</v>
       </c>
@@ -7299,16 +7299,16 @@
       <c r="AF6" s="257"/>
       <c r="AG6" s="257"/>
       <c r="AH6" s="257"/>
-      <c r="AI6" s="630"/>
+      <c r="AI6" s="650"/>
       <c r="AJ6" s="441" t="s">
         <v>458</v>
       </c>
-      <c r="AK6" s="630" t="s">
+      <c r="AK6" s="650" t="s">
         <v>251</v>
       </c>
       <c r="AL6" s="257"/>
       <c r="AM6" s="428"/>
-      <c r="AN6" s="641"/>
+      <c r="AN6" s="636"/>
       <c r="AO6" s="338" t="s">
         <v>470</v>
       </c>
@@ -7317,7 +7317,7 @@
       <c r="A7" s="232" t="s">
         <v>571</v>
       </c>
-      <c r="B7" s="681"/>
+      <c r="B7" s="632"/>
       <c r="C7" s="202" t="s">
         <v>374</v>
       </c>
@@ -7327,7 +7327,7 @@
       <c r="E7" s="265">
         <v>3</v>
       </c>
-      <c r="F7" s="620"/>
+      <c r="F7" s="641"/>
       <c r="G7" s="395">
         <v>0</v>
       </c>
@@ -7346,8 +7346,8 @@
       <c r="L7" s="212">
         <v>0</v>
       </c>
-      <c r="M7" s="620"/>
-      <c r="O7" s="650"/>
+      <c r="M7" s="641"/>
+      <c r="O7" s="645"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
       </c>
@@ -7361,7 +7361,7 @@
       <c r="X7" s="431" t="s">
         <v>161</v>
       </c>
-      <c r="Y7" s="658"/>
+      <c r="Y7" s="654"/>
       <c r="Z7" s="407">
         <v>1</v>
       </c>
@@ -7371,18 +7371,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="257"/>
       <c r="AF7" s="257"/>
-      <c r="AG7" s="631" t="s">
+      <c r="AG7" s="656" t="s">
         <v>454</v>
       </c>
       <c r="AH7" s="257"/>
-      <c r="AI7" s="630"/>
+      <c r="AI7" s="650"/>
       <c r="AJ7" s="257"/>
-      <c r="AK7" s="630"/>
+      <c r="AK7" s="650"/>
       <c r="AL7" s="80" t="s">
         <v>496</v>
       </c>
       <c r="AM7" s="428"/>
-      <c r="AN7" s="641"/>
+      <c r="AN7" s="636"/>
       <c r="AP7" s="76" t="s">
         <v>471</v>
       </c>
@@ -7399,27 +7399,27 @@
         <f>SUM(G7:N9)</f>
         <v>15</v>
       </c>
-      <c r="F8" s="620"/>
-      <c r="G8" s="675">
-        <v>0</v>
-      </c>
-      <c r="H8" s="672" t="s">
+      <c r="F8" s="641"/>
+      <c r="G8" s="626">
+        <v>0</v>
+      </c>
+      <c r="H8" s="623" t="s">
         <v>104</v>
       </c>
       <c r="I8" s="598">
         <v>0</v>
       </c>
-      <c r="J8" s="672" t="s">
+      <c r="J8" s="623" t="s">
         <v>104</v>
       </c>
-      <c r="K8" s="678"/>
-      <c r="L8" s="632"/>
-      <c r="M8" s="647"/>
-      <c r="N8" s="637">
+      <c r="K8" s="629"/>
+      <c r="L8" s="663"/>
+      <c r="M8" s="642"/>
+      <c r="N8" s="666">
         <f>N5+N11</f>
         <v>15</v>
       </c>
-      <c r="O8" s="650"/>
+      <c r="O8" s="645"/>
       <c r="T8" s="103" t="s">
         <v>44</v>
       </c>
@@ -7429,7 +7429,7 @@
       <c r="X8" s="431" t="s">
         <v>162</v>
       </c>
-      <c r="Y8" s="658"/>
+      <c r="Y8" s="654"/>
       <c r="Z8" s="409"/>
       <c r="AA8" s="307"/>
       <c r="AB8" s="209"/>
@@ -7437,14 +7437,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="257"/>
       <c r="AF8" s="257"/>
-      <c r="AG8" s="631"/>
+      <c r="AG8" s="656"/>
       <c r="AH8" s="257"/>
-      <c r="AI8" s="630"/>
+      <c r="AI8" s="650"/>
       <c r="AJ8" s="257"/>
       <c r="AK8" s="257"/>
       <c r="AL8" s="257"/>
       <c r="AM8" s="428"/>
-      <c r="AN8" s="641"/>
+      <c r="AN8" s="636"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="232" t="s">
@@ -7459,17 +7459,17 @@
       <c r="D9" s="348" t="s">
         <v>281</v>
       </c>
-      <c r="F9" s="620"/>
-      <c r="G9" s="677"/>
-      <c r="H9" s="673"/>
+      <c r="F9" s="641"/>
+      <c r="G9" s="628"/>
+      <c r="H9" s="624"/>
       <c r="I9" s="600"/>
-      <c r="J9" s="673"/>
-      <c r="K9" s="679"/>
-      <c r="L9" s="633"/>
-      <c r="M9" s="648"/>
-      <c r="N9" s="638"/>
-      <c r="O9" s="651"/>
-      <c r="S9" s="634" t="s">
+      <c r="J9" s="624"/>
+      <c r="K9" s="630"/>
+      <c r="L9" s="664"/>
+      <c r="M9" s="643"/>
+      <c r="N9" s="667"/>
+      <c r="O9" s="646"/>
+      <c r="S9" s="657" t="s">
         <v>61</v>
       </c>
       <c r="T9" s="89"/>
@@ -7481,7 +7481,7 @@
       <c r="X9" s="431" t="s">
         <v>163</v>
       </c>
-      <c r="Y9" s="658"/>
+      <c r="Y9" s="654"/>
       <c r="Z9" s="410"/>
       <c r="AA9" s="307"/>
       <c r="AB9" s="209"/>
@@ -7491,16 +7491,16 @@
       </c>
       <c r="AE9" s="257"/>
       <c r="AF9" s="257"/>
-      <c r="AG9" s="631"/>
+      <c r="AG9" s="656"/>
       <c r="AH9" s="257"/>
-      <c r="AI9" s="630"/>
+      <c r="AI9" s="650"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="630" t="s">
+      <c r="AK9" s="650" t="s">
         <v>251</v>
       </c>
       <c r="AL9" s="257"/>
       <c r="AM9" s="428"/>
-      <c r="AN9" s="641"/>
+      <c r="AN9" s="636"/>
       <c r="AP9" s="2" t="s">
         <v>508</v>
       </c>
@@ -7517,20 +7517,20 @@
         <f>Boat!W8</f>
         <v>37</v>
       </c>
-      <c r="F10" s="620"/>
+      <c r="F10" s="641"/>
       <c r="N10" s="418" t="s">
         <v>396</v>
       </c>
-      <c r="O10" s="622" t="s">
+      <c r="O10" s="678" t="s">
         <v>102</v>
       </c>
-      <c r="P10" s="652" t="s">
+      <c r="P10" s="647" t="s">
         <v>400</v>
       </c>
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="635"/>
+      <c r="S10" s="665"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>176</v>
@@ -7542,7 +7542,7 @@
       <c r="X10" s="431" t="s">
         <v>164</v>
       </c>
-      <c r="Y10" s="658"/>
+      <c r="Y10" s="654"/>
       <c r="Z10" s="409">
         <v>0</v>
       </c>
@@ -7560,16 +7560,16 @@
       <c r="AF10" s="238" t="s">
         <v>311</v>
       </c>
-      <c r="AG10" s="631"/>
+      <c r="AG10" s="656"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="630"/>
+      <c r="AI10" s="650"/>
       <c r="AJ10" s="257"/>
-      <c r="AK10" s="630"/>
+      <c r="AK10" s="650"/>
       <c r="AL10" s="257"/>
       <c r="AM10" s="442" t="s">
         <v>318</v>
       </c>
-      <c r="AN10" s="641"/>
+      <c r="AN10" s="636"/>
       <c r="AO10" s="204" t="s">
         <v>94</v>
       </c>
@@ -7587,18 +7587,18 @@
       <c r="D11" s="170" t="s">
         <v>355</v>
       </c>
-      <c r="F11" s="620"/>
+      <c r="F11" s="641"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="623"/>
-      <c r="P11" s="653"/>
+      <c r="O11" s="679"/>
+      <c r="P11" s="648"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>220</v>
       </c>
-      <c r="S11" s="635"/>
+      <c r="S11" s="665"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -7608,7 +7608,7 @@
       <c r="X11" s="431" t="s">
         <v>165</v>
       </c>
-      <c r="Y11" s="658"/>
+      <c r="Y11" s="654"/>
       <c r="Z11" s="409"/>
       <c r="AA11" s="307">
         <v>1</v>
@@ -7622,14 +7622,14 @@
       <c r="AF11" s="257" t="s">
         <v>476</v>
       </c>
-      <c r="AG11" s="631"/>
+      <c r="AG11" s="656"/>
       <c r="AH11" s="257"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="257"/>
       <c r="AK11" s="257"/>
       <c r="AL11" s="257"/>
       <c r="AM11" s="428"/>
-      <c r="AN11" s="641"/>
+      <c r="AN11" s="636"/>
       <c r="AP11" s="76" t="s">
         <v>484</v>
       </c>
@@ -7648,7 +7648,7 @@
       <c r="E12" s="224">
         <v>3</v>
       </c>
-      <c r="F12" s="620"/>
+      <c r="F12" s="641"/>
       <c r="G12" s="337" t="s">
         <v>400</v>
       </c>
@@ -7657,16 +7657,16 @@
       </c>
       <c r="I12" s="605"/>
       <c r="J12" s="605"/>
-      <c r="K12" s="627"/>
+      <c r="K12" s="683"/>
       <c r="L12" s="203"/>
       <c r="M12" s="203"/>
       <c r="N12" s="203"/>
-      <c r="O12" s="623"/>
-      <c r="P12" s="653"/>
+      <c r="O12" s="679"/>
+      <c r="P12" s="648"/>
       <c r="R12" s="122" t="s">
         <v>180</v>
       </c>
-      <c r="S12" s="636"/>
+      <c r="S12" s="658"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -7676,7 +7676,7 @@
       <c r="X12" s="431" t="s">
         <v>166</v>
       </c>
-      <c r="Y12" s="658"/>
+      <c r="Y12" s="654"/>
       <c r="Z12" s="407">
         <v>1</v>
       </c>
@@ -7687,16 +7687,16 @@
       <c r="AC12" s="100" t="s">
         <v>481</v>
       </c>
-      <c r="AD12" s="639" t="s">
+      <c r="AD12" s="668" t="s">
         <v>240</v>
       </c>
       <c r="AE12" s="441" t="s">
         <v>239</v>
       </c>
-      <c r="AF12" s="631" t="s">
+      <c r="AF12" s="656" t="s">
         <v>228</v>
       </c>
-      <c r="AG12" s="631"/>
+      <c r="AG12" s="656"/>
       <c r="AH12" s="238" t="s">
         <v>259</v>
       </c>
@@ -7706,10 +7706,10 @@
       <c r="AJ12" s="257"/>
       <c r="AK12" s="257"/>
       <c r="AL12" s="257"/>
-      <c r="AM12" s="655" t="s">
+      <c r="AM12" s="651" t="s">
         <v>249</v>
       </c>
-      <c r="AN12" s="641"/>
+      <c r="AN12" s="636"/>
       <c r="AO12" s="338" t="s">
         <v>96</v>
       </c>
@@ -7721,17 +7721,17 @@
       <c r="E13" s="448">
         <v>-3</v>
       </c>
-      <c r="F13" s="620"/>
+      <c r="F13" s="641"/>
       <c r="G13" s="605" t="s">
         <v>430</v>
       </c>
       <c r="H13" s="605"/>
       <c r="I13" s="605"/>
-      <c r="J13" s="627"/>
+      <c r="J13" s="683"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="623"/>
-      <c r="P13" s="654"/>
+      <c r="O13" s="679"/>
+      <c r="P13" s="649"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
       </c>
@@ -7741,7 +7741,7 @@
       <c r="X13" s="431" t="s">
         <v>167</v>
       </c>
-      <c r="Y13" s="658"/>
+      <c r="Y13" s="654"/>
       <c r="Z13" s="407">
         <v>1</v>
       </c>
@@ -7752,8 +7752,8 @@
         <v>500</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="639"/>
-      <c r="AF13" s="631"/>
+      <c r="AD13" s="668"/>
+      <c r="AF13" s="656"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="238" t="s">
         <v>308</v>
@@ -7764,8 +7764,8 @@
       <c r="AJ13" s="80"/>
       <c r="AK13" s="257"/>
       <c r="AL13" s="257"/>
-      <c r="AM13" s="655"/>
-      <c r="AN13" s="641"/>
+      <c r="AM13" s="651"/>
+      <c r="AN13" s="636"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="450"/>
@@ -7773,18 +7773,18 @@
       <c r="C14" s="459"/>
       <c r="D14" s="452"/>
       <c r="E14" s="453"/>
-      <c r="F14" s="620"/>
+      <c r="F14" s="641"/>
       <c r="G14" s="605" t="s">
         <v>429</v>
       </c>
       <c r="H14" s="605"/>
       <c r="I14" s="605"/>
-      <c r="J14" s="627"/>
+      <c r="J14" s="683"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="623"/>
+      <c r="O14" s="679"/>
       <c r="Q14" s="61" t="s">
         <v>532</v>
       </c>
@@ -7798,24 +7798,24 @@
       <c r="X14" s="431" t="s">
         <v>168</v>
       </c>
-      <c r="Y14" s="658"/>
+      <c r="Y14" s="654"/>
       <c r="Z14" s="407">
         <v>1</v>
       </c>
       <c r="AA14" s="307"/>
       <c r="AB14" s="209"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="639"/>
+      <c r="AD14" s="668"/>
       <c r="AE14" s="257"/>
-      <c r="AF14" s="631"/>
+      <c r="AF14" s="656"/>
       <c r="AG14" s="257"/>
       <c r="AH14" s="257"/>
       <c r="AI14" s="70"/>
       <c r="AJ14" s="257"/>
       <c r="AK14" s="257"/>
       <c r="AL14" s="257"/>
-      <c r="AM14" s="655"/>
-      <c r="AN14" s="641"/>
+      <c r="AM14" s="651"/>
+      <c r="AN14" s="636"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="449" t="s">
@@ -7824,8 +7824,8 @@
       <c r="C15" s="598" t="s">
         <v>373</v>
       </c>
-      <c r="F15" s="620"/>
-      <c r="O15" s="623"/>
+      <c r="F15" s="641"/>
+      <c r="O15" s="679"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -7838,7 +7838,7 @@
       <c r="X15" s="431" t="s">
         <v>169</v>
       </c>
-      <c r="Y15" s="658"/>
+      <c r="Y15" s="654"/>
       <c r="Z15" s="409">
         <v>1</v>
       </c>
@@ -7847,8 +7847,8 @@
       <c r="AC15" s="76" t="s">
         <v>479</v>
       </c>
-      <c r="AD15" s="639"/>
-      <c r="AF15" s="631"/>
+      <c r="AD15" s="668"/>
+      <c r="AF15" s="656"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="238" t="s">
         <v>448</v>
@@ -7861,8 +7861,8 @@
       </c>
       <c r="AK15" s="257"/>
       <c r="AL15" s="257"/>
-      <c r="AM15" s="655"/>
-      <c r="AN15" s="641"/>
+      <c r="AM15" s="651"/>
+      <c r="AN15" s="636"/>
       <c r="AP15" s="76" t="s">
         <v>73</v>
       </c>
@@ -7884,13 +7884,13 @@
       <c r="E16" s="224">
         <v>1</v>
       </c>
-      <c r="F16" s="620"/>
+      <c r="F16" s="641"/>
       <c r="G16" s="337" t="s">
         <v>488</v>
       </c>
       <c r="I16" s="469"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="623"/>
+      <c r="O16" s="679"/>
       <c r="R16" s="435" t="s">
         <v>184</v>
       </c>
@@ -7901,7 +7901,7 @@
       <c r="X16" s="431" t="s">
         <v>170</v>
       </c>
-      <c r="Y16" s="658"/>
+      <c r="Y16" s="654"/>
       <c r="Z16" s="407">
         <v>1</v>
       </c>
@@ -7922,18 +7922,18 @@
       <c r="AM16" s="428" t="s">
         <v>317</v>
       </c>
-      <c r="AN16" s="641"/>
+      <c r="AN16" s="636"/>
       <c r="AP16" s="76" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="620"/>
+      <c r="F17" s="641"/>
       <c r="I17" s="470"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="623"/>
+      <c r="O17" s="679"/>
       <c r="Q17" s="21" t="s">
         <v>530</v>
       </c>
@@ -7953,7 +7953,7 @@
       <c r="X17" s="431" t="s">
         <v>171</v>
       </c>
-      <c r="Y17" s="658"/>
+      <c r="Y17" s="654"/>
       <c r="Z17" s="409"/>
       <c r="AA17" s="307"/>
       <c r="AB17" s="209"/>
@@ -7978,7 +7978,7 @@
       <c r="AK17" s="257"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="428"/>
-      <c r="AN17" s="641"/>
+      <c r="AN17" s="636"/>
       <c r="AO17" s="204" t="s">
         <v>497</v>
       </c>
@@ -8002,21 +8002,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="620"/>
+      <c r="F18" s="641"/>
       <c r="G18" s="337" t="s">
         <v>527</v>
       </c>
       <c r="I18" s="24"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="623"/>
+      <c r="O18" s="679"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="615" t="s">
+      <c r="R18" s="673" t="s">
         <v>535</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="663" t="s">
+      <c r="U18" s="612" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -8026,7 +8026,7 @@
       <c r="X18" s="431" t="s">
         <v>172</v>
       </c>
-      <c r="Y18" s="658"/>
+      <c r="Y18" s="654"/>
       <c r="Z18" s="409">
         <v>1</v>
       </c>
@@ -8037,38 +8037,38 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="257"/>
-      <c r="AF18" s="630" t="s">
+      <c r="AF18" s="650" t="s">
         <v>475</v>
       </c>
       <c r="AG18" s="257"/>
       <c r="AH18" s="70"/>
       <c r="AI18" s="70"/>
-      <c r="AJ18" s="656" t="s">
+      <c r="AJ18" s="652" t="s">
         <v>315</v>
       </c>
       <c r="AK18" s="257"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="428"/>
-      <c r="AN18" s="641"/>
+      <c r="AN18" s="636"/>
       <c r="AP18" s="76" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="620"/>
+      <c r="F19" s="641"/>
       <c r="I19" s="219"/>
-      <c r="O19" s="623"/>
-      <c r="R19" s="616"/>
+      <c r="O19" s="679"/>
+      <c r="R19" s="674"/>
       <c r="S19" s="30" t="s">
         <v>533</v>
       </c>
-      <c r="U19" s="664"/>
+      <c r="U19" s="613"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="431" t="s">
         <v>173</v>
       </c>
-      <c r="Y19" s="658"/>
+      <c r="Y19" s="654"/>
       <c r="Z19" s="407">
         <v>1</v>
       </c>
@@ -8077,17 +8077,17 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="257"/>
-      <c r="AF19" s="630"/>
+      <c r="AF19" s="650"/>
       <c r="AG19" s="257"/>
       <c r="AH19" s="257"/>
       <c r="AI19" s="70"/>
-      <c r="AJ19" s="656"/>
+      <c r="AJ19" s="652"/>
       <c r="AK19" s="460" t="s">
         <v>251</v>
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="428"/>
-      <c r="AN19" s="641"/>
+      <c r="AN19" s="636"/>
       <c r="AP19" s="76" t="s">
         <v>468</v>
       </c>
@@ -8108,24 +8108,24 @@
       <c r="E20" s="437">
         <v>-1</v>
       </c>
-      <c r="F20" s="620"/>
+      <c r="F20" s="641"/>
       <c r="G20" s="337" t="s">
         <v>491</v>
       </c>
       <c r="I20" s="219"/>
-      <c r="O20" s="623"/>
-      <c r="Q20" s="625" t="s">
+      <c r="O20" s="679"/>
+      <c r="Q20" s="681" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="404" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="665"/>
+      <c r="U20" s="614"/>
       <c r="W20" s="405"/>
       <c r="X20" s="432" t="s">
         <v>174</v>
       </c>
-      <c r="Y20" s="658"/>
+      <c r="Y20" s="654"/>
       <c r="Z20" s="411">
         <v>1</v>
       </c>
@@ -8150,7 +8150,7 @@
       <c r="AM20" s="381" t="s">
         <v>249</v>
       </c>
-      <c r="AN20" s="641"/>
+      <c r="AN20" s="636"/>
       <c r="AO20" s="338" t="s">
         <v>460</v>
       </c>
@@ -8171,20 +8171,20 @@
       <c r="E21" s="265">
         <v>0</v>
       </c>
-      <c r="F21" s="620"/>
+      <c r="F21" s="641"/>
       <c r="I21" s="219"/>
-      <c r="O21" s="623"/>
-      <c r="Q21" s="626"/>
+      <c r="O21" s="679"/>
+      <c r="Q21" s="682"/>
       <c r="T21" s="422"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="660"/>
+      <c r="V21" s="609"/>
       <c r="W21" s="426" t="s">
         <v>175</v>
       </c>
       <c r="X21" s="429" t="s">
         <v>186</v>
       </c>
-      <c r="Y21" s="658"/>
+      <c r="Y21" s="654"/>
       <c r="Z21" s="445">
         <v>3</v>
       </c>
@@ -8215,15 +8215,15 @@
       <c r="AM21" s="428" t="s">
         <v>544</v>
       </c>
-      <c r="AN21" s="641"/>
+      <c r="AN21" s="636"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="620"/>
+      <c r="F22" s="641"/>
       <c r="G22" s="337" t="s">
         <v>489</v>
       </c>
       <c r="I22" s="219"/>
-      <c r="O22" s="623"/>
+      <c r="O22" s="679"/>
       <c r="R22" s="434" t="s">
         <v>44</v>
       </c>
@@ -8231,14 +8231,14 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="661"/>
+      <c r="V22" s="610"/>
       <c r="W22" s="426" t="s">
         <v>175</v>
       </c>
       <c r="X22" s="429" t="s">
         <v>187</v>
       </c>
-      <c r="Y22" s="658"/>
+      <c r="Y22" s="654"/>
       <c r="Z22" s="415"/>
       <c r="AA22" s="10"/>
       <c r="AB22" s="415"/>
@@ -8249,7 +8249,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="630" t="s">
+      <c r="AJ22" s="650" t="s">
         <v>472</v>
       </c>
       <c r="AK22" s="257"/>
@@ -8257,7 +8257,7 @@
         <v>478</v>
       </c>
       <c r="AM22" s="300"/>
-      <c r="AN22" s="641"/>
+      <c r="AN22" s="636"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="231" t="s">
@@ -8275,22 +8275,22 @@
       <c r="E23" s="225">
         <v>1</v>
       </c>
-      <c r="F23" s="620"/>
+      <c r="F23" s="641"/>
       <c r="I23" s="219"/>
-      <c r="O23" s="623"/>
-      <c r="Q23" s="625" t="s">
+      <c r="O23" s="679"/>
+      <c r="Q23" s="681" t="s">
         <v>144</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="420" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="661"/>
+      <c r="V23" s="610"/>
       <c r="W23" s="148"/>
       <c r="X23" s="429" t="s">
         <v>188</v>
       </c>
-      <c r="Y23" s="658"/>
+      <c r="Y23" s="654"/>
       <c r="Z23" s="17"/>
       <c r="AA23" s="10"/>
       <c r="AB23" s="415"/>
@@ -8301,13 +8301,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="630"/>
+      <c r="AJ23" s="650"/>
       <c r="AK23" s="257"/>
       <c r="AL23" s="80" t="s">
         <v>507</v>
       </c>
       <c r="AM23" s="300"/>
-      <c r="AN23" s="641"/>
+      <c r="AN23" s="636"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="440" t="s">
@@ -8325,23 +8325,23 @@
       <c r="E24" s="436">
         <v>1</v>
       </c>
-      <c r="F24" s="620"/>
+      <c r="F24" s="641"/>
       <c r="G24" s="61" t="s">
         <v>490</v>
       </c>
       <c r="I24" s="219"/>
-      <c r="O24" s="623"/>
-      <c r="Q24" s="626"/>
+      <c r="O24" s="679"/>
+      <c r="Q24" s="682"/>
       <c r="T24" s="17"/>
       <c r="U24" s="227" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="661"/>
+      <c r="V24" s="610"/>
       <c r="W24" s="148"/>
       <c r="X24" s="429" t="s">
         <v>185</v>
       </c>
-      <c r="Y24" s="658"/>
+      <c r="Y24" s="654"/>
       <c r="Z24" s="17"/>
       <c r="AA24" s="10"/>
       <c r="AB24" s="415"/>
@@ -8360,12 +8360,12 @@
         <v>463</v>
       </c>
       <c r="AM24" s="300"/>
-      <c r="AN24" s="641"/>
+      <c r="AN24" s="636"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="620"/>
+      <c r="F25" s="641"/>
       <c r="I25" s="219"/>
-      <c r="O25" s="623"/>
+      <c r="O25" s="679"/>
       <c r="P25" s="204" t="s">
         <v>280</v>
       </c>
@@ -8378,12 +8378,12 @@
       <c r="U25" s="400" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="662"/>
+      <c r="V25" s="611"/>
       <c r="W25" s="148"/>
       <c r="X25" s="429" t="s">
         <v>189</v>
       </c>
-      <c r="Y25" s="658"/>
+      <c r="Y25" s="654"/>
       <c r="Z25" s="17"/>
       <c r="AA25" s="10"/>
       <c r="AB25" s="415"/>
@@ -8400,7 +8400,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="300"/>
-      <c r="AN25" s="641"/>
+      <c r="AN25" s="636"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="231" t="s">
@@ -8418,17 +8418,17 @@
       <c r="E26" s="380">
         <v>1</v>
       </c>
-      <c r="F26" s="620"/>
+      <c r="F26" s="641"/>
       <c r="G26" s="337" t="s">
         <v>487</v>
       </c>
       <c r="I26" s="219"/>
-      <c r="O26" s="623"/>
-      <c r="P26" s="643" t="s">
+      <c r="O26" s="679"/>
+      <c r="P26" s="638" t="s">
         <v>525</v>
       </c>
-      <c r="Q26" s="644"/>
-      <c r="R26" s="617" t="s">
+      <c r="Q26" s="639"/>
+      <c r="R26" s="675" t="s">
         <v>534</v>
       </c>
       <c r="T26" s="178"/>
@@ -8440,7 +8440,7 @@
       <c r="X26" s="429" t="s">
         <v>181</v>
       </c>
-      <c r="Y26" s="658"/>
+      <c r="Y26" s="654"/>
       <c r="Z26" s="17"/>
       <c r="AA26" s="10"/>
       <c r="AB26" s="415"/>
@@ -8467,7 +8467,7 @@
       <c r="AM26" s="442" t="s">
         <v>456</v>
       </c>
-      <c r="AN26" s="641"/>
+      <c r="AN26" s="636"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -8479,13 +8479,13 @@
       <c r="E27" s="265" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="621"/>
+      <c r="F27" s="677"/>
       <c r="G27" s="61" t="s">
         <v>543</v>
       </c>
       <c r="I27" s="220"/>
-      <c r="O27" s="624"/>
-      <c r="R27" s="618"/>
+      <c r="O27" s="680"/>
+      <c r="R27" s="676"/>
       <c r="S27" s="421" t="s">
         <v>54</v>
       </c>
@@ -8498,7 +8498,7 @@
       <c r="X27" s="429" t="s">
         <v>529</v>
       </c>
-      <c r="Y27" s="659"/>
+      <c r="Y27" s="655"/>
       <c r="Z27" s="161"/>
       <c r="AA27" s="13"/>
       <c r="AB27" s="416"/>
@@ -8515,10 +8515,48 @@
       <c r="AM27" s="381" t="s">
         <v>319</v>
       </c>
-      <c r="AN27" s="642"/>
+      <c r="AN27" s="637"/>
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="O10:O27"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="AI6:AI10"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AG7:AG12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="AN1:AN27"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="M2:M9"/>
+    <mergeCell ref="O2:O9"/>
+    <mergeCell ref="P10:P13"/>
+    <mergeCell ref="AK6:AK7"/>
+    <mergeCell ref="AM12:AM15"/>
+    <mergeCell ref="AF18:AF19"/>
+    <mergeCell ref="AJ18:AJ19"/>
+    <mergeCell ref="Y1:Y27"/>
+    <mergeCell ref="AJ22:AJ23"/>
+    <mergeCell ref="AK9:AK10"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="R2:R3"/>
     <mergeCell ref="V21:V25"/>
     <mergeCell ref="U18:U20"/>
     <mergeCell ref="C2:C3"/>
@@ -8535,44 +8573,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="AN1:AN27"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="M2:M9"/>
-    <mergeCell ref="O2:O9"/>
-    <mergeCell ref="P10:P13"/>
-    <mergeCell ref="AK6:AK7"/>
-    <mergeCell ref="AM12:AM15"/>
-    <mergeCell ref="AF18:AF19"/>
-    <mergeCell ref="AJ18:AJ19"/>
-    <mergeCell ref="Y1:Y27"/>
-    <mergeCell ref="AJ22:AJ23"/>
-    <mergeCell ref="AK9:AK10"/>
-    <mergeCell ref="AD3:AD4"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AI6:AI10"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AG7:AG12"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="F2:F27"/>
-    <mergeCell ref="O10:O27"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8609,12 +8609,12 @@
       <c r="B1" s="603" t="s">
         <v>310</v>
       </c>
-      <c r="C1" s="627"/>
+      <c r="C1" s="683"/>
       <c r="D1" s="204"/>
       <c r="J1" s="603" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="627"/>
+      <c r="K1" s="683"/>
       <c r="L1" s="195" t="s">
         <v>330</v>
       </c>
@@ -9017,7 +9017,7 @@
       <c r="P1" s="398" t="s">
         <v>397</v>
       </c>
-      <c r="Q1" s="701" t="s">
+      <c r="Q1" s="714" t="s">
         <v>180</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -9041,7 +9041,7 @@
       <c r="AA1" s="517" t="s">
         <v>437</v>
       </c>
-      <c r="AB1" s="695" t="s">
+      <c r="AB1" s="708" t="s">
         <v>593</v>
       </c>
       <c r="AC1" s="99" t="s">
@@ -9063,32 +9063,32 @@
       </c>
     </row>
     <row r="2" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="706">
+      <c r="A2" s="693">
         <f ca="1">TODAY()</f>
-        <v>45293</v>
-      </c>
-      <c r="B2" s="708" t="s">
+        <v>45294</v>
+      </c>
+      <c r="B2" s="695" t="s">
         <v>379</v>
       </c>
-      <c r="C2" s="645" t="s">
+      <c r="C2" s="615" t="s">
         <v>357</v>
       </c>
-      <c r="D2" s="710" t="s">
+      <c r="D2" s="697" t="s">
         <v>102</v>
       </c>
-      <c r="E2" s="712" t="s">
+      <c r="E2" s="699" t="s">
         <v>64</v>
       </c>
       <c r="F2" s="191" t="s">
         <v>218</v>
       </c>
-      <c r="G2" s="613" t="s">
+      <c r="G2" s="659" t="s">
         <v>372</v>
       </c>
       <c r="H2" s="206" t="s">
         <v>218</v>
       </c>
-      <c r="I2" s="692" t="s">
+      <c r="I2" s="705" t="s">
         <v>102</v>
       </c>
       <c r="J2" s="396" t="s">
@@ -9112,7 +9112,7 @@
       <c r="P2" s="399">
         <v>40</v>
       </c>
-      <c r="Q2" s="702"/>
+      <c r="Q2" s="715"/>
       <c r="R2" s="21">
         <f>R7+R20</f>
         <v>2</v>
@@ -9137,7 +9137,7 @@
         <f>IF((Z2+T2)&gt;0,0,-1)</f>
         <v>0</v>
       </c>
-      <c r="AB2" s="696"/>
+      <c r="AB2" s="709"/>
       <c r="AC2" s="35"/>
       <c r="AH2" s="6" t="s">
         <v>344</v>
@@ -9152,14 +9152,14 @@
       </c>
     </row>
     <row r="3" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="707"/>
-      <c r="B3" s="709"/>
-      <c r="C3" s="646"/>
-      <c r="D3" s="711"/>
-      <c r="E3" s="713"/>
-      <c r="G3" s="614"/>
+      <c r="A3" s="694"/>
+      <c r="B3" s="696"/>
+      <c r="C3" s="616"/>
+      <c r="D3" s="698"/>
+      <c r="E3" s="700"/>
+      <c r="G3" s="660"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="693"/>
+      <c r="I3" s="706"/>
       <c r="K3" s="24">
         <v>2</v>
       </c>
@@ -9174,7 +9174,7 @@
       <c r="V3" s="470"/>
       <c r="W3" s="6"/>
       <c r="X3" s="470"/>
-      <c r="AB3" s="696"/>
+      <c r="AB3" s="709"/>
       <c r="AC3" s="35"/>
       <c r="AE3" s="100" t="s">
         <v>588</v>
@@ -9203,10 +9203,10 @@
         <v>380</v>
       </c>
       <c r="B4" s="243"/>
-      <c r="C4" s="714" t="s">
+      <c r="C4" s="701" t="s">
         <v>177</v>
       </c>
-      <c r="I4" s="693"/>
+      <c r="I4" s="706"/>
       <c r="R4" s="471" t="s">
         <v>588</v>
       </c>
@@ -9218,7 +9218,7 @@
       <c r="V4" s="470"/>
       <c r="W4" s="6"/>
       <c r="X4" s="470"/>
-      <c r="AB4" s="696"/>
+      <c r="AB4" s="709"/>
       <c r="AC4" s="35"/>
       <c r="AE4" s="20"/>
       <c r="AF4" s="100" t="s">
@@ -9247,7 +9247,7 @@
       <c r="B5" s="100" t="s">
         <v>357</v>
       </c>
-      <c r="C5" s="715"/>
+      <c r="C5" s="702"/>
       <c r="D5" s="222" t="s">
         <v>102</v>
       </c>
@@ -9263,7 +9263,7 @@
       <c r="H5" s="206" t="s">
         <v>218</v>
       </c>
-      <c r="I5" s="693"/>
+      <c r="I5" s="706"/>
       <c r="J5" s="397" t="s">
         <v>268</v>
       </c>
@@ -9290,7 +9290,7 @@
       <c r="V5" s="468"/>
       <c r="W5" s="6"/>
       <c r="X5" s="468"/>
-      <c r="AB5" s="696"/>
+      <c r="AB5" s="709"/>
       <c r="AC5" s="2" t="s">
         <v>591</v>
       </c>
@@ -9310,19 +9310,19 @@
       <c r="AL5" s="468"/>
     </row>
     <row r="6" spans="1:38" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="703" t="s">
+      <c r="A6" s="690" t="s">
         <v>285</v>
       </c>
       <c r="B6" s="105" t="s">
         <v>198</v>
       </c>
-      <c r="C6" s="628"/>
-      <c r="D6" s="629"/>
+      <c r="C6" s="661"/>
+      <c r="D6" s="662"/>
       <c r="E6" s="96">
         <v>1</v>
       </c>
       <c r="G6" s="599"/>
-      <c r="I6" s="693"/>
+      <c r="I6" s="706"/>
       <c r="P6" s="61" t="s">
         <v>591</v>
       </c>
@@ -9334,7 +9334,7 @@
         <f>S7+S11-SUM(V2:V10)</f>
         <v>3</v>
       </c>
-      <c r="AB6" s="696"/>
+      <c r="AB6" s="709"/>
       <c r="AC6" s="35"/>
       <c r="AE6" s="64">
         <f>AE7-SUM(AL2:AL10)+AE11</f>
@@ -9350,7 +9350,7 @@
       <c r="AL6" s="112"/>
     </row>
     <row r="7" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="704"/>
+      <c r="A7" s="691"/>
       <c r="B7" s="100" t="s">
         <v>154</v>
       </c>
@@ -9361,7 +9361,7 @@
         <v>135</v>
       </c>
       <c r="G7" s="599"/>
-      <c r="I7" s="693"/>
+      <c r="I7" s="706"/>
       <c r="M7" s="16" t="s">
         <v>347</v>
       </c>
@@ -9391,7 +9391,7 @@
         <v>249</v>
       </c>
       <c r="X7" s="469"/>
-      <c r="AB7" s="696"/>
+      <c r="AB7" s="709"/>
       <c r="AC7" s="99" t="s">
         <v>592</v>
       </c>
@@ -9419,7 +9419,7 @@
       <c r="AL7" s="24"/>
     </row>
     <row r="8" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="705"/>
+      <c r="A8" s="692"/>
       <c r="B8" s="212" t="s">
         <v>28</v>
       </c>
@@ -9428,7 +9428,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="599"/>
-      <c r="I8" s="693"/>
+      <c r="I8" s="706"/>
       <c r="N8" s="80"/>
       <c r="U8" s="6"/>
       <c r="V8" s="24"/>
@@ -9436,7 +9436,7 @@
         <v>611</v>
       </c>
       <c r="X8" s="470"/>
-      <c r="AB8" s="696"/>
+      <c r="AB8" s="709"/>
       <c r="AC8" s="515"/>
       <c r="AH8" s="6" t="s">
         <v>610</v>
@@ -9467,7 +9467,7 @@
       </c>
       <c r="G9" s="599"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="693"/>
+      <c r="I9" s="706"/>
       <c r="M9" s="19" t="s">
         <v>524</v>
       </c>
@@ -9478,7 +9478,7 @@
         <v>603</v>
       </c>
       <c r="X9" s="470"/>
-      <c r="AB9" s="696"/>
+      <c r="AB9" s="709"/>
       <c r="AC9" s="515"/>
       <c r="AE9" s="20"/>
       <c r="AF9" s="20"/>
@@ -9506,7 +9506,7 @@
         <v>37</v>
       </c>
       <c r="G10" s="599"/>
-      <c r="I10" s="693"/>
+      <c r="I10" s="706"/>
       <c r="J10" s="24" t="s">
         <v>372</v>
       </c>
@@ -9521,7 +9521,7 @@
       <c r="V10" s="470"/>
       <c r="W10" s="6"/>
       <c r="X10" s="470"/>
-      <c r="AB10" s="696"/>
+      <c r="AB10" s="709"/>
       <c r="AC10" s="515"/>
       <c r="AE10" s="20"/>
       <c r="AF10" s="20"/>
@@ -9549,7 +9549,7 @@
         <v>265</v>
       </c>
       <c r="G11" s="599"/>
-      <c r="I11" s="693"/>
+      <c r="I11" s="706"/>
       <c r="J11" s="24" t="s">
         <v>194</v>
       </c>
@@ -9575,13 +9575,13 @@
       <c r="S11" s="24">
         <v>3</v>
       </c>
-      <c r="U11" s="698" t="s">
+      <c r="U11" s="711" t="s">
         <v>557</v>
       </c>
-      <c r="V11" s="699"/>
-      <c r="W11" s="699"/>
-      <c r="X11" s="700"/>
-      <c r="AB11" s="697"/>
+      <c r="V11" s="712"/>
+      <c r="W11" s="712"/>
+      <c r="X11" s="713"/>
+      <c r="AB11" s="710"/>
       <c r="AC11" s="99" t="s">
         <v>594</v>
       </c>
@@ -9595,13 +9595,13 @@
         <v>3</v>
       </c>
       <c r="AG11" s="414"/>
-      <c r="AH11" s="698" t="s">
+      <c r="AH11" s="711" t="s">
         <v>602</v>
       </c>
-      <c r="AI11" s="699"/>
-      <c r="AJ11" s="699"/>
-      <c r="AK11" s="699"/>
-      <c r="AL11" s="700"/>
+      <c r="AI11" s="712"/>
+      <c r="AJ11" s="712"/>
+      <c r="AK11" s="712"/>
+      <c r="AL11" s="713"/>
     </row>
     <row r="12" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="227" t="s">
@@ -9612,7 +9612,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="599"/>
-      <c r="I12" s="693"/>
+      <c r="I12" s="706"/>
       <c r="J12" s="24" t="s">
         <v>515</v>
       </c>
@@ -9645,7 +9645,7 @@
       </c>
       <c r="D13" s="20"/>
       <c r="G13" s="599"/>
-      <c r="I13" s="693"/>
+      <c r="I13" s="706"/>
       <c r="J13" s="108" t="s">
         <v>547</v>
       </c>
@@ -9689,7 +9689,7 @@
       <c r="H14" s="206" t="s">
         <v>218</v>
       </c>
-      <c r="I14" s="693"/>
+      <c r="I14" s="706"/>
       <c r="U14" s="67" t="s">
         <v>80</v>
       </c>
@@ -9716,7 +9716,7 @@
       <c r="H15" s="271">
         <v>0</v>
       </c>
-      <c r="I15" s="693"/>
+      <c r="I15" s="706"/>
       <c r="J15" s="108" t="s">
         <v>153</v>
       </c>
@@ -9747,7 +9747,7 @@
       <c r="D16" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="I16" s="693"/>
+      <c r="I16" s="706"/>
       <c r="K16" s="100" t="s">
         <v>44</v>
       </c>
@@ -9791,7 +9791,7 @@
       <c r="G17" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="I17" s="693"/>
+      <c r="I17" s="706"/>
       <c r="L17" s="2" t="s">
         <v>426</v>
       </c>
@@ -9805,13 +9805,13 @@
     </row>
     <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
-      <c r="I18" s="693"/>
+      <c r="I18" s="706"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="690" t="s">
+      <c r="O18" s="703" t="s">
         <v>516</v>
       </c>
-      <c r="P18" s="691"/>
+      <c r="P18" s="704"/>
       <c r="Q18" s="127" t="s">
         <v>44</v>
       </c>
@@ -9833,7 +9833,7 @@
       </c>
     </row>
     <row r="19" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="693"/>
+      <c r="I19" s="706"/>
       <c r="M19" s="21" t="s">
         <v>425</v>
       </c>
@@ -9865,7 +9865,7 @@
       <c r="G20" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="I20" s="693"/>
+      <c r="I20" s="706"/>
       <c r="K20" s="19" t="s">
         <v>422</v>
       </c>
@@ -9894,7 +9894,7 @@
       <c r="X20" s="468"/>
     </row>
     <row r="21" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="693"/>
+      <c r="I21" s="706"/>
       <c r="M21" s="216" t="s">
         <v>411</v>
       </c>
@@ -9924,7 +9924,7 @@
       <c r="G22" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="I22" s="693"/>
+      <c r="I22" s="706"/>
       <c r="P22" s="99" t="s">
         <v>590</v>
       </c>
@@ -9939,7 +9939,7 @@
       <c r="E23" s="283" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="693"/>
+      <c r="I23" s="706"/>
       <c r="Q23" s="24">
         <f>SUM(V23:V31)</f>
         <v>7</v>
@@ -9956,7 +9956,7 @@
       </c>
     </row>
     <row r="24" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="693"/>
+      <c r="I24" s="706"/>
       <c r="U24" s="35"/>
       <c r="V24" s="509">
         <v>1</v>
@@ -9984,7 +9984,7 @@
       <c r="H25" s="191" t="s">
         <v>266</v>
       </c>
-      <c r="I25" s="693"/>
+      <c r="I25" s="706"/>
       <c r="J25" s="397" t="s">
         <v>269</v>
       </c>
@@ -10029,7 +10029,7 @@
       <c r="H26" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="I26" s="693"/>
+      <c r="I26" s="706"/>
       <c r="K26" s="24">
         <v>15</v>
       </c>
@@ -10064,7 +10064,7 @@
       </c>
     </row>
     <row r="27" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="693"/>
+      <c r="I27" s="706"/>
       <c r="O27" s="2" t="s">
         <v>98</v>
       </c>
@@ -10091,7 +10091,7 @@
       <c r="E28" s="215">
         <v>2</v>
       </c>
-      <c r="I28" s="693"/>
+      <c r="I28" s="706"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="142"/>
@@ -10113,7 +10113,7 @@
       <c r="H29" s="191" t="s">
         <v>267</v>
       </c>
-      <c r="I29" s="694"/>
+      <c r="I29" s="707"/>
       <c r="J29" s="324"/>
       <c r="L29" s="96" t="s">
         <v>273</v>
@@ -10171,6 +10171,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I2:I29"/>
+    <mergeCell ref="AB1:AB11"/>
+    <mergeCell ref="AH11:AL11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="U11:X11"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="G5:G14"/>
     <mergeCell ref="A2:A3"/>
@@ -10182,13 +10189,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I2:I29"/>
-    <mergeCell ref="AB1:AB11"/>
-    <mergeCell ref="AH11:AL11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="U11:X11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10199,8 +10199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AT37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10298,16 +10298,16 @@
       </c>
       <c r="S1" s="151">
         <f ca="1">TODAY()</f>
-        <v>45293</v>
-      </c>
-      <c r="T1" s="735"/>
+        <v>45294</v>
+      </c>
+      <c r="T1" s="742"/>
       <c r="U1" s="142"/>
       <c r="V1" s="6"/>
       <c r="W1" s="6"/>
-      <c r="X1" s="719" t="s">
+      <c r="X1" s="726" t="s">
         <v>441</v>
       </c>
-      <c r="Y1" s="720"/>
+      <c r="Y1" s="727"/>
       <c r="Z1" s="306">
         <f>68-(W8+Y3+X3+U3)</f>
         <v>0</v>
@@ -10323,27 +10323,27 @@
       <c r="AD1" s="302" t="s">
         <v>44</v>
       </c>
-      <c r="AE1" s="721" t="s">
+      <c r="AE1" s="728" t="s">
         <v>190</v>
       </c>
-      <c r="AF1" s="722"/>
-      <c r="AG1" s="723"/>
-      <c r="AH1" s="724" t="s">
+      <c r="AF1" s="729"/>
+      <c r="AG1" s="730"/>
+      <c r="AH1" s="731" t="s">
         <v>293</v>
       </c>
-      <c r="AI1" s="725"/>
-      <c r="AJ1" s="726"/>
-      <c r="AK1" s="613" t="s">
+      <c r="AI1" s="732"/>
+      <c r="AJ1" s="733"/>
+      <c r="AK1" s="659" t="s">
         <v>613</v>
       </c>
       <c r="AL1" s="550" t="s">
         <v>614</v>
       </c>
-      <c r="AM1" s="716" t="s">
+      <c r="AM1" s="723" t="s">
         <v>444</v>
       </c>
-      <c r="AN1" s="717"/>
-      <c r="AO1" s="718"/>
+      <c r="AN1" s="724"/>
+      <c r="AO1" s="725"/>
       <c r="AR1" s="142"/>
     </row>
     <row r="2" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10358,27 +10358,27 @@
         <f>K2+L2</f>
         <v>29</v>
       </c>
-      <c r="K2" s="743">
+      <c r="K2" s="721">
         <f>SUM(K4:K37)</f>
         <v>7</v>
       </c>
-      <c r="L2" s="741">
+      <c r="L2" s="719">
         <f>SUM(L4:L37)</f>
         <v>22</v>
       </c>
-      <c r="M2" s="727">
+      <c r="M2" s="734">
         <f>SUM(M5:M30)</f>
         <v>0</v>
       </c>
-      <c r="N2" s="729">
+      <c r="N2" s="736">
         <f>SUM(N4:N29)</f>
         <v>8</v>
       </c>
-      <c r="O2" s="731">
+      <c r="O2" s="738">
         <f>SUM(O4:O29)</f>
         <v>11</v>
       </c>
-      <c r="P2" s="637">
+      <c r="P2" s="666">
         <f>SUM(N30:N37)* (-1)</f>
         <v>-1</v>
       </c>
@@ -10391,14 +10391,14 @@
       <c r="S2" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="T2" s="736"/>
+      <c r="T2" s="743"/>
       <c r="U2" s="537" t="s">
         <v>262</v>
       </c>
       <c r="V2" s="482" t="s">
         <v>219</v>
       </c>
-      <c r="W2" s="733" t="s">
+      <c r="W2" s="740" t="s">
         <v>234</v>
       </c>
       <c r="X2" s="483" t="s">
@@ -10440,7 +10440,7 @@
       <c r="AJ2" s="150" t="s">
         <v>288</v>
       </c>
-      <c r="AK2" s="614"/>
+      <c r="AK2" s="660"/>
       <c r="AL2" s="591" t="s">
         <v>288</v>
       </c>
@@ -10468,12 +10468,12 @@
         <f>V3+X3+Y3+U3</f>
         <v>68</v>
       </c>
-      <c r="K3" s="744"/>
-      <c r="L3" s="742"/>
-      <c r="M3" s="728"/>
-      <c r="N3" s="730"/>
-      <c r="O3" s="732"/>
-      <c r="P3" s="638"/>
+      <c r="K3" s="722"/>
+      <c r="L3" s="720"/>
+      <c r="M3" s="735"/>
+      <c r="N3" s="737"/>
+      <c r="O3" s="739"/>
+      <c r="P3" s="667"/>
       <c r="Q3" s="172">
         <f>(M2+N2)-Y3</f>
         <v>0</v>
@@ -10481,7 +10481,7 @@
       <c r="S3" s="159" t="s">
         <v>244</v>
       </c>
-      <c r="T3" s="737"/>
+      <c r="T3" s="744"/>
       <c r="U3" s="538">
         <f>SUM(U4:U29)</f>
         <v>14</v>
@@ -10490,7 +10490,7 @@
         <f>SUM(V4:V29)</f>
         <v>37</v>
       </c>
-      <c r="W3" s="734"/>
+      <c r="W3" s="741"/>
       <c r="X3" s="485">
         <f t="shared" ref="X3:AC3" si="0">SUM(X4:X29)</f>
         <v>9</v>
@@ -10598,7 +10598,7 @@
         <f>AC4</f>
         <v>0</v>
       </c>
-      <c r="P4" s="738"/>
+      <c r="P4" s="716"/>
       <c r="Q4" s="20"/>
       <c r="R4" s="2" t="s">
         <v>334</v>
@@ -10682,7 +10682,7 @@
         <f>AC5</f>
         <v>0</v>
       </c>
-      <c r="P5" s="739"/>
+      <c r="P5" s="717"/>
       <c r="Q5" s="20"/>
       <c r="R5" s="2" t="s">
         <v>340</v>
@@ -10776,7 +10776,7 @@
         <f>AC6</f>
         <v>1</v>
       </c>
-      <c r="P6" s="739"/>
+      <c r="P6" s="717"/>
       <c r="Q6" s="54" t="s">
         <v>335</v>
       </c>
@@ -10881,7 +10881,7 @@
         <f>AC7</f>
         <v>1</v>
       </c>
-      <c r="P7" s="739"/>
+      <c r="P7" s="717"/>
       <c r="Q7" s="20"/>
       <c r="R7" s="2" t="s">
         <v>335</v>
@@ -10997,7 +10997,7 @@
         <f t="shared" ref="O8:O37" si="10">AC8</f>
         <v>0</v>
       </c>
-      <c r="P8" s="739"/>
+      <c r="P8" s="717"/>
       <c r="Q8" s="108" t="s">
         <v>233</v>
       </c>
@@ -11090,7 +11090,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P9" s="739"/>
+      <c r="P9" s="717"/>
       <c r="Q9" s="108" t="s">
         <v>335</v>
       </c>
@@ -11195,7 +11195,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P10" s="739"/>
+      <c r="P10" s="717"/>
       <c r="Q10" s="20"/>
       <c r="R10" s="2" t="s">
         <v>340</v>
@@ -11287,7 +11287,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P11" s="739"/>
+      <c r="P11" s="717"/>
       <c r="Q11" s="108" t="s">
         <v>335</v>
       </c>
@@ -11352,14 +11352,14 @@
       <c r="AR11" s="508"/>
     </row>
     <row r="12" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="675" t="s">
+      <c r="A12" s="626" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
         <v>13</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="E12" s="625" t="s">
+      <c r="E12" s="681" t="s">
         <v>56</v>
       </c>
       <c r="G12" s="262"/>
@@ -11384,7 +11384,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P12" s="739"/>
+      <c r="P12" s="717"/>
       <c r="Q12" s="108" t="s">
         <v>335</v>
       </c>
@@ -11461,14 +11461,14 @@
       </c>
     </row>
     <row r="13" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="677"/>
+      <c r="A13" s="628"/>
       <c r="B13" s="583">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="626"/>
+      <c r="E13" s="682"/>
       <c r="F13" s="172">
         <v>0</v>
       </c>
@@ -11492,7 +11492,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P13" s="739"/>
+      <c r="P13" s="717"/>
       <c r="Q13" s="108" t="s">
         <v>335</v>
       </c>
@@ -11574,7 +11574,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P14" s="739"/>
+      <c r="P14" s="717"/>
       <c r="Q14" s="20"/>
       <c r="R14" s="200" t="s">
         <v>339</v>
@@ -11677,7 +11677,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P15" s="739"/>
+      <c r="P15" s="717"/>
       <c r="Q15" s="20"/>
       <c r="R15" s="200" t="s">
         <v>339</v>
@@ -11771,7 +11771,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P16" s="739"/>
+      <c r="P16" s="717"/>
       <c r="Q16" s="108" t="s">
         <v>335</v>
       </c>
@@ -11872,7 +11872,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P17" s="739"/>
+      <c r="P17" s="717"/>
       <c r="Q17" s="20"/>
       <c r="R17" s="2" t="s">
         <v>341</v>
@@ -11972,7 +11972,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P18" s="739"/>
+      <c r="P18" s="717"/>
       <c r="Q18" s="108" t="s">
         <v>335</v>
       </c>
@@ -12060,7 +12060,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P19" s="739"/>
+      <c r="P19" s="717"/>
       <c r="Q19" s="20"/>
       <c r="R19" s="2" t="s">
         <v>334</v>
@@ -12168,11 +12168,11 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P20" s="740"/>
+      <c r="P20" s="718"/>
       <c r="Q20" s="605" t="s">
         <v>335</v>
       </c>
-      <c r="R20" s="627"/>
+      <c r="R20" s="683"/>
       <c r="S20" s="534" t="s">
         <v>85</v>
       </c>
@@ -12434,7 +12434,7 @@
     </row>
     <row r="23" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="24"/>
-      <c r="E23" s="682" t="s">
+      <c r="E23" s="633" t="s">
         <v>289</v>
       </c>
       <c r="F23" s="180"/>
@@ -12539,7 +12539,7 @@
       <c r="C24" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="E24" s="683"/>
+      <c r="E24" s="634"/>
       <c r="F24" s="172"/>
       <c r="H24" s="42"/>
       <c r="J24" s="570" t="s">
@@ -12563,7 +12563,7 @@
       <c r="Q24" s="605" t="s">
         <v>335</v>
       </c>
-      <c r="R24" s="627"/>
+      <c r="R24" s="683"/>
       <c r="S24" s="534" t="s">
         <v>249</v>
       </c>
@@ -13229,8 +13229,8 @@
       <c r="AR31" s="508"/>
     </row>
     <row r="32" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="630"/>
-      <c r="B32" s="630"/>
+      <c r="A32" s="650"/>
+      <c r="B32" s="650"/>
       <c r="J32" s="571"/>
       <c r="K32" s="586"/>
       <c r="L32" s="580">
@@ -13427,9 +13427,7 @@
       </c>
     </row>
     <row r="34" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="21">
-        <v>5</v>
-      </c>
+      <c r="B34" s="21"/>
       <c r="C34" s="2" t="s">
         <v>257</v>
       </c>
@@ -13814,15 +13812,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="P4:P20"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="Q20:R20"/>
     <mergeCell ref="AM1:AO1"/>
     <mergeCell ref="X1:Y1"/>
     <mergeCell ref="AE1:AG1"/>
@@ -13834,6 +13823,15 @@
     <mergeCell ref="W2:W3"/>
     <mergeCell ref="T1:T3"/>
     <mergeCell ref="AK1:AK2"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="P4:P20"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="Q20:R20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13896,12 +13894,12 @@
       <c r="P1" s="38"/>
       <c r="S1" s="58">
         <f ca="1">TODAY()</f>
-        <v>45293</v>
+        <v>45294</v>
       </c>
       <c r="V1" s="603" t="s">
         <v>70</v>
       </c>
-      <c r="W1" s="627"/>
+      <c r="W1" s="683"/>
       <c r="X1" s="62" t="s">
         <v>101</v>
       </c>
@@ -13920,7 +13918,7 @@
       <c r="AC1" s="116" t="s">
         <v>190</v>
       </c>
-      <c r="AD1" s="752" t="s">
+      <c r="AD1" s="759" t="s">
         <v>211</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -13937,10 +13935,10 @@
       <c r="E2" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="751" t="s">
+      <c r="F2" s="790" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="779" t="s">
+      <c r="G2" s="747" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -13968,10 +13966,10 @@
       <c r="U2" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="V2" s="719" t="s">
+      <c r="V2" s="726" t="s">
         <v>120</v>
       </c>
-      <c r="W2" s="720"/>
+      <c r="W2" s="727"/>
       <c r="X2" s="64" t="s">
         <v>109</v>
       </c>
@@ -13990,7 +13988,7 @@
       <c r="AC2" s="117" t="s">
         <v>98</v>
       </c>
-      <c r="AD2" s="753"/>
+      <c r="AD2" s="760"/>
       <c r="AE2" s="64" t="s">
         <v>98</v>
       </c>
@@ -14009,8 +14007,8 @@
       <c r="E3" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="F3" s="679"/>
-      <c r="G3" s="780"/>
+      <c r="F3" s="630"/>
+      <c r="G3" s="748"/>
       <c r="H3" s="40" t="s">
         <v>80</v>
       </c>
@@ -14021,13 +14019,13 @@
         <v>81</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="789" t="s">
+      <c r="O3" s="757" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="771" t="s">
+      <c r="P3" s="778" t="s">
         <v>217</v>
       </c>
-      <c r="Q3" s="772"/>
+      <c r="Q3" s="779"/>
       <c r="S3" s="57" t="s">
         <v>218</v>
       </c>
@@ -14037,15 +14035,15 @@
       <c r="W3" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="AD3" s="753"/>
+      <c r="AD3" s="760"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="780"/>
+      <c r="G4" s="748"/>
       <c r="H4" s="6"/>
       <c r="L4" s="687" t="s">
         <v>82</v>
       </c>
-      <c r="O4" s="790"/>
+      <c r="O4" s="758"/>
       <c r="T4" s="55" t="s">
         <v>97</v>
       </c>
@@ -14059,8 +14057,8 @@
         <v>194</v>
       </c>
       <c r="Z4" s="605"/>
-      <c r="AA4" s="627"/>
-      <c r="AD4" s="753"/>
+      <c r="AA4" s="683"/>
+      <c r="AD4" s="760"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -14075,21 +14073,21 @@
       <c r="F5" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="G5" s="780"/>
+      <c r="G5" s="748"/>
       <c r="H5" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="K5" s="758" t="s">
+      <c r="K5" s="765" t="s">
         <v>215</v>
       </c>
-      <c r="L5" s="773"/>
+      <c r="L5" s="780"/>
       <c r="M5" s="2" t="s">
         <v>213</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>212</v>
       </c>
-      <c r="O5" s="790"/>
+      <c r="O5" s="758"/>
       <c r="P5" s="108" t="s">
         <v>214</v>
       </c>
@@ -14105,11 +14103,11 @@
       <c r="U5" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="Y5" s="761" t="s">
+      <c r="Y5" s="768" t="s">
         <v>282</v>
       </c>
-      <c r="Z5" s="762"/>
-      <c r="AD5" s="753"/>
+      <c r="Z5" s="769"/>
+      <c r="AD5" s="760"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -14119,16 +14117,16 @@
       <c r="E6" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="G6" s="780"/>
+      <c r="G6" s="748"/>
       <c r="H6" s="46" t="s">
         <v>80</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="759"/>
-      <c r="L6" s="773"/>
-      <c r="O6" s="790"/>
+      <c r="K6" s="766"/>
+      <c r="L6" s="780"/>
+      <c r="O6" s="758"/>
       <c r="T6" s="2" t="s">
         <v>100</v>
       </c>
@@ -14138,23 +14136,23 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="753"/>
+      <c r="AD6" s="760"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="780"/>
+      <c r="G7" s="748"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="759"/>
-      <c r="L7" s="773"/>
+      <c r="K7" s="766"/>
+      <c r="L7" s="780"/>
       <c r="N7" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="O7" s="790"/>
+      <c r="O7" s="758"/>
       <c r="P7" s="73"/>
       <c r="U7" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="753"/>
+      <c r="AD7" s="760"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -14167,7 +14165,7 @@
       <c r="F8" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="G8" s="780"/>
+      <c r="G8" s="748"/>
       <c r="H8" s="50" t="s">
         <v>75</v>
       </c>
@@ -14177,41 +14175,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="759"/>
-      <c r="L8" s="773"/>
-      <c r="O8" s="790"/>
+      <c r="K8" s="766"/>
+      <c r="L8" s="780"/>
+      <c r="O8" s="758"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="755" t="s">
+      <c r="S8" s="762" t="s">
         <v>210</v>
       </c>
-      <c r="T8" s="756"/>
-      <c r="U8" s="756"/>
-      <c r="V8" s="756"/>
-      <c r="W8" s="756"/>
-      <c r="X8" s="756"/>
-      <c r="Y8" s="756"/>
-      <c r="Z8" s="756"/>
-      <c r="AA8" s="756"/>
-      <c r="AB8" s="756"/>
-      <c r="AC8" s="757"/>
-      <c r="AD8" s="753"/>
+      <c r="T8" s="763"/>
+      <c r="U8" s="763"/>
+      <c r="V8" s="763"/>
+      <c r="W8" s="763"/>
+      <c r="X8" s="763"/>
+      <c r="Y8" s="763"/>
+      <c r="Z8" s="763"/>
+      <c r="AA8" s="763"/>
+      <c r="AB8" s="763"/>
+      <c r="AC8" s="764"/>
+      <c r="AD8" s="760"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="745"/>
-      <c r="G9" s="780"/>
+      <c r="C9" s="784"/>
+      <c r="G9" s="748"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="759"/>
-      <c r="L9" s="783" t="s">
+      <c r="K9" s="766"/>
+      <c r="L9" s="751" t="s">
         <v>216</v>
       </c>
-      <c r="M9" s="784"/>
-      <c r="N9" s="785"/>
-      <c r="O9" s="790"/>
+      <c r="M9" s="752"/>
+      <c r="N9" s="753"/>
+      <c r="O9" s="758"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="753"/>
+      <c r="AD9" s="760"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="746"/>
+      <c r="C10" s="785"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>87</v>
@@ -14219,7 +14217,7 @@
       <c r="F10" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="G10" s="780"/>
+      <c r="G10" s="748"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>80</v>
@@ -14227,33 +14225,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="759"/>
-      <c r="M10" s="748" t="s">
+      <c r="K10" s="766"/>
+      <c r="M10" s="787" t="s">
         <v>89</v>
       </c>
-      <c r="N10" s="749"/>
-      <c r="O10" s="749"/>
-      <c r="P10" s="749"/>
-      <c r="Q10" s="749"/>
-      <c r="R10" s="749"/>
-      <c r="S10" s="749"/>
-      <c r="T10" s="749"/>
-      <c r="U10" s="749"/>
-      <c r="V10" s="749"/>
-      <c r="W10" s="749"/>
-      <c r="X10" s="749"/>
-      <c r="Y10" s="749"/>
-      <c r="Z10" s="749"/>
-      <c r="AA10" s="749"/>
-      <c r="AB10" s="749"/>
-      <c r="AC10" s="750"/>
-      <c r="AD10" s="753"/>
+      <c r="N10" s="788"/>
+      <c r="O10" s="788"/>
+      <c r="P10" s="788"/>
+      <c r="Q10" s="788"/>
+      <c r="R10" s="788"/>
+      <c r="S10" s="788"/>
+      <c r="T10" s="788"/>
+      <c r="U10" s="788"/>
+      <c r="V10" s="788"/>
+      <c r="W10" s="788"/>
+      <c r="X10" s="788"/>
+      <c r="Y10" s="788"/>
+      <c r="Z10" s="788"/>
+      <c r="AA10" s="788"/>
+      <c r="AB10" s="788"/>
+      <c r="AC10" s="789"/>
+      <c r="AD10" s="760"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="747"/>
-      <c r="G11" s="780"/>
+      <c r="C11" s="786"/>
+      <c r="G11" s="748"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="759"/>
+      <c r="K11" s="766"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -14261,17 +14259,17 @@
       <c r="Y11" s="68" t="s">
         <v>120</v>
       </c>
-      <c r="Z11" s="769" t="s">
+      <c r="Z11" s="776" t="s">
         <v>120</v>
       </c>
-      <c r="AA11" s="770"/>
+      <c r="AA11" s="777"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>120</v>
       </c>
-      <c r="AD11" s="753"/>
+      <c r="AD11" s="760"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -14284,7 +14282,7 @@
       <c r="F12" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="G12" s="780"/>
+      <c r="G12" s="748"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>80</v>
@@ -14292,8 +14290,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="759"/>
-      <c r="L12" s="774" t="s">
+      <c r="K12" s="766"/>
+      <c r="L12" s="781" t="s">
         <v>92</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -14324,25 +14322,25 @@
         <v>115</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="763" t="s">
+      <c r="AA12" s="770" t="s">
         <v>125</v>
       </c>
-      <c r="AB12" s="764"/>
+      <c r="AB12" s="771"/>
       <c r="AC12" s="21" t="s">
         <v>230</v>
       </c>
-      <c r="AD12" s="753"/>
+      <c r="AD12" s="760"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="745"/>
-      <c r="G13" s="780"/>
-      <c r="K13" s="759"/>
-      <c r="L13" s="775"/>
+      <c r="C13" s="784"/>
+      <c r="G13" s="748"/>
+      <c r="K13" s="766"/>
+      <c r="L13" s="782"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="782" t="s">
+      <c r="Q13" s="750" t="s">
         <v>208</v>
       </c>
-      <c r="R13" s="644"/>
+      <c r="R13" s="639"/>
       <c r="S13" s="599"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
@@ -14351,17 +14349,17 @@
       <c r="X13" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="AA13" s="765"/>
-      <c r="AB13" s="766"/>
-      <c r="AD13" s="753"/>
+      <c r="AA13" s="772"/>
+      <c r="AB13" s="773"/>
+      <c r="AD13" s="760"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="C14" s="747"/>
+      <c r="C14" s="786"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="780"/>
+      <c r="G14" s="748"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -14369,8 +14367,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="759"/>
-      <c r="L14" s="775"/>
+      <c r="K14" s="766"/>
+      <c r="L14" s="782"/>
       <c r="M14" s="21" t="s">
         <v>110</v>
       </c>
@@ -14391,9 +14389,9 @@
       <c r="Y14" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="AA14" s="765"/>
-      <c r="AB14" s="766"/>
-      <c r="AD14" s="753"/>
+      <c r="AA14" s="772"/>
+      <c r="AB14" s="773"/>
+      <c r="AD14" s="760"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -14408,19 +14406,19 @@
       <c r="F15" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="G15" s="780"/>
+      <c r="G15" s="748"/>
       <c r="H15" s="2" t="s">
         <v>80</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="K15" s="759"/>
-      <c r="L15" s="776"/>
-      <c r="Q15" s="782" t="s">
+      <c r="K15" s="766"/>
+      <c r="L15" s="783"/>
+      <c r="Q15" s="750" t="s">
         <v>209</v>
       </c>
-      <c r="R15" s="644"/>
+      <c r="R15" s="639"/>
       <c r="S15" s="599"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
@@ -14429,14 +14427,14 @@
       <c r="X15" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="AA15" s="765"/>
-      <c r="AB15" s="766"/>
-      <c r="AD15" s="753"/>
+      <c r="AA15" s="772"/>
+      <c r="AB15" s="773"/>
+      <c r="AD15" s="760"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="780"/>
-      <c r="K16" s="759"/>
+      <c r="G16" s="748"/>
+      <c r="K16" s="766"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>108</v>
@@ -14455,24 +14453,24 @@
       <c r="Z16" s="76" t="s">
         <v>126</v>
       </c>
-      <c r="AA16" s="765"/>
-      <c r="AB16" s="766"/>
-      <c r="AD16" s="753"/>
+      <c r="AA16" s="772"/>
+      <c r="AB16" s="773"/>
+      <c r="AD16" s="760"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F17" s="777" t="s">
+      <c r="F17" s="745" t="s">
         <v>95</v>
       </c>
-      <c r="G17" s="780"/>
+      <c r="G17" s="748"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>80</v>
       </c>
-      <c r="K17" s="759"/>
+      <c r="K17" s="766"/>
       <c r="S17" s="599"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
@@ -14480,9 +14478,9 @@
       <c r="X17" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA17" s="765"/>
-      <c r="AB17" s="766"/>
-      <c r="AD17" s="753"/>
+      <c r="AA17" s="772"/>
+      <c r="AB17" s="773"/>
+      <c r="AD17" s="760"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -14492,15 +14490,15 @@
       <c r="E18" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F18" s="778"/>
-      <c r="G18" s="780"/>
+      <c r="F18" s="746"/>
+      <c r="G18" s="748"/>
       <c r="H18" s="108" t="s">
         <v>75</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="K18" s="759"/>
+      <c r="K18" s="766"/>
       <c r="O18" s="64" t="s">
         <v>114</v>
       </c>
@@ -14511,42 +14509,39 @@
       <c r="X18" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AA18" s="767"/>
-      <c r="AB18" s="768"/>
-      <c r="AD18" s="753"/>
+      <c r="AA18" s="774"/>
+      <c r="AB18" s="775"/>
+      <c r="AD18" s="760"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>207</v>
       </c>
-      <c r="G19" s="781"/>
-      <c r="K19" s="760"/>
+      <c r="G19" s="749"/>
+      <c r="K19" s="767"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="786" t="s">
+      <c r="R19" s="754" t="s">
         <v>123</v>
       </c>
-      <c r="S19" s="787"/>
-      <c r="T19" s="788"/>
+      <c r="S19" s="755"/>
+      <c r="T19" s="756"/>
       <c r="V19" s="77" t="s">
         <v>114</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="AD19" s="754"/>
+      <c r="AD19" s="761"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G19"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="S12:S18"/>
-    <mergeCell ref="O3:O9"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="M10:AC10"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="AD1:AD19"/>
     <mergeCell ref="S8:AC8"/>
     <mergeCell ref="K5:K19"/>
@@ -14558,11 +14553,14 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L12:L15"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="M10:AC10"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="S12:S18"/>
+    <mergeCell ref="O3:O9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>